<commit_message>
Alterada a meta no Business Case, Criado novos gráficos(Carta de Controle A I-AM , Sequencial, Histrograma e Temporal por categoria)
</commit_message>
<xml_diff>
--- a/TRE_Dados_MapaRaciocinio.xlsx
+++ b/TRE_Dados_MapaRaciocinio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Historicos x Categoria" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t>Categoria</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>Conclusão</t>
   </si>
 </sst>
 </file>
@@ -221,7 +224,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -269,7 +272,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -336,11 +339,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -369,9 +421,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,15 +452,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:colOff>328612</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2838450</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>3228975</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -423,8 +484,173 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="323850" y="3048000"/>
-          <a:ext cx="5810250" cy="3873500"/>
+          <a:off x="328612" y="2981325"/>
+          <a:ext cx="6196013" cy="4130675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2971800</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="781050" y="7448550"/>
+          <a:ext cx="5486400" cy="3657600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2933700</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="742950" y="11468100"/>
+          <a:ext cx="5486400" cy="3657600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>485777</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="723900" y="15763874"/>
+          <a:ext cx="7286627" cy="4857751"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -737,7 +963,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,7 +991,7 @@
       </c>
       <c r="D1" s="12">
         <f ca="1">TODAY()</f>
-        <v>42677</v>
+        <v>42678</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>11</v>
@@ -1288,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B12"/>
+  <dimension ref="A2:J94"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,7 +1526,7 @@
     <col min="2" max="2" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
@@ -1396,6 +1622,382 @@
         <f>AVERAGEIF('Dados Historicos x Categoria'!$A$4:$A$21,'Dados Historicos x Categoria'!A18,'Dados Historicos x Categoria'!$E$4:$E$21)</f>
         <v>247</v>
       </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="23"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="24"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="26"/>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="24"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="24"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="26"/>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="24"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="24"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="26"/>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="24"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="26"/>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="24"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="26"/>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="24"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="26"/>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="24"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="26"/>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="24"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="26"/>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="24"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="26"/>
+    </row>
+    <row r="29" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="27"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="29"/>
+    </row>
+    <row r="37" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="23"/>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C39" s="24"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="26"/>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="24"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="26"/>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="24"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="26"/>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="24"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="26"/>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="24"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="26"/>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="24"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="26"/>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="24"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="26"/>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="24"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="26"/>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C47" s="24"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="26"/>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C48" s="24"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="26"/>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="24"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="26"/>
+    </row>
+    <row r="50" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="27"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="29"/>
+    </row>
+    <row r="58" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C59" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="23"/>
+    </row>
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C60" s="24"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="26"/>
+    </row>
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C61" s="24"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="26"/>
+    </row>
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C62" s="24"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="26"/>
+    </row>
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C63" s="24"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="25"/>
+      <c r="F63" s="25"/>
+      <c r="G63" s="26"/>
+    </row>
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C64" s="24"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="25"/>
+      <c r="G64" s="26"/>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C65" s="24"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="25"/>
+      <c r="G65" s="26"/>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C66" s="24"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="25"/>
+      <c r="G66" s="26"/>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C67" s="24"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="25"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="26"/>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C68" s="24"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="25"/>
+      <c r="F68" s="25"/>
+      <c r="G68" s="26"/>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C69" s="24"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="25"/>
+      <c r="G69" s="26"/>
+    </row>
+    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C70" s="24"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="25"/>
+      <c r="F70" s="25"/>
+      <c r="G70" s="26"/>
+    </row>
+    <row r="71" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C71" s="27"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="28"/>
+      <c r="G71" s="29"/>
+    </row>
+    <row r="81" spans="6:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F82" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="G82" s="22"/>
+      <c r="H82" s="22"/>
+      <c r="I82" s="22"/>
+      <c r="J82" s="23"/>
+    </row>
+    <row r="83" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F83" s="24"/>
+      <c r="G83" s="25"/>
+      <c r="H83" s="25"/>
+      <c r="I83" s="25"/>
+      <c r="J83" s="26"/>
+    </row>
+    <row r="84" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F84" s="24"/>
+      <c r="G84" s="25"/>
+      <c r="H84" s="25"/>
+      <c r="I84" s="25"/>
+      <c r="J84" s="26"/>
+    </row>
+    <row r="85" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F85" s="24"/>
+      <c r="G85" s="25"/>
+      <c r="H85" s="25"/>
+      <c r="I85" s="25"/>
+      <c r="J85" s="26"/>
+    </row>
+    <row r="86" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F86" s="24"/>
+      <c r="G86" s="25"/>
+      <c r="H86" s="25"/>
+      <c r="I86" s="25"/>
+      <c r="J86" s="26"/>
+    </row>
+    <row r="87" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F87" s="24"/>
+      <c r="G87" s="25"/>
+      <c r="H87" s="25"/>
+      <c r="I87" s="25"/>
+      <c r="J87" s="26"/>
+    </row>
+    <row r="88" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F88" s="24"/>
+      <c r="G88" s="25"/>
+      <c r="H88" s="25"/>
+      <c r="I88" s="25"/>
+      <c r="J88" s="26"/>
+    </row>
+    <row r="89" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F89" s="24"/>
+      <c r="G89" s="25"/>
+      <c r="H89" s="25"/>
+      <c r="I89" s="25"/>
+      <c r="J89" s="26"/>
+    </row>
+    <row r="90" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F90" s="24"/>
+      <c r="G90" s="25"/>
+      <c r="H90" s="25"/>
+      <c r="I90" s="25"/>
+      <c r="J90" s="26"/>
+    </row>
+    <row r="91" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F91" s="24"/>
+      <c r="G91" s="25"/>
+      <c r="H91" s="25"/>
+      <c r="I91" s="25"/>
+      <c r="J91" s="26"/>
+    </row>
+    <row r="92" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F92" s="24"/>
+      <c r="G92" s="25"/>
+      <c r="H92" s="25"/>
+      <c r="I92" s="25"/>
+      <c r="J92" s="26"/>
+    </row>
+    <row r="93" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F93" s="24"/>
+      <c r="G93" s="25"/>
+      <c r="H93" s="25"/>
+      <c r="I93" s="25"/>
+      <c r="J93" s="26"/>
+    </row>
+    <row r="94" spans="6:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F94" s="27"/>
+      <c r="G94" s="28"/>
+      <c r="H94" s="28"/>
+      <c r="I94" s="28"/>
+      <c r="J94" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1407,7 +2009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adicionado 2 novas TABs no documento Mapa de Raciocionio , ATA de Reunioes e  Controle do Projeto
</commit_message>
<xml_diff>
--- a/TRE_Dados_MapaRaciocinio.xlsx
+++ b/TRE_Dados_MapaRaciocinio.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -9,14 +9,16 @@
   <sheets>
     <sheet name="Dados Historicos x Categoria" sheetId="1" r:id="rId1"/>
     <sheet name="PARETO" sheetId="2" r:id="rId2"/>
-    <sheet name="PROCESSO PADRÃO" sheetId="4" r:id="rId3"/>
+    <sheet name="Ata de Reuniões" sheetId="5" r:id="rId3"/>
+    <sheet name="PROCESSO PADRÃO" sheetId="4" r:id="rId4"/>
+    <sheet name="Controle do Projeto" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="98">
   <si>
     <t>Categoria</t>
   </si>
@@ -217,16 +219,112 @@
   </si>
   <si>
     <t>Conclusão</t>
+  </si>
+  <si>
+    <t>Sl#</t>
+  </si>
+  <si>
+    <t>Data da Reunião</t>
+  </si>
+  <si>
+    <t>Participanates</t>
+  </si>
+  <si>
+    <t>Agenda Geral/Topico</t>
+  </si>
+  <si>
+    <t>Duração
+(hrs)</t>
+  </si>
+  <si>
+    <t>Action Items</t>
+  </si>
+  <si>
+    <t>Resp</t>
+  </si>
+  <si>
+    <t>Data Prevista</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Comentários/Notas</t>
+  </si>
+  <si>
+    <t>27/10/2016</t>
+  </si>
+  <si>
+    <t>Ruhan, André, Pedro, Ivanilda, Silmara e Hélcio</t>
+  </si>
+  <si>
+    <t>Discussão acerca do problema principal referente a contração/aquisição e preenchimento do documento Business Case</t>
+  </si>
+  <si>
+    <t>*Meta de redução ainda precisa de análise de dados históricos para coleta de médias. A partir destas será possível obter uma meta mais coerente.</t>
+  </si>
+  <si>
+    <t>*Ruhan, Ivis , Andre - Criar planilha para organizar dados históricos das diversas categorias de contratações
+*Ivanilda , Silmara e Hélcio - Coleta de dados histórios desde 2012 das mais diversas categorias</t>
+  </si>
+  <si>
+    <t>Em progresso</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Schedule Chart                  Plan                  Actual</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Reunião Inicial</t>
+  </si>
+  <si>
+    <t>27/10/16</t>
+  </si>
+  <si>
+    <t>Define</t>
+  </si>
+  <si>
+    <t>Measure</t>
+  </si>
+  <si>
+    <t>Analyze</t>
+  </si>
+  <si>
+    <t>Improve</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Status Geral</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="165" formatCode="dd\-mm\-yy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,8 +349,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,8 +385,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -388,11 +508,230 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -433,15 +772,151 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -672,10 +1147,359 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4924425" y="523875"/>
+          <a:ext cx="161925" cy="57150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0C0C0" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="22"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4943475" y="619125"/>
+          <a:ext cx="123825" cy="47625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0000FF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="12"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9527</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>581026</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 11"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4943476" y="771527"/>
+          <a:ext cx="1181100" cy="47624"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0C0C0" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="22"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 12"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6762750" y="981076"/>
+          <a:ext cx="1200150" cy="57149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0C0C0" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="22"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 13"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8334375" y="2752725"/>
+          <a:ext cx="1504950" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0000FF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="12"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Rectangle 14"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6943725" y="38100"/>
+          <a:ext cx="152400" cy="95250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0C0C0" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="22"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Rectangle 15"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7991475" y="38100"/>
+          <a:ext cx="152400" cy="104775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0000FF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="12"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>132522</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>132522</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Rectangle 16"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4943475" y="838199"/>
+          <a:ext cx="122997" cy="56323"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0000FF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="12"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -713,9 +1537,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -750,7 +1574,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -785,7 +1609,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -963,20 +1787,20 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.125" customWidth="1"/>
-    <col min="2" max="2" width="53.125" customWidth="1"/>
-    <col min="3" max="4" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" customWidth="1"/>
+    <col min="3" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="2.875" customWidth="1"/>
-    <col min="8" max="8" width="12.625" customWidth="1"/>
-    <col min="9" max="9" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
@@ -1516,17 +2340,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J94"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.25" customWidth="1"/>
-    <col min="2" max="2" width="46.5" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
@@ -2006,6 +2830,92 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="12">
+        <v>42440</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2016,8 +2926,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.25" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2045,4 +2955,442 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="38"/>
+      <c r="G1" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+    </row>
+    <row r="2" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="41"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="46">
+        <v>42690</v>
+      </c>
+      <c r="H2" s="46">
+        <v>42720</v>
+      </c>
+      <c r="I2" s="46">
+        <v>42751</v>
+      </c>
+      <c r="J2" s="46">
+        <v>42782</v>
+      </c>
+      <c r="K2" s="46">
+        <v>42810</v>
+      </c>
+      <c r="L2" s="46">
+        <v>42841</v>
+      </c>
+      <c r="M2" s="46">
+        <v>42871</v>
+      </c>
+      <c r="N2" s="46">
+        <v>42902</v>
+      </c>
+      <c r="O2" s="46">
+        <v>42932</v>
+      </c>
+      <c r="P2" s="46">
+        <v>42963</v>
+      </c>
+      <c r="Q2" s="46">
+        <v>42994</v>
+      </c>
+      <c r="R2" s="46">
+        <v>43024</v>
+      </c>
+      <c r="S2" s="46">
+        <v>43055</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="47">
+        <v>1</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="47"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="52"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="53">
+        <v>2</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="55"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="53">
+        <v>3</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="55"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="52"/>
+      <c r="S5" s="52"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="53">
+        <v>4</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="52"/>
+      <c r="Q6" s="52"/>
+      <c r="R6" s="52"/>
+      <c r="S6" s="52"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="53">
+        <v>5</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="55"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="52"/>
+      <c r="S7" s="52"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="53">
+        <v>6</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="55"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="52"/>
+      <c r="S8" s="52"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="53">
+        <v>7</v>
+      </c>
+      <c r="B9" s="54"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="52"/>
+      <c r="S9" s="52"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="53">
+        <v>8</v>
+      </c>
+      <c r="B10" s="54"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="52"/>
+      <c r="Q10" s="52"/>
+      <c r="R10" s="52"/>
+      <c r="S10" s="52"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="53">
+        <v>9</v>
+      </c>
+      <c r="B11" s="54"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="52"/>
+      <c r="Q11" s="52"/>
+      <c r="R11" s="52"/>
+      <c r="S11" s="52"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="53">
+        <v>10</v>
+      </c>
+      <c r="B12" s="54"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="52"/>
+      <c r="R12" s="52"/>
+      <c r="S12" s="52"/>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="53">
+        <v>11</v>
+      </c>
+      <c r="B13" s="54"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="52"/>
+      <c r="Q13" s="52"/>
+      <c r="R13" s="52"/>
+      <c r="S13" s="52"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="60">
+        <v>12</v>
+      </c>
+      <c r="B14" s="61"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="65"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="52"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="52"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="67"/>
+      <c r="B15" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" s="71"/>
+      <c r="G15" s="67">
+        <v>30</v>
+      </c>
+      <c r="H15" s="72">
+        <v>30</v>
+      </c>
+      <c r="I15" s="72"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="72"/>
+      <c r="L15" s="72"/>
+      <c r="M15" s="72"/>
+      <c r="N15" s="72"/>
+      <c r="O15" s="73"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="73"/>
+      <c r="R15" s="73"/>
+      <c r="S15" s="73"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ATa de reuniao atualizada. Alterado o nome da Aba PARETO. Inclusao do Grafico Histograma.
</commit_message>
<xml_diff>
--- a/TRE_Dados_MapaRaciocinio.xlsx
+++ b/TRE_Dados_MapaRaciocinio.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Historicos x Categoria" sheetId="1" r:id="rId1"/>
-    <sheet name="PARETO" sheetId="2" r:id="rId2"/>
-    <sheet name="Ata de Reuniões" sheetId="5" r:id="rId3"/>
+    <sheet name="Graficos" sheetId="2" r:id="rId2"/>
+    <sheet name="Atas das Reuniões" sheetId="5" r:id="rId3"/>
     <sheet name="PROCESSO PADRÃO" sheetId="4" r:id="rId4"/>
     <sheet name="Controle do Projeto" sheetId="6" r:id="rId5"/>
   </sheets>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="114">
   <si>
     <t>Categoria</t>
   </si>
@@ -261,16 +261,6 @@
     <t>Discussão acerca do problema principal referente a contração/aquisição e preenchimento do documento Business Case</t>
   </si>
   <si>
-    <t>*Meta de redução ainda precisa de análise de dados históricos para coleta de médias. A partir destas será possível obter uma meta mais coerente.</t>
-  </si>
-  <si>
-    <t>*Ruhan, Ivis , Andre - Criar planilha para organizar dados históricos das diversas categorias de contratações
-*Ivanilda , Silmara e Hélcio - Coleta de dados histórios desde 2012 das mais diversas categorias</t>
-  </si>
-  <si>
-    <t>Em progresso</t>
-  </si>
-  <si>
     <t>Activity</t>
   </si>
   <si>
@@ -314,6 +304,65 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>*Definir a Meta de redução ainda fazendo análise de dados históricos para coleta de médias. A partir destas será possível obter uma meta mais coerente.</t>
+  </si>
+  <si>
+    <t>Coleta de dados adicionais, para reajuste das médias.
+(coletar outos itens que não sejam Manutenção e Jardinagem)</t>
+  </si>
+  <si>
+    <t>16/11/2016</t>
+  </si>
+  <si>
+    <t>Ruhan, Ivis, Andre</t>
+  </si>
+  <si>
+    <t>Ivanilda , Silmara e Hélcio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t>Pendente</t>
+  </si>
+  <si>
+    <t>Silmara</t>
+  </si>
+  <si>
+    <t>Coleta dos principais processos à serem utilizados como exemplo para analise dos Tempos Médios.</t>
+  </si>
+  <si>
+    <t>Realizar os cálculos dos tempos médios dos processos selecionados</t>
+  </si>
+  <si>
+    <t>Fazer uma lista com os processos mais importantes.</t>
+  </si>
+  <si>
+    <t>Apresentar os Graficos com os resultados e resaltar a importancia da escolha de um processo simples.</t>
+  </si>
+  <si>
+    <t>Ruhan, André, Ivis, Silmara</t>
+  </si>
+  <si>
+    <t>Concluído</t>
+  </si>
+  <si>
+    <t>Revisar nome correto da categoria "Aquisição - Consumo"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar planilha para organizar dados históricos das diversas categorias de contratações
+</t>
+  </si>
+  <si>
+    <t>Coleta de dados histórios desde 2012 das mais diversas categorias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruhan, Ivis , Andre </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivanilda , Silmara e Hélcio </t>
   </si>
 </sst>
 </file>
@@ -366,7 +415,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,8 +440,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -726,12 +781,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -784,12 +863,117 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -799,110 +983,36 @@
     <xf numFmtId="165" fontId="5" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1126,6 +1236,61 @@
         <a:xfrm>
           <a:off x="723900" y="15763874"/>
           <a:ext cx="7286627" cy="4857751"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504824</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagem 49"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="761999" y="21107400"/>
+          <a:ext cx="6334125" cy="4826000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1785,9 +1950,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,7 +1980,7 @@
       </c>
       <c r="D1" s="12">
         <f ca="1">TODAY()</f>
-        <v>42678</v>
+        <v>42681</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>11</v>
@@ -2100,7 +2265,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="76" t="s">
         <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2340,8 +2505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J94"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2831,21 +2996,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="77"/>
+    <col min="2" max="2" width="10.7109375" style="77" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="77" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="77" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="77"/>
+    <col min="6" max="6" width="29.42578125" style="77" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" style="77" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="77" customWidth="1"/>
+    <col min="9" max="9" width="12" style="77" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" style="77" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -2880,37 +3048,209 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:10" s="74" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="78">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="75" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="75">
         <v>2</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2" s="12">
+      <c r="F2" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="79">
         <v>42440</v>
       </c>
-      <c r="I2" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="J2" s="1"/>
+      <c r="I2" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" s="51"/>
+    </row>
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="81"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" s="79">
+        <v>42440</v>
+      </c>
+      <c r="I3" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="J3" s="51"/>
+    </row>
+    <row r="4" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="75">
+        <v>2</v>
+      </c>
+      <c r="B4" s="82">
+        <v>42440</v>
+      </c>
+      <c r="C4" s="75" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="78">
+        <v>2</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="79">
+        <v>42440</v>
+      </c>
+      <c r="I4" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="J4" s="51"/>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="78"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="58" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="84">
+        <v>42440</v>
+      </c>
+      <c r="I5" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="J5" s="58"/>
+    </row>
+    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="75">
+        <v>3</v>
+      </c>
+      <c r="B6" s="83">
+        <v>42624</v>
+      </c>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6" s="79">
+        <v>42624</v>
+      </c>
+      <c r="I6" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="J6" s="51"/>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="75"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="H7" s="79">
+        <v>42624</v>
+      </c>
+      <c r="I7" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" s="51"/>
+    </row>
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="75"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" s="79">
+        <v>42624</v>
+      </c>
+      <c r="I8" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" s="51"/>
+    </row>
+    <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="51">
+        <v>4</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="J9" s="51"/>
     </row>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2920,7 +3260,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2971,417 +3311,417 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="69" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="71" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="73"/>
+      <c r="G1" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+    </row>
+    <row r="2" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="68"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37" t="s">
+      <c r="D2" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="39" t="s">
+      <c r="E2" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="39">
+        <v>42690</v>
+      </c>
+      <c r="H2" s="39">
+        <v>42720</v>
+      </c>
+      <c r="I2" s="39">
+        <v>42751</v>
+      </c>
+      <c r="J2" s="39">
+        <v>42782</v>
+      </c>
+      <c r="K2" s="39">
+        <v>42810</v>
+      </c>
+      <c r="L2" s="39">
+        <v>42841</v>
+      </c>
+      <c r="M2" s="39">
+        <v>42871</v>
+      </c>
+      <c r="N2" s="39">
+        <v>42902</v>
+      </c>
+      <c r="O2" s="39">
+        <v>42932</v>
+      </c>
+      <c r="P2" s="39">
+        <v>42963</v>
+      </c>
+      <c r="Q2" s="39">
+        <v>42994</v>
+      </c>
+      <c r="R2" s="39">
+        <v>43024</v>
+      </c>
+      <c r="S2" s="39">
+        <v>43055</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="40">
+        <v>1</v>
+      </c>
+      <c r="B3" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-    </row>
-    <row r="2" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="43" t="s">
+      <c r="C3" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D3" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="40"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="46">
+        <v>2</v>
+      </c>
+      <c r="B4" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="G2" s="46">
-        <v>42690</v>
-      </c>
-      <c r="H2" s="46">
-        <v>42720</v>
-      </c>
-      <c r="I2" s="46">
-        <v>42751</v>
-      </c>
-      <c r="J2" s="46">
-        <v>42782</v>
-      </c>
-      <c r="K2" s="46">
-        <v>42810</v>
-      </c>
-      <c r="L2" s="46">
-        <v>42841</v>
-      </c>
-      <c r="M2" s="46">
-        <v>42871</v>
-      </c>
-      <c r="N2" s="46">
-        <v>42902</v>
-      </c>
-      <c r="O2" s="46">
-        <v>42932</v>
-      </c>
-      <c r="P2" s="46">
-        <v>42963</v>
-      </c>
-      <c r="Q2" s="46">
-        <v>42994</v>
-      </c>
-      <c r="R2" s="46">
-        <v>43024</v>
-      </c>
-      <c r="S2" s="46">
-        <v>43055</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47">
-        <v>1</v>
-      </c>
-      <c r="B3" s="48" t="s">
+      <c r="C4" s="48"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="46">
+        <v>3</v>
+      </c>
+      <c r="B5" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="46">
+        <v>4</v>
+      </c>
+      <c r="B6" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53">
-        <v>2</v>
-      </c>
-      <c r="B4" s="54" t="s">
+      <c r="C6" s="48"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="46">
+        <v>5</v>
+      </c>
+      <c r="B7" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="52"/>
-      <c r="R4" s="52"/>
-      <c r="S4" s="52"/>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53">
-        <v>3</v>
-      </c>
-      <c r="B5" s="54" t="s">
+      <c r="C7" s="48"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="46">
+        <v>6</v>
+      </c>
+      <c r="B8" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="52"/>
-      <c r="R5" s="52"/>
-      <c r="S5" s="52"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="53">
-        <v>4</v>
-      </c>
-      <c r="B6" s="54" t="s">
+      <c r="C8" s="48"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="45"/>
+      <c r="S8" s="45"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="46">
+        <v>7</v>
+      </c>
+      <c r="B9" s="47"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="45"/>
+      <c r="Q9" s="45"/>
+      <c r="R9" s="45"/>
+      <c r="S9" s="45"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="46">
+        <v>8</v>
+      </c>
+      <c r="B10" s="47"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="45"/>
+      <c r="Q10" s="45"/>
+      <c r="R10" s="45"/>
+      <c r="S10" s="45"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="46">
+        <v>9</v>
+      </c>
+      <c r="B11" s="47"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="45"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="46">
+        <v>10</v>
+      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="46">
+        <v>11</v>
+      </c>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="52"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="53">
+        <v>12</v>
+      </c>
+      <c r="B14" s="54"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="59"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="60"/>
+      <c r="B15" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="52"/>
-      <c r="S6" s="52"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="53">
-        <v>5</v>
-      </c>
-      <c r="B7" s="54" t="s">
+      <c r="C15" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="52"/>
-      <c r="S7" s="52"/>
-    </row>
-    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="53">
-        <v>6</v>
-      </c>
-      <c r="B8" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="58"/>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="59"/>
-      <c r="P8" s="52"/>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="52"/>
-      <c r="S8" s="52"/>
-    </row>
-    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="53">
-        <v>7</v>
-      </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="58"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
-    </row>
-    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="53">
-        <v>8</v>
-      </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="52"/>
-      <c r="Q10" s="52"/>
-      <c r="R10" s="52"/>
-      <c r="S10" s="52"/>
-    </row>
-    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="53">
-        <v>9</v>
-      </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="59"/>
-      <c r="P11" s="52"/>
-      <c r="Q11" s="52"/>
-      <c r="R11" s="52"/>
-      <c r="S11" s="52"/>
-    </row>
-    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="53">
-        <v>10</v>
-      </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="59"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="52"/>
-      <c r="S12" s="52"/>
-    </row>
-    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="53">
-        <v>11</v>
-      </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="58"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="52"/>
-      <c r="R13" s="52"/>
-      <c r="S13" s="52"/>
-    </row>
-    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="60">
-        <v>12</v>
-      </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="65"/>
-      <c r="O14" s="66"/>
-      <c r="P14" s="52"/>
-      <c r="Q14" s="52"/>
-      <c r="R14" s="52"/>
-      <c r="S14" s="52"/>
-    </row>
-    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="67"/>
-      <c r="B15" s="68" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" s="69" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70" t="s">
-        <v>97</v>
-      </c>
-      <c r="F15" s="71"/>
-      <c r="G15" s="67">
+      <c r="D15" s="63"/>
+      <c r="E15" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="64"/>
+      <c r="G15" s="60">
         <v>30</v>
       </c>
-      <c r="H15" s="72">
+      <c r="H15" s="65">
         <v>30</v>
       </c>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="72"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="72"/>
-      <c r="N15" s="72"/>
-      <c r="O15" s="73"/>
-      <c r="P15" s="73"/>
-      <c r="Q15" s="73"/>
-      <c r="R15" s="73"/>
-      <c r="S15" s="73"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="65"/>
+      <c r="N15" s="65"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="66"/>
+      <c r="Q15" s="66"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Adicionado todas as conclusoes para todos os graficos
</commit_message>
<xml_diff>
--- a/TRE_Dados_MapaRaciocinio.xlsx
+++ b/TRE_Dados_MapaRaciocinio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Historicos x Categoria" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="118">
   <si>
     <t>Categoria</t>
   </si>
@@ -216,9 +216,6 @@
   </si>
   <si>
     <t>c</t>
-  </si>
-  <si>
-    <t>Conclusão</t>
   </si>
   <si>
     <t>Sl#</t>
@@ -363,6 +360,26 @@
   </si>
   <si>
     <t xml:space="preserve">Ivanilda , Silmara e Hélcio </t>
+  </si>
+  <si>
+    <t>Conclusão 
+A partir da análise de 18 processos de contratações descritos acima e na aba Dados Históricos x Categoria , conseguimos identificar um tempo total  de contratação de 3108 dias ou  equivalente à 8 anos caso não fossem conduzidos em paralelo. É possível observar também que os processos mais críticos são de aquisição de bens permanentes com tempo médio de 420 a 560 dias de contratação.</t>
+  </si>
+  <si>
+    <t>Conclusão 
+A partir desta carta  CEP - Análise de Capacidade de processo, é possível observar que o processo ainda  pode aceitar um tempo limite de 784 dias, dado o fato que não estabelecemos nenhum limite superior nem um inferior.</t>
+  </si>
+  <si>
+    <t>Conclusão
+Este gráfico nos apresenta de forma mais detalhada os registros dos tempos médios no tempo</t>
+  </si>
+  <si>
+    <t>Conclusão
+Este gráfico nos apresenta de forma mais detalhada por categoria de contratação os registros dos tempos médios no tempo</t>
+  </si>
+  <si>
+    <t>Conclusão
+O histrograma ao lado mostra a frequência de processos e seus respectivos tempos médios. Pode-se observar que  6 processos estão entre  300 e 400 dias, sendo que a média geral encontra-se em 340 dias</t>
   </si>
 </sst>
 </file>
@@ -447,7 +464,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -805,12 +822,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -842,15 +896,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -962,57 +1008,103 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1042,10 +1134,10 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3228975</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:rowOff>53975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1093,13 +1185,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2971800</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1148,13 +1240,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2933700</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>104</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1203,14 +1295,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>485777</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1254,22 +1346,17 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>107</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>504824</xdr:colOff>
-      <xdr:row>132</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="6334125" cy="4826000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Imagem 49"/>
+        <xdr:cNvPr id="9" name="Imagem 49"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1289,7 +1376,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="761999" y="21107400"/>
+          <a:off x="761999" y="29689425"/>
           <a:ext cx="6334125" cy="4826000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1308,7 +1395,7 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2265,7 +2352,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="76" t="s">
+      <c r="A18" s="60" t="s">
         <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2503,10 +2590,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J94"/>
+  <dimension ref="A2:J148"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="G127" sqref="G127"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2614,381 +2701,594 @@
     </row>
     <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="23"/>
+      <c r="C17" s="82" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="80"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="26"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="24"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="26"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="80"/>
+      <c r="G21" s="80"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="26"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="24"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="26"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="24"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="26"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="24"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="26"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="80"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="24"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="26"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="80"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="24"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="26"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="80"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="24"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="26"/>
-    </row>
-    <row r="29" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="27"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="29"/>
-    </row>
-    <row r="37" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="23"/>
-    </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="24"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="26"/>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="24"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="26"/>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="24"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="26"/>
-    </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="24"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="26"/>
-    </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="24"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="26"/>
-    </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="24"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="26"/>
-    </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="24"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="26"/>
-    </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="24"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="26"/>
-    </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="24"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="26"/>
-    </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C48" s="24"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="26"/>
-    </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C49" s="24"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="26"/>
-    </row>
-    <row r="50" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="27"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="29"/>
-    </row>
-    <row r="58" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="23"/>
-    </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C60" s="24"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="26"/>
-    </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C61" s="24"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="26"/>
-    </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="24"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="26"/>
-    </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="24"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="26"/>
-    </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C64" s="24"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="26"/>
-    </row>
+      <c r="C28" s="80"/>
+      <c r="D28" s="80"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="80"/>
+      <c r="G28" s="80"/>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="80"/>
+      <c r="D29" s="80"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="80"/>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="80"/>
+      <c r="D30" s="80"/>
+      <c r="E30" s="80"/>
+      <c r="F30" s="80"/>
+      <c r="G30" s="80"/>
+    </row>
+    <row r="38" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E39" s="89" t="s">
+        <v>117</v>
+      </c>
+      <c r="F39" s="79"/>
+      <c r="G39" s="79"/>
+      <c r="H39" s="79"/>
+      <c r="I39" s="83"/>
+    </row>
+    <row r="40" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E40" s="84"/>
+      <c r="F40" s="80"/>
+      <c r="G40" s="80"/>
+      <c r="H40" s="80"/>
+      <c r="I40" s="85"/>
+    </row>
+    <row r="41" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E41" s="84"/>
+      <c r="F41" s="80"/>
+      <c r="G41" s="80"/>
+      <c r="H41" s="80"/>
+      <c r="I41" s="85"/>
+    </row>
+    <row r="42" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E42" s="84"/>
+      <c r="F42" s="80"/>
+      <c r="G42" s="80"/>
+      <c r="H42" s="80"/>
+      <c r="I42" s="85"/>
+    </row>
+    <row r="43" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E43" s="84"/>
+      <c r="F43" s="80"/>
+      <c r="G43" s="80"/>
+      <c r="H43" s="80"/>
+      <c r="I43" s="85"/>
+    </row>
+    <row r="44" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E44" s="84"/>
+      <c r="F44" s="80"/>
+      <c r="G44" s="80"/>
+      <c r="H44" s="80"/>
+      <c r="I44" s="85"/>
+    </row>
+    <row r="45" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E45" s="84"/>
+      <c r="F45" s="80"/>
+      <c r="G45" s="80"/>
+      <c r="H45" s="80"/>
+      <c r="I45" s="85"/>
+    </row>
+    <row r="46" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E46" s="84"/>
+      <c r="F46" s="80"/>
+      <c r="G46" s="80"/>
+      <c r="H46" s="80"/>
+      <c r="I46" s="85"/>
+    </row>
+    <row r="47" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E47" s="84"/>
+      <c r="F47" s="80"/>
+      <c r="G47" s="80"/>
+      <c r="H47" s="80"/>
+      <c r="I47" s="85"/>
+    </row>
+    <row r="48" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E48" s="84"/>
+      <c r="F48" s="80"/>
+      <c r="G48" s="80"/>
+      <c r="H48" s="80"/>
+      <c r="I48" s="85"/>
+    </row>
+    <row r="49" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E49" s="84"/>
+      <c r="F49" s="80"/>
+      <c r="G49" s="80"/>
+      <c r="H49" s="80"/>
+      <c r="I49" s="85"/>
+    </row>
+    <row r="50" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E50" s="84"/>
+      <c r="F50" s="80"/>
+      <c r="G50" s="80"/>
+      <c r="H50" s="80"/>
+      <c r="I50" s="85"/>
+    </row>
+    <row r="51" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E51" s="86"/>
+      <c r="F51" s="87"/>
+      <c r="G51" s="87"/>
+      <c r="H51" s="87"/>
+      <c r="I51" s="88"/>
+    </row>
+    <row r="64" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="24"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="26"/>
+      <c r="C65" s="89" t="s">
+        <v>114</v>
+      </c>
+      <c r="D65" s="79"/>
+      <c r="E65" s="79"/>
+      <c r="F65" s="79"/>
+      <c r="G65" s="83"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="24"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
-      <c r="G66" s="26"/>
+      <c r="C66" s="84"/>
+      <c r="D66" s="80"/>
+      <c r="E66" s="80"/>
+      <c r="F66" s="80"/>
+      <c r="G66" s="85"/>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="24"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="25"/>
-      <c r="F67" s="25"/>
-      <c r="G67" s="26"/>
+      <c r="C67" s="84"/>
+      <c r="D67" s="80"/>
+      <c r="E67" s="80"/>
+      <c r="F67" s="80"/>
+      <c r="G67" s="85"/>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C68" s="24"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="26"/>
+      <c r="C68" s="84"/>
+      <c r="D68" s="80"/>
+      <c r="E68" s="80"/>
+      <c r="F68" s="80"/>
+      <c r="G68" s="85"/>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="24"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="26"/>
+      <c r="C69" s="84"/>
+      <c r="D69" s="80"/>
+      <c r="E69" s="80"/>
+      <c r="F69" s="80"/>
+      <c r="G69" s="85"/>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="24"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="26"/>
-    </row>
-    <row r="71" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C71" s="27"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="28"/>
-      <c r="F71" s="28"/>
-      <c r="G71" s="29"/>
-    </row>
-    <row r="81" spans="6:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="82" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F82" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="G82" s="22"/>
-      <c r="H82" s="22"/>
-      <c r="I82" s="22"/>
-      <c r="J82" s="23"/>
-    </row>
-    <row r="83" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F83" s="24"/>
-      <c r="G83" s="25"/>
-      <c r="H83" s="25"/>
-      <c r="I83" s="25"/>
-      <c r="J83" s="26"/>
-    </row>
-    <row r="84" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F84" s="24"/>
-      <c r="G84" s="25"/>
-      <c r="H84" s="25"/>
-      <c r="I84" s="25"/>
-      <c r="J84" s="26"/>
-    </row>
-    <row r="85" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F85" s="24"/>
-      <c r="G85" s="25"/>
-      <c r="H85" s="25"/>
-      <c r="I85" s="25"/>
-      <c r="J85" s="26"/>
-    </row>
-    <row r="86" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F86" s="24"/>
-      <c r="G86" s="25"/>
-      <c r="H86" s="25"/>
-      <c r="I86" s="25"/>
-      <c r="J86" s="26"/>
-    </row>
-    <row r="87" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F87" s="24"/>
-      <c r="G87" s="25"/>
-      <c r="H87" s="25"/>
-      <c r="I87" s="25"/>
-      <c r="J87" s="26"/>
-    </row>
-    <row r="88" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F88" s="24"/>
-      <c r="G88" s="25"/>
-      <c r="H88" s="25"/>
-      <c r="I88" s="25"/>
-      <c r="J88" s="26"/>
-    </row>
-    <row r="89" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F89" s="24"/>
-      <c r="G89" s="25"/>
-      <c r="H89" s="25"/>
-      <c r="I89" s="25"/>
-      <c r="J89" s="26"/>
-    </row>
-    <row r="90" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F90" s="24"/>
-      <c r="G90" s="25"/>
-      <c r="H90" s="25"/>
-      <c r="I90" s="25"/>
-      <c r="J90" s="26"/>
-    </row>
-    <row r="91" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F91" s="24"/>
-      <c r="G91" s="25"/>
-      <c r="H91" s="25"/>
-      <c r="I91" s="25"/>
-      <c r="J91" s="26"/>
-    </row>
-    <row r="92" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F92" s="24"/>
-      <c r="G92" s="25"/>
-      <c r="H92" s="25"/>
-      <c r="I92" s="25"/>
-      <c r="J92" s="26"/>
-    </row>
-    <row r="93" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F93" s="24"/>
-      <c r="G93" s="25"/>
-      <c r="H93" s="25"/>
-      <c r="I93" s="25"/>
-      <c r="J93" s="26"/>
-    </row>
-    <row r="94" spans="6:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F94" s="27"/>
-      <c r="G94" s="28"/>
-      <c r="H94" s="28"/>
-      <c r="I94" s="28"/>
-      <c r="J94" s="29"/>
+      <c r="C70" s="84"/>
+      <c r="D70" s="80"/>
+      <c r="E70" s="80"/>
+      <c r="F70" s="80"/>
+      <c r="G70" s="85"/>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C71" s="84"/>
+      <c r="D71" s="80"/>
+      <c r="E71" s="80"/>
+      <c r="F71" s="80"/>
+      <c r="G71" s="85"/>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C72" s="84"/>
+      <c r="D72" s="80"/>
+      <c r="E72" s="80"/>
+      <c r="F72" s="80"/>
+      <c r="G72" s="85"/>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C73" s="84"/>
+      <c r="D73" s="80"/>
+      <c r="E73" s="80"/>
+      <c r="F73" s="80"/>
+      <c r="G73" s="85"/>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C74" s="84"/>
+      <c r="D74" s="80"/>
+      <c r="E74" s="80"/>
+      <c r="F74" s="80"/>
+      <c r="G74" s="85"/>
+    </row>
+    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C75" s="84"/>
+      <c r="D75" s="80"/>
+      <c r="E75" s="80"/>
+      <c r="F75" s="80"/>
+      <c r="G75" s="85"/>
+    </row>
+    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C76" s="84"/>
+      <c r="D76" s="80"/>
+      <c r="E76" s="80"/>
+      <c r="F76" s="80"/>
+      <c r="G76" s="85"/>
+    </row>
+    <row r="77" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="86"/>
+      <c r="D77" s="87"/>
+      <c r="E77" s="87"/>
+      <c r="F77" s="87"/>
+      <c r="G77" s="88"/>
+    </row>
+    <row r="84" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J84" s="78"/>
+    </row>
+    <row r="85" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J85" s="78"/>
+    </row>
+    <row r="86" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C86" s="89" t="s">
+        <v>115</v>
+      </c>
+      <c r="D86" s="79"/>
+      <c r="E86" s="79"/>
+      <c r="F86" s="79"/>
+      <c r="G86" s="83"/>
+      <c r="J86" s="78"/>
+    </row>
+    <row r="87" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C87" s="84"/>
+      <c r="D87" s="80"/>
+      <c r="E87" s="80"/>
+      <c r="F87" s="80"/>
+      <c r="G87" s="85"/>
+      <c r="J87" s="78"/>
+    </row>
+    <row r="88" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C88" s="84"/>
+      <c r="D88" s="80"/>
+      <c r="E88" s="80"/>
+      <c r="F88" s="80"/>
+      <c r="G88" s="85"/>
+      <c r="J88" s="78"/>
+    </row>
+    <row r="89" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C89" s="84"/>
+      <c r="D89" s="80"/>
+      <c r="E89" s="80"/>
+      <c r="F89" s="80"/>
+      <c r="G89" s="85"/>
+      <c r="J89" s="78"/>
+    </row>
+    <row r="90" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C90" s="84"/>
+      <c r="D90" s="80"/>
+      <c r="E90" s="80"/>
+      <c r="F90" s="80"/>
+      <c r="G90" s="85"/>
+      <c r="J90" s="78"/>
+    </row>
+    <row r="91" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C91" s="84"/>
+      <c r="D91" s="80"/>
+      <c r="E91" s="80"/>
+      <c r="F91" s="80"/>
+      <c r="G91" s="85"/>
+      <c r="J91" s="78"/>
+    </row>
+    <row r="92" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C92" s="84"/>
+      <c r="D92" s="80"/>
+      <c r="E92" s="80"/>
+      <c r="F92" s="80"/>
+      <c r="G92" s="85"/>
+      <c r="J92" s="78"/>
+    </row>
+    <row r="93" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C93" s="84"/>
+      <c r="D93" s="80"/>
+      <c r="E93" s="80"/>
+      <c r="F93" s="80"/>
+      <c r="G93" s="85"/>
+      <c r="J93" s="78"/>
+    </row>
+    <row r="94" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C94" s="84"/>
+      <c r="D94" s="80"/>
+      <c r="E94" s="80"/>
+      <c r="F94" s="80"/>
+      <c r="G94" s="85"/>
+      <c r="J94" s="78"/>
+    </row>
+    <row r="95" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C95" s="84"/>
+      <c r="D95" s="80"/>
+      <c r="E95" s="80"/>
+      <c r="F95" s="80"/>
+      <c r="G95" s="85"/>
+      <c r="J95" s="78"/>
+    </row>
+    <row r="96" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C96" s="84"/>
+      <c r="D96" s="80"/>
+      <c r="E96" s="80"/>
+      <c r="F96" s="80"/>
+      <c r="G96" s="85"/>
+      <c r="J96" s="78"/>
+    </row>
+    <row r="97" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C97" s="84"/>
+      <c r="D97" s="80"/>
+      <c r="E97" s="80"/>
+      <c r="F97" s="80"/>
+      <c r="G97" s="85"/>
+    </row>
+    <row r="98" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C98" s="86"/>
+      <c r="D98" s="87"/>
+      <c r="E98" s="87"/>
+      <c r="F98" s="87"/>
+      <c r="G98" s="88"/>
+    </row>
+    <row r="108" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="3:10" ht="315" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F109" s="90" t="s">
+        <v>116</v>
+      </c>
+      <c r="G109" s="91"/>
+      <c r="H109" s="91"/>
+      <c r="I109" s="92"/>
+    </row>
+    <row r="110" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F110" s="77"/>
+      <c r="G110" s="78"/>
+      <c r="H110" s="78"/>
+      <c r="I110" s="78"/>
+    </row>
+    <row r="111" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F111" s="78"/>
+      <c r="G111" s="78"/>
+      <c r="H111" s="78"/>
+      <c r="I111" s="78"/>
+      <c r="J111" s="21"/>
+    </row>
+    <row r="112" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F112" s="78"/>
+      <c r="G112" s="78"/>
+      <c r="H112" s="78"/>
+      <c r="I112" s="78"/>
+      <c r="J112" s="21"/>
+    </row>
+    <row r="113" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F113" s="78"/>
+      <c r="G113" s="78"/>
+      <c r="H113" s="78"/>
+      <c r="I113" s="78"/>
+      <c r="J113" s="21"/>
+    </row>
+    <row r="114" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F114" s="78"/>
+      <c r="G114" s="78"/>
+      <c r="H114" s="78"/>
+      <c r="I114" s="78"/>
+      <c r="J114" s="21"/>
+    </row>
+    <row r="115" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F115" s="78"/>
+      <c r="G115" s="78"/>
+      <c r="H115" s="78"/>
+      <c r="I115" s="78"/>
+      <c r="J115" s="21"/>
+    </row>
+    <row r="116" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F116" s="78"/>
+      <c r="G116" s="78"/>
+      <c r="H116" s="78"/>
+      <c r="I116" s="78"/>
+      <c r="J116" s="21"/>
+    </row>
+    <row r="117" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F117" s="78"/>
+      <c r="G117" s="78"/>
+      <c r="H117" s="78"/>
+      <c r="I117" s="78"/>
+      <c r="J117" s="21"/>
+    </row>
+    <row r="118" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F118" s="78"/>
+      <c r="G118" s="78"/>
+      <c r="H118" s="78"/>
+      <c r="I118" s="78"/>
+      <c r="J118" s="21"/>
+    </row>
+    <row r="119" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F119" s="78"/>
+      <c r="G119" s="78"/>
+      <c r="H119" s="78"/>
+      <c r="I119" s="78"/>
+      <c r="J119" s="21"/>
+    </row>
+    <row r="120" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F120" s="78"/>
+      <c r="G120" s="78"/>
+      <c r="H120" s="78"/>
+      <c r="I120" s="78"/>
+      <c r="J120" s="21"/>
+    </row>
+    <row r="121" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F121" s="78"/>
+      <c r="G121" s="78"/>
+      <c r="H121" s="78"/>
+      <c r="I121" s="78"/>
+      <c r="J121" s="21"/>
+    </row>
+    <row r="136" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E136" s="81"/>
+      <c r="F136" s="81"/>
+      <c r="G136" s="81"/>
+      <c r="H136" s="81"/>
+      <c r="I136" s="81"/>
+    </row>
+    <row r="137" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E137" s="81"/>
+      <c r="F137" s="81"/>
+      <c r="G137" s="81"/>
+      <c r="H137" s="81"/>
+      <c r="I137" s="81"/>
+    </row>
+    <row r="138" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E138" s="81"/>
+      <c r="F138" s="81"/>
+      <c r="G138" s="81"/>
+      <c r="H138" s="81"/>
+      <c r="I138" s="81"/>
+    </row>
+    <row r="139" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E139" s="81"/>
+      <c r="F139" s="81"/>
+      <c r="G139" s="81"/>
+      <c r="H139" s="81"/>
+      <c r="I139" s="81"/>
+    </row>
+    <row r="140" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E140" s="81"/>
+      <c r="F140" s="81"/>
+      <c r="G140" s="81"/>
+      <c r="H140" s="81"/>
+      <c r="I140" s="81"/>
+    </row>
+    <row r="141" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E141" s="81"/>
+      <c r="F141" s="81"/>
+      <c r="G141" s="81"/>
+      <c r="H141" s="81"/>
+      <c r="I141" s="81"/>
+    </row>
+    <row r="142" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E142" s="81"/>
+      <c r="F142" s="81"/>
+      <c r="G142" s="81"/>
+      <c r="H142" s="81"/>
+      <c r="I142" s="81"/>
+    </row>
+    <row r="143" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E143" s="81"/>
+      <c r="F143" s="81"/>
+      <c r="G143" s="81"/>
+      <c r="H143" s="81"/>
+      <c r="I143" s="81"/>
+    </row>
+    <row r="144" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E144" s="81"/>
+      <c r="F144" s="81"/>
+      <c r="G144" s="81"/>
+      <c r="H144" s="81"/>
+      <c r="I144" s="81"/>
+    </row>
+    <row r="145" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E145" s="81"/>
+      <c r="F145" s="81"/>
+      <c r="G145" s="81"/>
+      <c r="H145" s="81"/>
+      <c r="I145" s="81"/>
+    </row>
+    <row r="146" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E146" s="81"/>
+      <c r="F146" s="81"/>
+      <c r="G146" s="81"/>
+      <c r="H146" s="81"/>
+      <c r="I146" s="81"/>
+    </row>
+    <row r="147" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E147" s="81"/>
+      <c r="F147" s="81"/>
+      <c r="G147" s="81"/>
+      <c r="H147" s="81"/>
+      <c r="I147" s="81"/>
+    </row>
+    <row r="148" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E148" s="81"/>
+      <c r="F148" s="81"/>
+      <c r="G148" s="81"/>
+      <c r="H148" s="81"/>
+      <c r="I148" s="81"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C17:G30"/>
+    <mergeCell ref="C65:G77"/>
+    <mergeCell ref="C86:G98"/>
+    <mergeCell ref="E39:I51"/>
+    <mergeCell ref="F109:I109"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2998,246 +3298,251 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="77"/>
-    <col min="2" max="2" width="10.7109375" style="77" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="77" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="77" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="77"/>
-    <col min="6" max="6" width="29.42578125" style="77" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="77" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="77" customWidth="1"/>
-    <col min="9" max="9" width="12" style="77" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" style="77" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="61"/>
+    <col min="2" max="2" width="10.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="61" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="61" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="61"/>
+    <col min="6" max="6" width="29.42578125" style="61" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" style="61" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="61" customWidth="1"/>
+    <col min="9" max="9" width="12" style="61" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" style="61" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="C1" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="E1" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="F1" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="G1" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="J1" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="33" t="s">
+    </row>
+    <row r="2" spans="1:10" s="59" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="64">
+        <v>1</v>
+      </c>
+      <c r="B2" s="66" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="74" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="78">
-        <v>1</v>
-      </c>
-      <c r="B2" s="75" t="s">
+      <c r="C2" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="D2" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="75" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="75">
+      <c r="E2" s="66">
         <v>2</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="62">
+        <v>42440</v>
+      </c>
+      <c r="I2" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="J2" s="43"/>
+    </row>
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="65"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="G3" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="79">
+      <c r="H3" s="62">
         <v>42440</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="I3" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" s="43"/>
+    </row>
+    <row r="4" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="66">
+        <v>2</v>
+      </c>
+      <c r="B4" s="69">
+        <v>42440</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="64">
+        <v>2</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="62">
+        <v>42440</v>
+      </c>
+      <c r="I4" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="J4" s="43"/>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="64"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" s="63">
+        <v>42440</v>
+      </c>
+      <c r="I5" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" s="50"/>
+    </row>
+    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="66">
+        <v>3</v>
+      </c>
+      <c r="B6" s="67">
+        <v>42624</v>
+      </c>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="62">
+        <v>42624</v>
+      </c>
+      <c r="I6" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="J6" s="43"/>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="66"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="J2" s="51"/>
-    </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="81"/>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="51" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="H3" s="79">
-        <v>42440</v>
-      </c>
-      <c r="I3" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="J3" s="51"/>
-    </row>
-    <row r="4" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="75">
-        <v>2</v>
-      </c>
-      <c r="B4" s="82">
-        <v>42440</v>
-      </c>
-      <c r="C4" s="75" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" s="75" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" s="78">
-        <v>2</v>
-      </c>
-      <c r="F4" s="51" t="s">
+      <c r="G7" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" s="62">
+        <v>42624</v>
+      </c>
+      <c r="I7" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="J7" s="43"/>
+    </row>
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="66"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="51" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" s="79">
-        <v>42440</v>
-      </c>
-      <c r="I4" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="J4" s="51"/>
-    </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="78"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="58" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" s="58" t="s">
+      <c r="G8" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="62">
+        <v>42624</v>
+      </c>
+      <c r="I8" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="J8" s="43"/>
+    </row>
+    <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="43">
+        <v>4</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="H5" s="84">
-        <v>42440</v>
-      </c>
-      <c r="I5" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="J5" s="58"/>
-    </row>
-    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="75">
-        <v>3</v>
-      </c>
-      <c r="B6" s="83">
-        <v>42624</v>
-      </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51" t="s">
+      <c r="H9" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="G6" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="79">
-        <v>42624</v>
-      </c>
-      <c r="I6" s="51" t="s">
-        <v>101</v>
-      </c>
-      <c r="J6" s="51"/>
-    </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="75"/>
-      <c r="B7" s="81"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51" t="s">
-        <v>109</v>
-      </c>
-      <c r="G7" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="H7" s="79">
-        <v>42624</v>
-      </c>
-      <c r="I7" s="51" t="s">
-        <v>101</v>
-      </c>
-      <c r="J7" s="51"/>
-    </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="75"/>
-      <c r="B8" s="80"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="G8" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="H8" s="79">
-        <v>42624</v>
-      </c>
-      <c r="I8" s="51" t="s">
-        <v>101</v>
-      </c>
-      <c r="J8" s="51"/>
-    </row>
-    <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="51">
-        <v>4</v>
-      </c>
-      <c r="B9" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="G9" s="51" t="s">
+      <c r="I9" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="H9" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="I9" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="J9" s="51"/>
+      <c r="J9" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
@@ -3245,11 +3550,6 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3311,417 +3611,417 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="69" t="s">
+      <c r="A1" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="72" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="D1" s="75"/>
+      <c r="E1" s="75" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72" t="s">
+      <c r="F1" s="76"/>
+      <c r="G1" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="34" t="s">
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+    </row>
+    <row r="2" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="71"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-    </row>
-    <row r="2" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="68"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="36" t="s">
+      <c r="D2" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="E2" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="31">
+        <v>42690</v>
+      </c>
+      <c r="H2" s="31">
+        <v>42720</v>
+      </c>
+      <c r="I2" s="31">
+        <v>42751</v>
+      </c>
+      <c r="J2" s="31">
+        <v>42782</v>
+      </c>
+      <c r="K2" s="31">
+        <v>42810</v>
+      </c>
+      <c r="L2" s="31">
+        <v>42841</v>
+      </c>
+      <c r="M2" s="31">
+        <v>42871</v>
+      </c>
+      <c r="N2" s="31">
+        <v>42902</v>
+      </c>
+      <c r="O2" s="31">
+        <v>42932</v>
+      </c>
+      <c r="P2" s="31">
+        <v>42963</v>
+      </c>
+      <c r="Q2" s="31">
+        <v>42994</v>
+      </c>
+      <c r="R2" s="31">
+        <v>43024</v>
+      </c>
+      <c r="S2" s="31">
+        <v>43055</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="32">
+        <v>1</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="G2" s="39">
-        <v>42690</v>
-      </c>
-      <c r="H2" s="39">
-        <v>42720</v>
-      </c>
-      <c r="I2" s="39">
-        <v>42751</v>
-      </c>
-      <c r="J2" s="39">
-        <v>42782</v>
-      </c>
-      <c r="K2" s="39">
-        <v>42810</v>
-      </c>
-      <c r="L2" s="39">
-        <v>42841</v>
-      </c>
-      <c r="M2" s="39">
-        <v>42871</v>
-      </c>
-      <c r="N2" s="39">
-        <v>42902</v>
-      </c>
-      <c r="O2" s="39">
-        <v>42932</v>
-      </c>
-      <c r="P2" s="39">
-        <v>42963</v>
-      </c>
-      <c r="Q2" s="39">
-        <v>42994</v>
-      </c>
-      <c r="R2" s="39">
-        <v>43024</v>
-      </c>
-      <c r="S2" s="39">
-        <v>43055</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40">
-        <v>1</v>
-      </c>
-      <c r="B3" s="41" t="s">
+      <c r="C3" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="D3" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="38">
+        <v>2</v>
+      </c>
+      <c r="B4" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" s="40"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="46">
-        <v>2</v>
-      </c>
-      <c r="B4" s="47" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="38">
+        <v>3</v>
+      </c>
+      <c r="B5" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="52"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46">
-        <v>3</v>
-      </c>
-      <c r="B5" s="47" t="s">
+      <c r="C5" s="40"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="38">
+        <v>4</v>
+      </c>
+      <c r="B6" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46">
-        <v>4</v>
-      </c>
-      <c r="B6" s="47" t="s">
+      <c r="C6" s="40"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="38">
+        <v>5</v>
+      </c>
+      <c r="B7" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="46">
-        <v>5</v>
-      </c>
-      <c r="B7" s="47" t="s">
+      <c r="C7" s="40"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="38">
+        <v>6</v>
+      </c>
+      <c r="B8" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-    </row>
-    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="46">
-        <v>6</v>
-      </c>
-      <c r="B8" s="47" t="s">
+      <c r="C8" s="40"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="38">
+        <v>7</v>
+      </c>
+      <c r="B9" s="39"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="38">
+        <v>8</v>
+      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="37"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="38">
+        <v>9</v>
+      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="38">
+        <v>10</v>
+      </c>
+      <c r="B12" s="39"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="38">
+        <v>11</v>
+      </c>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="45">
+        <v>12</v>
+      </c>
+      <c r="B14" s="46"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="52"/>
+      <c r="B15" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="51"/>
-      <c r="O8" s="52"/>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-    </row>
-    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="46">
-        <v>7</v>
-      </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="45"/>
-      <c r="R9" s="45"/>
-      <c r="S9" s="45"/>
-    </row>
-    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="46">
-        <v>8</v>
-      </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="52"/>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="45"/>
-      <c r="R10" s="45"/>
-      <c r="S10" s="45"/>
-    </row>
-    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="46">
-        <v>9</v>
-      </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="52"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="45"/>
-      <c r="S11" s="45"/>
-    </row>
-    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46">
-        <v>10</v>
-      </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="52"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="45"/>
-      <c r="R12" s="45"/>
-      <c r="S12" s="45"/>
-    </row>
-    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="46">
-        <v>11</v>
-      </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="52"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
-    </row>
-    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="53">
-        <v>12</v>
-      </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="58"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="58"/>
-      <c r="O14" s="59"/>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="45"/>
-      <c r="R14" s="45"/>
-      <c r="S14" s="45"/>
-    </row>
-    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="60"/>
-      <c r="B15" s="61" t="s">
+      <c r="C15" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="F15" s="64"/>
-      <c r="G15" s="60">
+      <c r="D15" s="55"/>
+      <c r="E15" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="56"/>
+      <c r="G15" s="52">
         <v>30</v>
       </c>
-      <c r="H15" s="65">
+      <c r="H15" s="57">
         <v>30</v>
       </c>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="65"/>
-      <c r="N15" s="65"/>
-      <c r="O15" s="66"/>
-      <c r="P15" s="66"/>
-      <c r="Q15" s="66"/>
-      <c r="R15" s="66"/>
-      <c r="S15" s="66"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="57"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="58"/>
+      <c r="Q15" s="58"/>
+      <c r="R15" s="58"/>
+      <c r="S15" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Criado SIPOC para processo de contratação.
</commit_message>
<xml_diff>
--- a/TRE_Dados_MapaRaciocinio.xlsx
+++ b/TRE_Dados_MapaRaciocinio.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Historicos x Categoria" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="PROCESSO PADRÃO" sheetId="4" r:id="rId4"/>
     <sheet name="Controle do Projeto" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1021,52 +1021,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1076,6 +1031,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1094,9 +1058,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1105,6 +1066,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1749,9 +1749,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1789,9 +1789,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1826,7 +1826,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1861,7 +1861,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2037,16 +2037,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.140625" customWidth="1"/>
     <col min="2" max="2" width="53.140625" customWidth="1"/>
-    <col min="3" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
     <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="2.85546875" customWidth="1"/>
@@ -2067,7 +2068,7 @@
       </c>
       <c r="D1" s="12">
         <f ca="1">TODAY()</f>
-        <v>42681</v>
+        <v>42683</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>11</v>
@@ -2592,8 +2593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J148"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView showGridLines="0" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2701,585 +2702,585 @@
     </row>
     <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="82" t="s">
+      <c r="C17" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="79"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="79"/>
-      <c r="G17" s="79"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="80"/>
-      <c r="D18" s="80"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="80"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
-      <c r="G19" s="80"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="80"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="80"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="80"/>
-      <c r="G21" s="80"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="80"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="80"/>
-      <c r="G23" s="80"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="80"/>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
-      <c r="G24" s="80"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="80"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="80"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="69"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="80"/>
-      <c r="D26" s="80"/>
-      <c r="E26" s="80"/>
-      <c r="F26" s="80"/>
-      <c r="G26" s="80"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="69"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="80"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="80"/>
-      <c r="G27" s="80"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="69"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="80"/>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="80"/>
-      <c r="G28" s="80"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="69"/>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="80"/>
-      <c r="D29" s="80"/>
-      <c r="E29" s="80"/>
-      <c r="F29" s="80"/>
-      <c r="G29" s="80"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="80"/>
-      <c r="D30" s="80"/>
-      <c r="E30" s="80"/>
-      <c r="F30" s="80"/>
-      <c r="G30" s="80"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
     </row>
     <row r="38" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="89" t="s">
+      <c r="E39" s="70" t="s">
         <v>117</v>
       </c>
-      <c r="F39" s="79"/>
-      <c r="G39" s="79"/>
-      <c r="H39" s="79"/>
-      <c r="I39" s="83"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="68"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="71"/>
     </row>
     <row r="40" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E40" s="84"/>
-      <c r="F40" s="80"/>
-      <c r="G40" s="80"/>
-      <c r="H40" s="80"/>
-      <c r="I40" s="85"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="69"/>
+      <c r="G40" s="69"/>
+      <c r="H40" s="69"/>
+      <c r="I40" s="73"/>
     </row>
     <row r="41" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="84"/>
-      <c r="F41" s="80"/>
-      <c r="G41" s="80"/>
-      <c r="H41" s="80"/>
-      <c r="I41" s="85"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="69"/>
+      <c r="G41" s="69"/>
+      <c r="H41" s="69"/>
+      <c r="I41" s="73"/>
     </row>
     <row r="42" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E42" s="84"/>
-      <c r="F42" s="80"/>
-      <c r="G42" s="80"/>
-      <c r="H42" s="80"/>
-      <c r="I42" s="85"/>
+      <c r="E42" s="72"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="69"/>
+      <c r="I42" s="73"/>
     </row>
     <row r="43" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E43" s="84"/>
-      <c r="F43" s="80"/>
-      <c r="G43" s="80"/>
-      <c r="H43" s="80"/>
-      <c r="I43" s="85"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="69"/>
+      <c r="G43" s="69"/>
+      <c r="H43" s="69"/>
+      <c r="I43" s="73"/>
     </row>
     <row r="44" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E44" s="84"/>
-      <c r="F44" s="80"/>
-      <c r="G44" s="80"/>
-      <c r="H44" s="80"/>
-      <c r="I44" s="85"/>
+      <c r="E44" s="72"/>
+      <c r="F44" s="69"/>
+      <c r="G44" s="69"/>
+      <c r="H44" s="69"/>
+      <c r="I44" s="73"/>
     </row>
     <row r="45" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E45" s="84"/>
-      <c r="F45" s="80"/>
-      <c r="G45" s="80"/>
-      <c r="H45" s="80"/>
-      <c r="I45" s="85"/>
+      <c r="E45" s="72"/>
+      <c r="F45" s="69"/>
+      <c r="G45" s="69"/>
+      <c r="H45" s="69"/>
+      <c r="I45" s="73"/>
     </row>
     <row r="46" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E46" s="84"/>
-      <c r="F46" s="80"/>
-      <c r="G46" s="80"/>
-      <c r="H46" s="80"/>
-      <c r="I46" s="85"/>
+      <c r="E46" s="72"/>
+      <c r="F46" s="69"/>
+      <c r="G46" s="69"/>
+      <c r="H46" s="69"/>
+      <c r="I46" s="73"/>
     </row>
     <row r="47" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E47" s="84"/>
-      <c r="F47" s="80"/>
-      <c r="G47" s="80"/>
-      <c r="H47" s="80"/>
-      <c r="I47" s="85"/>
+      <c r="E47" s="72"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="69"/>
+      <c r="I47" s="73"/>
     </row>
     <row r="48" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E48" s="84"/>
-      <c r="F48" s="80"/>
-      <c r="G48" s="80"/>
-      <c r="H48" s="80"/>
-      <c r="I48" s="85"/>
+      <c r="E48" s="72"/>
+      <c r="F48" s="69"/>
+      <c r="G48" s="69"/>
+      <c r="H48" s="69"/>
+      <c r="I48" s="73"/>
     </row>
     <row r="49" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E49" s="84"/>
-      <c r="F49" s="80"/>
-      <c r="G49" s="80"/>
-      <c r="H49" s="80"/>
-      <c r="I49" s="85"/>
+      <c r="E49" s="72"/>
+      <c r="F49" s="69"/>
+      <c r="G49" s="69"/>
+      <c r="H49" s="69"/>
+      <c r="I49" s="73"/>
     </row>
     <row r="50" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E50" s="84"/>
-      <c r="F50" s="80"/>
-      <c r="G50" s="80"/>
-      <c r="H50" s="80"/>
-      <c r="I50" s="85"/>
+      <c r="E50" s="72"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="73"/>
     </row>
     <row r="51" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E51" s="86"/>
-      <c r="F51" s="87"/>
-      <c r="G51" s="87"/>
-      <c r="H51" s="87"/>
-      <c r="I51" s="88"/>
+      <c r="E51" s="74"/>
+      <c r="F51" s="75"/>
+      <c r="G51" s="75"/>
+      <c r="H51" s="75"/>
+      <c r="I51" s="76"/>
     </row>
     <row r="64" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="89" t="s">
+      <c r="C65" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="D65" s="79"/>
-      <c r="E65" s="79"/>
-      <c r="F65" s="79"/>
-      <c r="G65" s="83"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="68"/>
+      <c r="F65" s="68"/>
+      <c r="G65" s="71"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="84"/>
-      <c r="D66" s="80"/>
-      <c r="E66" s="80"/>
-      <c r="F66" s="80"/>
-      <c r="G66" s="85"/>
+      <c r="C66" s="72"/>
+      <c r="D66" s="69"/>
+      <c r="E66" s="69"/>
+      <c r="F66" s="69"/>
+      <c r="G66" s="73"/>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="84"/>
-      <c r="D67" s="80"/>
-      <c r="E67" s="80"/>
-      <c r="F67" s="80"/>
-      <c r="G67" s="85"/>
+      <c r="C67" s="72"/>
+      <c r="D67" s="69"/>
+      <c r="E67" s="69"/>
+      <c r="F67" s="69"/>
+      <c r="G67" s="73"/>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C68" s="84"/>
-      <c r="D68" s="80"/>
-      <c r="E68" s="80"/>
-      <c r="F68" s="80"/>
-      <c r="G68" s="85"/>
+      <c r="C68" s="72"/>
+      <c r="D68" s="69"/>
+      <c r="E68" s="69"/>
+      <c r="F68" s="69"/>
+      <c r="G68" s="73"/>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="84"/>
-      <c r="D69" s="80"/>
-      <c r="E69" s="80"/>
-      <c r="F69" s="80"/>
-      <c r="G69" s="85"/>
+      <c r="C69" s="72"/>
+      <c r="D69" s="69"/>
+      <c r="E69" s="69"/>
+      <c r="F69" s="69"/>
+      <c r="G69" s="73"/>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="84"/>
-      <c r="D70" s="80"/>
-      <c r="E70" s="80"/>
-      <c r="F70" s="80"/>
-      <c r="G70" s="85"/>
+      <c r="C70" s="72"/>
+      <c r="D70" s="69"/>
+      <c r="E70" s="69"/>
+      <c r="F70" s="69"/>
+      <c r="G70" s="73"/>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C71" s="84"/>
-      <c r="D71" s="80"/>
-      <c r="E71" s="80"/>
-      <c r="F71" s="80"/>
-      <c r="G71" s="85"/>
+      <c r="C71" s="72"/>
+      <c r="D71" s="69"/>
+      <c r="E71" s="69"/>
+      <c r="F71" s="69"/>
+      <c r="G71" s="73"/>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="84"/>
-      <c r="D72" s="80"/>
-      <c r="E72" s="80"/>
-      <c r="F72" s="80"/>
-      <c r="G72" s="85"/>
+      <c r="C72" s="72"/>
+      <c r="D72" s="69"/>
+      <c r="E72" s="69"/>
+      <c r="F72" s="69"/>
+      <c r="G72" s="73"/>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="84"/>
-      <c r="D73" s="80"/>
-      <c r="E73" s="80"/>
-      <c r="F73" s="80"/>
-      <c r="G73" s="85"/>
+      <c r="C73" s="72"/>
+      <c r="D73" s="69"/>
+      <c r="E73" s="69"/>
+      <c r="F73" s="69"/>
+      <c r="G73" s="73"/>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="84"/>
-      <c r="D74" s="80"/>
-      <c r="E74" s="80"/>
-      <c r="F74" s="80"/>
-      <c r="G74" s="85"/>
+      <c r="C74" s="72"/>
+      <c r="D74" s="69"/>
+      <c r="E74" s="69"/>
+      <c r="F74" s="69"/>
+      <c r="G74" s="73"/>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="84"/>
-      <c r="D75" s="80"/>
-      <c r="E75" s="80"/>
-      <c r="F75" s="80"/>
-      <c r="G75" s="85"/>
+      <c r="C75" s="72"/>
+      <c r="D75" s="69"/>
+      <c r="E75" s="69"/>
+      <c r="F75" s="69"/>
+      <c r="G75" s="73"/>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="84"/>
-      <c r="D76" s="80"/>
-      <c r="E76" s="80"/>
-      <c r="F76" s="80"/>
-      <c r="G76" s="85"/>
+      <c r="C76" s="72"/>
+      <c r="D76" s="69"/>
+      <c r="E76" s="69"/>
+      <c r="F76" s="69"/>
+      <c r="G76" s="73"/>
     </row>
     <row r="77" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C77" s="86"/>
-      <c r="D77" s="87"/>
-      <c r="E77" s="87"/>
-      <c r="F77" s="87"/>
-      <c r="G77" s="88"/>
+      <c r="C77" s="74"/>
+      <c r="D77" s="75"/>
+      <c r="E77" s="75"/>
+      <c r="F77" s="75"/>
+      <c r="G77" s="76"/>
     </row>
     <row r="84" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="78"/>
+      <c r="J84" s="65"/>
     </row>
     <row r="85" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J85" s="78"/>
+      <c r="J85" s="65"/>
     </row>
     <row r="86" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C86" s="89" t="s">
+      <c r="C86" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="D86" s="79"/>
-      <c r="E86" s="79"/>
-      <c r="F86" s="79"/>
-      <c r="G86" s="83"/>
-      <c r="J86" s="78"/>
+      <c r="D86" s="68"/>
+      <c r="E86" s="68"/>
+      <c r="F86" s="68"/>
+      <c r="G86" s="71"/>
+      <c r="J86" s="65"/>
     </row>
     <row r="87" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C87" s="84"/>
-      <c r="D87" s="80"/>
-      <c r="E87" s="80"/>
-      <c r="F87" s="80"/>
-      <c r="G87" s="85"/>
-      <c r="J87" s="78"/>
+      <c r="C87" s="72"/>
+      <c r="D87" s="69"/>
+      <c r="E87" s="69"/>
+      <c r="F87" s="69"/>
+      <c r="G87" s="73"/>
+      <c r="J87" s="65"/>
     </row>
     <row r="88" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C88" s="84"/>
-      <c r="D88" s="80"/>
-      <c r="E88" s="80"/>
-      <c r="F88" s="80"/>
-      <c r="G88" s="85"/>
-      <c r="J88" s="78"/>
+      <c r="C88" s="72"/>
+      <c r="D88" s="69"/>
+      <c r="E88" s="69"/>
+      <c r="F88" s="69"/>
+      <c r="G88" s="73"/>
+      <c r="J88" s="65"/>
     </row>
     <row r="89" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C89" s="84"/>
-      <c r="D89" s="80"/>
-      <c r="E89" s="80"/>
-      <c r="F89" s="80"/>
-      <c r="G89" s="85"/>
-      <c r="J89" s="78"/>
+      <c r="C89" s="72"/>
+      <c r="D89" s="69"/>
+      <c r="E89" s="69"/>
+      <c r="F89" s="69"/>
+      <c r="G89" s="73"/>
+      <c r="J89" s="65"/>
     </row>
     <row r="90" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C90" s="84"/>
-      <c r="D90" s="80"/>
-      <c r="E90" s="80"/>
-      <c r="F90" s="80"/>
-      <c r="G90" s="85"/>
-      <c r="J90" s="78"/>
+      <c r="C90" s="72"/>
+      <c r="D90" s="69"/>
+      <c r="E90" s="69"/>
+      <c r="F90" s="69"/>
+      <c r="G90" s="73"/>
+      <c r="J90" s="65"/>
     </row>
     <row r="91" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C91" s="84"/>
-      <c r="D91" s="80"/>
-      <c r="E91" s="80"/>
-      <c r="F91" s="80"/>
-      <c r="G91" s="85"/>
-      <c r="J91" s="78"/>
+      <c r="C91" s="72"/>
+      <c r="D91" s="69"/>
+      <c r="E91" s="69"/>
+      <c r="F91" s="69"/>
+      <c r="G91" s="73"/>
+      <c r="J91" s="65"/>
     </row>
     <row r="92" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C92" s="84"/>
-      <c r="D92" s="80"/>
-      <c r="E92" s="80"/>
-      <c r="F92" s="80"/>
-      <c r="G92" s="85"/>
-      <c r="J92" s="78"/>
+      <c r="C92" s="72"/>
+      <c r="D92" s="69"/>
+      <c r="E92" s="69"/>
+      <c r="F92" s="69"/>
+      <c r="G92" s="73"/>
+      <c r="J92" s="65"/>
     </row>
     <row r="93" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C93" s="84"/>
-      <c r="D93" s="80"/>
-      <c r="E93" s="80"/>
-      <c r="F93" s="80"/>
-      <c r="G93" s="85"/>
-      <c r="J93" s="78"/>
+      <c r="C93" s="72"/>
+      <c r="D93" s="69"/>
+      <c r="E93" s="69"/>
+      <c r="F93" s="69"/>
+      <c r="G93" s="73"/>
+      <c r="J93" s="65"/>
     </row>
     <row r="94" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C94" s="84"/>
-      <c r="D94" s="80"/>
-      <c r="E94" s="80"/>
-      <c r="F94" s="80"/>
-      <c r="G94" s="85"/>
-      <c r="J94" s="78"/>
+      <c r="C94" s="72"/>
+      <c r="D94" s="69"/>
+      <c r="E94" s="69"/>
+      <c r="F94" s="69"/>
+      <c r="G94" s="73"/>
+      <c r="J94" s="65"/>
     </row>
     <row r="95" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C95" s="84"/>
-      <c r="D95" s="80"/>
-      <c r="E95" s="80"/>
-      <c r="F95" s="80"/>
-      <c r="G95" s="85"/>
-      <c r="J95" s="78"/>
+      <c r="C95" s="72"/>
+      <c r="D95" s="69"/>
+      <c r="E95" s="69"/>
+      <c r="F95" s="69"/>
+      <c r="G95" s="73"/>
+      <c r="J95" s="65"/>
     </row>
     <row r="96" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C96" s="84"/>
-      <c r="D96" s="80"/>
-      <c r="E96" s="80"/>
-      <c r="F96" s="80"/>
-      <c r="G96" s="85"/>
-      <c r="J96" s="78"/>
+      <c r="C96" s="72"/>
+      <c r="D96" s="69"/>
+      <c r="E96" s="69"/>
+      <c r="F96" s="69"/>
+      <c r="G96" s="73"/>
+      <c r="J96" s="65"/>
     </row>
     <row r="97" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C97" s="84"/>
-      <c r="D97" s="80"/>
-      <c r="E97" s="80"/>
-      <c r="F97" s="80"/>
-      <c r="G97" s="85"/>
+      <c r="C97" s="72"/>
+      <c r="D97" s="69"/>
+      <c r="E97" s="69"/>
+      <c r="F97" s="69"/>
+      <c r="G97" s="73"/>
     </row>
     <row r="98" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C98" s="86"/>
-      <c r="D98" s="87"/>
-      <c r="E98" s="87"/>
-      <c r="F98" s="87"/>
-      <c r="G98" s="88"/>
+      <c r="C98" s="74"/>
+      <c r="D98" s="75"/>
+      <c r="E98" s="75"/>
+      <c r="F98" s="75"/>
+      <c r="G98" s="76"/>
     </row>
     <row r="108" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="109" spans="3:10" ht="315" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F109" s="90" t="s">
+      <c r="F109" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="G109" s="91"/>
-      <c r="H109" s="91"/>
-      <c r="I109" s="92"/>
+      <c r="G109" s="78"/>
+      <c r="H109" s="78"/>
+      <c r="I109" s="79"/>
     </row>
     <row r="110" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F110" s="77"/>
-      <c r="G110" s="78"/>
-      <c r="H110" s="78"/>
-      <c r="I110" s="78"/>
+      <c r="F110" s="64"/>
+      <c r="G110" s="65"/>
+      <c r="H110" s="65"/>
+      <c r="I110" s="65"/>
     </row>
     <row r="111" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F111" s="78"/>
-      <c r="G111" s="78"/>
-      <c r="H111" s="78"/>
-      <c r="I111" s="78"/>
+      <c r="F111" s="65"/>
+      <c r="G111" s="65"/>
+      <c r="H111" s="65"/>
+      <c r="I111" s="65"/>
       <c r="J111" s="21"/>
     </row>
     <row r="112" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F112" s="78"/>
-      <c r="G112" s="78"/>
-      <c r="H112" s="78"/>
-      <c r="I112" s="78"/>
+      <c r="F112" s="65"/>
+      <c r="G112" s="65"/>
+      <c r="H112" s="65"/>
+      <c r="I112" s="65"/>
       <c r="J112" s="21"/>
     </row>
     <row r="113" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F113" s="78"/>
-      <c r="G113" s="78"/>
-      <c r="H113" s="78"/>
-      <c r="I113" s="78"/>
+      <c r="F113" s="65"/>
+      <c r="G113" s="65"/>
+      <c r="H113" s="65"/>
+      <c r="I113" s="65"/>
       <c r="J113" s="21"/>
     </row>
     <row r="114" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F114" s="78"/>
-      <c r="G114" s="78"/>
-      <c r="H114" s="78"/>
-      <c r="I114" s="78"/>
+      <c r="F114" s="65"/>
+      <c r="G114" s="65"/>
+      <c r="H114" s="65"/>
+      <c r="I114" s="65"/>
       <c r="J114" s="21"/>
     </row>
     <row r="115" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F115" s="78"/>
-      <c r="G115" s="78"/>
-      <c r="H115" s="78"/>
-      <c r="I115" s="78"/>
+      <c r="F115" s="65"/>
+      <c r="G115" s="65"/>
+      <c r="H115" s="65"/>
+      <c r="I115" s="65"/>
       <c r="J115" s="21"/>
     </row>
     <row r="116" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F116" s="78"/>
-      <c r="G116" s="78"/>
-      <c r="H116" s="78"/>
-      <c r="I116" s="78"/>
+      <c r="F116" s="65"/>
+      <c r="G116" s="65"/>
+      <c r="H116" s="65"/>
+      <c r="I116" s="65"/>
       <c r="J116" s="21"/>
     </row>
     <row r="117" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F117" s="78"/>
-      <c r="G117" s="78"/>
-      <c r="H117" s="78"/>
-      <c r="I117" s="78"/>
+      <c r="F117" s="65"/>
+      <c r="G117" s="65"/>
+      <c r="H117" s="65"/>
+      <c r="I117" s="65"/>
       <c r="J117" s="21"/>
     </row>
     <row r="118" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F118" s="78"/>
-      <c r="G118" s="78"/>
-      <c r="H118" s="78"/>
-      <c r="I118" s="78"/>
+      <c r="F118" s="65"/>
+      <c r="G118" s="65"/>
+      <c r="H118" s="65"/>
+      <c r="I118" s="65"/>
       <c r="J118" s="21"/>
     </row>
     <row r="119" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F119" s="78"/>
-      <c r="G119" s="78"/>
-      <c r="H119" s="78"/>
-      <c r="I119" s="78"/>
+      <c r="F119" s="65"/>
+      <c r="G119" s="65"/>
+      <c r="H119" s="65"/>
+      <c r="I119" s="65"/>
       <c r="J119" s="21"/>
     </row>
     <row r="120" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F120" s="78"/>
-      <c r="G120" s="78"/>
-      <c r="H120" s="78"/>
-      <c r="I120" s="78"/>
+      <c r="F120" s="65"/>
+      <c r="G120" s="65"/>
+      <c r="H120" s="65"/>
+      <c r="I120" s="65"/>
       <c r="J120" s="21"/>
     </row>
     <row r="121" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F121" s="78"/>
-      <c r="G121" s="78"/>
-      <c r="H121" s="78"/>
-      <c r="I121" s="78"/>
+      <c r="F121" s="65"/>
+      <c r="G121" s="65"/>
+      <c r="H121" s="65"/>
+      <c r="I121" s="65"/>
       <c r="J121" s="21"/>
     </row>
     <row r="136" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E136" s="81"/>
-      <c r="F136" s="81"/>
-      <c r="G136" s="81"/>
-      <c r="H136" s="81"/>
-      <c r="I136" s="81"/>
+      <c r="E136" s="66"/>
+      <c r="F136" s="66"/>
+      <c r="G136" s="66"/>
+      <c r="H136" s="66"/>
+      <c r="I136" s="66"/>
     </row>
     <row r="137" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E137" s="81"/>
-      <c r="F137" s="81"/>
-      <c r="G137" s="81"/>
-      <c r="H137" s="81"/>
-      <c r="I137" s="81"/>
+      <c r="E137" s="66"/>
+      <c r="F137" s="66"/>
+      <c r="G137" s="66"/>
+      <c r="H137" s="66"/>
+      <c r="I137" s="66"/>
     </row>
     <row r="138" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E138" s="81"/>
-      <c r="F138" s="81"/>
-      <c r="G138" s="81"/>
-      <c r="H138" s="81"/>
-      <c r="I138" s="81"/>
+      <c r="E138" s="66"/>
+      <c r="F138" s="66"/>
+      <c r="G138" s="66"/>
+      <c r="H138" s="66"/>
+      <c r="I138" s="66"/>
     </row>
     <row r="139" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E139" s="81"/>
-      <c r="F139" s="81"/>
-      <c r="G139" s="81"/>
-      <c r="H139" s="81"/>
-      <c r="I139" s="81"/>
+      <c r="E139" s="66"/>
+      <c r="F139" s="66"/>
+      <c r="G139" s="66"/>
+      <c r="H139" s="66"/>
+      <c r="I139" s="66"/>
     </row>
     <row r="140" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E140" s="81"/>
-      <c r="F140" s="81"/>
-      <c r="G140" s="81"/>
-      <c r="H140" s="81"/>
-      <c r="I140" s="81"/>
+      <c r="E140" s="66"/>
+      <c r="F140" s="66"/>
+      <c r="G140" s="66"/>
+      <c r="H140" s="66"/>
+      <c r="I140" s="66"/>
     </row>
     <row r="141" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E141" s="81"/>
-      <c r="F141" s="81"/>
-      <c r="G141" s="81"/>
-      <c r="H141" s="81"/>
-      <c r="I141" s="81"/>
+      <c r="E141" s="66"/>
+      <c r="F141" s="66"/>
+      <c r="G141" s="66"/>
+      <c r="H141" s="66"/>
+      <c r="I141" s="66"/>
     </row>
     <row r="142" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E142" s="81"/>
-      <c r="F142" s="81"/>
-      <c r="G142" s="81"/>
-      <c r="H142" s="81"/>
-      <c r="I142" s="81"/>
+      <c r="E142" s="66"/>
+      <c r="F142" s="66"/>
+      <c r="G142" s="66"/>
+      <c r="H142" s="66"/>
+      <c r="I142" s="66"/>
     </row>
     <row r="143" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E143" s="81"/>
-      <c r="F143" s="81"/>
-      <c r="G143" s="81"/>
-      <c r="H143" s="81"/>
-      <c r="I143" s="81"/>
+      <c r="E143" s="66"/>
+      <c r="F143" s="66"/>
+      <c r="G143" s="66"/>
+      <c r="H143" s="66"/>
+      <c r="I143" s="66"/>
     </row>
     <row r="144" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E144" s="81"/>
-      <c r="F144" s="81"/>
-      <c r="G144" s="81"/>
-      <c r="H144" s="81"/>
-      <c r="I144" s="81"/>
+      <c r="E144" s="66"/>
+      <c r="F144" s="66"/>
+      <c r="G144" s="66"/>
+      <c r="H144" s="66"/>
+      <c r="I144" s="66"/>
     </row>
     <row r="145" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E145" s="81"/>
-      <c r="F145" s="81"/>
-      <c r="G145" s="81"/>
-      <c r="H145" s="81"/>
-      <c r="I145" s="81"/>
+      <c r="E145" s="66"/>
+      <c r="F145" s="66"/>
+      <c r="G145" s="66"/>
+      <c r="H145" s="66"/>
+      <c r="I145" s="66"/>
     </row>
     <row r="146" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E146" s="81"/>
-      <c r="F146" s="81"/>
-      <c r="G146" s="81"/>
-      <c r="H146" s="81"/>
-      <c r="I146" s="81"/>
+      <c r="E146" s="66"/>
+      <c r="F146" s="66"/>
+      <c r="G146" s="66"/>
+      <c r="H146" s="66"/>
+      <c r="I146" s="66"/>
     </row>
     <row r="147" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E147" s="81"/>
-      <c r="F147" s="81"/>
-      <c r="G147" s="81"/>
-      <c r="H147" s="81"/>
-      <c r="I147" s="81"/>
+      <c r="E147" s="66"/>
+      <c r="F147" s="66"/>
+      <c r="G147" s="66"/>
+      <c r="H147" s="66"/>
+      <c r="I147" s="66"/>
     </row>
     <row r="148" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E148" s="81"/>
-      <c r="F148" s="81"/>
-      <c r="G148" s="81"/>
-      <c r="H148" s="81"/>
-      <c r="I148" s="81"/>
+      <c r="E148" s="66"/>
+      <c r="F148" s="66"/>
+      <c r="G148" s="66"/>
+      <c r="H148" s="66"/>
+      <c r="I148" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3298,8 +3299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3349,19 +3350,19 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="59" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64">
+      <c r="A2" s="81">
         <v>1</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="66">
+      <c r="E2" s="80">
         <v>2</v>
       </c>
       <c r="F2" s="43" t="s">
@@ -3379,11 +3380,11 @@
       <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
+      <c r="A3" s="82"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
       <c r="F3" s="43" t="s">
         <v>110</v>
       </c>
@@ -3399,19 +3400,19 @@
       <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="66">
+      <c r="A4" s="80">
         <v>2</v>
       </c>
-      <c r="B4" s="69">
+      <c r="B4" s="85">
         <v>42440</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="D4" s="66" t="s">
+      <c r="D4" s="80" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="64">
+      <c r="E4" s="81">
         <v>2</v>
       </c>
       <c r="F4" s="43" t="s">
@@ -3429,11 +3430,11 @@
       <c r="J4" s="43"/>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="64"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
+      <c r="A5" s="81"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="82"/>
       <c r="F5" s="50" t="s">
         <v>103</v>
       </c>
@@ -3449,10 +3450,10 @@
       <c r="J5" s="50"/>
     </row>
     <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="66">
+      <c r="A6" s="80">
         <v>3</v>
       </c>
-      <c r="B6" s="67">
+      <c r="B6" s="83">
         <v>42624</v>
       </c>
       <c r="C6" s="43"/>
@@ -3473,8 +3474,8 @@
       <c r="J6" s="43"/>
     </row>
     <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="66"/>
-      <c r="B7" s="65"/>
+      <c r="A7" s="80"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="43"/>
       <c r="D7" s="43"/>
       <c r="E7" s="43"/>
@@ -3493,8 +3494,8 @@
       <c r="J7" s="43"/>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="66"/>
-      <c r="B8" s="68"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="84"/>
       <c r="C8" s="43"/>
       <c r="D8" s="43"/>
       <c r="E8" s="43"/>
@@ -3538,11 +3539,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A2:A3"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
@@ -3550,6 +3546,11 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3611,20 +3612,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="86" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75" t="s">
+      <c r="D1" s="91"/>
+      <c r="E1" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="76"/>
+      <c r="F1" s="92"/>
       <c r="G1" s="26" t="s">
         <v>82</v>
       </c>
@@ -3642,8 +3643,8 @@
       <c r="S1" s="27"/>
     </row>
     <row r="2" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="71"/>
-      <c r="B2" s="73"/>
+      <c r="A2" s="87"/>
+      <c r="B2" s="89"/>
       <c r="C2" s="28" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Atualizado Ata de Reunião com base no email enviado pelo André . Atualizado Planilha Histórico com a coluna de Numero do Processo Atualizado SIPOC no RoadMap
</commit_message>
<xml_diff>
--- a/TRE_Dados_MapaRaciocinio.xlsx
+++ b/TRE_Dados_MapaRaciocinio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Historicos x Categoria" sheetId="1" r:id="rId1"/>
@@ -14,11 +14,46 @@
     <sheet name="Controle do Projeto" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="B4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Coletar novos Dados</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="127">
   <si>
     <t>Categoria</t>
   </si>
@@ -303,9 +338,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>*Definir a Meta de redução ainda fazendo análise de dados históricos para coleta de médias. A partir destas será possível obter uma meta mais coerente.</t>
-  </si>
-  <si>
     <t>Coleta de dados adicionais, para reajuste das médias.
 (coletar outos itens que não sejam Manutenção e Jardinagem)</t>
   </si>
@@ -319,9 +351,6 @@
     <t>Ivanilda , Silmara e Hélcio</t>
   </si>
   <si>
-    <t xml:space="preserve"> - </t>
-  </si>
-  <si>
     <t>Pendente</t>
   </si>
   <si>
@@ -335,9 +364,6 @@
   </si>
   <si>
     <t>Fazer uma lista com os processos mais importantes.</t>
-  </si>
-  <si>
-    <t>Apresentar os Graficos com os resultados e resaltar a importancia da escolha de um processo simples.</t>
   </si>
   <si>
     <t>Ruhan, André, Ivis, Silmara</t>
@@ -380,6 +406,46 @@
   <si>
     <t>Conclusão
 O histrograma ao lado mostra a frequência de processos e seus respectivos tempos médios. Pode-se observar que  6 processos estão entre  300 e 400 dias, sendo que a média geral encontra-se em 340 dias</t>
+  </si>
+  <si>
+    <t>NUMERO DO PROCESSO</t>
+  </si>
+  <si>
+    <t>Ruhan, André, Ivis, Silmara, Ivanilda, Hélcio, Flávio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Demonstrar Gráfico de Pareto com dados coletados até o momento.
+Analisar possibilidade para definição da Meta de redução.
+Apresentação da ferramenta SIPOC.</t>
+  </si>
+  <si>
+    <t>Apresentar os Graficos com os resultados e resaltar a importancia da escolha de um processo simples</t>
+  </si>
+  <si>
+    <t>Escolher 12 processos candidatos de sua área.</t>
+  </si>
+  <si>
+    <t>Hélcio, Flávio</t>
+  </si>
+  <si>
+    <t>Escolher outros 12 processos candidatos, mais relevantes de sua área.
+(Considerar fazer a separação de Servicos e Aquisição de Bens)</t>
+  </si>
+  <si>
+    <t>Verificar com Pedro a possibilidade de pegarmos 2 processos para análise</t>
+  </si>
+  <si>
+    <t>Silmara, Ivanilda</t>
+  </si>
+  <si>
+    <t>Definir a Meta de redução ainda fazendo análise de dados históricos para coleta de médias. A partir destas será possível obter uma meta mais coerente.</t>
+  </si>
+  <si>
+    <t>Analisar os tempos decorridos dos novos processos candidatos.
+(Considerar o tempo final = Nota de Empenho ou Homologação (RP)</t>
+  </si>
+  <si>
+    <t>REVISAR</t>
   </si>
 </sst>
 </file>
@@ -390,7 +456,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="dd\-mm\-yy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,8 +497,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,6 +549,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="32">
     <border>
@@ -864,14 +962,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1028,43 +1123,69 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1116,9 +1237,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2034,558 +2152,601 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.140625" customWidth="1"/>
-    <col min="2" max="2" width="53.140625" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="59.140625" customWidth="1"/>
+    <col min="3" max="3" width="53.140625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="75"/>
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="12">
+      <c r="E1" s="11">
         <f ca="1">TODAY()</f>
         <v>42683</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="2" spans="1:11" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="68" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="20">
+      <c r="F4" s="19">
         <v>298</v>
       </c>
-      <c r="H4" s="2">
-        <f>E22</f>
+      <c r="I4" s="2">
+        <f>F22</f>
         <v>340.77777777777777</v>
       </c>
-      <c r="I4" s="14">
+      <c r="J4" s="13">
         <v>0</v>
       </c>
-      <c r="J4" s="1">
-        <f>H4-(H4*I4)</f>
+      <c r="K4" s="1">
+        <f>I4-(I4*J4)</f>
         <v>340.77777777777777</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="12">
+      <c r="D5" s="11">
         <v>40668</v>
       </c>
-      <c r="D5" s="12">
+      <c r="E5" s="11">
         <v>41214</v>
       </c>
-      <c r="E5" s="20">
+      <c r="F5" s="19">
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="12">
+      <c r="E6" s="11">
         <v>40973</v>
       </c>
-      <c r="E6" s="20">
+      <c r="F6" s="19">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="12">
+      <c r="D7" s="11">
         <v>40882</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="20">
+      <c r="F7" s="19">
         <v>620</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="12">
+      <c r="D8" s="11">
         <v>40703</v>
       </c>
-      <c r="D8" s="12">
+      <c r="E8" s="11">
         <v>41190</v>
       </c>
-      <c r="E8" s="20">
+      <c r="F8" s="19">
         <v>338</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="12">
+      <c r="E9" s="11">
         <v>41035</v>
       </c>
-      <c r="E9" s="20">
+      <c r="F9" s="19">
         <v>449</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="20">
+      <c r="F10" s="19">
         <v>309</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="12">
+      <c r="D11" s="11">
         <v>41617</v>
       </c>
-      <c r="D11" s="12">
+      <c r="E11" s="11">
         <v>41737</v>
       </c>
-      <c r="E11" s="20">
+      <c r="F11" s="19">
         <v>326</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="12">
+      <c r="D12" s="11">
         <v>41590</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="20">
+      <c r="F12" s="19">
         <v>466</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="12">
+      <c r="D13" s="11">
         <v>41487</v>
       </c>
-      <c r="D13" s="12">
+      <c r="E13" s="11">
         <v>41342</v>
       </c>
-      <c r="E13" s="20">
+      <c r="F13" s="19">
         <v>238</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="12">
+      <c r="E14" s="11">
         <v>42042</v>
       </c>
-      <c r="E14" s="20">
+      <c r="F14" s="19">
         <v>567</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="20">
+      <c r="F15" s="19">
         <v>668</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="18">
+      <c r="D16" s="17">
         <v>42047</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="E16" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="20">
-        <f>DAYS360(C16,D16)</f>
+      <c r="F16" s="19">
+        <f t="shared" ref="F16:F21" si="0">DAYS360(D16,E16)</f>
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="E17" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="20">
-        <f>DAYS360(C17,D17)</f>
+      <c r="F17" s="19">
+        <f t="shared" si="0"/>
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="12">
+      <c r="D18" s="11">
         <v>42135</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="E18" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="20">
-        <f t="shared" ref="E18:E21" si="0">DAYS360(C18,D18)</f>
+      <c r="F18" s="19">
+        <f t="shared" si="0"/>
         <v>247</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="D19" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="12">
+      <c r="E19" s="11">
         <v>42339</v>
       </c>
-      <c r="E19" s="20">
+      <c r="F19" s="19">
         <f t="shared" si="0"/>
         <v>182</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="12">
+      <c r="D20" s="11">
         <v>42226</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="20">
+      <c r="F20" s="19">
         <f t="shared" si="0"/>
         <v>310</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="D21" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="12">
+      <c r="E21" s="11">
         <v>42381</v>
       </c>
-      <c r="E21" s="20">
+      <c r="F21" s="19">
         <f t="shared" si="0"/>
         <v>356</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1">
-        <f>AVERAGE(E4:E21)</f>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1">
+        <f>AVERAGE(F4:F21)</f>
         <v>340.77777777777777</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I45" t="s">
+      <c r="F37" s="1"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
         <v>63</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>1</v>
       </c>
-      <c r="K45">
-        <f>AVERAGEIF(I45:I49,I45,J45:J49)</f>
+      <c r="L45">
+        <f>AVERAGEIF(J45:J49,J45,K45:K49)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I46" t="s">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
         <v>64</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I47" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
         <v>63</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I48" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
         <v>64</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I49" t="s">
+    <row r="49" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
         <v>65</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2593,8 +2754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J148"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2603,15 +2764,18 @@
     <col min="2" max="2" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="74" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -2619,668 +2783,668 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$A$4:$A$21,'Dados Historicos x Categoria'!A4,'Dados Historicos x Categoria'!$E$4:$E$21)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$21,'Dados Historicos x Categoria'!B4,'Dados Historicos x Categoria'!$F$4:$F$21)</f>
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$A$4:$A$21,'Dados Historicos x Categoria'!A5,'Dados Historicos x Categoria'!$E$4:$E$21)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$21,'Dados Historicos x Categoria'!B5,'Dados Historicos x Categoria'!$F$4:$F$21)</f>
         <v>288</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$A$4:$A$21,'Dados Historicos x Categoria'!A6,'Dados Historicos x Categoria'!$E$4:$E$21)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$21,'Dados Historicos x Categoria'!B6,'Dados Historicos x Categoria'!$F$4:$F$21)</f>
         <v>299.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$A$4:$A$21,'Dados Historicos x Categoria'!A7,'Dados Historicos x Categoria'!$E$4:$E$21)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$21,'Dados Historicos x Categoria'!B7,'Dados Historicos x Categoria'!$F$4:$F$21)</f>
         <v>429</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$A$4:$A$21,'Dados Historicos x Categoria'!A8,'Dados Historicos x Categoria'!$E$4:$E$21)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$21,'Dados Historicos x Categoria'!B8,'Dados Historicos x Categoria'!$F$4:$F$21)</f>
         <v>452.5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$A$4:$A$21,'Dados Historicos x Categoria'!A9,'Dados Historicos x Categoria'!$E$4:$E$21)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$21,'Dados Historicos x Categoria'!B9,'Dados Historicos x Categoria'!$F$4:$F$21)</f>
         <v>558.5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$A$4:$A$21,'Dados Historicos x Categoria'!A10,'Dados Historicos x Categoria'!$E$4:$E$21)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$21,'Dados Historicos x Categoria'!B10,'Dados Historicos x Categoria'!$F$4:$F$21)</f>
         <v>309</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$A$4:$A$21,'Dados Historicos x Categoria'!A16,'Dados Historicos x Categoria'!$E$4:$E$21)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$21,'Dados Historicos x Categoria'!B16,'Dados Historicos x Categoria'!$F$4:$F$21)</f>
         <v>260.75</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B12" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$A$4:$A$21,'Dados Historicos x Categoria'!A18,'Dados Historicos x Categoria'!$E$4:$E$21)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$21,'Dados Historicos x Categoria'!B18,'Dados Historicos x Categoria'!$F$4:$F$21)</f>
         <v>247</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="67" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" s="68"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
+      <c r="C17" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="77"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="69"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="69"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="78"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="78"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="69"/>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="78"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="78"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="69"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="78"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="78"/>
+      <c r="E24" s="78"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="78"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69"/>
+      <c r="C25" s="78"/>
+      <c r="D25" s="78"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="78"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="69"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="78"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="69"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="78"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="69"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="78"/>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="69"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="69"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="78"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="69"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="69"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="78"/>
     </row>
     <row r="38" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="70" t="s">
-        <v>117</v>
-      </c>
-      <c r="F39" s="68"/>
-      <c r="G39" s="68"/>
-      <c r="H39" s="68"/>
-      <c r="I39" s="71"/>
+      <c r="E39" s="79" t="s">
+        <v>114</v>
+      </c>
+      <c r="F39" s="77"/>
+      <c r="G39" s="77"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="80"/>
     </row>
     <row r="40" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E40" s="72"/>
-      <c r="F40" s="69"/>
-      <c r="G40" s="69"/>
-      <c r="H40" s="69"/>
-      <c r="I40" s="73"/>
+      <c r="E40" s="81"/>
+      <c r="F40" s="78"/>
+      <c r="G40" s="78"/>
+      <c r="H40" s="78"/>
+      <c r="I40" s="82"/>
     </row>
     <row r="41" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="72"/>
-      <c r="F41" s="69"/>
-      <c r="G41" s="69"/>
-      <c r="H41" s="69"/>
-      <c r="I41" s="73"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="78"/>
+      <c r="G41" s="78"/>
+      <c r="H41" s="78"/>
+      <c r="I41" s="82"/>
     </row>
     <row r="42" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E42" s="72"/>
-      <c r="F42" s="69"/>
-      <c r="G42" s="69"/>
-      <c r="H42" s="69"/>
-      <c r="I42" s="73"/>
+      <c r="E42" s="81"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="78"/>
+      <c r="H42" s="78"/>
+      <c r="I42" s="82"/>
     </row>
     <row r="43" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E43" s="72"/>
-      <c r="F43" s="69"/>
-      <c r="G43" s="69"/>
-      <c r="H43" s="69"/>
-      <c r="I43" s="73"/>
+      <c r="E43" s="81"/>
+      <c r="F43" s="78"/>
+      <c r="G43" s="78"/>
+      <c r="H43" s="78"/>
+      <c r="I43" s="82"/>
     </row>
     <row r="44" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E44" s="72"/>
-      <c r="F44" s="69"/>
-      <c r="G44" s="69"/>
-      <c r="H44" s="69"/>
-      <c r="I44" s="73"/>
+      <c r="E44" s="81"/>
+      <c r="F44" s="78"/>
+      <c r="G44" s="78"/>
+      <c r="H44" s="78"/>
+      <c r="I44" s="82"/>
     </row>
     <row r="45" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E45" s="72"/>
-      <c r="F45" s="69"/>
-      <c r="G45" s="69"/>
-      <c r="H45" s="69"/>
-      <c r="I45" s="73"/>
+      <c r="E45" s="81"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="78"/>
+      <c r="H45" s="78"/>
+      <c r="I45" s="82"/>
     </row>
     <row r="46" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E46" s="72"/>
-      <c r="F46" s="69"/>
-      <c r="G46" s="69"/>
-      <c r="H46" s="69"/>
-      <c r="I46" s="73"/>
+      <c r="E46" s="81"/>
+      <c r="F46" s="78"/>
+      <c r="G46" s="78"/>
+      <c r="H46" s="78"/>
+      <c r="I46" s="82"/>
     </row>
     <row r="47" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E47" s="72"/>
-      <c r="F47" s="69"/>
-      <c r="G47" s="69"/>
-      <c r="H47" s="69"/>
-      <c r="I47" s="73"/>
+      <c r="E47" s="81"/>
+      <c r="F47" s="78"/>
+      <c r="G47" s="78"/>
+      <c r="H47" s="78"/>
+      <c r="I47" s="82"/>
     </row>
     <row r="48" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E48" s="72"/>
-      <c r="F48" s="69"/>
-      <c r="G48" s="69"/>
-      <c r="H48" s="69"/>
-      <c r="I48" s="73"/>
+      <c r="E48" s="81"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="78"/>
+      <c r="H48" s="78"/>
+      <c r="I48" s="82"/>
     </row>
     <row r="49" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E49" s="72"/>
-      <c r="F49" s="69"/>
-      <c r="G49" s="69"/>
-      <c r="H49" s="69"/>
-      <c r="I49" s="73"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="78"/>
+      <c r="G49" s="78"/>
+      <c r="H49" s="78"/>
+      <c r="I49" s="82"/>
     </row>
     <row r="50" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E50" s="72"/>
-      <c r="F50" s="69"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="69"/>
-      <c r="I50" s="73"/>
+      <c r="E50" s="81"/>
+      <c r="F50" s="78"/>
+      <c r="G50" s="78"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="82"/>
     </row>
     <row r="51" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E51" s="74"/>
-      <c r="F51" s="75"/>
-      <c r="G51" s="75"/>
-      <c r="H51" s="75"/>
-      <c r="I51" s="76"/>
+      <c r="E51" s="83"/>
+      <c r="F51" s="84"/>
+      <c r="G51" s="84"/>
+      <c r="H51" s="84"/>
+      <c r="I51" s="85"/>
     </row>
     <row r="64" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="70" t="s">
-        <v>114</v>
-      </c>
-      <c r="D65" s="68"/>
-      <c r="E65" s="68"/>
-      <c r="F65" s="68"/>
-      <c r="G65" s="71"/>
+      <c r="C65" s="79" t="s">
+        <v>111</v>
+      </c>
+      <c r="D65" s="77"/>
+      <c r="E65" s="77"/>
+      <c r="F65" s="77"/>
+      <c r="G65" s="80"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="72"/>
-      <c r="D66" s="69"/>
-      <c r="E66" s="69"/>
-      <c r="F66" s="69"/>
-      <c r="G66" s="73"/>
+      <c r="C66" s="81"/>
+      <c r="D66" s="78"/>
+      <c r="E66" s="78"/>
+      <c r="F66" s="78"/>
+      <c r="G66" s="82"/>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="72"/>
-      <c r="D67" s="69"/>
-      <c r="E67" s="69"/>
-      <c r="F67" s="69"/>
-      <c r="G67" s="73"/>
+      <c r="C67" s="81"/>
+      <c r="D67" s="78"/>
+      <c r="E67" s="78"/>
+      <c r="F67" s="78"/>
+      <c r="G67" s="82"/>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C68" s="72"/>
-      <c r="D68" s="69"/>
-      <c r="E68" s="69"/>
-      <c r="F68" s="69"/>
-      <c r="G68" s="73"/>
+      <c r="C68" s="81"/>
+      <c r="D68" s="78"/>
+      <c r="E68" s="78"/>
+      <c r="F68" s="78"/>
+      <c r="G68" s="82"/>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="72"/>
-      <c r="D69" s="69"/>
-      <c r="E69" s="69"/>
-      <c r="F69" s="69"/>
-      <c r="G69" s="73"/>
+      <c r="C69" s="81"/>
+      <c r="D69" s="78"/>
+      <c r="E69" s="78"/>
+      <c r="F69" s="78"/>
+      <c r="G69" s="82"/>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="72"/>
-      <c r="D70" s="69"/>
-      <c r="E70" s="69"/>
-      <c r="F70" s="69"/>
-      <c r="G70" s="73"/>
+      <c r="C70" s="81"/>
+      <c r="D70" s="78"/>
+      <c r="E70" s="78"/>
+      <c r="F70" s="78"/>
+      <c r="G70" s="82"/>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C71" s="72"/>
-      <c r="D71" s="69"/>
-      <c r="E71" s="69"/>
-      <c r="F71" s="69"/>
-      <c r="G71" s="73"/>
+      <c r="C71" s="81"/>
+      <c r="D71" s="78"/>
+      <c r="E71" s="78"/>
+      <c r="F71" s="78"/>
+      <c r="G71" s="82"/>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="72"/>
-      <c r="D72" s="69"/>
-      <c r="E72" s="69"/>
-      <c r="F72" s="69"/>
-      <c r="G72" s="73"/>
+      <c r="C72" s="81"/>
+      <c r="D72" s="78"/>
+      <c r="E72" s="78"/>
+      <c r="F72" s="78"/>
+      <c r="G72" s="82"/>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="72"/>
-      <c r="D73" s="69"/>
-      <c r="E73" s="69"/>
-      <c r="F73" s="69"/>
-      <c r="G73" s="73"/>
+      <c r="C73" s="81"/>
+      <c r="D73" s="78"/>
+      <c r="E73" s="78"/>
+      <c r="F73" s="78"/>
+      <c r="G73" s="82"/>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="72"/>
-      <c r="D74" s="69"/>
-      <c r="E74" s="69"/>
-      <c r="F74" s="69"/>
-      <c r="G74" s="73"/>
+      <c r="C74" s="81"/>
+      <c r="D74" s="78"/>
+      <c r="E74" s="78"/>
+      <c r="F74" s="78"/>
+      <c r="G74" s="82"/>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="72"/>
-      <c r="D75" s="69"/>
-      <c r="E75" s="69"/>
-      <c r="F75" s="69"/>
-      <c r="G75" s="73"/>
+      <c r="C75" s="81"/>
+      <c r="D75" s="78"/>
+      <c r="E75" s="78"/>
+      <c r="F75" s="78"/>
+      <c r="G75" s="82"/>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="72"/>
-      <c r="D76" s="69"/>
-      <c r="E76" s="69"/>
-      <c r="F76" s="69"/>
-      <c r="G76" s="73"/>
+      <c r="C76" s="81"/>
+      <c r="D76" s="78"/>
+      <c r="E76" s="78"/>
+      <c r="F76" s="78"/>
+      <c r="G76" s="82"/>
     </row>
     <row r="77" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C77" s="74"/>
-      <c r="D77" s="75"/>
-      <c r="E77" s="75"/>
-      <c r="F77" s="75"/>
-      <c r="G77" s="76"/>
+      <c r="C77" s="83"/>
+      <c r="D77" s="84"/>
+      <c r="E77" s="84"/>
+      <c r="F77" s="84"/>
+      <c r="G77" s="85"/>
     </row>
     <row r="84" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="65"/>
+      <c r="J84" s="64"/>
     </row>
     <row r="85" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J85" s="65"/>
+      <c r="J85" s="64"/>
     </row>
     <row r="86" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C86" s="70" t="s">
-        <v>115</v>
-      </c>
-      <c r="D86" s="68"/>
-      <c r="E86" s="68"/>
-      <c r="F86" s="68"/>
-      <c r="G86" s="71"/>
-      <c r="J86" s="65"/>
+      <c r="C86" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="D86" s="77"/>
+      <c r="E86" s="77"/>
+      <c r="F86" s="77"/>
+      <c r="G86" s="80"/>
+      <c r="J86" s="64"/>
     </row>
     <row r="87" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C87" s="72"/>
-      <c r="D87" s="69"/>
-      <c r="E87" s="69"/>
-      <c r="F87" s="69"/>
-      <c r="G87" s="73"/>
-      <c r="J87" s="65"/>
+      <c r="C87" s="81"/>
+      <c r="D87" s="78"/>
+      <c r="E87" s="78"/>
+      <c r="F87" s="78"/>
+      <c r="G87" s="82"/>
+      <c r="J87" s="64"/>
     </row>
     <row r="88" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C88" s="72"/>
-      <c r="D88" s="69"/>
-      <c r="E88" s="69"/>
-      <c r="F88" s="69"/>
-      <c r="G88" s="73"/>
-      <c r="J88" s="65"/>
+      <c r="C88" s="81"/>
+      <c r="D88" s="78"/>
+      <c r="E88" s="78"/>
+      <c r="F88" s="78"/>
+      <c r="G88" s="82"/>
+      <c r="J88" s="64"/>
     </row>
     <row r="89" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C89" s="72"/>
-      <c r="D89" s="69"/>
-      <c r="E89" s="69"/>
-      <c r="F89" s="69"/>
-      <c r="G89" s="73"/>
-      <c r="J89" s="65"/>
+      <c r="C89" s="81"/>
+      <c r="D89" s="78"/>
+      <c r="E89" s="78"/>
+      <c r="F89" s="78"/>
+      <c r="G89" s="82"/>
+      <c r="J89" s="64"/>
     </row>
     <row r="90" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C90" s="72"/>
-      <c r="D90" s="69"/>
-      <c r="E90" s="69"/>
-      <c r="F90" s="69"/>
-      <c r="G90" s="73"/>
-      <c r="J90" s="65"/>
+      <c r="C90" s="81"/>
+      <c r="D90" s="78"/>
+      <c r="E90" s="78"/>
+      <c r="F90" s="78"/>
+      <c r="G90" s="82"/>
+      <c r="J90" s="64"/>
     </row>
     <row r="91" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C91" s="72"/>
-      <c r="D91" s="69"/>
-      <c r="E91" s="69"/>
-      <c r="F91" s="69"/>
-      <c r="G91" s="73"/>
-      <c r="J91" s="65"/>
+      <c r="C91" s="81"/>
+      <c r="D91" s="78"/>
+      <c r="E91" s="78"/>
+      <c r="F91" s="78"/>
+      <c r="G91" s="82"/>
+      <c r="J91" s="64"/>
     </row>
     <row r="92" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C92" s="72"/>
-      <c r="D92" s="69"/>
-      <c r="E92" s="69"/>
-      <c r="F92" s="69"/>
-      <c r="G92" s="73"/>
-      <c r="J92" s="65"/>
+      <c r="C92" s="81"/>
+      <c r="D92" s="78"/>
+      <c r="E92" s="78"/>
+      <c r="F92" s="78"/>
+      <c r="G92" s="82"/>
+      <c r="J92" s="64"/>
     </row>
     <row r="93" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C93" s="72"/>
-      <c r="D93" s="69"/>
-      <c r="E93" s="69"/>
-      <c r="F93" s="69"/>
-      <c r="G93" s="73"/>
-      <c r="J93" s="65"/>
+      <c r="C93" s="81"/>
+      <c r="D93" s="78"/>
+      <c r="E93" s="78"/>
+      <c r="F93" s="78"/>
+      <c r="G93" s="82"/>
+      <c r="J93" s="64"/>
     </row>
     <row r="94" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C94" s="72"/>
-      <c r="D94" s="69"/>
-      <c r="E94" s="69"/>
-      <c r="F94" s="69"/>
-      <c r="G94" s="73"/>
-      <c r="J94" s="65"/>
+      <c r="C94" s="81"/>
+      <c r="D94" s="78"/>
+      <c r="E94" s="78"/>
+      <c r="F94" s="78"/>
+      <c r="G94" s="82"/>
+      <c r="J94" s="64"/>
     </row>
     <row r="95" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C95" s="72"/>
-      <c r="D95" s="69"/>
-      <c r="E95" s="69"/>
-      <c r="F95" s="69"/>
-      <c r="G95" s="73"/>
-      <c r="J95" s="65"/>
+      <c r="C95" s="81"/>
+      <c r="D95" s="78"/>
+      <c r="E95" s="78"/>
+      <c r="F95" s="78"/>
+      <c r="G95" s="82"/>
+      <c r="J95" s="64"/>
     </row>
     <row r="96" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C96" s="72"/>
-      <c r="D96" s="69"/>
-      <c r="E96" s="69"/>
-      <c r="F96" s="69"/>
-      <c r="G96" s="73"/>
-      <c r="J96" s="65"/>
+      <c r="C96" s="81"/>
+      <c r="D96" s="78"/>
+      <c r="E96" s="78"/>
+      <c r="F96" s="78"/>
+      <c r="G96" s="82"/>
+      <c r="J96" s="64"/>
     </row>
     <row r="97" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C97" s="72"/>
-      <c r="D97" s="69"/>
-      <c r="E97" s="69"/>
-      <c r="F97" s="69"/>
-      <c r="G97" s="73"/>
+      <c r="C97" s="81"/>
+      <c r="D97" s="78"/>
+      <c r="E97" s="78"/>
+      <c r="F97" s="78"/>
+      <c r="G97" s="82"/>
     </row>
     <row r="98" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C98" s="74"/>
-      <c r="D98" s="75"/>
-      <c r="E98" s="75"/>
-      <c r="F98" s="75"/>
-      <c r="G98" s="76"/>
+      <c r="C98" s="83"/>
+      <c r="D98" s="84"/>
+      <c r="E98" s="84"/>
+      <c r="F98" s="84"/>
+      <c r="G98" s="85"/>
     </row>
     <row r="108" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="109" spans="3:10" ht="315" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F109" s="77" t="s">
-        <v>116</v>
-      </c>
-      <c r="G109" s="78"/>
-      <c r="H109" s="78"/>
-      <c r="I109" s="79"/>
+      <c r="F109" s="86" t="s">
+        <v>113</v>
+      </c>
+      <c r="G109" s="87"/>
+      <c r="H109" s="87"/>
+      <c r="I109" s="88"/>
     </row>
     <row r="110" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F110" s="64"/>
-      <c r="G110" s="65"/>
-      <c r="H110" s="65"/>
-      <c r="I110" s="65"/>
+      <c r="F110" s="63"/>
+      <c r="G110" s="64"/>
+      <c r="H110" s="64"/>
+      <c r="I110" s="64"/>
     </row>
     <row r="111" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F111" s="65"/>
-      <c r="G111" s="65"/>
-      <c r="H111" s="65"/>
-      <c r="I111" s="65"/>
-      <c r="J111" s="21"/>
+      <c r="F111" s="64"/>
+      <c r="G111" s="64"/>
+      <c r="H111" s="64"/>
+      <c r="I111" s="64"/>
+      <c r="J111" s="20"/>
     </row>
     <row r="112" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F112" s="65"/>
-      <c r="G112" s="65"/>
-      <c r="H112" s="65"/>
-      <c r="I112" s="65"/>
-      <c r="J112" s="21"/>
+      <c r="F112" s="64"/>
+      <c r="G112" s="64"/>
+      <c r="H112" s="64"/>
+      <c r="I112" s="64"/>
+      <c r="J112" s="20"/>
     </row>
     <row r="113" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F113" s="65"/>
-      <c r="G113" s="65"/>
-      <c r="H113" s="65"/>
-      <c r="I113" s="65"/>
-      <c r="J113" s="21"/>
+      <c r="F113" s="64"/>
+      <c r="G113" s="64"/>
+      <c r="H113" s="64"/>
+      <c r="I113" s="64"/>
+      <c r="J113" s="20"/>
     </row>
     <row r="114" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F114" s="65"/>
-      <c r="G114" s="65"/>
-      <c r="H114" s="65"/>
-      <c r="I114" s="65"/>
-      <c r="J114" s="21"/>
+      <c r="F114" s="64"/>
+      <c r="G114" s="64"/>
+      <c r="H114" s="64"/>
+      <c r="I114" s="64"/>
+      <c r="J114" s="20"/>
     </row>
     <row r="115" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F115" s="65"/>
-      <c r="G115" s="65"/>
-      <c r="H115" s="65"/>
-      <c r="I115" s="65"/>
-      <c r="J115" s="21"/>
+      <c r="F115" s="64"/>
+      <c r="G115" s="64"/>
+      <c r="H115" s="64"/>
+      <c r="I115" s="64"/>
+      <c r="J115" s="20"/>
     </row>
     <row r="116" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F116" s="65"/>
-      <c r="G116" s="65"/>
-      <c r="H116" s="65"/>
-      <c r="I116" s="65"/>
-      <c r="J116" s="21"/>
+      <c r="F116" s="64"/>
+      <c r="G116" s="64"/>
+      <c r="H116" s="64"/>
+      <c r="I116" s="64"/>
+      <c r="J116" s="20"/>
     </row>
     <row r="117" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F117" s="65"/>
-      <c r="G117" s="65"/>
-      <c r="H117" s="65"/>
-      <c r="I117" s="65"/>
-      <c r="J117" s="21"/>
+      <c r="F117" s="64"/>
+      <c r="G117" s="64"/>
+      <c r="H117" s="64"/>
+      <c r="I117" s="64"/>
+      <c r="J117" s="20"/>
     </row>
     <row r="118" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F118" s="65"/>
-      <c r="G118" s="65"/>
-      <c r="H118" s="65"/>
-      <c r="I118" s="65"/>
-      <c r="J118" s="21"/>
+      <c r="F118" s="64"/>
+      <c r="G118" s="64"/>
+      <c r="H118" s="64"/>
+      <c r="I118" s="64"/>
+      <c r="J118" s="20"/>
     </row>
     <row r="119" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F119" s="65"/>
-      <c r="G119" s="65"/>
-      <c r="H119" s="65"/>
-      <c r="I119" s="65"/>
-      <c r="J119" s="21"/>
+      <c r="F119" s="64"/>
+      <c r="G119" s="64"/>
+      <c r="H119" s="64"/>
+      <c r="I119" s="64"/>
+      <c r="J119" s="20"/>
     </row>
     <row r="120" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F120" s="65"/>
-      <c r="G120" s="65"/>
-      <c r="H120" s="65"/>
-      <c r="I120" s="65"/>
-      <c r="J120" s="21"/>
+      <c r="F120" s="64"/>
+      <c r="G120" s="64"/>
+      <c r="H120" s="64"/>
+      <c r="I120" s="64"/>
+      <c r="J120" s="20"/>
     </row>
     <row r="121" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F121" s="65"/>
-      <c r="G121" s="65"/>
-      <c r="H121" s="65"/>
-      <c r="I121" s="65"/>
-      <c r="J121" s="21"/>
+      <c r="F121" s="64"/>
+      <c r="G121" s="64"/>
+      <c r="H121" s="64"/>
+      <c r="I121" s="64"/>
+      <c r="J121" s="20"/>
     </row>
     <row r="136" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E136" s="66"/>
-      <c r="F136" s="66"/>
-      <c r="G136" s="66"/>
-      <c r="H136" s="66"/>
-      <c r="I136" s="66"/>
+      <c r="E136" s="65"/>
+      <c r="F136" s="65"/>
+      <c r="G136" s="65"/>
+      <c r="H136" s="65"/>
+      <c r="I136" s="65"/>
     </row>
     <row r="137" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E137" s="66"/>
-      <c r="F137" s="66"/>
-      <c r="G137" s="66"/>
-      <c r="H137" s="66"/>
-      <c r="I137" s="66"/>
+      <c r="E137" s="65"/>
+      <c r="F137" s="65"/>
+      <c r="G137" s="65"/>
+      <c r="H137" s="65"/>
+      <c r="I137" s="65"/>
     </row>
     <row r="138" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E138" s="66"/>
-      <c r="F138" s="66"/>
-      <c r="G138" s="66"/>
-      <c r="H138" s="66"/>
-      <c r="I138" s="66"/>
+      <c r="E138" s="65"/>
+      <c r="F138" s="65"/>
+      <c r="G138" s="65"/>
+      <c r="H138" s="65"/>
+      <c r="I138" s="65"/>
     </row>
     <row r="139" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E139" s="66"/>
-      <c r="F139" s="66"/>
-      <c r="G139" s="66"/>
-      <c r="H139" s="66"/>
-      <c r="I139" s="66"/>
+      <c r="E139" s="65"/>
+      <c r="F139" s="65"/>
+      <c r="G139" s="65"/>
+      <c r="H139" s="65"/>
+      <c r="I139" s="65"/>
     </row>
     <row r="140" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E140" s="66"/>
-      <c r="F140" s="66"/>
-      <c r="G140" s="66"/>
-      <c r="H140" s="66"/>
-      <c r="I140" s="66"/>
+      <c r="E140" s="65"/>
+      <c r="F140" s="65"/>
+      <c r="G140" s="65"/>
+      <c r="H140" s="65"/>
+      <c r="I140" s="65"/>
     </row>
     <row r="141" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E141" s="66"/>
-      <c r="F141" s="66"/>
-      <c r="G141" s="66"/>
-      <c r="H141" s="66"/>
-      <c r="I141" s="66"/>
+      <c r="E141" s="65"/>
+      <c r="F141" s="65"/>
+      <c r="G141" s="65"/>
+      <c r="H141" s="65"/>
+      <c r="I141" s="65"/>
     </row>
     <row r="142" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E142" s="66"/>
-      <c r="F142" s="66"/>
-      <c r="G142" s="66"/>
-      <c r="H142" s="66"/>
-      <c r="I142" s="66"/>
+      <c r="E142" s="65"/>
+      <c r="F142" s="65"/>
+      <c r="G142" s="65"/>
+      <c r="H142" s="65"/>
+      <c r="I142" s="65"/>
     </row>
     <row r="143" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E143" s="66"/>
-      <c r="F143" s="66"/>
-      <c r="G143" s="66"/>
-      <c r="H143" s="66"/>
-      <c r="I143" s="66"/>
+      <c r="E143" s="65"/>
+      <c r="F143" s="65"/>
+      <c r="G143" s="65"/>
+      <c r="H143" s="65"/>
+      <c r="I143" s="65"/>
     </row>
     <row r="144" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E144" s="66"/>
-      <c r="F144" s="66"/>
-      <c r="G144" s="66"/>
-      <c r="H144" s="66"/>
-      <c r="I144" s="66"/>
+      <c r="E144" s="65"/>
+      <c r="F144" s="65"/>
+      <c r="G144" s="65"/>
+      <c r="H144" s="65"/>
+      <c r="I144" s="65"/>
     </row>
     <row r="145" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E145" s="66"/>
-      <c r="F145" s="66"/>
-      <c r="G145" s="66"/>
-      <c r="H145" s="66"/>
-      <c r="I145" s="66"/>
+      <c r="E145" s="65"/>
+      <c r="F145" s="65"/>
+      <c r="G145" s="65"/>
+      <c r="H145" s="65"/>
+      <c r="I145" s="65"/>
     </row>
     <row r="146" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E146" s="66"/>
-      <c r="F146" s="66"/>
-      <c r="G146" s="66"/>
-      <c r="H146" s="66"/>
-      <c r="I146" s="66"/>
+      <c r="E146" s="65"/>
+      <c r="F146" s="65"/>
+      <c r="G146" s="65"/>
+      <c r="H146" s="65"/>
+      <c r="I146" s="65"/>
     </row>
     <row r="147" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E147" s="66"/>
-      <c r="F147" s="66"/>
-      <c r="G147" s="66"/>
-      <c r="H147" s="66"/>
-      <c r="I147" s="66"/>
+      <c r="E147" s="65"/>
+      <c r="F147" s="65"/>
+      <c r="G147" s="65"/>
+      <c r="H147" s="65"/>
+      <c r="I147" s="65"/>
     </row>
     <row r="148" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E148" s="66"/>
-      <c r="F148" s="66"/>
-      <c r="G148" s="66"/>
-      <c r="H148" s="66"/>
-      <c r="I148" s="66"/>
+      <c r="E148" s="65"/>
+      <c r="F148" s="65"/>
+      <c r="G148" s="65"/>
+      <c r="H148" s="65"/>
+      <c r="I148" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3297,262 +3461,355 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="61"/>
-    <col min="2" max="2" width="10.7109375" style="61" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="61" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="61" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="61"/>
-    <col min="6" max="6" width="29.42578125" style="61" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="61" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="61" customWidth="1"/>
-    <col min="9" max="9" width="12" style="61" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" style="61" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="60"/>
+    <col min="2" max="2" width="15.5703125" style="60" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="60" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="60" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="60"/>
+    <col min="6" max="6" width="29.42578125" style="60" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" style="60" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="60" customWidth="1"/>
+    <col min="9" max="9" width="12" style="60" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="24" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="59" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81">
+    <row r="2" spans="1:10" s="58" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="90">
         <v>1</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="89" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="89" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="80" t="s">
+      <c r="D2" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="80">
+      <c r="E2" s="89">
         <v>2</v>
       </c>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="61">
+        <v>42440</v>
+      </c>
+      <c r="I2" s="72" t="s">
+        <v>104</v>
+      </c>
+      <c r="J2" s="42"/>
+    </row>
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="91"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="H2" s="62">
+      <c r="H3" s="61">
         <v>42440</v>
       </c>
-      <c r="I2" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="J2" s="43"/>
-    </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="82"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="G3" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="H3" s="62">
+      <c r="I3" s="72" t="s">
+        <v>104</v>
+      </c>
+      <c r="J3" s="42"/>
+    </row>
+    <row r="4" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="89">
+        <v>2</v>
+      </c>
+      <c r="B4" s="94">
         <v>42440</v>
       </c>
-      <c r="I3" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="J3" s="43"/>
-    </row>
-    <row r="4" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="80">
+      <c r="C4" s="89" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="89" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="90">
         <v>2</v>
       </c>
-      <c r="B4" s="85">
+      <c r="F4" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="61">
         <v>42440</v>
       </c>
-      <c r="C4" s="80" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="80" t="s">
-        <v>102</v>
-      </c>
-      <c r="E4" s="81">
+      <c r="I4" s="72" t="s">
+        <v>104</v>
+      </c>
+      <c r="J4" s="42"/>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="90"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="62">
+        <v>42440</v>
+      </c>
+      <c r="I5" s="72" t="s">
+        <v>104</v>
+      </c>
+      <c r="J5" s="49"/>
+    </row>
+    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="89">
+        <v>3</v>
+      </c>
+      <c r="B6" s="92">
+        <v>42624</v>
+      </c>
+      <c r="C6" s="90" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="90" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="90">
         <v>2</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F6" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="61">
+        <v>42624</v>
+      </c>
+      <c r="I6" s="72" t="s">
         <v>104</v>
       </c>
-      <c r="G4" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="H4" s="62">
-        <v>42440</v>
-      </c>
-      <c r="I4" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="J4" s="43"/>
-    </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="81"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="50" t="s">
-        <v>103</v>
-      </c>
-      <c r="G5" s="50" t="s">
+      <c r="J6" s="42"/>
+    </row>
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="89"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="69" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" s="70" t="s">
+        <v>120</v>
+      </c>
+      <c r="H7" s="61">
+        <v>42624</v>
+      </c>
+      <c r="I7" s="72" t="s">
+        <v>104</v>
+      </c>
+      <c r="J7" s="42"/>
+    </row>
+    <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="89"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="66" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="71">
+        <v>42691</v>
+      </c>
+      <c r="I8" s="73" t="s">
+        <v>98</v>
+      </c>
+      <c r="J8" s="66"/>
+    </row>
+    <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="89"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" s="71">
+        <v>42691</v>
+      </c>
+      <c r="I9" s="73" t="s">
+        <v>98</v>
+      </c>
+      <c r="J9" s="66"/>
+    </row>
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="89"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="H10" s="61">
+        <v>42624</v>
+      </c>
+      <c r="I10" s="73" t="s">
+        <v>98</v>
+      </c>
+      <c r="J10" s="42"/>
+    </row>
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="89">
+        <v>4</v>
+      </c>
+      <c r="B11" s="89" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="H5" s="63">
-        <v>42440</v>
-      </c>
-      <c r="I5" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="J5" s="50"/>
-    </row>
-    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="80">
-        <v>3</v>
-      </c>
-      <c r="B6" s="83">
-        <v>42624</v>
-      </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43" t="s">
+      <c r="H11" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="G6" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="H6" s="62">
-        <v>42624</v>
-      </c>
-      <c r="I6" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="J6" s="43"/>
-    </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="80"/>
-      <c r="B7" s="82"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43" t="s">
+      <c r="I11" s="73" t="s">
+        <v>98</v>
+      </c>
+      <c r="J11" s="66"/>
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="89"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="69" t="s">
+        <v>105</v>
+      </c>
+      <c r="G12" s="66" t="s">
         <v>108</v>
       </c>
-      <c r="G7" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="H7" s="62">
-        <v>42624</v>
-      </c>
-      <c r="I7" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="J7" s="43"/>
-    </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="80"/>
-      <c r="B8" s="84"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="G8" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="H8" s="62">
-        <v>42624</v>
-      </c>
-      <c r="I8" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="J8" s="43"/>
-    </row>
-    <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="43">
-        <v>4</v>
-      </c>
-      <c r="B9" s="43" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="G9" s="43" t="s">
+      <c r="H12" s="67">
+        <v>42690</v>
+      </c>
+      <c r="I12" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="H9" s="43" t="s">
-        <v>96</v>
-      </c>
-      <c r="I9" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="J9" s="43"/>
+      <c r="J12" s="66"/>
+    </row>
+    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="89"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="69" t="s">
+        <v>124</v>
+      </c>
+      <c r="G13" s="66" t="s">
+        <v>108</v>
+      </c>
+      <c r="H13" s="67">
+        <v>42690</v>
+      </c>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="20">
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B6:B10"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="E6:E10"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3572,7 +3829,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3586,10 +3843,10 @@
       <c r="C2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>41883</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="16">
         <v>51</v>
       </c>
     </row>
@@ -3612,417 +3869,417 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="97" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="99" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91" t="s">
+      <c r="D1" s="100"/>
+      <c r="E1" s="100" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="92"/>
-      <c r="G1" s="26" t="s">
+      <c r="F1" s="101"/>
+      <c r="G1" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
     </row>
     <row r="2" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="87"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="28" t="s">
+      <c r="A2" s="96"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="G2" s="31">
+      <c r="G2" s="30">
         <v>42690</v>
       </c>
-      <c r="H2" s="31">
+      <c r="H2" s="30">
         <v>42720</v>
       </c>
-      <c r="I2" s="31">
+      <c r="I2" s="30">
         <v>42751</v>
       </c>
-      <c r="J2" s="31">
+      <c r="J2" s="30">
         <v>42782</v>
       </c>
-      <c r="K2" s="31">
+      <c r="K2" s="30">
         <v>42810</v>
       </c>
-      <c r="L2" s="31">
+      <c r="L2" s="30">
         <v>42841</v>
       </c>
-      <c r="M2" s="31">
+      <c r="M2" s="30">
         <v>42871</v>
       </c>
-      <c r="N2" s="31">
+      <c r="N2" s="30">
         <v>42902</v>
       </c>
-      <c r="O2" s="31">
+      <c r="O2" s="30">
         <v>42932</v>
       </c>
-      <c r="P2" s="31">
+      <c r="P2" s="30">
         <v>42963</v>
       </c>
-      <c r="Q2" s="31">
+      <c r="Q2" s="30">
         <v>42994</v>
       </c>
-      <c r="R2" s="31">
+      <c r="R2" s="30">
         <v>43024</v>
       </c>
-      <c r="S2" s="31">
+      <c r="S2" s="30">
         <v>43055</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32">
+      <c r="A3" s="31">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="36"/>
+      <c r="S3" s="36"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38">
+      <c r="A4" s="37">
         <v>2</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
     </row>
     <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38">
+      <c r="A5" s="37">
         <v>3</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="36"/>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="36"/>
+      <c r="S5" s="36"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38">
+      <c r="A6" s="37">
         <v>4</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38">
+      <c r="A7" s="37">
         <v>5</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="44"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="36"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="36"/>
+      <c r="S7" s="36"/>
     </row>
     <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38">
+      <c r="A8" s="37">
         <v>6</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="44"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="37"/>
-      <c r="S8" s="37"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="36"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="36"/>
+      <c r="S8" s="36"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="38">
+      <c r="A9" s="37">
         <v>7</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="36"/>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="36"/>
+      <c r="S9" s="36"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="38">
+      <c r="A10" s="37">
         <v>8</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="37"/>
-      <c r="S10" s="37"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="36"/>
+      <c r="S10" s="36"/>
     </row>
     <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="38">
+      <c r="A11" s="37">
         <v>9</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="44"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="37"/>
-      <c r="S11" s="37"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="36"/>
+      <c r="S11" s="36"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="38">
+      <c r="A12" s="37">
         <v>10</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="37"/>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="37"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="42"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="36"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="38">
+      <c r="A13" s="37">
         <v>11</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="44"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="37"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="45">
+      <c r="A14" s="44">
         <v>12</v>
       </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="51"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="37"/>
-      <c r="S14" s="37"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="36"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="52"/>
-      <c r="B15" s="53" t="s">
+      <c r="A15" s="51"/>
+      <c r="B15" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="54" t="s">
+      <c r="C15" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55" t="s">
+      <c r="D15" s="54"/>
+      <c r="E15" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="F15" s="56"/>
-      <c r="G15" s="52">
+      <c r="F15" s="55"/>
+      <c r="G15" s="51">
         <v>30</v>
       </c>
-      <c r="H15" s="57">
+      <c r="H15" s="56">
         <v>30</v>
       </c>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="57"/>
-      <c r="N15" s="57"/>
-      <c r="O15" s="58"/>
-      <c r="P15" s="58"/>
-      <c r="Q15" s="58"/>
-      <c r="R15" s="58"/>
-      <c r="S15" s="58"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Atualizado dados da Ata para a reunião do dia 01/12 Atuallizado Lista de Processos com os novos processos de Dispensa enviado pelo Helcio
</commit_message>
<xml_diff>
--- a/TRE_Dados_MapaRaciocinio.xlsx
+++ b/TRE_Dados_MapaRaciocinio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Historicos x Categoria" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="143">
   <si>
     <t>Categoria</t>
   </si>
@@ -388,6 +388,78 @@
   </si>
   <si>
     <t>Analisar SIPOC e FluxoGrama , se for possível usar um bypass para chegar a um ponto comum poderemos aplicar soluções semelhantes que abordem as 2 áreas.</t>
+  </si>
+  <si>
+    <t>Licitação</t>
+  </si>
+  <si>
+    <t>Forma de Contratação</t>
+  </si>
+  <si>
+    <t>Dispença</t>
+  </si>
+  <si>
+    <t>Ruhan, Ivis, Iva, Alceu,Silmara, Jeronimo e Helcio</t>
+  </si>
+  <si>
+    <t>Definição das médias por 3 grandes grupos (Licitação, Dispensa e Registro de Preços)</t>
+  </si>
+  <si>
+    <t>Definição da Meta</t>
+  </si>
+  <si>
+    <t>Início do FluxoGrama</t>
+  </si>
+  <si>
+    <t>Termo de dispença e abertura de licitação – Levantar mais categorias</t>
+  </si>
+  <si>
+    <t>Iva</t>
+  </si>
+  <si>
+    <t>Repassar pra Iva/Helcio coletar os dados de forma de contratação (licitação/dispença)</t>
+  </si>
+  <si>
+    <t>Iva / Helcio</t>
+  </si>
+  <si>
+    <t>Ajustar o Grafico de Pareto por Dispença/RP</t>
+  </si>
+  <si>
+    <t>Atacar o processo de Serviço de Mão de Obra continuada</t>
+  </si>
+  <si>
+    <t>Flavio</t>
+  </si>
+  <si>
+    <t>Incluir os telefones do Alceu (99605-4979) e Jerônimo (99631-9673)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2462/2015 </t>
+  </si>
+  <si>
+    <t>Dispensa</t>
+  </si>
+  <si>
+    <t>Alarme-Monitoramento</t>
+  </si>
+  <si>
+    <t>6475/2015</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>12566/2016</t>
+  </si>
+  <si>
+    <t>1247/2016</t>
+  </si>
+  <si>
+    <t>8379/2014</t>
+  </si>
+  <si>
+    <t>2370/2014</t>
   </si>
 </sst>
 </file>
@@ -398,7 +470,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="dd\-mm\-yy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -452,6 +524,13 @@
       <color rgb="FF0000FF"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12.1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -922,7 +1001,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1100,106 +1179,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1207,6 +1192,138 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2133,606 +2250,828 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:F17"/>
+      <pane ySplit="3" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="59.140625" customWidth="1"/>
-    <col min="3" max="3" width="53.140625" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" customWidth="1"/>
+    <col min="4" max="4" width="53.140625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+    <row r="1" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="10">
+      <c r="F1" s="10">
         <f ca="1">TODAY()</f>
-        <v>42691</v>
-      </c>
-      <c r="F1" s="11" t="s">
+        <v>42703</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="105" t="s">
+    <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="10">
+      <c r="E4" s="10">
         <v>42311</v>
       </c>
-      <c r="E4" s="10">
+      <c r="F4" s="10">
         <v>42446</v>
       </c>
-      <c r="F4" s="17">
-        <f>DAYS360(D4,E4)</f>
+      <c r="G4" s="17">
+        <f>DAYS360(E4,F4)</f>
         <v>134</v>
       </c>
-      <c r="I4" s="110">
-        <f>AVERAGE(F8,F20)</f>
-        <v>199.55</v>
-      </c>
-      <c r="J4" s="12">
+      <c r="J4" s="78">
+        <f>AVERAGE(G14,G26)</f>
+        <v>223.55</v>
+      </c>
+      <c r="K4" s="12">
         <v>0</v>
       </c>
-      <c r="K4" s="1">
-        <f>I4-(I4*J4)</f>
-        <v>199.55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="105" t="s">
+      <c r="L4" s="1">
+        <f>J4-(J4*K4)</f>
+        <v>223.55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" s="10">
+        <v>42118</v>
+      </c>
+      <c r="F5" s="10">
+        <v>42221</v>
+      </c>
+      <c r="G5" s="17">
+        <f t="shared" ref="G5:G10" si="0">DAYS360(E5,F5)</f>
+        <v>101</v>
+      </c>
+      <c r="J5" s="119"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="18"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="74" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="10">
+        <v>42263</v>
+      </c>
+      <c r="F6" s="10">
+        <v>42342</v>
+      </c>
+      <c r="G6" s="17">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="J6" s="119"/>
+      <c r="K6" s="120"/>
+      <c r="L6" s="18"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="74" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="10">
+        <v>42633</v>
+      </c>
+      <c r="F7" s="10">
+        <v>42695</v>
+      </c>
+      <c r="G7" s="17">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="J7" s="119"/>
+      <c r="K7" s="120"/>
+      <c r="L7" s="18"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="74" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" s="74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" s="10">
+        <v>42422</v>
+      </c>
+      <c r="F8" s="10">
+        <v>42643</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="0"/>
+        <v>218</v>
+      </c>
+      <c r="J8" s="119"/>
+      <c r="K8" s="120"/>
+      <c r="L8" s="18"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="74" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="10">
+        <v>41955</v>
+      </c>
+      <c r="F9" s="10">
+        <v>42179</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="0"/>
+        <v>222</v>
+      </c>
+      <c r="K9" s="84"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="74" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" s="74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="10">
+        <v>41738</v>
+      </c>
+      <c r="F10" s="10">
+        <v>41850</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B11" s="83" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="D11" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="10">
+      <c r="E11" s="76">
         <v>41225</v>
       </c>
-      <c r="E5" s="10">
+      <c r="F11" s="76">
         <v>41263</v>
       </c>
-      <c r="F5" s="17">
-        <f>DAYS360(D5,E5)</f>
+      <c r="G11" s="77">
+        <f>DAYS360(E11,F11)</f>
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="105" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B12" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="10">
+      <c r="E12" s="10">
         <v>41337</v>
       </c>
-      <c r="E6" s="10">
+      <c r="F12" s="10">
         <v>41430</v>
       </c>
-      <c r="F6" s="17">
-        <f>DAYS360(D6,E6)</f>
+      <c r="G12" s="17">
+        <f>DAYS360(E12,F12)</f>
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="105" t="s">
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B13" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D13" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="10">
+      <c r="E13" s="10">
         <v>42209</v>
       </c>
-      <c r="E7" s="10">
+      <c r="F13" s="10">
         <v>42683</v>
       </c>
-      <c r="F7" s="17">
-        <f>DAYS360(D7,E7)</f>
+      <c r="G13" s="17">
+        <f>DAYS360(E13,F13)</f>
         <v>465</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="102" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="103"/>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="101">
-        <f>AVERAGE(F4:F7)</f>
-        <v>182</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B14" s="87"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="73">
+        <f>AVERAGE(G13,G12,G4)</f>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B15" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="D15" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="10">
+      <c r="E15" s="10">
         <v>42020</v>
       </c>
-      <c r="E9" s="10">
+      <c r="F15" s="10">
         <v>42671</v>
       </c>
-      <c r="F9" s="17">
-        <f>DAYS360(D9,E9)</f>
+      <c r="G15" s="17">
+        <f t="shared" ref="G15:G25" si="1">DAYS360(E15,F15)</f>
         <v>642</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="106" t="s">
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B16" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="D16" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="10">
+      <c r="E16" s="10">
         <v>42439</v>
       </c>
-      <c r="E10" s="10">
+      <c r="F16" s="10">
         <v>42668</v>
       </c>
-      <c r="F10" s="17">
-        <f>DAYS360(D10,E10)</f>
+      <c r="G16" s="17">
+        <f t="shared" si="1"/>
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="106" t="s">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B17" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="D17" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="10">
+      <c r="E17" s="10">
         <v>42521</v>
       </c>
-      <c r="E11" s="10">
+      <c r="F17" s="10">
         <v>42661</v>
       </c>
-      <c r="F11" s="17">
-        <f>DAYS360(D11,E11)</f>
+      <c r="G17" s="17">
+        <f t="shared" si="1"/>
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="74" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B18" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D12" s="10">
+      <c r="E18" s="10">
         <v>41242</v>
       </c>
-      <c r="E12" s="10">
+      <c r="F18" s="10">
         <v>41472</v>
       </c>
-      <c r="F12" s="17">
-        <f>DAYS360(D12,E12)</f>
+      <c r="G18" s="17">
+        <f t="shared" si="1"/>
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B19" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="10">
+      <c r="E19" s="10">
         <v>41698</v>
       </c>
-      <c r="E13" s="10">
+      <c r="F19" s="10">
         <v>41932</v>
       </c>
-      <c r="F13" s="17">
-        <f>DAYS360(D13,E13)</f>
+      <c r="G19" s="17">
+        <f t="shared" si="1"/>
         <v>230</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="74" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B20" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="10">
+      <c r="E20" s="10">
         <v>42277</v>
       </c>
-      <c r="E14" s="10">
+      <c r="F20" s="10">
         <v>42681</v>
       </c>
-      <c r="F14" s="17">
-        <f>DAYS360(D14,E14)</f>
+      <c r="G20" s="17">
+        <f t="shared" si="1"/>
         <v>397</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="74" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B21" s="74" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="10">
+      <c r="E21" s="10">
         <v>42136</v>
       </c>
-      <c r="E15" s="15">
+      <c r="F21" s="15">
         <v>42171</v>
       </c>
-      <c r="F15" s="17">
-        <f>DAYS360(D15,E15)</f>
+      <c r="G21" s="17">
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B22" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D16" s="10">
+      <c r="E22" s="10">
         <v>41541</v>
       </c>
-      <c r="E16" s="10">
+      <c r="F22" s="10">
         <v>41634</v>
       </c>
-      <c r="F16" s="17">
-        <f>DAYS360(D16,E16)</f>
+      <c r="G22" s="17">
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="74" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="100" t="s">
+      <c r="B23" s="74" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="D17" s="10">
+      <c r="E23" s="10">
         <v>41575</v>
       </c>
-      <c r="E17" s="10">
+      <c r="F23" s="10">
         <v>41638</v>
       </c>
-      <c r="F17" s="17">
-        <f>DAYS360(D17,E17)</f>
+      <c r="G23" s="17">
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="57" t="s">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="74" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B24" s="74"/>
+      <c r="C24" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="107" t="s">
+      <c r="D24" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="108">
+      <c r="E24" s="76">
         <v>42143</v>
       </c>
-      <c r="E18" s="108">
+      <c r="F24" s="76">
         <v>42156</v>
       </c>
-      <c r="F18" s="109">
-        <f>DAYS360(D18,E18)</f>
+      <c r="G24" s="77">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B25" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="D25" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D19" s="10">
+      <c r="E25" s="10">
         <v>42229</v>
       </c>
-      <c r="E19" s="10">
+      <c r="F25" s="10">
         <v>42354</v>
       </c>
-      <c r="F19" s="17">
-        <f>DAYS360(D19,E19)</f>
+      <c r="G25" s="17">
+        <f t="shared" si="1"/>
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="102" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="86" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="103"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="103"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="17">
-        <f>AVERAGE(F19,F17,F16,F15,F14,F13,F12,F11,F10,F9)</f>
+      <c r="B26" s="87"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="88"/>
+      <c r="G26" s="17">
+        <f>AVERAGE(G25,G23,G22,G21,G20,G19,G18,G17,G16,G15)</f>
         <v>217.1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J45" t="s">
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="49" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K49" t="s">
         <v>16</v>
       </c>
-      <c r="K45">
+      <c r="L49">
         <v>1</v>
       </c>
-      <c r="L45">
-        <f>AVERAGEIF(J45:J49,J45,K45:K49)</f>
+      <c r="M49">
+        <f>AVERAGEIF(K49:K53,K49,L49:L53)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J46" t="s">
+    <row r="50" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K50" t="s">
         <v>17</v>
       </c>
-      <c r="K46">
+      <c r="L50">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J47" t="s">
+    <row r="51" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K51" t="s">
         <v>16</v>
       </c>
-      <c r="K47">
+      <c r="L51">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J48" t="s">
+    <row r="52" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K52" t="s">
         <v>17</v>
       </c>
-      <c r="K48">
+      <c r="L52">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J49" t="s">
+    <row r="53" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K53" t="s">
         <v>18</v>
       </c>
-      <c r="K49">
+      <c r="L53">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A26:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2743,8 +3082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J148"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2760,7 +3099,7 @@
       <c r="B2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="111"/>
+      <c r="C2" s="79"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2775,7 +3114,7 @@
         <v>88</v>
       </c>
       <c r="B4" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$20,'Dados Historicos x Categoria'!B7,'Dados Historicos x Categoria'!$F$4:$F$20)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$C$4:$C$26,'Dados Historicos x Categoria'!C13,'Dados Historicos x Categoria'!$G$4:$G$26)</f>
         <v>307.66666666666669</v>
       </c>
     </row>
@@ -2784,7 +3123,7 @@
         <v>104</v>
       </c>
       <c r="B5" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$20,'Dados Historicos x Categoria'!B14,'Dados Historicos x Categoria'!$F$4:$F$20)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$C$4:$C$26,'Dados Historicos x Categoria'!C20,'Dados Historicos x Categoria'!$G$4:$G$26)</f>
         <v>397</v>
       </c>
     </row>
@@ -2793,7 +3132,7 @@
         <v>81</v>
       </c>
       <c r="B6" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$20,'Dados Historicos x Categoria'!B10,'Dados Historicos x Categoria'!$F$4:$F$20)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$C$4:$C$26,'Dados Historicos x Categoria'!C16,'Dados Historicos x Categoria'!$G$4:$G$26)</f>
         <v>433.5</v>
       </c>
     </row>
@@ -2802,7 +3141,7 @@
         <v>113</v>
       </c>
       <c r="B7" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$20,'Dados Historicos x Categoria'!B19,'Dados Historicos x Categoria'!$F$4:$F$20)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$C$4:$C$26,'Dados Historicos x Categoria'!C25,'Dados Historicos x Categoria'!$G$4:$G$26)</f>
         <v>123</v>
       </c>
     </row>
@@ -2811,7 +3150,7 @@
         <v>97</v>
       </c>
       <c r="B8" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$20,'Dados Historicos x Categoria'!B11,'Dados Historicos x Categoria'!$F$4:$F$20)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$C$4:$C$26,'Dados Historicos x Categoria'!C17,'Dados Historicos x Categoria'!$G$4:$G$26)</f>
         <v>138</v>
       </c>
     </row>
@@ -2820,7 +3159,7 @@
         <v>82</v>
       </c>
       <c r="B9" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$20,'Dados Historicos x Categoria'!B4,'Dados Historicos x Categoria'!$F$4:$F$20)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$C$4:$C$26,'Dados Historicos x Categoria'!C4,'Dados Historicos x Categoria'!$G$4:$G$26)</f>
         <v>134</v>
       </c>
     </row>
@@ -2838,292 +3177,292 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="91"/>
+      <c r="E18" s="91"/>
+      <c r="F18" s="91"/>
+      <c r="G18" s="91"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="76"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="91"/>
+      <c r="G19" s="91"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
+      <c r="C20" s="91"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="91"/>
+      <c r="G20" s="91"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="76"/>
-      <c r="G21" s="76"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="91"/>
+      <c r="G21" s="91"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="76"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="76"/>
-      <c r="G22" s="76"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="91"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
-      <c r="G23" s="76"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="91"/>
+      <c r="G23" s="91"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="76"/>
-      <c r="D24" s="76"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="76"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="91"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="91"/>
+      <c r="G24" s="91"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="76"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="76"/>
-      <c r="G25" s="76"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="91"/>
+      <c r="G25" s="91"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="76"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="76"/>
-      <c r="F26" s="76"/>
-      <c r="G26" s="76"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="91"/>
+      <c r="F26" s="91"/>
+      <c r="G26" s="91"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="76"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="76"/>
-      <c r="G27" s="76"/>
+      <c r="C27" s="91"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="91"/>
+      <c r="F27" s="91"/>
+      <c r="G27" s="91"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="76"/>
-      <c r="G28" s="76"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="91"/>
+      <c r="G28" s="91"/>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="76"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="76"/>
-      <c r="G29" s="76"/>
+      <c r="C29" s="91"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="91"/>
+      <c r="F29" s="91"/>
+      <c r="G29" s="91"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="76"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="76"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="91"/>
+      <c r="F30" s="91"/>
+      <c r="G30" s="91"/>
     </row>
     <row r="38" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="77" t="s">
+      <c r="E39" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="F39" s="75"/>
-      <c r="G39" s="75"/>
-      <c r="H39" s="75"/>
-      <c r="I39" s="78"/>
+      <c r="F39" s="90"/>
+      <c r="G39" s="90"/>
+      <c r="H39" s="90"/>
+      <c r="I39" s="93"/>
     </row>
     <row r="40" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E40" s="79"/>
-      <c r="F40" s="76"/>
-      <c r="G40" s="76"/>
-      <c r="H40" s="76"/>
-      <c r="I40" s="80"/>
+      <c r="E40" s="94"/>
+      <c r="F40" s="91"/>
+      <c r="G40" s="91"/>
+      <c r="H40" s="91"/>
+      <c r="I40" s="95"/>
     </row>
     <row r="41" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="79"/>
-      <c r="F41" s="76"/>
-      <c r="G41" s="76"/>
-      <c r="H41" s="76"/>
-      <c r="I41" s="80"/>
+      <c r="E41" s="94"/>
+      <c r="F41" s="91"/>
+      <c r="G41" s="91"/>
+      <c r="H41" s="91"/>
+      <c r="I41" s="95"/>
     </row>
     <row r="42" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E42" s="79"/>
-      <c r="F42" s="76"/>
-      <c r="G42" s="76"/>
-      <c r="H42" s="76"/>
-      <c r="I42" s="80"/>
+      <c r="E42" s="94"/>
+      <c r="F42" s="91"/>
+      <c r="G42" s="91"/>
+      <c r="H42" s="91"/>
+      <c r="I42" s="95"/>
     </row>
     <row r="43" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E43" s="79"/>
-      <c r="F43" s="76"/>
-      <c r="G43" s="76"/>
-      <c r="H43" s="76"/>
-      <c r="I43" s="80"/>
+      <c r="E43" s="94"/>
+      <c r="F43" s="91"/>
+      <c r="G43" s="91"/>
+      <c r="H43" s="91"/>
+      <c r="I43" s="95"/>
     </row>
     <row r="44" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E44" s="79"/>
-      <c r="F44" s="76"/>
-      <c r="G44" s="76"/>
-      <c r="H44" s="76"/>
-      <c r="I44" s="80"/>
+      <c r="E44" s="94"/>
+      <c r="F44" s="91"/>
+      <c r="G44" s="91"/>
+      <c r="H44" s="91"/>
+      <c r="I44" s="95"/>
     </row>
     <row r="45" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E45" s="79"/>
-      <c r="F45" s="76"/>
-      <c r="G45" s="76"/>
-      <c r="H45" s="76"/>
-      <c r="I45" s="80"/>
+      <c r="E45" s="94"/>
+      <c r="F45" s="91"/>
+      <c r="G45" s="91"/>
+      <c r="H45" s="91"/>
+      <c r="I45" s="95"/>
     </row>
     <row r="46" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E46" s="79"/>
-      <c r="F46" s="76"/>
-      <c r="G46" s="76"/>
-      <c r="H46" s="76"/>
-      <c r="I46" s="80"/>
+      <c r="E46" s="94"/>
+      <c r="F46" s="91"/>
+      <c r="G46" s="91"/>
+      <c r="H46" s="91"/>
+      <c r="I46" s="95"/>
     </row>
     <row r="47" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E47" s="79"/>
-      <c r="F47" s="76"/>
-      <c r="G47" s="76"/>
-      <c r="H47" s="76"/>
-      <c r="I47" s="80"/>
+      <c r="E47" s="94"/>
+      <c r="F47" s="91"/>
+      <c r="G47" s="91"/>
+      <c r="H47" s="91"/>
+      <c r="I47" s="95"/>
     </row>
     <row r="48" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E48" s="79"/>
-      <c r="F48" s="76"/>
-      <c r="G48" s="76"/>
-      <c r="H48" s="76"/>
-      <c r="I48" s="80"/>
+      <c r="E48" s="94"/>
+      <c r="F48" s="91"/>
+      <c r="G48" s="91"/>
+      <c r="H48" s="91"/>
+      <c r="I48" s="95"/>
     </row>
     <row r="49" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E49" s="79"/>
-      <c r="F49" s="76"/>
-      <c r="G49" s="76"/>
-      <c r="H49" s="76"/>
-      <c r="I49" s="80"/>
+      <c r="E49" s="94"/>
+      <c r="F49" s="91"/>
+      <c r="G49" s="91"/>
+      <c r="H49" s="91"/>
+      <c r="I49" s="95"/>
     </row>
     <row r="50" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E50" s="79"/>
-      <c r="F50" s="76"/>
-      <c r="G50" s="76"/>
-      <c r="H50" s="76"/>
-      <c r="I50" s="80"/>
+      <c r="E50" s="94"/>
+      <c r="F50" s="91"/>
+      <c r="G50" s="91"/>
+      <c r="H50" s="91"/>
+      <c r="I50" s="95"/>
     </row>
     <row r="51" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E51" s="81"/>
-      <c r="F51" s="82"/>
-      <c r="G51" s="82"/>
-      <c r="H51" s="82"/>
-      <c r="I51" s="83"/>
+      <c r="E51" s="96"/>
+      <c r="F51" s="97"/>
+      <c r="G51" s="97"/>
+      <c r="H51" s="97"/>
+      <c r="I51" s="98"/>
     </row>
     <row r="64" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="77" t="s">
+      <c r="C65" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="78"/>
+      <c r="D65" s="90"/>
+      <c r="E65" s="90"/>
+      <c r="F65" s="90"/>
+      <c r="G65" s="93"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="79"/>
-      <c r="D66" s="76"/>
-      <c r="E66" s="76"/>
-      <c r="F66" s="76"/>
-      <c r="G66" s="80"/>
+      <c r="C66" s="94"/>
+      <c r="D66" s="91"/>
+      <c r="E66" s="91"/>
+      <c r="F66" s="91"/>
+      <c r="G66" s="95"/>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="79"/>
-      <c r="D67" s="76"/>
-      <c r="E67" s="76"/>
-      <c r="F67" s="76"/>
-      <c r="G67" s="80"/>
+      <c r="C67" s="94"/>
+      <c r="D67" s="91"/>
+      <c r="E67" s="91"/>
+      <c r="F67" s="91"/>
+      <c r="G67" s="95"/>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C68" s="79"/>
-      <c r="D68" s="76"/>
-      <c r="E68" s="76"/>
-      <c r="F68" s="76"/>
-      <c r="G68" s="80"/>
+      <c r="C68" s="94"/>
+      <c r="D68" s="91"/>
+      <c r="E68" s="91"/>
+      <c r="F68" s="91"/>
+      <c r="G68" s="95"/>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="79"/>
-      <c r="D69" s="76"/>
-      <c r="E69" s="76"/>
-      <c r="F69" s="76"/>
-      <c r="G69" s="80"/>
+      <c r="C69" s="94"/>
+      <c r="D69" s="91"/>
+      <c r="E69" s="91"/>
+      <c r="F69" s="91"/>
+      <c r="G69" s="95"/>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="79"/>
-      <c r="D70" s="76"/>
-      <c r="E70" s="76"/>
-      <c r="F70" s="76"/>
-      <c r="G70" s="80"/>
+      <c r="C70" s="94"/>
+      <c r="D70" s="91"/>
+      <c r="E70" s="91"/>
+      <c r="F70" s="91"/>
+      <c r="G70" s="95"/>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C71" s="79"/>
-      <c r="D71" s="76"/>
-      <c r="E71" s="76"/>
-      <c r="F71" s="76"/>
-      <c r="G71" s="80"/>
+      <c r="C71" s="94"/>
+      <c r="D71" s="91"/>
+      <c r="E71" s="91"/>
+      <c r="F71" s="91"/>
+      <c r="G71" s="95"/>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="79"/>
-      <c r="D72" s="76"/>
-      <c r="E72" s="76"/>
-      <c r="F72" s="76"/>
-      <c r="G72" s="80"/>
+      <c r="C72" s="94"/>
+      <c r="D72" s="91"/>
+      <c r="E72" s="91"/>
+      <c r="F72" s="91"/>
+      <c r="G72" s="95"/>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="79"/>
-      <c r="D73" s="76"/>
-      <c r="E73" s="76"/>
-      <c r="F73" s="76"/>
-      <c r="G73" s="80"/>
+      <c r="C73" s="94"/>
+      <c r="D73" s="91"/>
+      <c r="E73" s="91"/>
+      <c r="F73" s="91"/>
+      <c r="G73" s="95"/>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="79"/>
-      <c r="D74" s="76"/>
-      <c r="E74" s="76"/>
-      <c r="F74" s="76"/>
-      <c r="G74" s="80"/>
+      <c r="C74" s="94"/>
+      <c r="D74" s="91"/>
+      <c r="E74" s="91"/>
+      <c r="F74" s="91"/>
+      <c r="G74" s="95"/>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="79"/>
-      <c r="D75" s="76"/>
-      <c r="E75" s="76"/>
-      <c r="F75" s="76"/>
-      <c r="G75" s="80"/>
+      <c r="C75" s="94"/>
+      <c r="D75" s="91"/>
+      <c r="E75" s="91"/>
+      <c r="F75" s="91"/>
+      <c r="G75" s="95"/>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="79"/>
-      <c r="D76" s="76"/>
-      <c r="E76" s="76"/>
-      <c r="F76" s="76"/>
-      <c r="G76" s="80"/>
+      <c r="C76" s="94"/>
+      <c r="D76" s="91"/>
+      <c r="E76" s="91"/>
+      <c r="F76" s="91"/>
+      <c r="G76" s="95"/>
     </row>
     <row r="77" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C77" s="81"/>
-      <c r="D77" s="82"/>
-      <c r="E77" s="82"/>
-      <c r="F77" s="82"/>
-      <c r="G77" s="83"/>
+      <c r="C77" s="96"/>
+      <c r="D77" s="97"/>
+      <c r="E77" s="97"/>
+      <c r="F77" s="97"/>
+      <c r="G77" s="98"/>
     </row>
     <row r="84" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J84" s="62"/>
@@ -3132,117 +3471,117 @@
       <c r="J85" s="62"/>
     </row>
     <row r="86" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C86" s="77" t="s">
+      <c r="C86" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="D86" s="75"/>
-      <c r="E86" s="75"/>
-      <c r="F86" s="75"/>
-      <c r="G86" s="78"/>
+      <c r="D86" s="90"/>
+      <c r="E86" s="90"/>
+      <c r="F86" s="90"/>
+      <c r="G86" s="93"/>
       <c r="J86" s="62"/>
     </row>
     <row r="87" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C87" s="79"/>
-      <c r="D87" s="76"/>
-      <c r="E87" s="76"/>
-      <c r="F87" s="76"/>
-      <c r="G87" s="80"/>
+      <c r="C87" s="94"/>
+      <c r="D87" s="91"/>
+      <c r="E87" s="91"/>
+      <c r="F87" s="91"/>
+      <c r="G87" s="95"/>
       <c r="J87" s="62"/>
     </row>
     <row r="88" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C88" s="79"/>
-      <c r="D88" s="76"/>
-      <c r="E88" s="76"/>
-      <c r="F88" s="76"/>
-      <c r="G88" s="80"/>
+      <c r="C88" s="94"/>
+      <c r="D88" s="91"/>
+      <c r="E88" s="91"/>
+      <c r="F88" s="91"/>
+      <c r="G88" s="95"/>
       <c r="J88" s="62"/>
     </row>
     <row r="89" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C89" s="79"/>
-      <c r="D89" s="76"/>
-      <c r="E89" s="76"/>
-      <c r="F89" s="76"/>
-      <c r="G89" s="80"/>
+      <c r="C89" s="94"/>
+      <c r="D89" s="91"/>
+      <c r="E89" s="91"/>
+      <c r="F89" s="91"/>
+      <c r="G89" s="95"/>
       <c r="J89" s="62"/>
     </row>
     <row r="90" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C90" s="79"/>
-      <c r="D90" s="76"/>
-      <c r="E90" s="76"/>
-      <c r="F90" s="76"/>
-      <c r="G90" s="80"/>
+      <c r="C90" s="94"/>
+      <c r="D90" s="91"/>
+      <c r="E90" s="91"/>
+      <c r="F90" s="91"/>
+      <c r="G90" s="95"/>
       <c r="J90" s="62"/>
     </row>
     <row r="91" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C91" s="79"/>
-      <c r="D91" s="76"/>
-      <c r="E91" s="76"/>
-      <c r="F91" s="76"/>
-      <c r="G91" s="80"/>
+      <c r="C91" s="94"/>
+      <c r="D91" s="91"/>
+      <c r="E91" s="91"/>
+      <c r="F91" s="91"/>
+      <c r="G91" s="95"/>
       <c r="J91" s="62"/>
     </row>
     <row r="92" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C92" s="79"/>
-      <c r="D92" s="76"/>
-      <c r="E92" s="76"/>
-      <c r="F92" s="76"/>
-      <c r="G92" s="80"/>
+      <c r="C92" s="94"/>
+      <c r="D92" s="91"/>
+      <c r="E92" s="91"/>
+      <c r="F92" s="91"/>
+      <c r="G92" s="95"/>
       <c r="J92" s="62"/>
     </row>
     <row r="93" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C93" s="79"/>
-      <c r="D93" s="76"/>
-      <c r="E93" s="76"/>
-      <c r="F93" s="76"/>
-      <c r="G93" s="80"/>
+      <c r="C93" s="94"/>
+      <c r="D93" s="91"/>
+      <c r="E93" s="91"/>
+      <c r="F93" s="91"/>
+      <c r="G93" s="95"/>
       <c r="J93" s="62"/>
     </row>
     <row r="94" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C94" s="79"/>
-      <c r="D94" s="76"/>
-      <c r="E94" s="76"/>
-      <c r="F94" s="76"/>
-      <c r="G94" s="80"/>
+      <c r="C94" s="94"/>
+      <c r="D94" s="91"/>
+      <c r="E94" s="91"/>
+      <c r="F94" s="91"/>
+      <c r="G94" s="95"/>
       <c r="J94" s="62"/>
     </row>
     <row r="95" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C95" s="79"/>
-      <c r="D95" s="76"/>
-      <c r="E95" s="76"/>
-      <c r="F95" s="76"/>
-      <c r="G95" s="80"/>
+      <c r="C95" s="94"/>
+      <c r="D95" s="91"/>
+      <c r="E95" s="91"/>
+      <c r="F95" s="91"/>
+      <c r="G95" s="95"/>
       <c r="J95" s="62"/>
     </row>
     <row r="96" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C96" s="79"/>
-      <c r="D96" s="76"/>
-      <c r="E96" s="76"/>
-      <c r="F96" s="76"/>
-      <c r="G96" s="80"/>
+      <c r="C96" s="94"/>
+      <c r="D96" s="91"/>
+      <c r="E96" s="91"/>
+      <c r="F96" s="91"/>
+      <c r="G96" s="95"/>
       <c r="J96" s="62"/>
     </row>
     <row r="97" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C97" s="79"/>
-      <c r="D97" s="76"/>
-      <c r="E97" s="76"/>
-      <c r="F97" s="76"/>
-      <c r="G97" s="80"/>
+      <c r="C97" s="94"/>
+      <c r="D97" s="91"/>
+      <c r="E97" s="91"/>
+      <c r="F97" s="91"/>
+      <c r="G97" s="95"/>
     </row>
     <row r="98" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C98" s="81"/>
-      <c r="D98" s="82"/>
-      <c r="E98" s="82"/>
-      <c r="F98" s="82"/>
-      <c r="G98" s="83"/>
+      <c r="C98" s="96"/>
+      <c r="D98" s="97"/>
+      <c r="E98" s="97"/>
+      <c r="F98" s="97"/>
+      <c r="G98" s="98"/>
     </row>
     <row r="108" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="109" spans="3:10" ht="315" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F109" s="84" t="s">
+      <c r="F109" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="G109" s="85"/>
-      <c r="H109" s="85"/>
-      <c r="I109" s="86"/>
+      <c r="G109" s="100"/>
+      <c r="H109" s="100"/>
+      <c r="I109" s="101"/>
     </row>
     <row r="110" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F110" s="61"/>
@@ -3433,10 +3772,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3448,7 +3787,7 @@
     <col min="5" max="5" width="9.140625" style="58"/>
     <col min="6" max="6" width="29.42578125" style="58" customWidth="1"/>
     <col min="7" max="7" width="31.7109375" style="58" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="58" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="58" customWidth="1"/>
     <col min="9" max="9" width="12" style="58" customWidth="1"/>
     <col min="10" max="10" width="27.42578125" style="58" customWidth="1"/>
   </cols>
@@ -3486,19 +3825,19 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="56" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="88">
+      <c r="A2" s="103">
         <v>1</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="87" t="s">
+      <c r="D2" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="87">
+      <c r="E2" s="102">
         <v>2</v>
       </c>
       <c r="F2" s="40" t="s">
@@ -3516,11 +3855,11 @@
       <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
+      <c r="A3" s="104"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
       <c r="F3" s="40" t="s">
         <v>60</v>
       </c>
@@ -3536,19 +3875,19 @@
       <c r="J3" s="40"/>
     </row>
     <row r="4" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="87">
+      <c r="A4" s="102">
         <v>2</v>
       </c>
-      <c r="B4" s="92">
+      <c r="B4" s="107">
         <v>42440</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="102" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="88">
+      <c r="E4" s="103">
         <v>2</v>
       </c>
       <c r="F4" s="40" t="s">
@@ -3566,11 +3905,11 @@
       <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="88"/>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="89"/>
+      <c r="A5" s="103"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="104"/>
       <c r="F5" s="47" t="s">
         <v>54</v>
       </c>
@@ -3586,19 +3925,19 @@
       <c r="J5" s="47"/>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="87">
+      <c r="A6" s="102">
         <v>3</v>
       </c>
-      <c r="B6" s="90">
-        <v>42624</v>
-      </c>
-      <c r="C6" s="88" t="s">
+      <c r="B6" s="105">
+        <v>42683</v>
+      </c>
+      <c r="C6" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="88" t="s">
+      <c r="D6" s="103" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="88">
+      <c r="E6" s="103">
         <v>2</v>
       </c>
       <c r="F6" s="40" t="s">
@@ -3616,11 +3955,11 @@
       <c r="J6" s="40"/>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="87"/>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
+      <c r="A7" s="102"/>
+      <c r="B7" s="104"/>
+      <c r="C7" s="104"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="104"/>
       <c r="F7" s="67" t="s">
         <v>71</v>
       </c>
@@ -3636,11 +3975,11 @@
       <c r="J7" s="40"/>
     </row>
     <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="87"/>
-      <c r="B8" s="89"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
+      <c r="A8" s="102"/>
+      <c r="B8" s="104"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
       <c r="F8" s="64" t="s">
         <v>73</v>
       </c>
@@ -3656,11 +3995,11 @@
       <c r="J8" s="64"/>
     </row>
     <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="87"/>
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="89"/>
+      <c r="A9" s="102"/>
+      <c r="B9" s="104"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="104"/>
+      <c r="E9" s="104"/>
       <c r="F9" s="64" t="s">
         <v>77</v>
       </c>
@@ -3670,17 +4009,17 @@
       <c r="H9" s="69">
         <v>42691</v>
       </c>
-      <c r="I9" s="71" t="s">
-        <v>117</v>
+      <c r="I9" s="70" t="s">
+        <v>57</v>
       </c>
       <c r="J9" s="64"/>
     </row>
     <row r="10" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="87"/>
-      <c r="B10" s="91"/>
-      <c r="C10" s="91"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="91"/>
+      <c r="A10" s="102"/>
+      <c r="B10" s="106"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="106"/>
+      <c r="E10" s="106"/>
       <c r="F10" s="40" t="s">
         <v>74</v>
       </c>
@@ -3690,23 +4029,29 @@
       <c r="H10" s="59">
         <v>42624</v>
       </c>
-      <c r="I10" s="71" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10" s="72" t="s">
+      <c r="I10" s="70" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="71" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="87">
+      <c r="A11" s="102">
         <v>4</v>
       </c>
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="87"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="87"/>
+      <c r="C11" s="102" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="102" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" s="102">
+        <v>2</v>
+      </c>
       <c r="F11" s="64" t="s">
         <v>47</v>
       </c>
@@ -3716,17 +4061,17 @@
       <c r="H11" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="I11" s="71" t="s">
-        <v>51</v>
+      <c r="I11" s="70" t="s">
+        <v>57</v>
       </c>
       <c r="J11" s="64"/>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="87"/>
-      <c r="B12" s="87"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
+      <c r="A12" s="102"/>
+      <c r="B12" s="102"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
       <c r="F12" s="67" t="s">
         <v>58</v>
       </c>
@@ -3736,31 +4081,158 @@
       <c r="H12" s="65">
         <v>42690</v>
       </c>
-      <c r="I12" s="71" t="s">
+      <c r="I12" s="70" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" s="64"/>
+    </row>
+    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="103"/>
+      <c r="B13" s="103"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="115" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="80" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="82">
+        <v>42690</v>
+      </c>
+      <c r="I13" s="118" t="s">
         <v>51</v>
       </c>
-      <c r="J12" s="64"/>
-    </row>
-    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="87"/>
-      <c r="B13" s="87"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="67" t="s">
-        <v>76</v>
-      </c>
-      <c r="G13" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="65">
-        <v>42690</v>
-      </c>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
+      <c r="J13" s="80"/>
+    </row>
+    <row r="14" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="103">
+        <v>5</v>
+      </c>
+      <c r="B14" s="105">
+        <v>42705</v>
+      </c>
+      <c r="C14" s="103"/>
+      <c r="D14" s="103" t="s">
+        <v>123</v>
+      </c>
+      <c r="E14" s="103">
+        <v>2</v>
+      </c>
+      <c r="F14" s="116" t="s">
+        <v>126</v>
+      </c>
+      <c r="G14" s="116" t="s">
+        <v>127</v>
+      </c>
+      <c r="H14" s="117">
+        <v>42705</v>
+      </c>
+      <c r="I14" s="121" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="81"/>
+    </row>
+    <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+      <c r="A15" s="104"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="116" t="s">
+        <v>128</v>
+      </c>
+      <c r="G15" s="116" t="s">
+        <v>129</v>
+      </c>
+      <c r="H15" s="117">
+        <v>42705</v>
+      </c>
+      <c r="I15" s="122" t="s">
+        <v>117</v>
+      </c>
+      <c r="J15" s="81"/>
+    </row>
+    <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="104"/>
+      <c r="B16" s="123"/>
+      <c r="C16" s="104"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="116" t="s">
+        <v>130</v>
+      </c>
+      <c r="G16" s="116" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="117">
+        <v>42705</v>
+      </c>
+      <c r="I16" s="121" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" s="81"/>
+    </row>
+    <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="104"/>
+      <c r="B17" s="123"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="81" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="104"/>
+      <c r="F17" s="116" t="s">
+        <v>131</v>
+      </c>
+      <c r="G17" s="116" t="s">
+        <v>132</v>
+      </c>
+      <c r="H17" s="117">
+        <v>42705</v>
+      </c>
+      <c r="I17" s="121" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="81"/>
+    </row>
+    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="104"/>
+      <c r="B18" s="123"/>
+      <c r="C18" s="104"/>
+      <c r="D18" s="103" t="s">
+        <v>125</v>
+      </c>
+      <c r="E18" s="104"/>
+      <c r="F18" s="116" t="s">
+        <v>133</v>
+      </c>
+      <c r="G18" s="116" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="117">
+        <v>42705</v>
+      </c>
+      <c r="I18" s="125" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="81"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="106"/>
+      <c r="B19" s="124"/>
+      <c r="C19" s="106"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="106"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="26">
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="A14:A19"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="B6:B10"/>
@@ -3792,7 +4264,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3810,8 +4282,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A2" s="105" t="s">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="74" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -3856,7 +4328,7 @@
       <c r="A4" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="72" t="s">
         <v>81</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -3892,20 +4364,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98" t="s">
+      <c r="D1" s="113"/>
+      <c r="E1" s="113" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="99"/>
+      <c r="F1" s="114"/>
       <c r="G1" s="23" t="s">
         <v>35</v>
       </c>
@@ -3923,8 +4395,8 @@
       <c r="S1" s="24"/>
     </row>
     <row r="2" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="94"/>
-      <c r="B2" s="96"/>
+      <c r="A2" s="109"/>
+      <c r="B2" s="111"/>
       <c r="C2" s="25" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Atualizado gráfico com o lote de processos 3 enviado pela Iva no dia 14/12/2016
</commit_message>
<xml_diff>
--- a/TRE_Dados_MapaRaciocinio.xlsx
+++ b/TRE_Dados_MapaRaciocinio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Historicos x Categoria" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,33 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Autor:
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="168">
   <si>
     <t>Categoria</t>
   </si>
@@ -210,22 +235,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ivanilda , Silmara e Hélcio </t>
-  </si>
-  <si>
-    <t>Conclusão 
-A partir desta carta  CEP - Análise de Capacidade de processo, é possível observar que o processo ainda  pode aceitar um tempo limite de 784 dias, dado o fato que não estabelecemos nenhum limite superior nem um inferior.</t>
-  </si>
-  <si>
-    <t>Conclusão
-Este gráfico nos apresenta de forma mais detalhada os registros dos tempos médios no tempo</t>
-  </si>
-  <si>
-    <t>Conclusão
-Este gráfico nos apresenta de forma mais detalhada por categoria de contratação os registros dos tempos médios no tempo</t>
-  </si>
-  <si>
-    <t>Conclusão
-O histrograma ao lado mostra a frequência de processos e seus respectivos tempos médios. Pode-se observar que  6 processos estão entre  300 e 400 dias, sendo que a média geral encontra-se em 340 dias</t>
   </si>
   <si>
     <t>NUMERO DO PROCESSO</t>
@@ -308,9 +317,6 @@
     <t>Serviço de Manutenção</t>
   </si>
   <si>
-    <t>CONTRATAÇÃO - SERVIÇO DE MANUTENÇÃO PREDIAL -   LIMPEZA DE VIDROS - CAPITAL/ INTERIOR</t>
-  </si>
-  <si>
     <t>CONTRATAÇÃO - SERVIÇO DE MANUTENÇÃO PREDIAL -  BENS IMÓVEIS</t>
   </si>
   <si>
@@ -505,6 +511,52 @@
   </si>
   <si>
     <t>Contratação de serviços de manutenção predial para os prédios de Curitiba e interior do Estado -PGE INCORPORADORA DE OBRAS LTDA - ME - Contrato 17/2013.</t>
+  </si>
+  <si>
+    <t>Contratação Manutenção Predial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solicitação de aquisição, mediante registro de preços, de extintores de pó químico classes "A", "B" e "C" </t>
+  </si>
+  <si>
+    <t>455/2012</t>
+  </si>
+  <si>
+    <t>6761/2014</t>
+  </si>
+  <si>
+    <t>CONTRATAÇÃO DE EMPRESA PARA FORNECIMENTO ATRAVÉS DE REGISTRO DE PREÇOS DE LÂMPADAS TUBOLED PARA PRÉDIO SEDE E FÓRUM ELEITORAL DE CURITIBA</t>
+  </si>
+  <si>
+    <t>1060/2012</t>
+  </si>
+  <si>
+    <t>CONTRATAÇÃO SERVIÇO DE MANUTENÇÃO PREDIAL  DETETIZAÇÃO E CONTROLE DE PRAGAS - CAPITAL/INTERIOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contratação de serviços de desinsetização, desratização, esgotamento de fossas, esgotamento de caixas de gordura e de passagem e limpeza de dutos de esgoto para os Fóruns Eleitorais do Interior. </t>
+  </si>
+  <si>
+    <t>3819/2016</t>
+  </si>
+  <si>
+    <t>Contratação de  Serviço de Reformas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projeto Básico para contratação de serviços de pintura para 08 Fóruns Eleitorais. </t>
+  </si>
+  <si>
+    <t>7017/2016</t>
+  </si>
+  <si>
+    <t>Contratação de  Serviço de Manutenção Predial - DIVISÓRIAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contratação de empresa para fornecimento de materiais e serviços para montagem/desmontagem e readequação de forros e divisórias, através de Registro de Preços. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conclusão
+</t>
   </si>
 </sst>
 </file>
@@ -515,7 +567,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="dd\-mm\-yy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -577,6 +629,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -628,7 +687,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -987,43 +1046,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1052,7 +1074,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1279,102 +1301,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1386,8 +1312,99 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1408,19 +1425,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>181841</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>181841</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2971800</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>2782166</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19916</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPr id="11" name="Imagem 10"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1440,8 +1457,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="781050" y="7448550"/>
-          <a:ext cx="5486400" cy="3657600"/>
+          <a:off x="181841" y="3229841"/>
+          <a:ext cx="5483802" cy="3656734"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1463,19 +1480,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>86591</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2933700</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>2695574</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>106507</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagem 3"/>
+        <xdr:cNvPr id="13" name="Imagem 12"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1495,168 +1512,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="742950" y="11468100"/>
-          <a:ext cx="5486400" cy="3657600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>107</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>485777</xdr:colOff>
-      <xdr:row>112</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Imagem 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="723900" y="15763874"/>
-          <a:ext cx="7286627" cy="4857751"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="6334125" cy="4826000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Imagem 49"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="761999" y="29689425"/>
-          <a:ext cx="6334125" cy="4826000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2724150</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Imagem 9"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="123825" y="3228975"/>
-          <a:ext cx="5486400" cy="3657600"/>
+          <a:off x="95249" y="7715250"/>
+          <a:ext cx="5483802" cy="3656734"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2314,11 +2171,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2338,11 +2195,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
       <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
@@ -2351,7 +2208,7 @@
       </c>
       <c r="F1" s="10">
         <f ca="1">TODAY()</f>
-        <v>42712</v>
+        <v>42718</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>11</v>
@@ -2360,10 +2217,10 @@
     <row r="2" spans="1:12" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3" s="66" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>0</v>
@@ -2392,16 +2249,16 @@
     </row>
     <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="74" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="74" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="D4" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E4" s="10">
         <v>42311</v>
@@ -2410,34 +2267,34 @@
         <v>42446</v>
       </c>
       <c r="G4" s="17">
-        <f>DAYS360(E4,F4)</f>
+        <f t="shared" ref="G4:G12" si="0">DAYS360(E4,F4)</f>
         <v>134</v>
       </c>
-      <c r="H4" s="134"/>
-      <c r="J4" s="78" t="e">
-        <f>AVERAGE(G13,G29)</f>
-        <v>#DIV/0!</v>
+      <c r="H4" s="102"/>
+      <c r="J4" s="78">
+        <f>AVERAGE(G13,G34)</f>
+        <v>169.75277777777777</v>
       </c>
       <c r="K4" s="12">
         <v>0</v>
       </c>
-      <c r="L4" s="1" t="e">
+      <c r="L4" s="1">
         <f>J4-(J4*K4)</f>
-        <v>#DIV/0!</v>
+        <v>169.75277777777777</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="74" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B5" s="74" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E5" s="10">
         <v>42118</v>
@@ -2446,7 +2303,7 @@
         <v>42221</v>
       </c>
       <c r="G5" s="17">
-        <f>DAYS360(E5,F5)</f>
+        <f t="shared" si="0"/>
         <v>101</v>
       </c>
       <c r="J5" s="89"/>
@@ -2455,16 +2312,16 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="74" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B6" s="74" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E6" s="10">
         <v>42263</v>
@@ -2473,7 +2330,7 @@
         <v>42342</v>
       </c>
       <c r="G6" s="17">
-        <f>DAYS360(E6,F6)</f>
+        <f t="shared" si="0"/>
         <v>78</v>
       </c>
       <c r="J6" s="89"/>
@@ -2482,16 +2339,16 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B7" s="74" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E7" s="10">
         <v>42633</v>
@@ -2500,7 +2357,7 @@
         <v>42695</v>
       </c>
       <c r="G7" s="17">
-        <f>DAYS360(E7,F7)</f>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="J7" s="89"/>
@@ -2509,16 +2366,16 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="74" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B8" s="74" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E8" s="10">
         <v>42422</v>
@@ -2527,7 +2384,7 @@
         <v>42643</v>
       </c>
       <c r="G8" s="17">
-        <f>DAYS360(E8,F8)</f>
+        <f t="shared" si="0"/>
         <v>218</v>
       </c>
       <c r="J8" s="89"/>
@@ -2536,16 +2393,16 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B9" s="74" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E9" s="10">
         <v>41955</v>
@@ -2554,23 +2411,23 @@
         <v>42179</v>
       </c>
       <c r="G9" s="17">
-        <f>DAYS360(E9,F9)</f>
+        <f t="shared" si="0"/>
         <v>222</v>
       </c>
       <c r="K9" s="84"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B10" s="74" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E10" s="10">
         <v>41738</v>
@@ -2579,22 +2436,22 @@
         <v>41850</v>
       </c>
       <c r="G10" s="17">
-        <f>DAYS360(E10,F10)</f>
+        <f t="shared" si="0"/>
         <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="74" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B11" s="74" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="E11" s="10">
         <v>41337</v>
@@ -2603,22 +2460,22 @@
         <v>41430</v>
       </c>
       <c r="G11" s="17">
-        <f>DAYS360(E11,F11)</f>
+        <f t="shared" si="0"/>
         <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B12" s="74" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E12" s="10">
         <v>42209</v>
@@ -2627,37 +2484,37 @@
         <v>42683</v>
       </c>
       <c r="G12" s="17">
-        <f>DAYS360(E12,F12)</f>
+        <f t="shared" si="0"/>
         <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="132"/>
-      <c r="B13" s="133"/>
-      <c r="C13" s="96" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="96"/>
-      <c r="E13" s="96"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73">
+      <c r="A13" s="100"/>
+      <c r="B13" s="101"/>
+      <c r="C13" s="105" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="73">
         <f>AVERAGE(G4:G12)</f>
         <v>164.55555555555554</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="74" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B14" s="74" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>92</v>
+        <v>87</v>
+      </c>
+      <c r="D14" s="11" t="str">
+        <f>LOWER("CONTRATAÇÃO - SERVIÇO DE MANUTENÇÃO PREDIAL -   LIMPEZA DE VIDROS - CAPITAL/ INTERIOR")</f>
+        <v>contratação - serviço de manutenção predial -   limpeza de vidros - capital/ interior</v>
       </c>
       <c r="E14" s="10">
         <v>42020</v>
@@ -2666,22 +2523,22 @@
         <v>42671</v>
       </c>
       <c r="G14" s="17">
-        <f>DAYS360(E14,F14)</f>
+        <f t="shared" ref="G14:G34" si="1">DAYS360(E14,F14)</f>
         <v>642</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="74" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B15" s="74" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E15" s="10">
         <v>42439</v>
@@ -2690,22 +2547,22 @@
         <v>42668</v>
       </c>
       <c r="G15" s="17">
-        <f>DAYS360(E15,F15)</f>
+        <f t="shared" si="1"/>
         <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="74" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B16" s="74" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E16" s="10">
         <v>42521</v>
@@ -2714,22 +2571,22 @@
         <v>42661</v>
       </c>
       <c r="G16" s="17">
-        <f>DAYS360(E16,F16)</f>
+        <f t="shared" si="1"/>
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="74" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B17" s="74" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E17" s="10">
         <v>41242</v>
@@ -2738,22 +2595,22 @@
         <v>41472</v>
       </c>
       <c r="G17" s="17">
-        <f>DAYS360(E17,F17)</f>
+        <f t="shared" si="1"/>
         <v>228</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B18" s="74" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E18" s="10">
         <v>41698</v>
@@ -2762,22 +2619,22 @@
         <v>41932</v>
       </c>
       <c r="G18" s="17">
-        <f>DAYS360(E18,F18)</f>
+        <f t="shared" si="1"/>
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B19" s="74" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E19" s="10">
         <v>42277</v>
@@ -2786,22 +2643,22 @@
         <v>42681</v>
       </c>
       <c r="G19" s="17">
-        <f>DAYS360(E19,F19)</f>
+        <f t="shared" si="1"/>
         <v>397</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="74" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B20" s="74" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E20" s="10">
         <v>42136</v>
@@ -2810,22 +2667,22 @@
         <v>42171</v>
       </c>
       <c r="G20" s="17">
-        <f>DAYS360(E20,F20)</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E21" s="10">
         <v>41541</v>
@@ -2834,22 +2691,22 @@
         <v>41634</v>
       </c>
       <c r="G21" s="17">
-        <f>DAYS360(E21,F21)</f>
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="74" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B22" s="74" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C22" s="72" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E22" s="10">
         <v>41575</v>
@@ -2858,215 +2715,289 @@
         <v>41638</v>
       </c>
       <c r="G22" s="17">
-        <f>DAYS360(E22,F22)</f>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="74" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="74" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="98" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="94" t="s">
+        <v>139</v>
+      </c>
+      <c r="E23" s="96">
+        <v>42580</v>
+      </c>
+      <c r="F23" s="96">
+        <v>42641</v>
+      </c>
+      <c r="G23" s="97">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="74" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" s="74" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="94" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="95" t="s">
+        <v>141</v>
+      </c>
+      <c r="E24" s="96">
+        <v>42612</v>
+      </c>
+      <c r="F24" s="96">
+        <v>42704</v>
+      </c>
+      <c r="G24" s="97">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="74" t="s">
         <v>143</v>
       </c>
-      <c r="B23" s="74" t="s">
-        <v>135</v>
-      </c>
-      <c r="C23" s="130" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="126" t="s">
+      <c r="B25" s="74" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="128">
-        <v>42580</v>
-      </c>
-      <c r="F23" s="128">
-        <v>42641</v>
-      </c>
-      <c r="G23" s="129">
-        <f>DAYS360(E23,F23)</f>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="74" t="s">
+      <c r="C25" s="94" t="s">
         <v>145</v>
       </c>
-      <c r="B24" s="74" t="s">
-        <v>135</v>
-      </c>
-      <c r="C24" s="126" t="s">
+      <c r="D25" s="95" t="s">
+        <v>146</v>
+      </c>
+      <c r="E25" s="96">
+        <v>42068</v>
+      </c>
+      <c r="F25" s="96">
+        <v>42149</v>
+      </c>
+      <c r="G25" s="97">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="74" t="s">
         <v>147</v>
       </c>
-      <c r="D24" s="127" t="s">
-        <v>146</v>
-      </c>
-      <c r="E24" s="128">
-        <v>42612</v>
-      </c>
-      <c r="F24" s="128">
-        <v>42704</v>
-      </c>
-      <c r="G24" s="129">
-        <f>DAYS360(E24,F24)</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="74" t="s">
+      <c r="B26" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26" s="94" t="s">
         <v>148</v>
       </c>
-      <c r="B25" s="74" t="s">
+      <c r="D26" s="95" t="s">
         <v>149</v>
       </c>
-      <c r="C25" s="126" t="s">
+      <c r="E26" s="96">
+        <v>42410</v>
+      </c>
+      <c r="F26" s="96">
+        <v>42690</v>
+      </c>
+      <c r="G26" s="97">
+        <f t="shared" si="1"/>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="74" t="s">
         <v>150</v>
       </c>
-      <c r="D25" s="127" t="s">
+      <c r="B27" s="74" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="94" t="s">
         <v>151</v>
       </c>
-      <c r="E25" s="128">
-        <v>42068</v>
-      </c>
-      <c r="F25" s="128">
-        <v>42149</v>
-      </c>
-      <c r="G25" s="129">
-        <f>DAYS360(E25,F25)</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="74" t="s">
+      <c r="D27" s="95" t="s">
         <v>152</v>
       </c>
-      <c r="B26" s="74" t="s">
-        <v>149</v>
-      </c>
-      <c r="C26" s="126" t="s">
+      <c r="E27" s="96">
+        <v>41208</v>
+      </c>
+      <c r="F27" s="96">
+        <v>41348</v>
+      </c>
+      <c r="G27" s="97">
+        <f t="shared" si="1"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="74" t="s">
+        <v>155</v>
+      </c>
+      <c r="B28" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="94" t="s">
         <v>153</v>
       </c>
-      <c r="D26" s="127" t="s">
+      <c r="D28" s="95" t="s">
         <v>154</v>
       </c>
-      <c r="E26" s="128">
-        <v>42410</v>
-      </c>
-      <c r="F26" s="128">
-        <v>42690</v>
-      </c>
-      <c r="G26" s="129">
-        <f>DAYS360(E26,F26)</f>
-        <v>276</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="74" t="s">
-        <v>155</v>
-      </c>
-      <c r="B27" s="74" t="s">
-        <v>119</v>
-      </c>
-      <c r="C27" s="126" t="s">
+      <c r="E28" s="96">
+        <v>40927</v>
+      </c>
+      <c r="F28" s="96">
+        <v>41012</v>
+      </c>
+      <c r="G28" s="97">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="132" t="s">
         <v>156</v>
       </c>
-      <c r="D27" s="127" t="s">
+      <c r="B29" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="94" t="s">
+        <v>145</v>
+      </c>
+      <c r="D29" s="95" t="s">
         <v>157</v>
       </c>
-      <c r="E27" s="128">
-        <v>41208</v>
-      </c>
-      <c r="F27" s="128">
-        <v>41348</v>
-      </c>
-      <c r="G27" s="129">
-        <f>DAYS360(E27,F27)</f>
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="74" t="s">
-        <v>112</v>
-      </c>
-      <c r="B28" s="74" t="s">
-        <v>119</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D28" s="11" t="s">
+      <c r="E29" s="96">
+        <v>41885</v>
+      </c>
+      <c r="F29" s="96">
+        <v>41996</v>
+      </c>
+      <c r="G29" s="97">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="74" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="D30" s="133" t="s">
+        <v>160</v>
+      </c>
+      <c r="E30" s="96">
+        <v>40945</v>
+      </c>
+      <c r="F30" s="96">
+        <v>41093</v>
+      </c>
+      <c r="G30" s="97">
+        <f t="shared" si="1"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="74" t="s">
+        <v>161</v>
+      </c>
+      <c r="B31" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" s="94" t="s">
+        <v>162</v>
+      </c>
+      <c r="D31" s="95" t="s">
+        <v>163</v>
+      </c>
+      <c r="E31" s="96">
+        <v>41411</v>
+      </c>
+      <c r="F31" s="96">
+        <v>41666</v>
+      </c>
+      <c r="G31" s="97">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="74" t="s">
+        <v>164</v>
+      </c>
+      <c r="B32" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" s="94" t="s">
+        <v>165</v>
+      </c>
+      <c r="D32" s="95" t="s">
+        <v>166</v>
+      </c>
+      <c r="E32" s="96">
+        <v>41905</v>
+      </c>
+      <c r="F32" s="96">
+        <v>41999</v>
+      </c>
+      <c r="G32" s="97">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="10">
+      <c r="C33" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="10">
         <v>42229</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F33" s="10">
         <v>42354</v>
       </c>
-      <c r="G28" s="17">
-        <f>DAYS360(E28,F28)</f>
+      <c r="G33" s="17">
+        <f t="shared" si="1"/>
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="95" t="s">
-        <v>115</v>
-      </c>
-      <c r="B29" s="96"/>
-      <c r="C29" s="96"/>
-      <c r="D29" s="96"/>
-      <c r="E29" s="96"/>
-      <c r="F29" s="97"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17">
-        <f>AVERAGE(G14:G28)</f>
-        <v>187.66666666666666</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="104" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" s="105"/>
+      <c r="C34" s="105"/>
+      <c r="D34" s="105"/>
+      <c r="E34" s="105"/>
+      <c r="F34" s="106"/>
+      <c r="G34" s="17">
+        <f>AVERAGE(G14:G33)</f>
+        <v>174.95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3074,8 +3005,9 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="17"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3084,7 +3016,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3093,7 +3025,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3102,7 +3034,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3111,7 +3043,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3120,7 +3052,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3129,7 +3061,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3138,7 +3070,7 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3147,7 +3079,7 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3156,7 +3088,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3165,54 +3097,99 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="52" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K52" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K58" t="s">
         <v>16</v>
       </c>
-      <c r="L52">
+      <c r="L58">
         <v>1</v>
       </c>
-      <c r="M52">
-        <f>AVERAGEIF(K52:K56,K52,L52:L56)</f>
+      <c r="M58">
+        <f>AVERAGEIF(K58:K62,K58,L58:L62)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K53" t="s">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K59" t="s">
         <v>17</v>
       </c>
-      <c r="L53">
+      <c r="L59">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K54" t="s">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K60" t="s">
         <v>16</v>
       </c>
-      <c r="L54">
+      <c r="L60">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K55" t="s">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K61" t="s">
         <v>17</v>
       </c>
-      <c r="L55">
+      <c r="L61">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K56" t="s">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K62" t="s">
         <v>18</v>
       </c>
-      <c r="L56">
+      <c r="L62">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A34:F34"/>
     <mergeCell ref="C13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3221,11 +3198,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J148"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3253,29 +3230,29 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B4" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$28,A4,'Dados Historicos x Categoria'!$G$4:$G$28)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$33,A4,'Dados Historicos x Categoria'!$G$4:$G$33)</f>
         <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B5" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$28,A5,'Dados Historicos x Categoria'!$G$4:$G$28)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$33,A5,'Dados Historicos x Categoria'!$G$4:$G$33)</f>
         <v>117.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B6" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$28,A6,'Dados Historicos x Categoria'!$G$4:$G$28)</f>
-        <v>178</v>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$33,A6,'Dados Historicos x Categoria'!$G$4:$G$33)</f>
+        <v>148.57142857142858</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3304,426 +3281,253 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="98" t="s">
-        <v>116</v>
-      </c>
-      <c r="D17" s="99"/>
-      <c r="E17" s="99"/>
-      <c r="F17" s="99"/>
-      <c r="G17" s="99"/>
+      <c r="C17" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="108"/>
+      <c r="E17" s="108"/>
+      <c r="F17" s="108"/>
+      <c r="G17" s="108"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="100"/>
-      <c r="D18" s="100"/>
-      <c r="E18" s="100"/>
-      <c r="F18" s="100"/>
-      <c r="G18" s="100"/>
+      <c r="C18" s="109"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="109"/>
+      <c r="G18" s="109"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="100"/>
+      <c r="C19" s="109"/>
+      <c r="D19" s="109"/>
+      <c r="E19" s="109"/>
+      <c r="F19" s="109"/>
+      <c r="G19" s="109"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="100"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="100"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="100"/>
+      <c r="C20" s="109"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="109"/>
+      <c r="F20" s="109"/>
+      <c r="G20" s="109"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="100"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="100"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="109"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="100"/>
-      <c r="D22" s="100"/>
-      <c r="E22" s="100"/>
-      <c r="F22" s="100"/>
-      <c r="G22" s="100"/>
+      <c r="C22" s="109"/>
+      <c r="D22" s="109"/>
+      <c r="E22" s="109"/>
+      <c r="F22" s="109"/>
+      <c r="G22" s="109"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="100"/>
-      <c r="D23" s="100"/>
-      <c r="E23" s="100"/>
-      <c r="F23" s="100"/>
-      <c r="G23" s="100"/>
+      <c r="C23" s="109"/>
+      <c r="D23" s="109"/>
+      <c r="E23" s="109"/>
+      <c r="F23" s="109"/>
+      <c r="G23" s="109"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="100"/>
-      <c r="D24" s="100"/>
-      <c r="E24" s="100"/>
-      <c r="F24" s="100"/>
-      <c r="G24" s="100"/>
+      <c r="C24" s="109"/>
+      <c r="D24" s="109"/>
+      <c r="E24" s="109"/>
+      <c r="F24" s="109"/>
+      <c r="G24" s="109"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="100"/>
-      <c r="D25" s="100"/>
-      <c r="E25" s="100"/>
-      <c r="F25" s="100"/>
-      <c r="G25" s="100"/>
+      <c r="C25" s="109"/>
+      <c r="D25" s="109"/>
+      <c r="E25" s="109"/>
+      <c r="F25" s="109"/>
+      <c r="G25" s="109"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="100"/>
-      <c r="D26" s="100"/>
-      <c r="E26" s="100"/>
-      <c r="F26" s="100"/>
-      <c r="G26" s="100"/>
+      <c r="C26" s="109"/>
+      <c r="D26" s="109"/>
+      <c r="E26" s="109"/>
+      <c r="F26" s="109"/>
+      <c r="G26" s="109"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="100"/>
-      <c r="D27" s="100"/>
-      <c r="E27" s="100"/>
-      <c r="F27" s="100"/>
-      <c r="G27" s="100"/>
+      <c r="C27" s="109"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="109"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="100"/>
-      <c r="D28" s="100"/>
-      <c r="E28" s="100"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="100"/>
+      <c r="C28" s="109"/>
+      <c r="D28" s="109"/>
+      <c r="E28" s="109"/>
+      <c r="F28" s="109"/>
+      <c r="G28" s="109"/>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="100"/>
-      <c r="D29" s="100"/>
-      <c r="E29" s="100"/>
-      <c r="F29" s="100"/>
-      <c r="G29" s="100"/>
+      <c r="C29" s="109"/>
+      <c r="D29" s="109"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="109"/>
+      <c r="G29" s="109"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="100"/>
-      <c r="D30" s="100"/>
-      <c r="E30" s="100"/>
-      <c r="F30" s="100"/>
-      <c r="G30" s="100"/>
+      <c r="C30" s="109"/>
+      <c r="D30" s="109"/>
+      <c r="E30" s="109"/>
+      <c r="F30" s="109"/>
+      <c r="G30" s="109"/>
     </row>
     <row r="38" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="101" t="s">
-        <v>66</v>
-      </c>
-      <c r="F39" s="99"/>
-      <c r="G39" s="99"/>
-      <c r="H39" s="99"/>
-      <c r="I39" s="102"/>
+      <c r="E39" s="110" t="s">
+        <v>167</v>
+      </c>
+      <c r="F39" s="108"/>
+      <c r="G39" s="108"/>
+      <c r="H39" s="108"/>
+      <c r="I39" s="111"/>
     </row>
     <row r="40" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E40" s="103"/>
-      <c r="F40" s="100"/>
-      <c r="G40" s="100"/>
-      <c r="H40" s="100"/>
-      <c r="I40" s="104"/>
+      <c r="E40" s="112"/>
+      <c r="F40" s="109"/>
+      <c r="G40" s="109"/>
+      <c r="H40" s="109"/>
+      <c r="I40" s="113"/>
     </row>
     <row r="41" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="103"/>
-      <c r="F41" s="100"/>
-      <c r="G41" s="100"/>
-      <c r="H41" s="100"/>
-      <c r="I41" s="104"/>
+      <c r="E41" s="112"/>
+      <c r="F41" s="109"/>
+      <c r="G41" s="109"/>
+      <c r="H41" s="109"/>
+      <c r="I41" s="113"/>
     </row>
     <row r="42" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E42" s="103"/>
-      <c r="F42" s="100"/>
-      <c r="G42" s="100"/>
-      <c r="H42" s="100"/>
-      <c r="I42" s="104"/>
+      <c r="E42" s="112"/>
+      <c r="F42" s="109"/>
+      <c r="G42" s="109"/>
+      <c r="H42" s="109"/>
+      <c r="I42" s="113"/>
     </row>
     <row r="43" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E43" s="103"/>
-      <c r="F43" s="100"/>
-      <c r="G43" s="100"/>
-      <c r="H43" s="100"/>
-      <c r="I43" s="104"/>
+      <c r="E43" s="112"/>
+      <c r="F43" s="109"/>
+      <c r="G43" s="109"/>
+      <c r="H43" s="109"/>
+      <c r="I43" s="113"/>
     </row>
     <row r="44" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E44" s="103"/>
-      <c r="F44" s="100"/>
-      <c r="G44" s="100"/>
-      <c r="H44" s="100"/>
-      <c r="I44" s="104"/>
+      <c r="E44" s="112"/>
+      <c r="F44" s="109"/>
+      <c r="G44" s="109"/>
+      <c r="H44" s="109"/>
+      <c r="I44" s="113"/>
     </row>
     <row r="45" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E45" s="103"/>
-      <c r="F45" s="100"/>
-      <c r="G45" s="100"/>
-      <c r="H45" s="100"/>
-      <c r="I45" s="104"/>
+      <c r="E45" s="112"/>
+      <c r="F45" s="109"/>
+      <c r="G45" s="109"/>
+      <c r="H45" s="109"/>
+      <c r="I45" s="113"/>
     </row>
     <row r="46" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E46" s="103"/>
-      <c r="F46" s="100"/>
-      <c r="G46" s="100"/>
-      <c r="H46" s="100"/>
-      <c r="I46" s="104"/>
+      <c r="E46" s="112"/>
+      <c r="F46" s="109"/>
+      <c r="G46" s="109"/>
+      <c r="H46" s="109"/>
+      <c r="I46" s="113"/>
     </row>
     <row r="47" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E47" s="103"/>
-      <c r="F47" s="100"/>
-      <c r="G47" s="100"/>
-      <c r="H47" s="100"/>
-      <c r="I47" s="104"/>
+      <c r="E47" s="112"/>
+      <c r="F47" s="109"/>
+      <c r="G47" s="109"/>
+      <c r="H47" s="109"/>
+      <c r="I47" s="113"/>
     </row>
     <row r="48" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E48" s="103"/>
-      <c r="F48" s="100"/>
-      <c r="G48" s="100"/>
-      <c r="H48" s="100"/>
-      <c r="I48" s="104"/>
+      <c r="E48" s="112"/>
+      <c r="F48" s="109"/>
+      <c r="G48" s="109"/>
+      <c r="H48" s="109"/>
+      <c r="I48" s="113"/>
     </row>
     <row r="49" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E49" s="103"/>
-      <c r="F49" s="100"/>
-      <c r="G49" s="100"/>
-      <c r="H49" s="100"/>
-      <c r="I49" s="104"/>
+      <c r="E49" s="112"/>
+      <c r="F49" s="109"/>
+      <c r="G49" s="109"/>
+      <c r="H49" s="109"/>
+      <c r="I49" s="113"/>
     </row>
     <row r="50" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E50" s="103"/>
-      <c r="F50" s="100"/>
-      <c r="G50" s="100"/>
-      <c r="H50" s="100"/>
-      <c r="I50" s="104"/>
+      <c r="E50" s="112"/>
+      <c r="F50" s="109"/>
+      <c r="G50" s="109"/>
+      <c r="H50" s="109"/>
+      <c r="I50" s="113"/>
     </row>
     <row r="51" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E51" s="105"/>
-      <c r="F51" s="106"/>
-      <c r="G51" s="106"/>
-      <c r="H51" s="106"/>
-      <c r="I51" s="107"/>
-    </row>
-    <row r="64" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="101" t="s">
-        <v>63</v>
-      </c>
-      <c r="D65" s="99"/>
-      <c r="E65" s="99"/>
-      <c r="F65" s="99"/>
-      <c r="G65" s="102"/>
-    </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="103"/>
-      <c r="D66" s="100"/>
-      <c r="E66" s="100"/>
-      <c r="F66" s="100"/>
-      <c r="G66" s="104"/>
-    </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="103"/>
-      <c r="D67" s="100"/>
-      <c r="E67" s="100"/>
-      <c r="F67" s="100"/>
-      <c r="G67" s="104"/>
-    </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C68" s="103"/>
-      <c r="D68" s="100"/>
-      <c r="E68" s="100"/>
-      <c r="F68" s="100"/>
-      <c r="G68" s="104"/>
-    </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="103"/>
-      <c r="D69" s="100"/>
-      <c r="E69" s="100"/>
-      <c r="F69" s="100"/>
-      <c r="G69" s="104"/>
-    </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="103"/>
-      <c r="D70" s="100"/>
-      <c r="E70" s="100"/>
-      <c r="F70" s="100"/>
-      <c r="G70" s="104"/>
-    </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C71" s="103"/>
-      <c r="D71" s="100"/>
-      <c r="E71" s="100"/>
-      <c r="F71" s="100"/>
-      <c r="G71" s="104"/>
-    </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="103"/>
-      <c r="D72" s="100"/>
-      <c r="E72" s="100"/>
-      <c r="F72" s="100"/>
-      <c r="G72" s="104"/>
-    </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="103"/>
-      <c r="D73" s="100"/>
-      <c r="E73" s="100"/>
-      <c r="F73" s="100"/>
-      <c r="G73" s="104"/>
-    </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="103"/>
-      <c r="D74" s="100"/>
-      <c r="E74" s="100"/>
-      <c r="F74" s="100"/>
-      <c r="G74" s="104"/>
-    </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="103"/>
-      <c r="D75" s="100"/>
-      <c r="E75" s="100"/>
-      <c r="F75" s="100"/>
-      <c r="G75" s="104"/>
-    </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="103"/>
-      <c r="D76" s="100"/>
-      <c r="E76" s="100"/>
-      <c r="F76" s="100"/>
-      <c r="G76" s="104"/>
-    </row>
-    <row r="77" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C77" s="105"/>
-      <c r="D77" s="106"/>
-      <c r="E77" s="106"/>
-      <c r="F77" s="106"/>
-      <c r="G77" s="107"/>
-    </row>
-    <row r="84" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E51" s="114"/>
+      <c r="F51" s="115"/>
+      <c r="G51" s="115"/>
+      <c r="H51" s="115"/>
+      <c r="I51" s="116"/>
+    </row>
+    <row r="84" spans="10:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J84" s="62"/>
     </row>
-    <row r="85" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J85" s="62"/>
     </row>
-    <row r="86" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C86" s="101" t="s">
-        <v>64</v>
-      </c>
-      <c r="D86" s="99"/>
-      <c r="E86" s="99"/>
-      <c r="F86" s="99"/>
-      <c r="G86" s="102"/>
+    <row r="86" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J86" s="62"/>
     </row>
-    <row r="87" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C87" s="103"/>
-      <c r="D87" s="100"/>
-      <c r="E87" s="100"/>
-      <c r="F87" s="100"/>
-      <c r="G87" s="104"/>
+    <row r="87" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J87" s="62"/>
     </row>
-    <row r="88" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C88" s="103"/>
-      <c r="D88" s="100"/>
-      <c r="E88" s="100"/>
-      <c r="F88" s="100"/>
-      <c r="G88" s="104"/>
+    <row r="88" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J88" s="62"/>
     </row>
-    <row r="89" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C89" s="103"/>
-      <c r="D89" s="100"/>
-      <c r="E89" s="100"/>
-      <c r="F89" s="100"/>
-      <c r="G89" s="104"/>
+    <row r="89" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J89" s="62"/>
     </row>
-    <row r="90" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C90" s="103"/>
-      <c r="D90" s="100"/>
-      <c r="E90" s="100"/>
-      <c r="F90" s="100"/>
-      <c r="G90" s="104"/>
+    <row r="90" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J90" s="62"/>
     </row>
-    <row r="91" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C91" s="103"/>
-      <c r="D91" s="100"/>
-      <c r="E91" s="100"/>
-      <c r="F91" s="100"/>
-      <c r="G91" s="104"/>
+    <row r="91" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J91" s="62"/>
     </row>
-    <row r="92" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C92" s="103"/>
-      <c r="D92" s="100"/>
-      <c r="E92" s="100"/>
-      <c r="F92" s="100"/>
-      <c r="G92" s="104"/>
+    <row r="92" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J92" s="62"/>
     </row>
-    <row r="93" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C93" s="103"/>
-      <c r="D93" s="100"/>
-      <c r="E93" s="100"/>
-      <c r="F93" s="100"/>
-      <c r="G93" s="104"/>
+    <row r="93" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J93" s="62"/>
     </row>
-    <row r="94" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C94" s="103"/>
-      <c r="D94" s="100"/>
-      <c r="E94" s="100"/>
-      <c r="F94" s="100"/>
-      <c r="G94" s="104"/>
+    <row r="94" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J94" s="62"/>
     </row>
-    <row r="95" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C95" s="103"/>
-      <c r="D95" s="100"/>
-      <c r="E95" s="100"/>
-      <c r="F95" s="100"/>
-      <c r="G95" s="104"/>
+    <row r="95" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J95" s="62"/>
     </row>
-    <row r="96" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C96" s="103"/>
-      <c r="D96" s="100"/>
-      <c r="E96" s="100"/>
-      <c r="F96" s="100"/>
-      <c r="G96" s="104"/>
+    <row r="96" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J96" s="62"/>
     </row>
-    <row r="97" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C97" s="103"/>
-      <c r="D97" s="100"/>
-      <c r="E97" s="100"/>
-      <c r="F97" s="100"/>
-      <c r="G97" s="104"/>
-    </row>
-    <row r="98" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C98" s="105"/>
-      <c r="D98" s="106"/>
-      <c r="E98" s="106"/>
-      <c r="F98" s="106"/>
-      <c r="G98" s="107"/>
-    </row>
-    <row r="108" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="109" spans="3:10" ht="315" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F109" s="108" t="s">
-        <v>65</v>
-      </c>
-      <c r="G109" s="109"/>
-      <c r="H109" s="109"/>
-      <c r="I109" s="110"/>
-    </row>
-    <row r="110" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="6:10" ht="315" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F110" s="61"/>
       <c r="G110" s="62"/>
       <c r="H110" s="62"/>
       <c r="I110" s="62"/>
     </row>
-    <row r="111" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F111" s="62"/>
       <c r="G111" s="62"/>
       <c r="H111" s="62"/>
       <c r="I111" s="62"/>
       <c r="J111" s="18"/>
     </row>
-    <row r="112" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F112" s="62"/>
       <c r="G112" s="62"/>
       <c r="H112" s="62"/>
@@ -3885,15 +3689,13 @@
       <c r="I148" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="2">
     <mergeCell ref="C17:G30"/>
-    <mergeCell ref="C65:G77"/>
-    <mergeCell ref="C86:G98"/>
     <mergeCell ref="E39:I51"/>
-    <mergeCell ref="F109:I109"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3901,8 +3703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3952,19 +3754,19 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="56" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="111">
+      <c r="A2" s="117">
         <v>1</v>
       </c>
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="117" t="s">
+      <c r="C2" s="123" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="117" t="s">
+      <c r="D2" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="117">
+      <c r="E2" s="123">
         <v>2</v>
       </c>
       <c r="F2" s="40" t="s">
@@ -3982,11 +3784,11 @@
       <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="112"/>
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
+      <c r="A3" s="118"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
       <c r="F3" s="40" t="s">
         <v>60</v>
       </c>
@@ -4002,19 +3804,19 @@
       <c r="J3" s="40"/>
     </row>
     <row r="4" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="117">
+      <c r="A4" s="123">
         <v>2</v>
       </c>
-      <c r="B4" s="118">
+      <c r="B4" s="124">
         <v>42440</v>
       </c>
-      <c r="C4" s="117" t="s">
+      <c r="C4" s="123" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="117" t="s">
+      <c r="D4" s="123" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="111">
+      <c r="E4" s="117">
         <v>2</v>
       </c>
       <c r="F4" s="40" t="s">
@@ -4032,11 +3834,11 @@
       <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="111"/>
-      <c r="B5" s="111"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="112"/>
+      <c r="A5" s="117"/>
+      <c r="B5" s="117"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="118"/>
       <c r="F5" s="47" t="s">
         <v>54</v>
       </c>
@@ -4052,23 +3854,23 @@
       <c r="J5" s="47"/>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="117">
+      <c r="A6" s="123">
         <v>3</v>
       </c>
-      <c r="B6" s="114">
+      <c r="B6" s="120">
         <v>42683</v>
       </c>
-      <c r="C6" s="111" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="111" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="111">
+      <c r="C6" s="117" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="117" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="117">
         <v>2</v>
       </c>
       <c r="F6" s="40" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G6" s="40" t="s">
         <v>49</v>
@@ -4082,16 +3884,16 @@
       <c r="J6" s="40"/>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="117"/>
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
+      <c r="A7" s="123"/>
+      <c r="B7" s="118"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="118"/>
+      <c r="E7" s="118"/>
       <c r="F7" s="67" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G7" s="68" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H7" s="59">
         <v>42624</v>
@@ -4102,16 +3904,16 @@
       <c r="J7" s="40"/>
     </row>
     <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="117"/>
-      <c r="B8" s="112"/>
-      <c r="C8" s="112"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
+      <c r="A8" s="123"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118"/>
       <c r="F8" s="64" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G8" s="64" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H8" s="69">
         <v>42691</v>
@@ -4122,13 +3924,13 @@
       <c r="J8" s="64"/>
     </row>
     <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="117"/>
-      <c r="B9" s="112"/>
-      <c r="C9" s="112"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
+      <c r="A9" s="123"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="118"/>
+      <c r="D9" s="118"/>
+      <c r="E9" s="118"/>
       <c r="F9" s="64" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G9" s="64" t="s">
         <v>49</v>
@@ -4142,13 +3944,13 @@
       <c r="J9" s="64"/>
     </row>
     <row r="10" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="117"/>
-      <c r="B10" s="113"/>
-      <c r="C10" s="113"/>
-      <c r="D10" s="113"/>
-      <c r="E10" s="113"/>
+      <c r="A10" s="123"/>
+      <c r="B10" s="119"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="119"/>
       <c r="F10" s="40" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G10" s="40" t="s">
         <v>49</v>
@@ -4160,23 +3962,23 @@
         <v>57</v>
       </c>
       <c r="J10" s="71" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="123">
+        <v>4</v>
+      </c>
+      <c r="B11" s="123" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="123" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="123" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="117">
-        <v>4</v>
-      </c>
-      <c r="B11" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="117" t="s">
-        <v>122</v>
-      </c>
-      <c r="D11" s="117" t="s">
-        <v>123</v>
-      </c>
-      <c r="E11" s="117">
+      <c r="E11" s="123">
         <v>2</v>
       </c>
       <c r="F11" s="64" t="s">
@@ -4194,11 +3996,11 @@
       <c r="J11" s="64"/>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="117"/>
-      <c r="B12" s="117"/>
-      <c r="C12" s="117"/>
-      <c r="D12" s="117"/>
-      <c r="E12" s="117"/>
+      <c r="A12" s="123"/>
+      <c r="B12" s="123"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="123"/>
       <c r="F12" s="67" t="s">
         <v>58</v>
       </c>
@@ -4214,13 +4016,13 @@
       <c r="J12" s="64"/>
     </row>
     <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="111"/>
-      <c r="B13" s="111"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
+      <c r="A13" s="117"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
       <c r="F13" s="85" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G13" s="80" t="s">
         <v>61</v>
@@ -4234,24 +4036,24 @@
       <c r="J13" s="80"/>
     </row>
     <row r="14" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="111">
+      <c r="A14" s="117">
         <v>5</v>
       </c>
-      <c r="B14" s="114">
+      <c r="B14" s="120">
         <v>42705</v>
       </c>
-      <c r="C14" s="111"/>
-      <c r="D14" s="111" t="s">
-        <v>123</v>
-      </c>
-      <c r="E14" s="111">
+      <c r="C14" s="117"/>
+      <c r="D14" s="117" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="117">
         <v>2</v>
       </c>
       <c r="F14" s="86" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G14" s="86" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H14" s="87">
         <v>42705</v>
@@ -4262,33 +4064,33 @@
       <c r="J14" s="81"/>
     </row>
     <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A15" s="112"/>
-      <c r="B15" s="115"/>
-      <c r="C15" s="112"/>
-      <c r="D15" s="112"/>
-      <c r="E15" s="112"/>
+      <c r="A15" s="118"/>
+      <c r="B15" s="121"/>
+      <c r="C15" s="118"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="118"/>
       <c r="F15" s="86" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G15" s="86" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H15" s="87">
         <v>42705</v>
       </c>
       <c r="I15" s="92" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J15" s="81"/>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="112"/>
-      <c r="B16" s="115"/>
-      <c r="C16" s="112"/>
-      <c r="D16" s="113"/>
-      <c r="E16" s="112"/>
+      <c r="A16" s="118"/>
+      <c r="B16" s="121"/>
+      <c r="C16" s="118"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="118"/>
       <c r="F16" s="86" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G16" s="86" t="s">
         <v>49</v>
@@ -4302,18 +4104,18 @@
       <c r="J16" s="81"/>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="112"/>
-      <c r="B17" s="115"/>
-      <c r="C17" s="112"/>
+      <c r="A17" s="118"/>
+      <c r="B17" s="121"/>
+      <c r="C17" s="118"/>
       <c r="D17" s="81" t="s">
-        <v>124</v>
-      </c>
-      <c r="E17" s="112"/>
+        <v>119</v>
+      </c>
+      <c r="E17" s="118"/>
       <c r="F17" s="86" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="G17" s="86" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H17" s="87">
         <v>42705</v>
@@ -4324,15 +4126,15 @@
       <c r="J17" s="81"/>
     </row>
     <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="112"/>
-      <c r="B18" s="115"/>
-      <c r="C18" s="112"/>
-      <c r="D18" s="111" t="s">
-        <v>125</v>
-      </c>
-      <c r="E18" s="112"/>
+      <c r="A18" s="118"/>
+      <c r="B18" s="121"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="118"/>
       <c r="F18" s="86" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G18" s="86" t="s">
         <v>49</v>
@@ -4346,17 +4148,17 @@
       <c r="J18" s="81"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="113"/>
-      <c r="B19" s="116"/>
-      <c r="C19" s="113"/>
-      <c r="D19" s="113"/>
-      <c r="E19" s="113"/>
+      <c r="A19" s="119"/>
+      <c r="B19" s="122"/>
+      <c r="C19" s="119"/>
+      <c r="D19" s="119"/>
+      <c r="E19" s="119"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="58">
         <v>6</v>
       </c>
-      <c r="B20" s="131">
+      <c r="B20" s="99">
         <v>42387</v>
       </c>
     </row>
@@ -4421,14 +4223,14 @@
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B2" s="74"/>
       <c r="C2" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E2" s="10">
         <v>41225</v>
@@ -4443,14 +4245,14 @@
     </row>
     <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E3" s="10">
         <v>42136</v>
@@ -4465,14 +4267,14 @@
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="72" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E4" s="10">
         <v>41575</v>
@@ -4487,16 +4289,16 @@
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="83" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D5" s="75" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E5" s="76">
         <v>41225</v>
@@ -4509,16 +4311,16 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="74" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B6" s="74"/>
       <c r="C6" s="57" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D6" s="75" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E6" s="76">
         <v>42143</v>
@@ -4550,20 +4352,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="125" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="121" t="s">
+      <c r="B1" s="127" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="123" t="s">
+      <c r="C1" s="129" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124" t="s">
+      <c r="D1" s="130"/>
+      <c r="E1" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="125"/>
+      <c r="F1" s="131"/>
       <c r="G1" s="23" t="s">
         <v>35</v>
       </c>
@@ -4581,8 +4383,8 @@
       <c r="S1" s="24"/>
     </row>
     <row r="2" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="120"/>
-      <c r="B2" s="122"/>
+      <c r="A2" s="126"/>
+      <c r="B2" s="128"/>
       <c r="C2" s="25" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Criada apresentação do Projeto para  Reunião do dia 15/12 Alterado os gráficos e médias gerais
</commit_message>
<xml_diff>
--- a/TRE_Dados_MapaRaciocinio.xlsx
+++ b/TRE_Dados_MapaRaciocinio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Historicos x Categoria" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="168">
   <si>
     <t>Categoria</t>
   </si>
@@ -555,19 +555,19 @@
     <t xml:space="preserve">Contratação de empresa para fornecimento de materiais e serviços para montagem/desmontagem e readequação de forros e divisórias, através de Registro de Preços. </t>
   </si>
   <si>
-    <t xml:space="preserve">Conclusão
-</t>
+    <t>Contratação Serviço de Manutenção Predial Detização e Controle de Pragas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="dd\-mm\-yy"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,8 +636,15 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -686,8 +693,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="31">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -761,46 +774,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1102,115 +1075,115 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="5" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="5" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1223,7 +1196,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1265,20 +1238,20 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1287,7 +1260,7 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1307,23 +1280,27 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1335,76 +1312,58 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="10" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="10" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1418,6 +1377,320 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graficos!$D$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tempo TOTAL (Dias) =Lead Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graficos!$A$48:$A$76</c:f>
+              <c:strCache>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>Serviços Combustível</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Alarme-Monitoramento</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Alarme-Monitoramento</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Alarme-Monitoramento</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Alarme-Monitoramento</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Alarme-Monitoramento</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Alarme-Monitoramento</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Serviços de Manutenção</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Serviços de Mão de Obra</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Serviço de Manutenção</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Serviço de Manutenção</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Aquisição Bens de Consumo</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Serviços de Mão de Obra</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Serviços de Mão de Obra</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Aquisição de Software</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Serviços de Manutenção</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Serviços de Manutenção</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Serviços de Manutenção</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Serviços de Manutenção</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Serviços de Manutenção Reformas</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Aquisição de Bens de Consumo -Mat Hidraulicos e Eletricos</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Aquisição de Bens de Consumo Placas Indicaticas</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Contratação Eletricista Capital</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Contratação Manutenção Predial</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Aquisição de Bens de Consumo -Mat Hidraulicos e Eletricos</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Contratação Serviço de Manutenção Predial Detização e Controle de Pragas</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Contratação de  Serviço de Reformas</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Contratação de  Serviço de Manutenção Predial - DIVISÓRIAS</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Serviços de Engenharia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graficos!$D$48:$D$76</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>465</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>642</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>397</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>123</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="168800768"/>
+        <c:axId val="149224768"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="168800768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="149224768"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="149224768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="168800768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1477,59 +1750,34 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>86591</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>155863</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2695574</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>106507</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>251114</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>2407226</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Imagem 12"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="95249" y="7715250"/>
-          <a:ext cx="5483802" cy="3656734"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2173,9 +2421,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2195,11 +2443,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
       <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
@@ -2208,7 +2456,7 @@
       </c>
       <c r="F1" s="10">
         <f ca="1">TODAY()</f>
-        <v>42718</v>
+        <v>42719</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>11</v>
@@ -2491,12 +2739,12 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="100"/>
       <c r="B13" s="101"/>
-      <c r="C13" s="105" t="s">
+      <c r="C13" s="107" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="106"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="107"/>
+      <c r="F13" s="108"/>
       <c r="G13" s="73">
         <f>AVERAGE(G4:G12)</f>
         <v>164.55555555555554</v>
@@ -2523,7 +2771,7 @@
         <v>42671</v>
       </c>
       <c r="G14" s="17">
-        <f t="shared" ref="G14:G34" si="1">DAYS360(E14,F14)</f>
+        <f t="shared" ref="G14:G33" si="1">DAYS360(E14,F14)</f>
         <v>642</v>
       </c>
     </row>
@@ -2864,7 +3112,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="132" t="s">
+      <c r="A29" s="103" t="s">
         <v>156</v>
       </c>
       <c r="B29" s="74" t="s">
@@ -2897,7 +3145,7 @@
       <c r="C30" s="95" t="s">
         <v>159</v>
       </c>
-      <c r="D30" s="133" t="s">
+      <c r="D30" s="104" t="s">
         <v>160</v>
       </c>
       <c r="E30" s="96">
@@ -2984,14 +3232,14 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="104" t="s">
+      <c r="A34" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="B34" s="105"/>
-      <c r="C34" s="105"/>
-      <c r="D34" s="105"/>
-      <c r="E34" s="105"/>
-      <c r="F34" s="106"/>
+      <c r="B34" s="107"/>
+      <c r="C34" s="107"/>
+      <c r="D34" s="107"/>
+      <c r="E34" s="107"/>
+      <c r="F34" s="108"/>
       <c r="G34" s="17">
         <f>AVERAGE(G14:G33)</f>
         <v>174.95</v>
@@ -3201,14 +3449,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J148"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.28515625" customWidth="1"/>
     <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -3250,7 +3500,7 @@
       <c r="A6" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="127">
         <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$33,A6,'Dados Historicos x Categoria'!$G$4:$G$33)</f>
         <v>148.57142857142858</v>
       </c>
@@ -3281,198 +3531,524 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="107" t="s">
+      <c r="C17" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="D17" s="108"/>
-      <c r="E17" s="108"/>
-      <c r="F17" s="108"/>
-      <c r="G17" s="108"/>
+      <c r="D17" s="110"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="110"/>
+      <c r="G17" s="110"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="109"/>
-      <c r="D18" s="109"/>
-      <c r="E18" s="109"/>
-      <c r="F18" s="109"/>
-      <c r="G18" s="109"/>
+      <c r="C18" s="111"/>
+      <c r="D18" s="111"/>
+      <c r="E18" s="111"/>
+      <c r="F18" s="111"/>
+      <c r="G18" s="111"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="109"/>
-      <c r="D19" s="109"/>
-      <c r="E19" s="109"/>
-      <c r="F19" s="109"/>
-      <c r="G19" s="109"/>
+      <c r="C19" s="111"/>
+      <c r="D19" s="111"/>
+      <c r="E19" s="111"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="111"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="109"/>
-      <c r="D20" s="109"/>
-      <c r="E20" s="109"/>
-      <c r="F20" s="109"/>
-      <c r="G20" s="109"/>
+      <c r="C20" s="111"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="111"/>
+      <c r="F20" s="111"/>
+      <c r="G20" s="111"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="109"/>
-      <c r="D21" s="109"/>
-      <c r="E21" s="109"/>
-      <c r="F21" s="109"/>
-      <c r="G21" s="109"/>
+      <c r="C21" s="111"/>
+      <c r="D21" s="111"/>
+      <c r="E21" s="111"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="111"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="109"/>
-      <c r="D22" s="109"/>
-      <c r="E22" s="109"/>
-      <c r="F22" s="109"/>
-      <c r="G22" s="109"/>
+      <c r="C22" s="111"/>
+      <c r="D22" s="111"/>
+      <c r="E22" s="111"/>
+      <c r="F22" s="111"/>
+      <c r="G22" s="111"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="109"/>
-      <c r="D23" s="109"/>
-      <c r="E23" s="109"/>
-      <c r="F23" s="109"/>
-      <c r="G23" s="109"/>
+      <c r="C23" s="111"/>
+      <c r="D23" s="111"/>
+      <c r="E23" s="111"/>
+      <c r="F23" s="111"/>
+      <c r="G23" s="111"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="109"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="109"/>
-      <c r="G24" s="109"/>
+      <c r="C24" s="111"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="111"/>
+      <c r="F24" s="111"/>
+      <c r="G24" s="111"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="109"/>
-      <c r="D25" s="109"/>
-      <c r="E25" s="109"/>
-      <c r="F25" s="109"/>
-      <c r="G25" s="109"/>
+      <c r="C25" s="111"/>
+      <c r="D25" s="111"/>
+      <c r="E25" s="111"/>
+      <c r="F25" s="111"/>
+      <c r="G25" s="111"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="109"/>
-      <c r="D26" s="109"/>
-      <c r="E26" s="109"/>
-      <c r="F26" s="109"/>
-      <c r="G26" s="109"/>
+      <c r="C26" s="111"/>
+      <c r="D26" s="111"/>
+      <c r="E26" s="111"/>
+      <c r="F26" s="111"/>
+      <c r="G26" s="111"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="109"/>
-      <c r="D27" s="109"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="109"/>
-      <c r="G27" s="109"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="111"/>
+      <c r="E27" s="111"/>
+      <c r="F27" s="111"/>
+      <c r="G27" s="111"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="109"/>
-      <c r="D28" s="109"/>
-      <c r="E28" s="109"/>
-      <c r="F28" s="109"/>
-      <c r="G28" s="109"/>
+      <c r="C28" s="111"/>
+      <c r="D28" s="111"/>
+      <c r="E28" s="111"/>
+      <c r="F28" s="111"/>
+      <c r="G28" s="111"/>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="109"/>
-      <c r="D29" s="109"/>
-      <c r="E29" s="109"/>
-      <c r="F29" s="109"/>
-      <c r="G29" s="109"/>
+      <c r="C29" s="111"/>
+      <c r="D29" s="111"/>
+      <c r="E29" s="111"/>
+      <c r="F29" s="111"/>
+      <c r="G29" s="111"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="109"/>
-      <c r="D30" s="109"/>
-      <c r="E30" s="109"/>
-      <c r="F30" s="109"/>
-      <c r="G30" s="109"/>
-    </row>
-    <row r="38" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="110" t="s">
+      <c r="C30" s="111"/>
+      <c r="D30" s="111"/>
+      <c r="E30" s="111"/>
+      <c r="F30" s="111"/>
+      <c r="G30" s="111"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="131" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="132" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="132" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="133" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="128" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="129">
+        <v>42311</v>
+      </c>
+      <c r="C48" s="129">
+        <v>42446</v>
+      </c>
+      <c r="D48" s="130">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="128" t="s">
+        <v>131</v>
+      </c>
+      <c r="B49" s="129">
+        <v>42118</v>
+      </c>
+      <c r="C49" s="129">
+        <v>42221</v>
+      </c>
+      <c r="D49" s="130">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="128" t="s">
+        <v>131</v>
+      </c>
+      <c r="B50" s="129">
+        <v>42263</v>
+      </c>
+      <c r="C50" s="129">
+        <v>42342</v>
+      </c>
+      <c r="D50" s="130">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="128" t="s">
+        <v>131</v>
+      </c>
+      <c r="B51" s="129">
+        <v>42633</v>
+      </c>
+      <c r="C51" s="129">
+        <v>42695</v>
+      </c>
+      <c r="D51" s="130">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="128" t="s">
+        <v>131</v>
+      </c>
+      <c r="B52" s="129">
+        <v>42422</v>
+      </c>
+      <c r="C52" s="129">
+        <v>42643</v>
+      </c>
+      <c r="D52" s="130">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="128" t="s">
+        <v>131</v>
+      </c>
+      <c r="B53" s="129">
+        <v>41955</v>
+      </c>
+      <c r="C53" s="129">
+        <v>42179</v>
+      </c>
+      <c r="D53" s="130">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="128" t="s">
+        <v>131</v>
+      </c>
+      <c r="B54" s="129">
+        <v>41738</v>
+      </c>
+      <c r="C54" s="129">
+        <v>41850</v>
+      </c>
+      <c r="D54" s="130">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="128" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="129">
+        <v>41337</v>
+      </c>
+      <c r="C55" s="129">
+        <v>41430</v>
+      </c>
+      <c r="D55" s="130">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="128" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" s="129">
+        <v>42209</v>
+      </c>
+      <c r="C56" s="129">
+        <v>42683</v>
+      </c>
+      <c r="D56" s="130">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="128" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="129">
+        <v>42020</v>
+      </c>
+      <c r="C57" s="129">
+        <v>42671</v>
+      </c>
+      <c r="D57" s="130">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="128" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" s="129">
+        <v>42439</v>
+      </c>
+      <c r="C58" s="129">
+        <v>42668</v>
+      </c>
+      <c r="D58" s="130">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="128" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59" s="129">
+        <v>42521</v>
+      </c>
+      <c r="C59" s="129">
+        <v>42661</v>
+      </c>
+      <c r="D59" s="130">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="128" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" s="129">
+        <v>41242</v>
+      </c>
+      <c r="C60" s="129">
+        <v>41472</v>
+      </c>
+      <c r="D60" s="130">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="128" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" s="129">
+        <v>41698</v>
+      </c>
+      <c r="C61" s="129">
+        <v>41932</v>
+      </c>
+      <c r="D61" s="130">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="128" t="s">
+        <v>99</v>
+      </c>
+      <c r="B62" s="129">
+        <v>42277</v>
+      </c>
+      <c r="C62" s="129">
+        <v>42681</v>
+      </c>
+      <c r="D62" s="130">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="128" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" s="129">
+        <v>42136</v>
+      </c>
+      <c r="C63" s="129">
+        <v>42171</v>
+      </c>
+      <c r="D63" s="130">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="128" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" s="129">
+        <v>41541</v>
+      </c>
+      <c r="C64" s="129">
+        <v>41634</v>
+      </c>
+      <c r="D64" s="130">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="128" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" s="129">
+        <v>41575</v>
+      </c>
+      <c r="C65" s="129">
+        <v>41638</v>
+      </c>
+      <c r="D65" s="130">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="128" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" s="129">
+        <v>42580</v>
+      </c>
+      <c r="C66" s="129">
+        <v>42641</v>
+      </c>
+      <c r="D66" s="130">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="128" t="s">
+        <v>142</v>
+      </c>
+      <c r="B67" s="129">
+        <v>42612</v>
+      </c>
+      <c r="C67" s="129">
+        <v>42704</v>
+      </c>
+      <c r="D67" s="130">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="128" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68" s="129">
+        <v>42068</v>
+      </c>
+      <c r="C68" s="129">
+        <v>42149</v>
+      </c>
+      <c r="D68" s="130">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="128" t="s">
+        <v>148</v>
+      </c>
+      <c r="B69" s="129">
+        <v>42410</v>
+      </c>
+      <c r="C69" s="129">
+        <v>42690</v>
+      </c>
+      <c r="D69" s="130">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="128" t="s">
+        <v>151</v>
+      </c>
+      <c r="B70" s="129">
+        <v>41208</v>
+      </c>
+      <c r="C70" s="129">
+        <v>41348</v>
+      </c>
+      <c r="D70" s="130">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="128" t="s">
+        <v>153</v>
+      </c>
+      <c r="B71" s="129">
+        <v>40927</v>
+      </c>
+      <c r="C71" s="129">
+        <v>41012</v>
+      </c>
+      <c r="D71" s="130">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="128" t="s">
+        <v>145</v>
+      </c>
+      <c r="B72" s="129">
+        <v>41885</v>
+      </c>
+      <c r="C72" s="129">
+        <v>41996</v>
+      </c>
+      <c r="D72" s="130">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="128" t="s">
         <v>167</v>
       </c>
-      <c r="F39" s="108"/>
-      <c r="G39" s="108"/>
-      <c r="H39" s="108"/>
-      <c r="I39" s="111"/>
-    </row>
-    <row r="40" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E40" s="112"/>
-      <c r="F40" s="109"/>
-      <c r="G40" s="109"/>
-      <c r="H40" s="109"/>
-      <c r="I40" s="113"/>
-    </row>
-    <row r="41" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="112"/>
-      <c r="F41" s="109"/>
-      <c r="G41" s="109"/>
-      <c r="H41" s="109"/>
-      <c r="I41" s="113"/>
-    </row>
-    <row r="42" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E42" s="112"/>
-      <c r="F42" s="109"/>
-      <c r="G42" s="109"/>
-      <c r="H42" s="109"/>
-      <c r="I42" s="113"/>
-    </row>
-    <row r="43" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E43" s="112"/>
-      <c r="F43" s="109"/>
-      <c r="G43" s="109"/>
-      <c r="H43" s="109"/>
-      <c r="I43" s="113"/>
-    </row>
-    <row r="44" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E44" s="112"/>
-      <c r="F44" s="109"/>
-      <c r="G44" s="109"/>
-      <c r="H44" s="109"/>
-      <c r="I44" s="113"/>
-    </row>
-    <row r="45" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E45" s="112"/>
-      <c r="F45" s="109"/>
-      <c r="G45" s="109"/>
-      <c r="H45" s="109"/>
-      <c r="I45" s="113"/>
-    </row>
-    <row r="46" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E46" s="112"/>
-      <c r="F46" s="109"/>
-      <c r="G46" s="109"/>
-      <c r="H46" s="109"/>
-      <c r="I46" s="113"/>
-    </row>
-    <row r="47" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E47" s="112"/>
-      <c r="F47" s="109"/>
-      <c r="G47" s="109"/>
-      <c r="H47" s="109"/>
-      <c r="I47" s="113"/>
-    </row>
-    <row r="48" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E48" s="112"/>
-      <c r="F48" s="109"/>
-      <c r="G48" s="109"/>
-      <c r="H48" s="109"/>
-      <c r="I48" s="113"/>
-    </row>
-    <row r="49" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E49" s="112"/>
-      <c r="F49" s="109"/>
-      <c r="G49" s="109"/>
-      <c r="H49" s="109"/>
-      <c r="I49" s="113"/>
-    </row>
-    <row r="50" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E50" s="112"/>
-      <c r="F50" s="109"/>
-      <c r="G50" s="109"/>
-      <c r="H50" s="109"/>
-      <c r="I50" s="113"/>
-    </row>
-    <row r="51" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E51" s="114"/>
-      <c r="F51" s="115"/>
-      <c r="G51" s="115"/>
-      <c r="H51" s="115"/>
-      <c r="I51" s="116"/>
+      <c r="B73" s="129">
+        <v>40945</v>
+      </c>
+      <c r="C73" s="129">
+        <v>41093</v>
+      </c>
+      <c r="D73" s="130">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="128" t="s">
+        <v>162</v>
+      </c>
+      <c r="B74" s="129">
+        <v>41411</v>
+      </c>
+      <c r="C74" s="129">
+        <v>41666</v>
+      </c>
+      <c r="D74" s="130">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="128" t="s">
+        <v>165</v>
+      </c>
+      <c r="B75" s="129">
+        <v>41905</v>
+      </c>
+      <c r="C75" s="129">
+        <v>41999</v>
+      </c>
+      <c r="D75" s="130">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="128" t="s">
+        <v>108</v>
+      </c>
+      <c r="B76" s="129">
+        <v>42229</v>
+      </c>
+      <c r="C76" s="129">
+        <v>42354</v>
+      </c>
+      <c r="D76" s="130">
+        <v>123</v>
+      </c>
     </row>
     <row r="84" spans="10:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J84" s="62"/>
@@ -3689,9 +4265,8 @@
       <c r="I148" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="C17:G30"/>
-    <mergeCell ref="E39:I51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3754,19 +4329,19 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="56" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="117">
+      <c r="A2" s="113">
         <v>1</v>
       </c>
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="123" t="s">
+      <c r="C2" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="123" t="s">
+      <c r="D2" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="123">
+      <c r="E2" s="112">
         <v>2</v>
       </c>
       <c r="F2" s="40" t="s">
@@ -3784,11 +4359,11 @@
       <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="118"/>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
+      <c r="A3" s="114"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
       <c r="F3" s="40" t="s">
         <v>60</v>
       </c>
@@ -3804,19 +4379,19 @@
       <c r="J3" s="40"/>
     </row>
     <row r="4" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="123">
+      <c r="A4" s="112">
         <v>2</v>
       </c>
-      <c r="B4" s="124">
+      <c r="B4" s="117">
         <v>42440</v>
       </c>
-      <c r="C4" s="123" t="s">
+      <c r="C4" s="112" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="123" t="s">
+      <c r="D4" s="112" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="117">
+      <c r="E4" s="113">
         <v>2</v>
       </c>
       <c r="F4" s="40" t="s">
@@ -3834,11 +4409,11 @@
       <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="117"/>
-      <c r="B5" s="117"/>
-      <c r="C5" s="117"/>
-      <c r="D5" s="117"/>
-      <c r="E5" s="118"/>
+      <c r="A5" s="113"/>
+      <c r="B5" s="113"/>
+      <c r="C5" s="113"/>
+      <c r="D5" s="113"/>
+      <c r="E5" s="114"/>
       <c r="F5" s="47" t="s">
         <v>54</v>
       </c>
@@ -3854,19 +4429,19 @@
       <c r="J5" s="47"/>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="123">
+      <c r="A6" s="112">
         <v>3</v>
       </c>
-      <c r="B6" s="120">
+      <c r="B6" s="116">
         <v>42683</v>
       </c>
-      <c r="C6" s="117" t="s">
+      <c r="C6" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="117" t="s">
+      <c r="D6" s="113" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="117">
+      <c r="E6" s="113">
         <v>2</v>
       </c>
       <c r="F6" s="40" t="s">
@@ -3884,11 +4459,11 @@
       <c r="J6" s="40"/>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="123"/>
-      <c r="B7" s="118"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
-      <c r="E7" s="118"/>
+      <c r="A7" s="112"/>
+      <c r="B7" s="114"/>
+      <c r="C7" s="114"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="114"/>
       <c r="F7" s="67" t="s">
         <v>67</v>
       </c>
@@ -3904,11 +4479,11 @@
       <c r="J7" s="40"/>
     </row>
     <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="123"/>
-      <c r="B8" s="118"/>
-      <c r="C8" s="118"/>
-      <c r="D8" s="118"/>
-      <c r="E8" s="118"/>
+      <c r="A8" s="112"/>
+      <c r="B8" s="114"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="114"/>
+      <c r="E8" s="114"/>
       <c r="F8" s="64" t="s">
         <v>69</v>
       </c>
@@ -3924,11 +4499,11 @@
       <c r="J8" s="64"/>
     </row>
     <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="123"/>
-      <c r="B9" s="118"/>
-      <c r="C9" s="118"/>
-      <c r="D9" s="118"/>
-      <c r="E9" s="118"/>
+      <c r="A9" s="112"/>
+      <c r="B9" s="114"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
       <c r="F9" s="64" t="s">
         <v>73</v>
       </c>
@@ -3944,11 +4519,11 @@
       <c r="J9" s="64"/>
     </row>
     <row r="10" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="123"/>
-      <c r="B10" s="119"/>
-      <c r="C10" s="119"/>
-      <c r="D10" s="119"/>
-      <c r="E10" s="119"/>
+      <c r="A10" s="112"/>
+      <c r="B10" s="115"/>
+      <c r="C10" s="115"/>
+      <c r="D10" s="115"/>
+      <c r="E10" s="115"/>
       <c r="F10" s="40" t="s">
         <v>70</v>
       </c>
@@ -3966,19 +4541,19 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="123">
+      <c r="A11" s="112">
         <v>4</v>
       </c>
-      <c r="B11" s="123" t="s">
+      <c r="B11" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="123" t="s">
+      <c r="C11" s="112" t="s">
         <v>117</v>
       </c>
-      <c r="D11" s="123" t="s">
+      <c r="D11" s="112" t="s">
         <v>118</v>
       </c>
-      <c r="E11" s="123">
+      <c r="E11" s="112">
         <v>2</v>
       </c>
       <c r="F11" s="64" t="s">
@@ -3996,11 +4571,11 @@
       <c r="J11" s="64"/>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="123"/>
-      <c r="B12" s="123"/>
-      <c r="C12" s="123"/>
-      <c r="D12" s="123"/>
-      <c r="E12" s="123"/>
+      <c r="A12" s="112"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
       <c r="F12" s="67" t="s">
         <v>58</v>
       </c>
@@ -4016,11 +4591,11 @@
       <c r="J12" s="64"/>
     </row>
     <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="117"/>
-      <c r="B13" s="117"/>
-      <c r="C13" s="117"/>
-      <c r="D13" s="117"/>
-      <c r="E13" s="117"/>
+      <c r="A13" s="113"/>
+      <c r="B13" s="113"/>
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
       <c r="F13" s="85" t="s">
         <v>72</v>
       </c>
@@ -4036,17 +4611,17 @@
       <c r="J13" s="80"/>
     </row>
     <row r="14" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="117">
+      <c r="A14" s="113">
         <v>5</v>
       </c>
-      <c r="B14" s="120">
+      <c r="B14" s="116">
         <v>42705</v>
       </c>
-      <c r="C14" s="117"/>
-      <c r="D14" s="117" t="s">
+      <c r="C14" s="113"/>
+      <c r="D14" s="113" t="s">
         <v>118</v>
       </c>
-      <c r="E14" s="117">
+      <c r="E14" s="113">
         <v>2</v>
       </c>
       <c r="F14" s="86" t="s">
@@ -4064,11 +4639,11 @@
       <c r="J14" s="81"/>
     </row>
     <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A15" s="118"/>
-      <c r="B15" s="121"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
+      <c r="A15" s="114"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="114"/>
+      <c r="D15" s="114"/>
+      <c r="E15" s="114"/>
       <c r="F15" s="86" t="s">
         <v>123</v>
       </c>
@@ -4084,11 +4659,11 @@
       <c r="J15" s="81"/>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="118"/>
-      <c r="B16" s="121"/>
-      <c r="C16" s="118"/>
-      <c r="D16" s="119"/>
-      <c r="E16" s="118"/>
+      <c r="A16" s="114"/>
+      <c r="B16" s="118"/>
+      <c r="C16" s="114"/>
+      <c r="D16" s="115"/>
+      <c r="E16" s="114"/>
       <c r="F16" s="86" t="s">
         <v>125</v>
       </c>
@@ -4104,13 +4679,13 @@
       <c r="J16" s="81"/>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="118"/>
-      <c r="B17" s="121"/>
-      <c r="C17" s="118"/>
+      <c r="A17" s="114"/>
+      <c r="B17" s="118"/>
+      <c r="C17" s="114"/>
       <c r="D17" s="81" t="s">
         <v>119</v>
       </c>
-      <c r="E17" s="118"/>
+      <c r="E17" s="114"/>
       <c r="F17" s="86" t="s">
         <v>126</v>
       </c>
@@ -4126,13 +4701,13 @@
       <c r="J17" s="81"/>
     </row>
     <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="118"/>
-      <c r="B18" s="121"/>
-      <c r="C18" s="118"/>
-      <c r="D18" s="117" t="s">
+      <c r="A18" s="114"/>
+      <c r="B18" s="118"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="E18" s="118"/>
+      <c r="E18" s="114"/>
       <c r="F18" s="86" t="s">
         <v>128</v>
       </c>
@@ -4148,11 +4723,11 @@
       <c r="J18" s="81"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="119"/>
-      <c r="B19" s="122"/>
-      <c r="C19" s="119"/>
-      <c r="D19" s="119"/>
-      <c r="E19" s="119"/>
+      <c r="A19" s="115"/>
+      <c r="B19" s="119"/>
+      <c r="C19" s="115"/>
+      <c r="D19" s="115"/>
+      <c r="E19" s="115"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="58">
@@ -4164,11 +4739,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C14:C19"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="A6:A10"/>
@@ -4185,11 +4760,11 @@
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="E11:E13"/>
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4198,10 +4773,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4239,7 +4814,7 @@
         <v>41263</v>
       </c>
       <c r="G2" s="17">
-        <f>DAYS360(E2,F2)</f>
+        <f t="shared" ref="G2:G7" si="0">DAYS360(E2,F2)</f>
         <v>38</v>
       </c>
     </row>
@@ -4261,7 +4836,7 @@
         <v>42171</v>
       </c>
       <c r="G3" s="17">
-        <f>DAYS360(E3,F3)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
     </row>
@@ -4283,7 +4858,7 @@
         <v>41638</v>
       </c>
       <c r="G4" s="17">
-        <f>DAYS360(E4,F4)</f>
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
     </row>
@@ -4307,7 +4882,7 @@
         <v>41263</v>
       </c>
       <c r="G5" s="77">
-        <f>DAYS360(E5,F5)</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
@@ -4329,8 +4904,33 @@
         <v>42156</v>
       </c>
       <c r="G6" s="77">
-        <f>DAYS360(E6,F6)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="74" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="11" t="str">
+        <f>LOWER("CONTRATAÇÃO - SERVIÇO DE MANUTENÇÃO PREDIAL -   LIMPEZA DE VIDROS - CAPITAL/ INTERIOR")</f>
+        <v>contratação - serviço de manutenção predial -   limpeza de vidros - capital/ interior</v>
+      </c>
+      <c r="E7" s="10">
+        <v>42020</v>
+      </c>
+      <c r="F7" s="10">
+        <v>42671</v>
+      </c>
+      <c r="G7" s="17">
+        <f t="shared" si="0"/>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -4352,20 +4952,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="122" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="129" t="s">
+      <c r="C1" s="124" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130" t="s">
+      <c r="D1" s="125"/>
+      <c r="E1" s="125" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="131"/>
+      <c r="F1" s="126"/>
       <c r="G1" s="23" t="s">
         <v>35</v>
       </c>
@@ -4383,8 +4983,8 @@
       <c r="S1" s="24"/>
     </row>
     <row r="2" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="126"/>
-      <c r="B2" s="128"/>
+      <c r="A2" s="121"/>
+      <c r="B2" s="123"/>
       <c r="C2" s="25" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Adicionado milestones para aba Controle do Projeto
</commit_message>
<xml_diff>
--- a/TRE_Dados_MapaRaciocinio.xlsx
+++ b/TRE_Dados_MapaRaciocinio.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Historicos x Categoria" sheetId="1" r:id="rId1"/>
@@ -13,17 +13,17 @@
     <sheet name="PROCESSO PADRÃO" sheetId="4" r:id="rId4"/>
     <sheet name="Controle do Projeto" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -33,7 +33,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Autor:
+          <t xml:space="preserve">Author:
 </t>
         </r>
       </text>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="177">
   <si>
     <t>Categoria</t>
   </si>
@@ -556,6 +556,33 @@
   </si>
   <si>
     <t>Contratação Serviço de Manutenção Predial Detização e Controle de Pragas</t>
+  </si>
+  <si>
+    <t>Conexão</t>
+  </si>
+  <si>
+    <t>oct/2016</t>
+  </si>
+  <si>
+    <t>dec/2016</t>
+  </si>
+  <si>
+    <t>apr/2017</t>
+  </si>
+  <si>
+    <t>may/2017</t>
+  </si>
+  <si>
+    <t>aug/2017</t>
+  </si>
+  <si>
+    <t>oct/2017</t>
+  </si>
+  <si>
+    <t>sep/2017</t>
+  </si>
+  <si>
+    <t>dec/2017</t>
   </si>
 </sst>
 </file>
@@ -565,7 +592,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="dd\-mm\-yy"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -644,7 +671,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -699,8 +726,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1042,12 +1075,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1120,9 +1227,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1141,9 +1245,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1160,9 +1261,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1291,79 +1389,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="10" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="10" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="10" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1374,6 +1514,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1394,7 +1537,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1420,6 +1562,13 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1427,6 +1576,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:trendline>
             <c:trendlineType val="linear"/>
@@ -1634,16 +1788,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="168800768"/>
-        <c:axId val="149224768"/>
+        <c:axId val="147124936"/>
+        <c:axId val="147096400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="168800768"/>
+        <c:axId val="147124936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1657,7 +1812,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149224768"/>
+        <c:crossAx val="147096400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1665,7 +1820,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149224768"/>
+        <c:axId val="147096400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1676,7 +1831,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168800768"/>
+        <c:crossAx val="147124936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1874,15 +2029,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
+      <xdr:colOff>325406</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>9527</xdr:rowOff>
+      <xdr:rowOff>28577</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>581026</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>588996</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1893,51 +2048,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4943476" y="771527"/>
-          <a:ext cx="1181100" cy="47624"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0C0C0" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="22"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Rectangle 12"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6762750" y="981076"/>
-          <a:ext cx="1200150" cy="57149"/>
+          <a:off x="5259356" y="752477"/>
+          <a:ext cx="2092390" cy="47624"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1961,13 +2073,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2089,15 +2201,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>338149</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>132522</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>451598</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>132522</xdr:rowOff>
+      <xdr:rowOff>151572</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2108,8 +2220,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4943475" y="838199"/>
-          <a:ext cx="122997" cy="56323"/>
+          <a:off x="5272099" y="819149"/>
+          <a:ext cx="1332649" cy="56323"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2129,13 +2241,185 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38102</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Rectangle 17"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7372351" y="962027"/>
+          <a:ext cx="1181100" cy="47624"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0C0C0" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="22"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19052</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>590551</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Rectangle 18"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8610601" y="1143002"/>
+          <a:ext cx="1181100" cy="47624"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0C0C0" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="22"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>544340</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19052</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>8113</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Rectangle 19"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10355090" y="1304927"/>
+          <a:ext cx="1902173" cy="47624"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0C0C0" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="22"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>23185</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>62544</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Rectangle 20"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12296776" y="1499560"/>
+          <a:ext cx="1181100" cy="39359"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0C0C0" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="22"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2173,9 +2457,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2210,7 +2494,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2245,7 +2529,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2421,8 +2705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -2443,11 +2727,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
       <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
@@ -2456,7 +2740,7 @@
       </c>
       <c r="F1" s="10">
         <f ca="1">TODAY()</f>
-        <v>42719</v>
+        <v>42723</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>11</v>
@@ -2464,10 +2748,10 @@
     </row>
     <row r="2" spans="1:12" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="63" t="s">
         <v>115</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -2496,10 +2780,10 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="71" t="s">
         <v>114</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -2518,8 +2802,8 @@
         <f t="shared" ref="G4:G12" si="0">DAYS360(E4,F4)</f>
         <v>134</v>
       </c>
-      <c r="H4" s="102"/>
-      <c r="J4" s="78">
+      <c r="H4" s="99"/>
+      <c r="J4" s="75">
         <f>AVERAGE(G13,G34)</f>
         <v>169.75277777777777</v>
       </c>
@@ -2532,10 +2816,10 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="71" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="71" t="s">
         <v>130</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2554,15 +2838,15 @@
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
-      <c r="J5" s="89"/>
-      <c r="K5" s="90"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="87"/>
       <c r="L5" s="18"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="74" t="s">
+      <c r="A6" s="71" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="71" t="s">
         <v>130</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2581,15 +2865,15 @@
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
-      <c r="J6" s="89"/>
-      <c r="K6" s="90"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="87"/>
       <c r="L6" s="18"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="71" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="71" t="s">
         <v>130</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2608,15 +2892,15 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="J7" s="89"/>
-      <c r="K7" s="90"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="87"/>
       <c r="L7" s="18"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="71" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="71" t="s">
         <v>130</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -2635,15 +2919,15 @@
         <f t="shared" si="0"/>
         <v>218</v>
       </c>
-      <c r="J8" s="89"/>
-      <c r="K8" s="90"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="87"/>
       <c r="L8" s="18"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="74" t="s">
+      <c r="A9" s="71" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="71" t="s">
         <v>130</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2662,13 +2946,13 @@
         <f t="shared" si="0"/>
         <v>222</v>
       </c>
-      <c r="K9" s="84"/>
+      <c r="K9" s="81"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="74" t="s">
+      <c r="A10" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="71" t="s">
         <v>130</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -2689,10 +2973,10 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="71" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="71" t="s">
         <v>114</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2713,10 +2997,10 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="74" t="s">
+      <c r="A12" s="71" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="71" t="s">
         <v>114</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2737,24 +3021,24 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="100"/>
-      <c r="B13" s="101"/>
-      <c r="C13" s="107" t="s">
+      <c r="A13" s="97"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="113" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="107"/>
-      <c r="E13" s="107"/>
-      <c r="F13" s="108"/>
-      <c r="G13" s="73">
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="114"/>
+      <c r="G13" s="70">
         <f>AVERAGE(G4:G12)</f>
         <v>164.55555555555554</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="74" t="s">
+      <c r="B14" s="71" t="s">
         <v>114</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2776,10 +3060,10 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="B15" s="74" t="s">
+      <c r="B15" s="71" t="s">
         <v>114</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2800,10 +3084,10 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="74" t="s">
+      <c r="A16" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="B16" s="74" t="s">
+      <c r="B16" s="71" t="s">
         <v>114</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -2824,10 +3108,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="74" t="s">
+      <c r="A17" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="71" t="s">
         <v>114</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2848,10 +3132,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="74" t="s">
+      <c r="A18" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="71" t="s">
         <v>114</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -2872,10 +3156,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="74" t="s">
+      <c r="A19" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="71" t="s">
         <v>114</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -2896,10 +3180,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="74" t="s">
+      <c r="A20" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="74" t="s">
+      <c r="B20" s="71" t="s">
         <v>116</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2920,10 +3204,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="74" t="s">
+      <c r="A21" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="74" t="s">
+      <c r="B21" s="71" t="s">
         <v>114</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -2944,13 +3228,13 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="74" t="s">
+      <c r="A22" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="B22" s="74" t="s">
+      <c r="B22" s="71" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="69" t="s">
         <v>77</v>
       </c>
       <c r="D22" s="11" t="s">
@@ -2968,250 +3252,250 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="71" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="71" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="98" t="s">
+      <c r="C23" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="94" t="s">
+      <c r="D23" s="91" t="s">
         <v>139</v>
       </c>
-      <c r="E23" s="96">
+      <c r="E23" s="93">
         <v>42580</v>
       </c>
-      <c r="F23" s="96">
+      <c r="F23" s="93">
         <v>42641</v>
       </c>
-      <c r="G23" s="97">
+      <c r="G23" s="94">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="74" t="s">
+      <c r="A24" s="71" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="74" t="s">
+      <c r="B24" s="71" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="94" t="s">
+      <c r="C24" s="91" t="s">
         <v>142</v>
       </c>
-      <c r="D24" s="95" t="s">
+      <c r="D24" s="92" t="s">
         <v>141</v>
       </c>
-      <c r="E24" s="96">
+      <c r="E24" s="93">
         <v>42612</v>
       </c>
-      <c r="F24" s="96">
+      <c r="F24" s="93">
         <v>42704</v>
       </c>
-      <c r="G24" s="97">
+      <c r="G24" s="94">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="74" t="s">
+      <c r="A25" s="71" t="s">
         <v>143</v>
       </c>
-      <c r="B25" s="74" t="s">
+      <c r="B25" s="71" t="s">
         <v>144</v>
       </c>
-      <c r="C25" s="94" t="s">
+      <c r="C25" s="91" t="s">
         <v>145</v>
       </c>
-      <c r="D25" s="95" t="s">
+      <c r="D25" s="92" t="s">
         <v>146</v>
       </c>
-      <c r="E25" s="96">
+      <c r="E25" s="93">
         <v>42068</v>
       </c>
-      <c r="F25" s="96">
+      <c r="F25" s="93">
         <v>42149</v>
       </c>
-      <c r="G25" s="97">
+      <c r="G25" s="94">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="71" t="s">
         <v>147</v>
       </c>
-      <c r="B26" s="74" t="s">
+      <c r="B26" s="71" t="s">
         <v>144</v>
       </c>
-      <c r="C26" s="94" t="s">
+      <c r="C26" s="91" t="s">
         <v>148</v>
       </c>
-      <c r="D26" s="95" t="s">
+      <c r="D26" s="92" t="s">
         <v>149</v>
       </c>
-      <c r="E26" s="96">
+      <c r="E26" s="93">
         <v>42410</v>
       </c>
-      <c r="F26" s="96">
+      <c r="F26" s="93">
         <v>42690</v>
       </c>
-      <c r="G26" s="97">
+      <c r="G26" s="94">
         <f t="shared" si="1"/>
         <v>276</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="74" t="s">
+      <c r="A27" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="B27" s="74" t="s">
+      <c r="B27" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="C27" s="94" t="s">
+      <c r="C27" s="91" t="s">
         <v>151</v>
       </c>
-      <c r="D27" s="95" t="s">
+      <c r="D27" s="92" t="s">
         <v>152</v>
       </c>
-      <c r="E27" s="96">
+      <c r="E27" s="93">
         <v>41208</v>
       </c>
-      <c r="F27" s="96">
+      <c r="F27" s="93">
         <v>41348</v>
       </c>
-      <c r="G27" s="97">
+      <c r="G27" s="94">
         <f t="shared" si="1"/>
         <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="74" t="s">
+      <c r="A28" s="71" t="s">
         <v>155</v>
       </c>
-      <c r="B28" s="74" t="s">
+      <c r="B28" s="71" t="s">
         <v>144</v>
       </c>
-      <c r="C28" s="94" t="s">
+      <c r="C28" s="91" t="s">
         <v>153</v>
       </c>
-      <c r="D28" s="95" t="s">
+      <c r="D28" s="92" t="s">
         <v>154</v>
       </c>
-      <c r="E28" s="96">
+      <c r="E28" s="93">
         <v>40927</v>
       </c>
-      <c r="F28" s="96">
+      <c r="F28" s="93">
         <v>41012</v>
       </c>
-      <c r="G28" s="97">
+      <c r="G28" s="94">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="103" t="s">
+      <c r="A29" s="100" t="s">
         <v>156</v>
       </c>
-      <c r="B29" s="74" t="s">
+      <c r="B29" s="71" t="s">
         <v>144</v>
       </c>
-      <c r="C29" s="94" t="s">
+      <c r="C29" s="91" t="s">
         <v>145</v>
       </c>
-      <c r="D29" s="95" t="s">
+      <c r="D29" s="92" t="s">
         <v>157</v>
       </c>
-      <c r="E29" s="96">
+      <c r="E29" s="93">
         <v>41885</v>
       </c>
-      <c r="F29" s="96">
+      <c r="F29" s="93">
         <v>41996</v>
       </c>
-      <c r="G29" s="97">
+      <c r="G29" s="94">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="74" t="s">
+      <c r="A30" s="71" t="s">
         <v>158</v>
       </c>
-      <c r="B30" s="74" t="s">
+      <c r="B30" s="71" t="s">
         <v>144</v>
       </c>
-      <c r="C30" s="95" t="s">
+      <c r="C30" s="92" t="s">
         <v>159</v>
       </c>
-      <c r="D30" s="104" t="s">
+      <c r="D30" s="101" t="s">
         <v>160</v>
       </c>
-      <c r="E30" s="96">
+      <c r="E30" s="93">
         <v>40945</v>
       </c>
-      <c r="F30" s="96">
+      <c r="F30" s="93">
         <v>41093</v>
       </c>
-      <c r="G30" s="97">
+      <c r="G30" s="94">
         <f t="shared" si="1"/>
         <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="71" t="s">
         <v>161</v>
       </c>
-      <c r="B31" s="74" t="s">
+      <c r="B31" s="71" t="s">
         <v>144</v>
       </c>
-      <c r="C31" s="94" t="s">
+      <c r="C31" s="91" t="s">
         <v>162</v>
       </c>
-      <c r="D31" s="95" t="s">
+      <c r="D31" s="92" t="s">
         <v>163</v>
       </c>
-      <c r="E31" s="96">
+      <c r="E31" s="93">
         <v>41411</v>
       </c>
-      <c r="F31" s="96">
+      <c r="F31" s="93">
         <v>41666</v>
       </c>
-      <c r="G31" s="97">
+      <c r="G31" s="94">
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="71" t="s">
         <v>164</v>
       </c>
-      <c r="B32" s="74" t="s">
+      <c r="B32" s="71" t="s">
         <v>144</v>
       </c>
-      <c r="C32" s="94" t="s">
+      <c r="C32" s="91" t="s">
         <v>165</v>
       </c>
-      <c r="D32" s="95" t="s">
+      <c r="D32" s="92" t="s">
         <v>166</v>
       </c>
-      <c r="E32" s="96">
+      <c r="E32" s="93">
         <v>41905</v>
       </c>
-      <c r="F32" s="96">
+      <c r="F32" s="93">
         <v>41999</v>
       </c>
-      <c r="G32" s="97">
+      <c r="G32" s="94">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="74" t="s">
+      <c r="A33" s="71" t="s">
         <v>107</v>
       </c>
-      <c r="B33" s="74" t="s">
+      <c r="B33" s="71" t="s">
         <v>114</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -3232,14 +3516,14 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="106" t="s">
+      <c r="A34" s="112" t="s">
         <v>110</v>
       </c>
-      <c r="B34" s="107"/>
-      <c r="C34" s="107"/>
-      <c r="D34" s="107"/>
-      <c r="E34" s="107"/>
-      <c r="F34" s="108"/>
+      <c r="B34" s="113"/>
+      <c r="C34" s="113"/>
+      <c r="D34" s="113"/>
+      <c r="E34" s="113"/>
+      <c r="F34" s="114"/>
       <c r="G34" s="17">
         <f>AVERAGE(G14:G33)</f>
         <v>174.95</v>
@@ -3468,7 +3752,7 @@
       <c r="B2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="79"/>
+      <c r="C2" s="76"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3500,7 +3784,7 @@
       <c r="A6" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="127">
+      <c r="B6" s="104">
         <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$33,A6,'Dados Historicos x Categoria'!$G$4:$G$33)</f>
         <v>148.57142857142858</v>
       </c>
@@ -3531,738 +3815,738 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="109" t="s">
+      <c r="C17" s="115" t="s">
         <v>111</v>
       </c>
-      <c r="D17" s="110"/>
-      <c r="E17" s="110"/>
-      <c r="F17" s="110"/>
-      <c r="G17" s="110"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="116"/>
+      <c r="F17" s="116"/>
+      <c r="G17" s="116"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="111"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="111"/>
-      <c r="F18" s="111"/>
-      <c r="G18" s="111"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="117"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="111"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="111"/>
-      <c r="G19" s="111"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
+      <c r="G19" s="117"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="111"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="111"/>
-      <c r="F20" s="111"/>
-      <c r="G20" s="111"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="117"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="117"/>
+      <c r="G20" s="117"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="111"/>
-      <c r="D21" s="111"/>
-      <c r="E21" s="111"/>
-      <c r="F21" s="111"/>
-      <c r="G21" s="111"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="117"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="117"/>
+      <c r="G21" s="117"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="111"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="111"/>
-      <c r="F22" s="111"/>
-      <c r="G22" s="111"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="117"/>
+      <c r="E22" s="117"/>
+      <c r="F22" s="117"/>
+      <c r="G22" s="117"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="111"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="111"/>
-      <c r="F23" s="111"/>
-      <c r="G23" s="111"/>
+      <c r="C23" s="117"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="117"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="111"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="111"/>
-      <c r="F24" s="111"/>
-      <c r="G24" s="111"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="117"/>
+      <c r="E24" s="117"/>
+      <c r="F24" s="117"/>
+      <c r="G24" s="117"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="111"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="111"/>
-      <c r="F25" s="111"/>
-      <c r="G25" s="111"/>
+      <c r="C25" s="117"/>
+      <c r="D25" s="117"/>
+      <c r="E25" s="117"/>
+      <c r="F25" s="117"/>
+      <c r="G25" s="117"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="111"/>
-      <c r="D26" s="111"/>
-      <c r="E26" s="111"/>
-      <c r="F26" s="111"/>
-      <c r="G26" s="111"/>
+      <c r="C26" s="117"/>
+      <c r="D26" s="117"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="117"/>
+      <c r="G26" s="117"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="111"/>
-      <c r="D27" s="111"/>
-      <c r="E27" s="111"/>
-      <c r="F27" s="111"/>
-      <c r="G27" s="111"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
+      <c r="G27" s="117"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="111"/>
-      <c r="D28" s="111"/>
-      <c r="E28" s="111"/>
-      <c r="F28" s="111"/>
-      <c r="G28" s="111"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="117"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
+      <c r="G28" s="117"/>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="111"/>
-      <c r="D29" s="111"/>
-      <c r="E29" s="111"/>
-      <c r="F29" s="111"/>
-      <c r="G29" s="111"/>
+      <c r="C29" s="117"/>
+      <c r="D29" s="117"/>
+      <c r="E29" s="117"/>
+      <c r="F29" s="117"/>
+      <c r="G29" s="117"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="111"/>
-      <c r="D30" s="111"/>
-      <c r="E30" s="111"/>
-      <c r="F30" s="111"/>
-      <c r="G30" s="111"/>
+      <c r="C30" s="117"/>
+      <c r="D30" s="117"/>
+      <c r="E30" s="117"/>
+      <c r="F30" s="117"/>
+      <c r="G30" s="117"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="131" t="s">
+      <c r="A47" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="132" t="s">
+      <c r="B47" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="132" t="s">
+      <c r="C47" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="133" t="s">
+      <c r="D47" s="110" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="128" t="s">
+      <c r="A48" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="129">
+      <c r="B48" s="106">
         <v>42311</v>
       </c>
-      <c r="C48" s="129">
+      <c r="C48" s="106">
         <v>42446</v>
       </c>
-      <c r="D48" s="130">
+      <c r="D48" s="107">
         <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="128" t="s">
+      <c r="A49" s="105" t="s">
         <v>131</v>
       </c>
-      <c r="B49" s="129">
+      <c r="B49" s="106">
         <v>42118</v>
       </c>
-      <c r="C49" s="129">
+      <c r="C49" s="106">
         <v>42221</v>
       </c>
-      <c r="D49" s="130">
+      <c r="D49" s="107">
         <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="128" t="s">
+      <c r="A50" s="105" t="s">
         <v>131</v>
       </c>
-      <c r="B50" s="129">
+      <c r="B50" s="106">
         <v>42263</v>
       </c>
-      <c r="C50" s="129">
+      <c r="C50" s="106">
         <v>42342</v>
       </c>
-      <c r="D50" s="130">
+      <c r="D50" s="107">
         <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="128" t="s">
+      <c r="A51" s="105" t="s">
         <v>131</v>
       </c>
-      <c r="B51" s="129">
+      <c r="B51" s="106">
         <v>42633</v>
       </c>
-      <c r="C51" s="129">
+      <c r="C51" s="106">
         <v>42695</v>
       </c>
-      <c r="D51" s="130">
+      <c r="D51" s="107">
         <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="128" t="s">
+      <c r="A52" s="105" t="s">
         <v>131</v>
       </c>
-      <c r="B52" s="129">
+      <c r="B52" s="106">
         <v>42422</v>
       </c>
-      <c r="C52" s="129">
+      <c r="C52" s="106">
         <v>42643</v>
       </c>
-      <c r="D52" s="130">
+      <c r="D52" s="107">
         <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="128" t="s">
+      <c r="A53" s="105" t="s">
         <v>131</v>
       </c>
-      <c r="B53" s="129">
+      <c r="B53" s="106">
         <v>41955</v>
       </c>
-      <c r="C53" s="129">
+      <c r="C53" s="106">
         <v>42179</v>
       </c>
-      <c r="D53" s="130">
+      <c r="D53" s="107">
         <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="128" t="s">
+      <c r="A54" s="105" t="s">
         <v>131</v>
       </c>
-      <c r="B54" s="129">
+      <c r="B54" s="106">
         <v>41738</v>
       </c>
-      <c r="C54" s="129">
+      <c r="C54" s="106">
         <v>41850</v>
       </c>
-      <c r="D54" s="130">
+      <c r="D54" s="107">
         <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="128" t="s">
+      <c r="A55" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="B55" s="129">
+      <c r="B55" s="106">
         <v>41337</v>
       </c>
-      <c r="C55" s="129">
+      <c r="C55" s="106">
         <v>41430</v>
       </c>
-      <c r="D55" s="130">
+      <c r="D55" s="107">
         <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="128" t="s">
+      <c r="A56" s="105" t="s">
         <v>84</v>
       </c>
-      <c r="B56" s="129">
+      <c r="B56" s="106">
         <v>42209</v>
       </c>
-      <c r="C56" s="129">
+      <c r="C56" s="106">
         <v>42683</v>
       </c>
-      <c r="D56" s="130">
+      <c r="D56" s="107">
         <v>465</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="128" t="s">
+      <c r="A57" s="105" t="s">
         <v>87</v>
       </c>
-      <c r="B57" s="129">
+      <c r="B57" s="106">
         <v>42020</v>
       </c>
-      <c r="C57" s="129">
+      <c r="C57" s="106">
         <v>42671</v>
       </c>
-      <c r="D57" s="130">
+      <c r="D57" s="107">
         <v>642</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="128" t="s">
+      <c r="A58" s="105" t="s">
         <v>87</v>
       </c>
-      <c r="B58" s="129">
+      <c r="B58" s="106">
         <v>42439</v>
       </c>
-      <c r="C58" s="129">
+      <c r="C58" s="106">
         <v>42668</v>
       </c>
-      <c r="D58" s="130">
+      <c r="D58" s="107">
         <v>225</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="128" t="s">
+      <c r="A59" s="105" t="s">
         <v>92</v>
       </c>
-      <c r="B59" s="129">
+      <c r="B59" s="106">
         <v>42521</v>
       </c>
-      <c r="C59" s="129">
+      <c r="C59" s="106">
         <v>42661</v>
       </c>
-      <c r="D59" s="130">
+      <c r="D59" s="107">
         <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="128" t="s">
+      <c r="A60" s="105" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="129">
+      <c r="B60" s="106">
         <v>41242</v>
       </c>
-      <c r="C60" s="129">
+      <c r="C60" s="106">
         <v>41472</v>
       </c>
-      <c r="D60" s="130">
+      <c r="D60" s="107">
         <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="128" t="s">
+      <c r="A61" s="105" t="s">
         <v>84</v>
       </c>
-      <c r="B61" s="129">
+      <c r="B61" s="106">
         <v>41698</v>
       </c>
-      <c r="C61" s="129">
+      <c r="C61" s="106">
         <v>41932</v>
       </c>
-      <c r="D61" s="130">
+      <c r="D61" s="107">
         <v>230</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="128" t="s">
+      <c r="A62" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="B62" s="129">
+      <c r="B62" s="106">
         <v>42277</v>
       </c>
-      <c r="C62" s="129">
+      <c r="C62" s="106">
         <v>42681</v>
       </c>
-      <c r="D62" s="130">
+      <c r="D62" s="107">
         <v>397</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="128" t="s">
+      <c r="A63" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="B63" s="129">
+      <c r="B63" s="106">
         <v>42136</v>
       </c>
-      <c r="C63" s="129">
+      <c r="C63" s="106">
         <v>42171</v>
       </c>
-      <c r="D63" s="130">
+      <c r="D63" s="107">
         <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="128" t="s">
+      <c r="A64" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="B64" s="129">
+      <c r="B64" s="106">
         <v>41541</v>
       </c>
-      <c r="C64" s="129">
+      <c r="C64" s="106">
         <v>41634</v>
       </c>
-      <c r="D64" s="130">
+      <c r="D64" s="107">
         <v>92</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="128" t="s">
+      <c r="A65" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="B65" s="129">
+      <c r="B65" s="106">
         <v>41575</v>
       </c>
-      <c r="C65" s="129">
+      <c r="C65" s="106">
         <v>41638</v>
       </c>
-      <c r="D65" s="130">
+      <c r="D65" s="107">
         <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="128" t="s">
+      <c r="A66" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="B66" s="129">
+      <c r="B66" s="106">
         <v>42580</v>
       </c>
-      <c r="C66" s="129">
+      <c r="C66" s="106">
         <v>42641</v>
       </c>
-      <c r="D66" s="130">
+      <c r="D66" s="107">
         <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="128" t="s">
+      <c r="A67" s="105" t="s">
         <v>142</v>
       </c>
-      <c r="B67" s="129">
+      <c r="B67" s="106">
         <v>42612</v>
       </c>
-      <c r="C67" s="129">
+      <c r="C67" s="106">
         <v>42704</v>
       </c>
-      <c r="D67" s="130">
+      <c r="D67" s="107">
         <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="128" t="s">
+      <c r="A68" s="105" t="s">
         <v>145</v>
       </c>
-      <c r="B68" s="129">
+      <c r="B68" s="106">
         <v>42068</v>
       </c>
-      <c r="C68" s="129">
+      <c r="C68" s="106">
         <v>42149</v>
       </c>
-      <c r="D68" s="130">
+      <c r="D68" s="107">
         <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="128" t="s">
+      <c r="A69" s="105" t="s">
         <v>148</v>
       </c>
-      <c r="B69" s="129">
+      <c r="B69" s="106">
         <v>42410</v>
       </c>
-      <c r="C69" s="129">
+      <c r="C69" s="106">
         <v>42690</v>
       </c>
-      <c r="D69" s="130">
+      <c r="D69" s="107">
         <v>276</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="128" t="s">
+      <c r="A70" s="105" t="s">
         <v>151</v>
       </c>
-      <c r="B70" s="129">
+      <c r="B70" s="106">
         <v>41208</v>
       </c>
-      <c r="C70" s="129">
+      <c r="C70" s="106">
         <v>41348</v>
       </c>
-      <c r="D70" s="130">
+      <c r="D70" s="107">
         <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="128" t="s">
+      <c r="A71" s="105" t="s">
         <v>153</v>
       </c>
-      <c r="B71" s="129">
+      <c r="B71" s="106">
         <v>40927</v>
       </c>
-      <c r="C71" s="129">
+      <c r="C71" s="106">
         <v>41012</v>
       </c>
-      <c r="D71" s="130">
+      <c r="D71" s="107">
         <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="128" t="s">
+      <c r="A72" s="105" t="s">
         <v>145</v>
       </c>
-      <c r="B72" s="129">
+      <c r="B72" s="106">
         <v>41885</v>
       </c>
-      <c r="C72" s="129">
+      <c r="C72" s="106">
         <v>41996</v>
       </c>
-      <c r="D72" s="130">
+      <c r="D72" s="107">
         <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="128" t="s">
+      <c r="A73" s="105" t="s">
         <v>167</v>
       </c>
-      <c r="B73" s="129">
+      <c r="B73" s="106">
         <v>40945</v>
       </c>
-      <c r="C73" s="129">
+      <c r="C73" s="106">
         <v>41093</v>
       </c>
-      <c r="D73" s="130">
+      <c r="D73" s="107">
         <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="128" t="s">
+      <c r="A74" s="105" t="s">
         <v>162</v>
       </c>
-      <c r="B74" s="129">
+      <c r="B74" s="106">
         <v>41411</v>
       </c>
-      <c r="C74" s="129">
+      <c r="C74" s="106">
         <v>41666</v>
       </c>
-      <c r="D74" s="130">
+      <c r="D74" s="107">
         <v>250</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="128" t="s">
+      <c r="A75" s="105" t="s">
         <v>165</v>
       </c>
-      <c r="B75" s="129">
+      <c r="B75" s="106">
         <v>41905</v>
       </c>
-      <c r="C75" s="129">
+      <c r="C75" s="106">
         <v>41999</v>
       </c>
-      <c r="D75" s="130">
+      <c r="D75" s="107">
         <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="128" t="s">
+      <c r="A76" s="105" t="s">
         <v>108</v>
       </c>
-      <c r="B76" s="129">
+      <c r="B76" s="106">
         <v>42229</v>
       </c>
-      <c r="C76" s="129">
+      <c r="C76" s="106">
         <v>42354</v>
       </c>
-      <c r="D76" s="130">
+      <c r="D76" s="107">
         <v>123</v>
       </c>
     </row>
     <row r="84" spans="10:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="62"/>
+      <c r="J84" s="59"/>
     </row>
     <row r="85" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J85" s="62"/>
+      <c r="J85" s="59"/>
     </row>
     <row r="86" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J86" s="62"/>
+      <c r="J86" s="59"/>
     </row>
     <row r="87" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J87" s="62"/>
+      <c r="J87" s="59"/>
     </row>
     <row r="88" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J88" s="62"/>
+      <c r="J88" s="59"/>
     </row>
     <row r="89" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J89" s="62"/>
+      <c r="J89" s="59"/>
     </row>
     <row r="90" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J90" s="62"/>
+      <c r="J90" s="59"/>
     </row>
     <row r="91" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J91" s="62"/>
+      <c r="J91" s="59"/>
     </row>
     <row r="92" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J92" s="62"/>
+      <c r="J92" s="59"/>
     </row>
     <row r="93" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J93" s="62"/>
+      <c r="J93" s="59"/>
     </row>
     <row r="94" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J94" s="62"/>
+      <c r="J94" s="59"/>
     </row>
     <row r="95" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J95" s="62"/>
+      <c r="J95" s="59"/>
     </row>
     <row r="96" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J96" s="62"/>
+      <c r="J96" s="59"/>
     </row>
     <row r="109" spans="6:10" ht="315" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="110" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F110" s="61"/>
-      <c r="G110" s="62"/>
-      <c r="H110" s="62"/>
-      <c r="I110" s="62"/>
+      <c r="F110" s="58"/>
+      <c r="G110" s="59"/>
+      <c r="H110" s="59"/>
+      <c r="I110" s="59"/>
     </row>
     <row r="111" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F111" s="62"/>
-      <c r="G111" s="62"/>
-      <c r="H111" s="62"/>
-      <c r="I111" s="62"/>
+      <c r="F111" s="59"/>
+      <c r="G111" s="59"/>
+      <c r="H111" s="59"/>
+      <c r="I111" s="59"/>
       <c r="J111" s="18"/>
     </row>
     <row r="112" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F112" s="62"/>
-      <c r="G112" s="62"/>
-      <c r="H112" s="62"/>
-      <c r="I112" s="62"/>
+      <c r="F112" s="59"/>
+      <c r="G112" s="59"/>
+      <c r="H112" s="59"/>
+      <c r="I112" s="59"/>
       <c r="J112" s="18"/>
     </row>
     <row r="113" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F113" s="62"/>
-      <c r="G113" s="62"/>
-      <c r="H113" s="62"/>
-      <c r="I113" s="62"/>
+      <c r="F113" s="59"/>
+      <c r="G113" s="59"/>
+      <c r="H113" s="59"/>
+      <c r="I113" s="59"/>
       <c r="J113" s="18"/>
     </row>
     <row r="114" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F114" s="62"/>
-      <c r="G114" s="62"/>
-      <c r="H114" s="62"/>
-      <c r="I114" s="62"/>
+      <c r="F114" s="59"/>
+      <c r="G114" s="59"/>
+      <c r="H114" s="59"/>
+      <c r="I114" s="59"/>
       <c r="J114" s="18"/>
     </row>
     <row r="115" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F115" s="62"/>
-      <c r="G115" s="62"/>
-      <c r="H115" s="62"/>
-      <c r="I115" s="62"/>
+      <c r="F115" s="59"/>
+      <c r="G115" s="59"/>
+      <c r="H115" s="59"/>
+      <c r="I115" s="59"/>
       <c r="J115" s="18"/>
     </row>
     <row r="116" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F116" s="62"/>
-      <c r="G116" s="62"/>
-      <c r="H116" s="62"/>
-      <c r="I116" s="62"/>
+      <c r="F116" s="59"/>
+      <c r="G116" s="59"/>
+      <c r="H116" s="59"/>
+      <c r="I116" s="59"/>
       <c r="J116" s="18"/>
     </row>
     <row r="117" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F117" s="62"/>
-      <c r="G117" s="62"/>
-      <c r="H117" s="62"/>
-      <c r="I117" s="62"/>
+      <c r="F117" s="59"/>
+      <c r="G117" s="59"/>
+      <c r="H117" s="59"/>
+      <c r="I117" s="59"/>
       <c r="J117" s="18"/>
     </row>
     <row r="118" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F118" s="62"/>
-      <c r="G118" s="62"/>
-      <c r="H118" s="62"/>
-      <c r="I118" s="62"/>
+      <c r="F118" s="59"/>
+      <c r="G118" s="59"/>
+      <c r="H118" s="59"/>
+      <c r="I118" s="59"/>
       <c r="J118" s="18"/>
     </row>
     <row r="119" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F119" s="62"/>
-      <c r="G119" s="62"/>
-      <c r="H119" s="62"/>
-      <c r="I119" s="62"/>
+      <c r="F119" s="59"/>
+      <c r="G119" s="59"/>
+      <c r="H119" s="59"/>
+      <c r="I119" s="59"/>
       <c r="J119" s="18"/>
     </row>
     <row r="120" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F120" s="62"/>
-      <c r="G120" s="62"/>
-      <c r="H120" s="62"/>
-      <c r="I120" s="62"/>
+      <c r="F120" s="59"/>
+      <c r="G120" s="59"/>
+      <c r="H120" s="59"/>
+      <c r="I120" s="59"/>
       <c r="J120" s="18"/>
     </row>
     <row r="121" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F121" s="62"/>
-      <c r="G121" s="62"/>
-      <c r="H121" s="62"/>
-      <c r="I121" s="62"/>
+      <c r="F121" s="59"/>
+      <c r="G121" s="59"/>
+      <c r="H121" s="59"/>
+      <c r="I121" s="59"/>
       <c r="J121" s="18"/>
     </row>
     <row r="136" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E136" s="63"/>
-      <c r="F136" s="63"/>
-      <c r="G136" s="63"/>
-      <c r="H136" s="63"/>
-      <c r="I136" s="63"/>
+      <c r="E136" s="60"/>
+      <c r="F136" s="60"/>
+      <c r="G136" s="60"/>
+      <c r="H136" s="60"/>
+      <c r="I136" s="60"/>
     </row>
     <row r="137" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E137" s="63"/>
-      <c r="F137" s="63"/>
-      <c r="G137" s="63"/>
-      <c r="H137" s="63"/>
-      <c r="I137" s="63"/>
+      <c r="E137" s="60"/>
+      <c r="F137" s="60"/>
+      <c r="G137" s="60"/>
+      <c r="H137" s="60"/>
+      <c r="I137" s="60"/>
     </row>
     <row r="138" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E138" s="63"/>
-      <c r="F138" s="63"/>
-      <c r="G138" s="63"/>
-      <c r="H138" s="63"/>
-      <c r="I138" s="63"/>
+      <c r="E138" s="60"/>
+      <c r="F138" s="60"/>
+      <c r="G138" s="60"/>
+      <c r="H138" s="60"/>
+      <c r="I138" s="60"/>
     </row>
     <row r="139" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E139" s="63"/>
-      <c r="F139" s="63"/>
-      <c r="G139" s="63"/>
-      <c r="H139" s="63"/>
-      <c r="I139" s="63"/>
+      <c r="E139" s="60"/>
+      <c r="F139" s="60"/>
+      <c r="G139" s="60"/>
+      <c r="H139" s="60"/>
+      <c r="I139" s="60"/>
     </row>
     <row r="140" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E140" s="63"/>
-      <c r="F140" s="63"/>
-      <c r="G140" s="63"/>
-      <c r="H140" s="63"/>
-      <c r="I140" s="63"/>
+      <c r="E140" s="60"/>
+      <c r="F140" s="60"/>
+      <c r="G140" s="60"/>
+      <c r="H140" s="60"/>
+      <c r="I140" s="60"/>
     </row>
     <row r="141" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E141" s="63"/>
-      <c r="F141" s="63"/>
-      <c r="G141" s="63"/>
-      <c r="H141" s="63"/>
-      <c r="I141" s="63"/>
+      <c r="E141" s="60"/>
+      <c r="F141" s="60"/>
+      <c r="G141" s="60"/>
+      <c r="H141" s="60"/>
+      <c r="I141" s="60"/>
     </row>
     <row r="142" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E142" s="63"/>
-      <c r="F142" s="63"/>
-      <c r="G142" s="63"/>
-      <c r="H142" s="63"/>
-      <c r="I142" s="63"/>
+      <c r="E142" s="60"/>
+      <c r="F142" s="60"/>
+      <c r="G142" s="60"/>
+      <c r="H142" s="60"/>
+      <c r="I142" s="60"/>
     </row>
     <row r="143" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E143" s="63"/>
-      <c r="F143" s="63"/>
-      <c r="G143" s="63"/>
-      <c r="H143" s="63"/>
-      <c r="I143" s="63"/>
+      <c r="E143" s="60"/>
+      <c r="F143" s="60"/>
+      <c r="G143" s="60"/>
+      <c r="H143" s="60"/>
+      <c r="I143" s="60"/>
     </row>
     <row r="144" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E144" s="63"/>
-      <c r="F144" s="63"/>
-      <c r="G144" s="63"/>
-      <c r="H144" s="63"/>
-      <c r="I144" s="63"/>
+      <c r="E144" s="60"/>
+      <c r="F144" s="60"/>
+      <c r="G144" s="60"/>
+      <c r="H144" s="60"/>
+      <c r="I144" s="60"/>
     </row>
     <row r="145" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E145" s="63"/>
-      <c r="F145" s="63"/>
-      <c r="G145" s="63"/>
-      <c r="H145" s="63"/>
-      <c r="I145" s="63"/>
+      <c r="E145" s="60"/>
+      <c r="F145" s="60"/>
+      <c r="G145" s="60"/>
+      <c r="H145" s="60"/>
+      <c r="I145" s="60"/>
     </row>
     <row r="146" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E146" s="63"/>
-      <c r="F146" s="63"/>
-      <c r="G146" s="63"/>
-      <c r="H146" s="63"/>
-      <c r="I146" s="63"/>
+      <c r="E146" s="60"/>
+      <c r="F146" s="60"/>
+      <c r="G146" s="60"/>
+      <c r="H146" s="60"/>
+      <c r="I146" s="60"/>
     </row>
     <row r="147" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E147" s="63"/>
-      <c r="F147" s="63"/>
-      <c r="G147" s="63"/>
-      <c r="H147" s="63"/>
-      <c r="I147" s="63"/>
+      <c r="E147" s="60"/>
+      <c r="F147" s="60"/>
+      <c r="G147" s="60"/>
+      <c r="H147" s="60"/>
+      <c r="I147" s="60"/>
     </row>
     <row r="148" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E148" s="63"/>
-      <c r="F148" s="63"/>
-      <c r="G148" s="63"/>
-      <c r="H148" s="63"/>
-      <c r="I148" s="63"/>
+      <c r="E148" s="60"/>
+      <c r="F148" s="60"/>
+      <c r="G148" s="60"/>
+      <c r="H148" s="60"/>
+      <c r="I148" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4284,16 +4568,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="58"/>
-    <col min="2" max="2" width="15.5703125" style="58" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="58" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="58" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="58"/>
-    <col min="6" max="6" width="29.42578125" style="58" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="58" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="58" customWidth="1"/>
-    <col min="9" max="9" width="12" style="58" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" style="58" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="55"/>
+    <col min="2" max="2" width="15.5703125" style="55" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="55" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="55" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="55"/>
+    <col min="6" max="6" width="29.42578125" style="55" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" style="55" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="55" customWidth="1"/>
+    <col min="9" max="9" width="12" style="55" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" style="55" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -4328,422 +4612,422 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="56" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="113">
+    <row r="2" spans="1:10" s="53" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="118">
         <v>1</v>
       </c>
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="112" t="s">
+      <c r="C2" s="124" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="124" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="112">
+      <c r="E2" s="124">
         <v>2</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="59">
+      <c r="H2" s="56">
         <v>42440</v>
       </c>
-      <c r="I2" s="70" t="s">
+      <c r="I2" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="40"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="114"/>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="40" t="s">
+      <c r="A3" s="119"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="59">
+      <c r="H3" s="56">
         <v>42440</v>
       </c>
-      <c r="I3" s="70" t="s">
+      <c r="I3" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="40"/>
+      <c r="J3" s="39"/>
     </row>
     <row r="4" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="112">
+      <c r="A4" s="124">
         <v>2</v>
       </c>
-      <c r="B4" s="117">
+      <c r="B4" s="125">
         <v>42440</v>
       </c>
-      <c r="C4" s="112" t="s">
+      <c r="C4" s="124" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="112" t="s">
+      <c r="D4" s="124" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="113">
+      <c r="E4" s="118">
         <v>2</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="59">
+      <c r="H4" s="56">
         <v>42440</v>
       </c>
-      <c r="I4" s="70" t="s">
+      <c r="I4" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="J4" s="40"/>
+      <c r="J4" s="39"/>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="113"/>
-      <c r="B5" s="113"/>
-      <c r="C5" s="113"/>
-      <c r="D5" s="113"/>
-      <c r="E5" s="114"/>
-      <c r="F5" s="47" t="s">
+      <c r="A5" s="118"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="47" t="s">
+      <c r="G5" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="60">
+      <c r="H5" s="57">
         <v>42440</v>
       </c>
-      <c r="I5" s="70" t="s">
+      <c r="I5" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="J5" s="47"/>
+      <c r="J5" s="45"/>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="112">
+      <c r="A6" s="124">
         <v>3</v>
       </c>
-      <c r="B6" s="116">
+      <c r="B6" s="121">
         <v>42683</v>
       </c>
-      <c r="C6" s="113" t="s">
+      <c r="C6" s="118" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="113" t="s">
+      <c r="D6" s="118" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="113">
+      <c r="E6" s="118">
         <v>2</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="40" t="s">
+      <c r="G6" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="59">
+      <c r="H6" s="56">
         <v>42624</v>
       </c>
-      <c r="I6" s="70" t="s">
+      <c r="I6" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="J6" s="40"/>
+      <c r="J6" s="39"/>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="112"/>
-      <c r="B7" s="114"/>
-      <c r="C7" s="114"/>
-      <c r="D7" s="114"/>
-      <c r="E7" s="114"/>
-      <c r="F7" s="67" t="s">
+      <c r="A7" s="124"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="68" t="s">
+      <c r="G7" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="H7" s="59">
+      <c r="H7" s="56">
         <v>42624</v>
       </c>
-      <c r="I7" s="70" t="s">
+      <c r="I7" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="J7" s="40"/>
+      <c r="J7" s="39"/>
     </row>
     <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="112"/>
-      <c r="B8" s="114"/>
-      <c r="C8" s="114"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="64" t="s">
+      <c r="A8" s="124"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="119"/>
+      <c r="D8" s="119"/>
+      <c r="E8" s="119"/>
+      <c r="F8" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="64" t="s">
+      <c r="G8" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="69">
+      <c r="H8" s="66">
         <v>42691</v>
       </c>
-      <c r="I8" s="70" t="s">
+      <c r="I8" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="64"/>
+      <c r="J8" s="61"/>
     </row>
     <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="112"/>
-      <c r="B9" s="114"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="64" t="s">
+      <c r="A9" s="124"/>
+      <c r="B9" s="119"/>
+      <c r="C9" s="119"/>
+      <c r="D9" s="119"/>
+      <c r="E9" s="119"/>
+      <c r="F9" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="G9" s="64" t="s">
+      <c r="G9" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="69">
+      <c r="H9" s="66">
         <v>42691</v>
       </c>
-      <c r="I9" s="70" t="s">
+      <c r="I9" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="64"/>
+      <c r="J9" s="61"/>
     </row>
     <row r="10" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="112"/>
-      <c r="B10" s="115"/>
-      <c r="C10" s="115"/>
-      <c r="D10" s="115"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="40" t="s">
+      <c r="A10" s="124"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="120"/>
+      <c r="D10" s="120"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="40" t="s">
+      <c r="G10" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="59">
+      <c r="H10" s="56">
         <v>42624</v>
       </c>
-      <c r="I10" s="70" t="s">
+      <c r="I10" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="71" t="s">
+      <c r="J10" s="68" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="112">
+      <c r="A11" s="124">
         <v>4</v>
       </c>
-      <c r="B11" s="112" t="s">
+      <c r="B11" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="112" t="s">
+      <c r="C11" s="124" t="s">
         <v>117</v>
       </c>
-      <c r="D11" s="112" t="s">
+      <c r="D11" s="124" t="s">
         <v>118</v>
       </c>
-      <c r="E11" s="112">
+      <c r="E11" s="124">
         <v>2</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="64" t="s">
+      <c r="G11" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="64" t="s">
+      <c r="H11" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="I11" s="70" t="s">
+      <c r="I11" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="J11" s="64"/>
+      <c r="J11" s="61"/>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="112"/>
-      <c r="B12" s="112"/>
-      <c r="C12" s="112"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="112"/>
-      <c r="F12" s="67" t="s">
+      <c r="A12" s="124"/>
+      <c r="B12" s="124"/>
+      <c r="C12" s="124"/>
+      <c r="D12" s="124"/>
+      <c r="E12" s="124"/>
+      <c r="F12" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="G12" s="64" t="s">
+      <c r="G12" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="65">
+      <c r="H12" s="62">
         <v>42690</v>
       </c>
-      <c r="I12" s="70" t="s">
+      <c r="I12" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="64"/>
+      <c r="J12" s="61"/>
     </row>
     <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="113"/>
-      <c r="B13" s="113"/>
-      <c r="C13" s="113"/>
-      <c r="D13" s="113"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="85" t="s">
+      <c r="A13" s="118"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="118"/>
+      <c r="D13" s="118"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="82" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="80" t="s">
+      <c r="G13" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="H13" s="82">
+      <c r="H13" s="79">
         <v>42690</v>
       </c>
-      <c r="I13" s="88" t="s">
+      <c r="I13" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="J13" s="80"/>
+      <c r="J13" s="77"/>
     </row>
     <row r="14" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="113">
+      <c r="A14" s="118">
         <v>5</v>
       </c>
-      <c r="B14" s="116">
+      <c r="B14" s="121">
         <v>42705</v>
       </c>
-      <c r="C14" s="113"/>
-      <c r="D14" s="113" t="s">
+      <c r="C14" s="118"/>
+      <c r="D14" s="118" t="s">
         <v>118</v>
       </c>
-      <c r="E14" s="113">
+      <c r="E14" s="118">
         <v>2</v>
       </c>
-      <c r="F14" s="86" t="s">
+      <c r="F14" s="83" t="s">
         <v>121</v>
       </c>
-      <c r="G14" s="86" t="s">
+      <c r="G14" s="83" t="s">
         <v>122</v>
       </c>
-      <c r="H14" s="87">
+      <c r="H14" s="84">
         <v>42705</v>
       </c>
-      <c r="I14" s="91" t="s">
+      <c r="I14" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="J14" s="81"/>
+      <c r="J14" s="78"/>
     </row>
     <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A15" s="114"/>
-      <c r="B15" s="118"/>
-      <c r="C15" s="114"/>
-      <c r="D15" s="114"/>
-      <c r="E15" s="114"/>
-      <c r="F15" s="86" t="s">
+      <c r="A15" s="119"/>
+      <c r="B15" s="122"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="83" t="s">
         <v>123</v>
       </c>
-      <c r="G15" s="86" t="s">
+      <c r="G15" s="83" t="s">
         <v>124</v>
       </c>
-      <c r="H15" s="87">
+      <c r="H15" s="84">
         <v>42705</v>
       </c>
-      <c r="I15" s="92" t="s">
+      <c r="I15" s="89" t="s">
         <v>112</v>
       </c>
-      <c r="J15" s="81"/>
+      <c r="J15" s="78"/>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="114"/>
-      <c r="B16" s="118"/>
-      <c r="C16" s="114"/>
-      <c r="D16" s="115"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="86" t="s">
+      <c r="A16" s="119"/>
+      <c r="B16" s="122"/>
+      <c r="C16" s="119"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="119"/>
+      <c r="F16" s="83" t="s">
         <v>125</v>
       </c>
-      <c r="G16" s="86" t="s">
+      <c r="G16" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="H16" s="87">
+      <c r="H16" s="84">
         <v>42705</v>
       </c>
-      <c r="I16" s="91" t="s">
+      <c r="I16" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="J16" s="81"/>
+      <c r="J16" s="78"/>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="114"/>
-      <c r="B17" s="118"/>
-      <c r="C17" s="114"/>
-      <c r="D17" s="81" t="s">
+      <c r="A17" s="119"/>
+      <c r="B17" s="122"/>
+      <c r="C17" s="119"/>
+      <c r="D17" s="78" t="s">
         <v>119</v>
       </c>
-      <c r="E17" s="114"/>
-      <c r="F17" s="86" t="s">
+      <c r="E17" s="119"/>
+      <c r="F17" s="83" t="s">
         <v>126</v>
       </c>
-      <c r="G17" s="86" t="s">
+      <c r="G17" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="H17" s="87">
+      <c r="H17" s="84">
         <v>42705</v>
       </c>
-      <c r="I17" s="91" t="s">
+      <c r="I17" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="J17" s="81"/>
+      <c r="J17" s="78"/>
     </row>
     <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="114"/>
-      <c r="B18" s="118"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="113" t="s">
+      <c r="A18" s="119"/>
+      <c r="B18" s="122"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="E18" s="114"/>
-      <c r="F18" s="86" t="s">
+      <c r="E18" s="119"/>
+      <c r="F18" s="83" t="s">
         <v>128</v>
       </c>
-      <c r="G18" s="86" t="s">
+      <c r="G18" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="87">
+      <c r="H18" s="84">
         <v>42705</v>
       </c>
-      <c r="I18" s="93" t="s">
+      <c r="I18" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="J18" s="81"/>
+      <c r="J18" s="78"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="115"/>
-      <c r="B19" s="119"/>
-      <c r="C19" s="115"/>
-      <c r="D19" s="115"/>
-      <c r="E19" s="115"/>
+      <c r="A19" s="120"/>
+      <c r="B19" s="123"/>
+      <c r="C19" s="120"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="120"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="58">
+      <c r="A20" s="55">
         <v>6</v>
       </c>
-      <c r="B20" s="99">
+      <c r="B20" s="96">
         <v>42387</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="A6:A10"/>
@@ -4760,11 +5044,11 @@
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="E11:E13"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C14:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4797,10 +5081,10 @@
       <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="74"/>
+      <c r="B2" s="71"/>
       <c r="C2" s="1" t="s">
         <v>77</v>
       </c>
@@ -4845,7 +5129,7 @@
         <v>104</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="69" t="s">
         <v>77</v>
       </c>
       <c r="D4" s="11" t="s">
@@ -4863,56 +5147,56 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="80" t="s">
         <v>116</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="72" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="76">
+      <c r="E5" s="73">
         <v>41225</v>
       </c>
-      <c r="F5" s="76">
+      <c r="F5" s="73">
         <v>41263</v>
       </c>
-      <c r="G5" s="77">
+      <c r="G5" s="74">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="74" t="s">
+      <c r="A6" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="74"/>
-      <c r="C6" s="57" t="s">
+      <c r="B6" s="71"/>
+      <c r="C6" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="76">
+      <c r="E6" s="73">
         <v>42143</v>
       </c>
-      <c r="F6" s="76">
+      <c r="F6" s="73">
         <v>42156</v>
       </c>
-      <c r="G6" s="77">
+      <c r="G6" s="74">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="71" t="s">
         <v>114</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -4940,10 +5224,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4951,21 +5235,21 @@
     <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="122" t="s">
+      <c r="B1" s="128" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="124" t="s">
+      <c r="C1" s="130" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125" t="s">
+      <c r="D1" s="131"/>
+      <c r="E1" s="131" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="126"/>
+      <c r="F1" s="132"/>
       <c r="G1" s="23" t="s">
         <v>35</v>
       </c>
@@ -4981,10 +5265,12 @@
       <c r="Q1" s="24"/>
       <c r="R1" s="24"/>
       <c r="S1" s="24"/>
-    </row>
-    <row r="2" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="121"/>
-      <c r="B2" s="123"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+    </row>
+    <row r="2" spans="1:21" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="127"/>
+      <c r="B2" s="129"/>
       <c r="C2" s="25" t="s">
         <v>36</v>
       </c>
@@ -4997,47 +5283,53 @@
       <c r="F2" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="28">
-        <v>42690</v>
+      <c r="G2" s="28" t="s">
+        <v>169</v>
       </c>
       <c r="H2" s="28">
-        <v>42720</v>
-      </c>
-      <c r="I2" s="28">
-        <v>42751</v>
+        <v>42675</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>170</v>
       </c>
       <c r="J2" s="28">
-        <v>42782</v>
+        <v>42736</v>
       </c>
       <c r="K2" s="28">
-        <v>42810</v>
+        <v>42767</v>
       </c>
       <c r="L2" s="28">
-        <v>42841</v>
-      </c>
-      <c r="M2" s="28">
-        <v>42871</v>
-      </c>
-      <c r="N2" s="28">
-        <v>42902</v>
-      </c>
-      <c r="O2" s="28">
-        <v>42932</v>
+        <v>42795</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="O2" s="139">
+        <v>42887</v>
       </c>
       <c r="P2" s="28">
-        <v>42963</v>
-      </c>
-      <c r="Q2" s="28">
-        <v>42994</v>
-      </c>
-      <c r="R2" s="28">
-        <v>43024</v>
-      </c>
-      <c r="S2" s="28">
-        <v>43055</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42917</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="R2" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="T2" s="28">
+        <v>43040</v>
+      </c>
+      <c r="U2" s="139" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="29">
         <v>1</v>
       </c>
@@ -5064,305 +5356,366 @@
       <c r="L3" s="33"/>
       <c r="M3" s="33"/>
       <c r="N3" s="33"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34"/>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35">
+      <c r="O3" s="140"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="102"/>
+      <c r="R3" s="102"/>
+      <c r="S3" s="102"/>
+      <c r="T3" s="102"/>
+      <c r="U3" s="144"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="133">
         <v>2</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="134" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="135">
+        <v>42670</v>
+      </c>
+      <c r="D4" s="136">
+        <v>42794</v>
+      </c>
+      <c r="E4" s="136">
+        <v>42670</v>
+      </c>
+      <c r="F4" s="137">
+        <v>42794</v>
+      </c>
+      <c r="G4" s="133"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="103"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="103"/>
+      <c r="M4" s="103"/>
+      <c r="N4" s="103"/>
+      <c r="O4" s="141"/>
+      <c r="P4" s="102"/>
+      <c r="Q4" s="102"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="144"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="34">
+        <v>3</v>
+      </c>
+      <c r="B5" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
-      <c r="S4" s="34"/>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35">
-        <v>3</v>
-      </c>
-      <c r="B5" s="36" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="142"/>
+      <c r="P5" s="102"/>
+      <c r="Q5" s="102"/>
+      <c r="R5" s="102"/>
+      <c r="S5" s="102"/>
+      <c r="T5" s="102"/>
+      <c r="U5" s="144"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="34">
+        <v>4</v>
+      </c>
+      <c r="B6" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35">
-        <v>4</v>
-      </c>
-      <c r="B6" s="36" t="s">
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="142"/>
+      <c r="P6" s="102"/>
+      <c r="Q6" s="102"/>
+      <c r="R6" s="102"/>
+      <c r="S6" s="102"/>
+      <c r="T6" s="102"/>
+      <c r="U6" s="144"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="34">
+        <v>5</v>
+      </c>
+      <c r="B7" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="34"/>
-      <c r="S6" s="34"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35">
-        <v>5</v>
-      </c>
-      <c r="B7" s="36" t="s">
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="142"/>
+      <c r="P7" s="102"/>
+      <c r="Q7" s="102"/>
+      <c r="R7" s="102"/>
+      <c r="S7" s="102"/>
+      <c r="T7" s="102"/>
+      <c r="U7" s="144"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="34">
+        <v>6</v>
+      </c>
+      <c r="B8" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="41"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="34"/>
-      <c r="R7" s="34"/>
-      <c r="S7" s="34"/>
-    </row>
-    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35">
-        <v>6</v>
-      </c>
-      <c r="B8" s="36" t="s">
+      <c r="C8" s="36"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="142"/>
+      <c r="P8" s="102"/>
+      <c r="Q8" s="102"/>
+      <c r="R8" s="102"/>
+      <c r="S8" s="102"/>
+      <c r="T8" s="102"/>
+      <c r="U8" s="144"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="34">
+        <v>7</v>
+      </c>
+      <c r="B9" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34"/>
-      <c r="R8" s="34"/>
-      <c r="S8" s="34"/>
-    </row>
-    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35">
-        <v>7</v>
-      </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="41"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
-    </row>
-    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35">
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="142"/>
+      <c r="P9" s="102"/>
+      <c r="Q9" s="102"/>
+      <c r="R9" s="102"/>
+      <c r="S9" s="102"/>
+      <c r="T9" s="102"/>
+      <c r="U9" s="144"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="34">
         <v>8</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="34"/>
-    </row>
-    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="35">
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="142"/>
+      <c r="P10" s="102"/>
+      <c r="Q10" s="102"/>
+      <c r="R10" s="102"/>
+      <c r="S10" s="102"/>
+      <c r="T10" s="102"/>
+      <c r="U10" s="144"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="34">
         <v>9</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="40"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="34"/>
-    </row>
-    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="35">
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="142"/>
+      <c r="P11" s="102"/>
+      <c r="Q11" s="102"/>
+      <c r="R11" s="102"/>
+      <c r="S11" s="102"/>
+      <c r="T11" s="102"/>
+      <c r="U11" s="144"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="34">
         <v>10</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="40"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="34"/>
-      <c r="Q12" s="34"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="34"/>
-    </row>
-    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="35">
+      <c r="B12" s="35"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="142"/>
+      <c r="P12" s="102"/>
+      <c r="Q12" s="102"/>
+      <c r="R12" s="102"/>
+      <c r="S12" s="102"/>
+      <c r="T12" s="102"/>
+      <c r="U12" s="144"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="34">
         <v>11</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="40"/>
-      <c r="M13" s="40"/>
-      <c r="N13" s="40"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="34"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="34"/>
-    </row>
-    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="42">
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="142"/>
+      <c r="P13" s="102"/>
+      <c r="Q13" s="102"/>
+      <c r="R13" s="102"/>
+      <c r="S13" s="102"/>
+      <c r="T13" s="102"/>
+      <c r="U13" s="144"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="34">
         <v>12</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="34"/>
-      <c r="Q14" s="34"/>
-      <c r="R14" s="34"/>
-      <c r="S14" s="34"/>
-    </row>
-    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
-      <c r="B15" s="50" t="s">
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="142"/>
+      <c r="P14" s="102"/>
+      <c r="Q14" s="102"/>
+      <c r="R14" s="102"/>
+      <c r="S14" s="102"/>
+      <c r="T14" s="102"/>
+      <c r="U14" s="144"/>
+    </row>
+    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="34">
+        <v>13</v>
+      </c>
+      <c r="B15" s="41"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="143"/>
+      <c r="P15" s="102"/>
+      <c r="Q15" s="102"/>
+      <c r="R15" s="102"/>
+      <c r="S15" s="102"/>
+      <c r="T15" s="102"/>
+      <c r="U15" s="144"/>
+    </row>
+    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="46"/>
+      <c r="B16" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C16" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52" t="s">
+      <c r="D16" s="49"/>
+      <c r="E16" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="53"/>
-      <c r="G15" s="49">
+      <c r="F16" s="50"/>
+      <c r="G16" s="46">
         <v>30</v>
       </c>
-      <c r="H15" s="54">
+      <c r="H16" s="51">
         <v>30</v>
       </c>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="55"/>
-      <c r="P15" s="55"/>
-      <c r="Q15" s="55"/>
-      <c r="R15" s="55"/>
-      <c r="S15" s="55"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="51"/>
+      <c r="O16" s="52"/>
+      <c r="P16" s="138"/>
+      <c r="Q16" s="138"/>
+      <c r="R16" s="138"/>
+      <c r="S16" s="138"/>
+      <c r="T16" s="138"/>
+      <c r="U16" s="138"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Atualizado PAD com áreas selecionadas
</commit_message>
<xml_diff>
--- a/TRE_Dados_MapaRaciocinio.xlsx
+++ b/TRE_Dados_MapaRaciocinio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Historicos x Categoria" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Autor:
 </t>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="185">
   <si>
     <t>Categoria</t>
   </si>
@@ -601,6 +601,12 @@
   </si>
   <si>
     <t>Redefinição de escopo e médias</t>
+  </si>
+  <si>
+    <t>A3 - Contendo , objetivo do Projeto , histórico do projeto, lead time do processo inteiro(Pareto)</t>
+  </si>
+  <si>
+    <t>Ruhan, Ivis e Ruhan</t>
   </si>
 </sst>
 </file>
@@ -640,6 +646,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -679,7 +686,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1181,7 +1188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1406,9 +1413,6 @@
     <xf numFmtId="14" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1486,34 +1490,31 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1536,6 +1537,15 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1821,11 +1831,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="11733504"/>
-        <c:axId val="11155648"/>
+        <c:axId val="278735360"/>
+        <c:axId val="165007296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="11733504"/>
+        <c:axId val="278735360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1845,7 +1855,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11155648"/>
+        <c:crossAx val="165007296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1853,7 +1863,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11155648"/>
+        <c:axId val="165007296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1864,7 +1874,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="11733504"/>
+        <c:crossAx val="278735360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2738,8 +2748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2760,11 +2770,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
       <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
@@ -2773,7 +2783,7 @@
       </c>
       <c r="F1" s="10">
         <f ca="1">TODAY()</f>
-        <v>42771</v>
+        <v>42773</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>11</v>
@@ -2835,7 +2845,7 @@
         <f t="shared" ref="G4:G12" si="0">DAYS360(E4,F4)</f>
         <v>134</v>
       </c>
-      <c r="H4" s="99"/>
+      <c r="H4" s="98"/>
       <c r="J4" s="75">
         <f>AVERAGE(G13,G34)</f>
         <v>169.75277777777777</v>
@@ -3054,14 +3064,14 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="97"/>
-      <c r="B13" s="98"/>
-      <c r="C13" s="125" t="s">
+      <c r="A13" s="96"/>
+      <c r="B13" s="97"/>
+      <c r="C13" s="124" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="125"/>
-      <c r="E13" s="125"/>
-      <c r="F13" s="126"/>
+      <c r="D13" s="124"/>
+      <c r="E13" s="124"/>
+      <c r="F13" s="125"/>
       <c r="G13" s="70">
         <f>AVERAGE(G4:G12)</f>
         <v>164.55555555555554</v>
@@ -3429,7 +3439,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="100" t="s">
+      <c r="A29" s="99" t="s">
         <v>156</v>
       </c>
       <c r="B29" s="71" t="s">
@@ -3462,7 +3472,7 @@
       <c r="C30" s="92" t="s">
         <v>159</v>
       </c>
-      <c r="D30" s="101" t="s">
+      <c r="D30" s="100" t="s">
         <v>160</v>
       </c>
       <c r="E30" s="93">
@@ -3549,14 +3559,14 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="124" t="s">
+      <c r="A34" s="123" t="s">
         <v>110</v>
       </c>
-      <c r="B34" s="125"/>
-      <c r="C34" s="125"/>
-      <c r="D34" s="125"/>
-      <c r="E34" s="125"/>
-      <c r="F34" s="126"/>
+      <c r="B34" s="124"/>
+      <c r="C34" s="124"/>
+      <c r="D34" s="124"/>
+      <c r="E34" s="124"/>
+      <c r="F34" s="125"/>
       <c r="G34" s="17">
         <f>AVERAGE(G14:G33)</f>
         <v>174.95</v>
@@ -3817,7 +3827,7 @@
       <c r="A6" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="104">
+      <c r="B6" s="103">
         <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$33,A6,'Dados Historicos x Categoria'!$G$4:$G$33)</f>
         <v>148.57142857142858</v>
       </c>
@@ -3848,522 +3858,522 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="127" t="s">
+      <c r="C17" s="126" t="s">
         <v>111</v>
       </c>
-      <c r="D17" s="128"/>
-      <c r="E17" s="128"/>
-      <c r="F17" s="128"/>
-      <c r="G17" s="128"/>
+      <c r="D17" s="127"/>
+      <c r="E17" s="127"/>
+      <c r="F17" s="127"/>
+      <c r="G17" s="127"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="129"/>
-      <c r="D18" s="129"/>
-      <c r="E18" s="129"/>
-      <c r="F18" s="129"/>
-      <c r="G18" s="129"/>
+      <c r="C18" s="128"/>
+      <c r="D18" s="128"/>
+      <c r="E18" s="128"/>
+      <c r="F18" s="128"/>
+      <c r="G18" s="128"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="129"/>
-      <c r="D19" s="129"/>
-      <c r="E19" s="129"/>
-      <c r="F19" s="129"/>
-      <c r="G19" s="129"/>
+      <c r="C19" s="128"/>
+      <c r="D19" s="128"/>
+      <c r="E19" s="128"/>
+      <c r="F19" s="128"/>
+      <c r="G19" s="128"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="129"/>
-      <c r="D20" s="129"/>
-      <c r="E20" s="129"/>
-      <c r="F20" s="129"/>
-      <c r="G20" s="129"/>
+      <c r="C20" s="128"/>
+      <c r="D20" s="128"/>
+      <c r="E20" s="128"/>
+      <c r="F20" s="128"/>
+      <c r="G20" s="128"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="129"/>
-      <c r="D21" s="129"/>
-      <c r="E21" s="129"/>
-      <c r="F21" s="129"/>
-      <c r="G21" s="129"/>
+      <c r="C21" s="128"/>
+      <c r="D21" s="128"/>
+      <c r="E21" s="128"/>
+      <c r="F21" s="128"/>
+      <c r="G21" s="128"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="129"/>
-      <c r="D22" s="129"/>
-      <c r="E22" s="129"/>
-      <c r="F22" s="129"/>
-      <c r="G22" s="129"/>
+      <c r="C22" s="128"/>
+      <c r="D22" s="128"/>
+      <c r="E22" s="128"/>
+      <c r="F22" s="128"/>
+      <c r="G22" s="128"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="129"/>
-      <c r="D23" s="129"/>
-      <c r="E23" s="129"/>
-      <c r="F23" s="129"/>
-      <c r="G23" s="129"/>
+      <c r="C23" s="128"/>
+      <c r="D23" s="128"/>
+      <c r="E23" s="128"/>
+      <c r="F23" s="128"/>
+      <c r="G23" s="128"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="129"/>
-      <c r="D24" s="129"/>
-      <c r="E24" s="129"/>
-      <c r="F24" s="129"/>
-      <c r="G24" s="129"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="128"/>
+      <c r="F24" s="128"/>
+      <c r="G24" s="128"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="129"/>
-      <c r="D25" s="129"/>
-      <c r="E25" s="129"/>
-      <c r="F25" s="129"/>
-      <c r="G25" s="129"/>
+      <c r="C25" s="128"/>
+      <c r="D25" s="128"/>
+      <c r="E25" s="128"/>
+      <c r="F25" s="128"/>
+      <c r="G25" s="128"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="129"/>
-      <c r="D26" s="129"/>
-      <c r="E26" s="129"/>
-      <c r="F26" s="129"/>
-      <c r="G26" s="129"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="128"/>
+      <c r="F26" s="128"/>
+      <c r="G26" s="128"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="129"/>
-      <c r="D27" s="129"/>
-      <c r="E27" s="129"/>
-      <c r="F27" s="129"/>
-      <c r="G27" s="129"/>
+      <c r="C27" s="128"/>
+      <c r="D27" s="128"/>
+      <c r="E27" s="128"/>
+      <c r="F27" s="128"/>
+      <c r="G27" s="128"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="129"/>
-      <c r="D28" s="129"/>
-      <c r="E28" s="129"/>
-      <c r="F28" s="129"/>
-      <c r="G28" s="129"/>
+      <c r="C28" s="128"/>
+      <c r="D28" s="128"/>
+      <c r="E28" s="128"/>
+      <c r="F28" s="128"/>
+      <c r="G28" s="128"/>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="129"/>
-      <c r="D29" s="129"/>
-      <c r="E29" s="129"/>
-      <c r="F29" s="129"/>
-      <c r="G29" s="129"/>
+      <c r="C29" s="128"/>
+      <c r="D29" s="128"/>
+      <c r="E29" s="128"/>
+      <c r="F29" s="128"/>
+      <c r="G29" s="128"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="129"/>
-      <c r="D30" s="129"/>
-      <c r="E30" s="129"/>
-      <c r="F30" s="129"/>
-      <c r="G30" s="129"/>
+      <c r="C30" s="128"/>
+      <c r="D30" s="128"/>
+      <c r="E30" s="128"/>
+      <c r="F30" s="128"/>
+      <c r="G30" s="128"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="108" t="s">
+      <c r="A47" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="109" t="s">
+      <c r="B47" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="109" t="s">
+      <c r="C47" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="110" t="s">
+      <c r="D47" s="109" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="105" t="s">
+      <c r="A48" s="104" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="106">
+      <c r="B48" s="105">
         <v>42311</v>
       </c>
-      <c r="C48" s="106">
+      <c r="C48" s="105">
         <v>42446</v>
       </c>
-      <c r="D48" s="107">
+      <c r="D48" s="106">
         <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="105" t="s">
+      <c r="A49" s="104" t="s">
         <v>131</v>
       </c>
-      <c r="B49" s="106">
+      <c r="B49" s="105">
         <v>42118</v>
       </c>
-      <c r="C49" s="106">
+      <c r="C49" s="105">
         <v>42221</v>
       </c>
-      <c r="D49" s="107">
+      <c r="D49" s="106">
         <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="105" t="s">
+      <c r="A50" s="104" t="s">
         <v>131</v>
       </c>
-      <c r="B50" s="106">
+      <c r="B50" s="105">
         <v>42263</v>
       </c>
-      <c r="C50" s="106">
+      <c r="C50" s="105">
         <v>42342</v>
       </c>
-      <c r="D50" s="107">
+      <c r="D50" s="106">
         <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="105" t="s">
+      <c r="A51" s="104" t="s">
         <v>131</v>
       </c>
-      <c r="B51" s="106">
+      <c r="B51" s="105">
         <v>42633</v>
       </c>
-      <c r="C51" s="106">
+      <c r="C51" s="105">
         <v>42695</v>
       </c>
-      <c r="D51" s="107">
+      <c r="D51" s="106">
         <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="105" t="s">
+      <c r="A52" s="104" t="s">
         <v>131</v>
       </c>
-      <c r="B52" s="106">
+      <c r="B52" s="105">
         <v>42422</v>
       </c>
-      <c r="C52" s="106">
+      <c r="C52" s="105">
         <v>42643</v>
       </c>
-      <c r="D52" s="107">
+      <c r="D52" s="106">
         <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="105" t="s">
+      <c r="A53" s="104" t="s">
         <v>131</v>
       </c>
-      <c r="B53" s="106">
+      <c r="B53" s="105">
         <v>41955</v>
       </c>
-      <c r="C53" s="106">
+      <c r="C53" s="105">
         <v>42179</v>
       </c>
-      <c r="D53" s="107">
+      <c r="D53" s="106">
         <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="105" t="s">
+      <c r="A54" s="104" t="s">
         <v>131</v>
       </c>
-      <c r="B54" s="106">
+      <c r="B54" s="105">
         <v>41738</v>
       </c>
-      <c r="C54" s="106">
+      <c r="C54" s="105">
         <v>41850</v>
       </c>
-      <c r="D54" s="107">
+      <c r="D54" s="106">
         <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="105" t="s">
+      <c r="A55" s="104" t="s">
         <v>77</v>
       </c>
-      <c r="B55" s="106">
+      <c r="B55" s="105">
         <v>41337</v>
       </c>
-      <c r="C55" s="106">
+      <c r="C55" s="105">
         <v>41430</v>
       </c>
-      <c r="D55" s="107">
+      <c r="D55" s="106">
         <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="105" t="s">
+      <c r="A56" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="B56" s="106">
+      <c r="B56" s="105">
         <v>42209</v>
       </c>
-      <c r="C56" s="106">
+      <c r="C56" s="105">
         <v>42683</v>
       </c>
-      <c r="D56" s="107">
+      <c r="D56" s="106">
         <v>465</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="105" t="s">
+      <c r="A57" s="104" t="s">
         <v>87</v>
       </c>
-      <c r="B57" s="106">
+      <c r="B57" s="105">
         <v>42020</v>
       </c>
-      <c r="C57" s="106">
+      <c r="C57" s="105">
         <v>42671</v>
       </c>
-      <c r="D57" s="107">
+      <c r="D57" s="106">
         <v>642</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="105" t="s">
+      <c r="A58" s="104" t="s">
         <v>87</v>
       </c>
-      <c r="B58" s="106">
+      <c r="B58" s="105">
         <v>42439</v>
       </c>
-      <c r="C58" s="106">
+      <c r="C58" s="105">
         <v>42668</v>
       </c>
-      <c r="D58" s="107">
+      <c r="D58" s="106">
         <v>225</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="105" t="s">
+      <c r="A59" s="104" t="s">
         <v>92</v>
       </c>
-      <c r="B59" s="106">
+      <c r="B59" s="105">
         <v>42521</v>
       </c>
-      <c r="C59" s="106">
+      <c r="C59" s="105">
         <v>42661</v>
       </c>
-      <c r="D59" s="107">
+      <c r="D59" s="106">
         <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="105" t="s">
+      <c r="A60" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="106">
+      <c r="B60" s="105">
         <v>41242</v>
       </c>
-      <c r="C60" s="106">
+      <c r="C60" s="105">
         <v>41472</v>
       </c>
-      <c r="D60" s="107">
+      <c r="D60" s="106">
         <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="105" t="s">
+      <c r="A61" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="B61" s="106">
+      <c r="B61" s="105">
         <v>41698</v>
       </c>
-      <c r="C61" s="106">
+      <c r="C61" s="105">
         <v>41932</v>
       </c>
-      <c r="D61" s="107">
+      <c r="D61" s="106">
         <v>230</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="105" t="s">
+      <c r="A62" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="B62" s="106">
+      <c r="B62" s="105">
         <v>42277</v>
       </c>
-      <c r="C62" s="106">
+      <c r="C62" s="105">
         <v>42681</v>
       </c>
-      <c r="D62" s="107">
+      <c r="D62" s="106">
         <v>397</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="105" t="s">
+      <c r="A63" s="104" t="s">
         <v>77</v>
       </c>
-      <c r="B63" s="106">
+      <c r="B63" s="105">
         <v>42136</v>
       </c>
-      <c r="C63" s="106">
+      <c r="C63" s="105">
         <v>42171</v>
       </c>
-      <c r="D63" s="107">
+      <c r="D63" s="106">
         <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="105" t="s">
+      <c r="A64" s="104" t="s">
         <v>77</v>
       </c>
-      <c r="B64" s="106">
+      <c r="B64" s="105">
         <v>41541</v>
       </c>
-      <c r="C64" s="106">
+      <c r="C64" s="105">
         <v>41634</v>
       </c>
-      <c r="D64" s="107">
+      <c r="D64" s="106">
         <v>92</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="105" t="s">
+      <c r="A65" s="104" t="s">
         <v>77</v>
       </c>
-      <c r="B65" s="106">
+      <c r="B65" s="105">
         <v>41575</v>
       </c>
-      <c r="C65" s="106">
+      <c r="C65" s="105">
         <v>41638</v>
       </c>
-      <c r="D65" s="107">
+      <c r="D65" s="106">
         <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="105" t="s">
+      <c r="A66" s="104" t="s">
         <v>77</v>
       </c>
-      <c r="B66" s="106">
+      <c r="B66" s="105">
         <v>42580</v>
       </c>
-      <c r="C66" s="106">
+      <c r="C66" s="105">
         <v>42641</v>
       </c>
-      <c r="D66" s="107">
+      <c r="D66" s="106">
         <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="105" t="s">
+      <c r="A67" s="104" t="s">
         <v>142</v>
       </c>
-      <c r="B67" s="106">
+      <c r="B67" s="105">
         <v>42612</v>
       </c>
-      <c r="C67" s="106">
+      <c r="C67" s="105">
         <v>42704</v>
       </c>
-      <c r="D67" s="107">
+      <c r="D67" s="106">
         <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="105" t="s">
+      <c r="A68" s="104" t="s">
         <v>145</v>
       </c>
-      <c r="B68" s="106">
+      <c r="B68" s="105">
         <v>42068</v>
       </c>
-      <c r="C68" s="106">
+      <c r="C68" s="105">
         <v>42149</v>
       </c>
-      <c r="D68" s="107">
+      <c r="D68" s="106">
         <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="105" t="s">
+      <c r="A69" s="104" t="s">
         <v>148</v>
       </c>
-      <c r="B69" s="106">
+      <c r="B69" s="105">
         <v>42410</v>
       </c>
-      <c r="C69" s="106">
+      <c r="C69" s="105">
         <v>42690</v>
       </c>
-      <c r="D69" s="107">
+      <c r="D69" s="106">
         <v>276</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="105" t="s">
+      <c r="A70" s="104" t="s">
         <v>151</v>
       </c>
-      <c r="B70" s="106">
+      <c r="B70" s="105">
         <v>41208</v>
       </c>
-      <c r="C70" s="106">
+      <c r="C70" s="105">
         <v>41348</v>
       </c>
-      <c r="D70" s="107">
+      <c r="D70" s="106">
         <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="105" t="s">
+      <c r="A71" s="104" t="s">
         <v>153</v>
       </c>
-      <c r="B71" s="106">
+      <c r="B71" s="105">
         <v>40927</v>
       </c>
-      <c r="C71" s="106">
+      <c r="C71" s="105">
         <v>41012</v>
       </c>
-      <c r="D71" s="107">
+      <c r="D71" s="106">
         <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="105" t="s">
+      <c r="A72" s="104" t="s">
         <v>145</v>
       </c>
-      <c r="B72" s="106">
+      <c r="B72" s="105">
         <v>41885</v>
       </c>
-      <c r="C72" s="106">
+      <c r="C72" s="105">
         <v>41996</v>
       </c>
-      <c r="D72" s="107">
+      <c r="D72" s="106">
         <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="105" t="s">
+      <c r="A73" s="104" t="s">
         <v>167</v>
       </c>
-      <c r="B73" s="106">
+      <c r="B73" s="105">
         <v>40945</v>
       </c>
-      <c r="C73" s="106">
+      <c r="C73" s="105">
         <v>41093</v>
       </c>
-      <c r="D73" s="107">
+      <c r="D73" s="106">
         <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="105" t="s">
+      <c r="A74" s="104" t="s">
         <v>162</v>
       </c>
-      <c r="B74" s="106">
+      <c r="B74" s="105">
         <v>41411</v>
       </c>
-      <c r="C74" s="106">
+      <c r="C74" s="105">
         <v>41666</v>
       </c>
-      <c r="D74" s="107">
+      <c r="D74" s="106">
         <v>250</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="105" t="s">
+      <c r="A75" s="104" t="s">
         <v>165</v>
       </c>
-      <c r="B75" s="106">
+      <c r="B75" s="105">
         <v>41905</v>
       </c>
-      <c r="C75" s="106">
+      <c r="C75" s="105">
         <v>41999</v>
       </c>
-      <c r="D75" s="107">
+      <c r="D75" s="106">
         <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="105" t="s">
+      <c r="A76" s="104" t="s">
         <v>108</v>
       </c>
-      <c r="B76" s="106">
+      <c r="B76" s="105">
         <v>42229</v>
       </c>
-      <c r="C76" s="106">
+      <c r="C76" s="105">
         <v>42354</v>
       </c>
-      <c r="D76" s="107">
+      <c r="D76" s="106">
         <v>123</v>
       </c>
     </row>
@@ -4593,10 +4603,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4646,19 +4656,19 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="53" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="132">
+      <c r="A2" s="130">
         <v>1</v>
       </c>
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="129" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="138" t="s">
+      <c r="C2" s="129" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="138" t="s">
+      <c r="D2" s="129" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="138">
+      <c r="E2" s="129">
         <v>2</v>
       </c>
       <c r="F2" s="39" t="s">
@@ -4676,11 +4686,11 @@
       <c r="J2" s="39"/>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="133"/>
-      <c r="B3" s="138"/>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
+      <c r="A3" s="131"/>
+      <c r="B3" s="129"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
       <c r="F3" s="39" t="s">
         <v>60</v>
       </c>
@@ -4696,19 +4706,19 @@
       <c r="J3" s="39"/>
     </row>
     <row r="4" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="138">
+      <c r="A4" s="129">
         <v>2</v>
       </c>
-      <c r="B4" s="139">
+      <c r="B4" s="134">
         <v>42440</v>
       </c>
-      <c r="C4" s="138" t="s">
+      <c r="C4" s="129" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="138" t="s">
+      <c r="D4" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="132">
+      <c r="E4" s="130">
         <v>2</v>
       </c>
       <c r="F4" s="39" t="s">
@@ -4726,11 +4736,11 @@
       <c r="J4" s="39"/>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="132"/>
-      <c r="B5" s="132"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="133"/>
+      <c r="A5" s="130"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="131"/>
       <c r="F5" s="45" t="s">
         <v>54</v>
       </c>
@@ -4746,19 +4756,19 @@
       <c r="J5" s="45"/>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="138">
+      <c r="A6" s="129">
         <v>3</v>
       </c>
-      <c r="B6" s="135">
+      <c r="B6" s="133">
         <v>42683</v>
       </c>
-      <c r="C6" s="132" t="s">
+      <c r="C6" s="130" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="132" t="s">
+      <c r="D6" s="130" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="132">
+      <c r="E6" s="130">
         <v>2</v>
       </c>
       <c r="F6" s="39" t="s">
@@ -4776,11 +4786,11 @@
       <c r="J6" s="39"/>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="138"/>
-      <c r="B7" s="133"/>
-      <c r="C7" s="133"/>
-      <c r="D7" s="133"/>
-      <c r="E7" s="133"/>
+      <c r="A7" s="129"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="131"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="131"/>
       <c r="F7" s="64" t="s">
         <v>67</v>
       </c>
@@ -4796,11 +4806,11 @@
       <c r="J7" s="39"/>
     </row>
     <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="138"/>
-      <c r="B8" s="133"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
+      <c r="A8" s="129"/>
+      <c r="B8" s="131"/>
+      <c r="C8" s="131"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="131"/>
       <c r="F8" s="61" t="s">
         <v>69</v>
       </c>
@@ -4816,11 +4826,11 @@
       <c r="J8" s="61"/>
     </row>
     <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="138"/>
-      <c r="B9" s="133"/>
-      <c r="C9" s="133"/>
-      <c r="D9" s="133"/>
-      <c r="E9" s="133"/>
+      <c r="A9" s="129"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="131"/>
+      <c r="D9" s="131"/>
+      <c r="E9" s="131"/>
       <c r="F9" s="61" t="s">
         <v>73</v>
       </c>
@@ -4836,11 +4846,11 @@
       <c r="J9" s="61"/>
     </row>
     <row r="10" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="138"/>
-      <c r="B10" s="134"/>
-      <c r="C10" s="134"/>
-      <c r="D10" s="134"/>
-      <c r="E10" s="134"/>
+      <c r="A10" s="129"/>
+      <c r="B10" s="132"/>
+      <c r="C10" s="132"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="132"/>
       <c r="F10" s="39" t="s">
         <v>70</v>
       </c>
@@ -4858,19 +4868,19 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="138">
+      <c r="A11" s="129">
         <v>4</v>
       </c>
-      <c r="B11" s="138" t="s">
+      <c r="B11" s="129" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="138" t="s">
+      <c r="C11" s="129" t="s">
         <v>117</v>
       </c>
-      <c r="D11" s="138" t="s">
+      <c r="D11" s="129" t="s">
         <v>118</v>
       </c>
-      <c r="E11" s="138">
+      <c r="E11" s="129">
         <v>2</v>
       </c>
       <c r="F11" s="61" t="s">
@@ -4888,11 +4898,11 @@
       <c r="J11" s="61"/>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="138"/>
-      <c r="B12" s="138"/>
-      <c r="C12" s="138"/>
-      <c r="D12" s="138"/>
-      <c r="E12" s="138"/>
+      <c r="A12" s="129"/>
+      <c r="B12" s="129"/>
+      <c r="C12" s="129"/>
+      <c r="D12" s="129"/>
+      <c r="E12" s="129"/>
       <c r="F12" s="64" t="s">
         <v>58</v>
       </c>
@@ -4908,11 +4918,11 @@
       <c r="J12" s="61"/>
     </row>
     <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="132"/>
-      <c r="B13" s="132"/>
-      <c r="C13" s="132"/>
-      <c r="D13" s="132"/>
-      <c r="E13" s="132"/>
+      <c r="A13" s="130"/>
+      <c r="B13" s="130"/>
+      <c r="C13" s="130"/>
+      <c r="D13" s="130"/>
+      <c r="E13" s="130"/>
       <c r="F13" s="82" t="s">
         <v>72</v>
       </c>
@@ -4928,17 +4938,17 @@
       <c r="J13" s="77"/>
     </row>
     <row r="14" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="132">
+      <c r="A14" s="130">
         <v>5</v>
       </c>
-      <c r="B14" s="135">
+      <c r="B14" s="133">
         <v>42705</v>
       </c>
-      <c r="C14" s="132"/>
-      <c r="D14" s="132" t="s">
+      <c r="C14" s="130"/>
+      <c r="D14" s="130" t="s">
         <v>118</v>
       </c>
-      <c r="E14" s="132">
+      <c r="E14" s="130">
         <v>2</v>
       </c>
       <c r="F14" s="83" t="s">
@@ -4956,11 +4966,11 @@
       <c r="J14" s="78"/>
     </row>
     <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A15" s="133"/>
+      <c r="A15" s="131"/>
       <c r="B15" s="136"/>
-      <c r="C15" s="133"/>
-      <c r="D15" s="133"/>
-      <c r="E15" s="133"/>
+      <c r="C15" s="131"/>
+      <c r="D15" s="131"/>
+      <c r="E15" s="131"/>
       <c r="F15" s="83" t="s">
         <v>123</v>
       </c>
@@ -4976,11 +4986,11 @@
       <c r="J15" s="78"/>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="133"/>
+      <c r="A16" s="131"/>
       <c r="B16" s="136"/>
-      <c r="C16" s="133"/>
-      <c r="D16" s="134"/>
-      <c r="E16" s="133"/>
+      <c r="C16" s="131"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="131"/>
       <c r="F16" s="83" t="s">
         <v>125</v>
       </c>
@@ -4996,13 +5006,13 @@
       <c r="J16" s="78"/>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="133"/>
+      <c r="A17" s="131"/>
       <c r="B17" s="136"/>
-      <c r="C17" s="133"/>
+      <c r="C17" s="131"/>
       <c r="D17" s="78" t="s">
         <v>119</v>
       </c>
-      <c r="E17" s="133"/>
+      <c r="E17" s="131"/>
       <c r="F17" s="83" t="s">
         <v>126</v>
       </c>
@@ -5018,13 +5028,13 @@
       <c r="J17" s="78"/>
     </row>
     <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="133"/>
+      <c r="A18" s="131"/>
       <c r="B18" s="136"/>
-      <c r="C18" s="133"/>
-      <c r="D18" s="132" t="s">
+      <c r="C18" s="131"/>
+      <c r="D18" s="130" t="s">
         <v>120</v>
       </c>
-      <c r="E18" s="133"/>
+      <c r="E18" s="131"/>
       <c r="F18" s="83" t="s">
         <v>128</v>
       </c>
@@ -5040,51 +5050,74 @@
       <c r="J18" s="78"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="134"/>
+      <c r="A19" s="132"/>
       <c r="B19" s="137"/>
-      <c r="C19" s="134"/>
-      <c r="D19" s="134"/>
-      <c r="E19" s="134"/>
+      <c r="C19" s="132"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="132"/>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="55">
         <v>6</v>
       </c>
-      <c r="B20" s="96">
+      <c r="B20" s="146">
         <v>42773</v>
       </c>
-      <c r="D20" s="130" t="s">
+      <c r="D20" s="135" t="s">
         <v>182</v>
       </c>
       <c r="F20" s="55" t="s">
         <v>177</v>
       </c>
+      <c r="I20" s="55" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="D21" s="131"/>
+      <c r="B21" s="145"/>
+      <c r="D21" s="147"/>
       <c r="F21" s="55" t="s">
         <v>178</v>
       </c>
       <c r="G21" s="55" t="s">
         <v>179</v>
       </c>
+      <c r="I21" s="55" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="D22" s="131"/>
+      <c r="B22" s="145"/>
+      <c r="D22" s="147"/>
       <c r="F22" s="55" t="s">
         <v>180</v>
       </c>
       <c r="G22" s="55" t="s">
         <v>181</v>
       </c>
+      <c r="I22" s="55" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B23" s="145"/>
+      <c r="D23" s="147"/>
+      <c r="F23" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="G23" s="55" t="s">
+        <v>184</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A2:A3"/>
+  <mergeCells count="28">
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="D20:D23"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="A6:A10"/>
@@ -5101,12 +5134,11 @@
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="E11:E13"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5294,20 +5326,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="138" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="142" t="s">
+      <c r="B1" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="144" t="s">
+      <c r="C1" s="142" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145" t="s">
+      <c r="D1" s="143"/>
+      <c r="E1" s="143" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="146"/>
+      <c r="F1" s="144"/>
       <c r="G1" s="23" t="s">
         <v>35</v>
       </c>
@@ -5327,8 +5359,8 @@
       <c r="U1" s="24"/>
     </row>
     <row r="2" spans="1:21" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="141"/>
-      <c r="B2" s="143"/>
+      <c r="A2" s="139"/>
+      <c r="B2" s="141"/>
       <c r="C2" s="25" t="s">
         <v>36</v>
       </c>
@@ -5365,7 +5397,7 @@
       <c r="N2" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="O2" s="117">
+      <c r="O2" s="116">
         <v>42887</v>
       </c>
       <c r="P2" s="28">
@@ -5383,7 +5415,7 @@
       <c r="T2" s="28">
         <v>43040</v>
       </c>
-      <c r="U2" s="117" t="s">
+      <c r="U2" s="116" t="s">
         <v>176</v>
       </c>
     </row>
@@ -5414,48 +5446,48 @@
       <c r="L3" s="33"/>
       <c r="M3" s="33"/>
       <c r="N3" s="33"/>
-      <c r="O3" s="118"/>
-      <c r="P3" s="102"/>
-      <c r="Q3" s="102"/>
-      <c r="R3" s="102"/>
-      <c r="S3" s="102"/>
-      <c r="T3" s="102"/>
-      <c r="U3" s="122"/>
+      <c r="O3" s="117"/>
+      <c r="P3" s="101"/>
+      <c r="Q3" s="101"/>
+      <c r="R3" s="101"/>
+      <c r="S3" s="101"/>
+      <c r="T3" s="101"/>
+      <c r="U3" s="121"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="111">
+      <c r="A4" s="110">
         <v>2</v>
       </c>
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="111" t="s">
         <v>168</v>
       </c>
-      <c r="C4" s="113">
+      <c r="C4" s="112">
         <v>42670</v>
       </c>
-      <c r="D4" s="114">
+      <c r="D4" s="113">
         <v>42794</v>
       </c>
-      <c r="E4" s="114">
+      <c r="E4" s="113">
         <v>42670</v>
       </c>
-      <c r="F4" s="115">
+      <c r="F4" s="114">
         <v>42794</v>
       </c>
-      <c r="G4" s="111"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="103"/>
-      <c r="K4" s="103"/>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103"/>
-      <c r="N4" s="103"/>
-      <c r="O4" s="119"/>
-      <c r="P4" s="102"/>
-      <c r="Q4" s="102"/>
-      <c r="R4" s="102"/>
-      <c r="S4" s="102"/>
-      <c r="T4" s="102"/>
-      <c r="U4" s="122"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="102"/>
+      <c r="N4" s="102"/>
+      <c r="O4" s="118"/>
+      <c r="P4" s="101"/>
+      <c r="Q4" s="101"/>
+      <c r="R4" s="101"/>
+      <c r="S4" s="101"/>
+      <c r="T4" s="101"/>
+      <c r="U4" s="121"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="34">
@@ -5476,13 +5508,13 @@
       <c r="L5" s="39"/>
       <c r="M5" s="39"/>
       <c r="N5" s="39"/>
-      <c r="O5" s="120"/>
-      <c r="P5" s="102"/>
-      <c r="Q5" s="102"/>
-      <c r="R5" s="102"/>
-      <c r="S5" s="102"/>
-      <c r="T5" s="102"/>
-      <c r="U5" s="122"/>
+      <c r="O5" s="119"/>
+      <c r="P5" s="101"/>
+      <c r="Q5" s="101"/>
+      <c r="R5" s="101"/>
+      <c r="S5" s="101"/>
+      <c r="T5" s="101"/>
+      <c r="U5" s="121"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="34">
@@ -5503,13 +5535,13 @@
       <c r="L6" s="39"/>
       <c r="M6" s="39"/>
       <c r="N6" s="39"/>
-      <c r="O6" s="120"/>
-      <c r="P6" s="102"/>
-      <c r="Q6" s="102"/>
-      <c r="R6" s="102"/>
-      <c r="S6" s="102"/>
-      <c r="T6" s="102"/>
-      <c r="U6" s="122"/>
+      <c r="O6" s="119"/>
+      <c r="P6" s="101"/>
+      <c r="Q6" s="101"/>
+      <c r="R6" s="101"/>
+      <c r="S6" s="101"/>
+      <c r="T6" s="101"/>
+      <c r="U6" s="121"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="34">
@@ -5530,13 +5562,13 @@
       <c r="L7" s="39"/>
       <c r="M7" s="39"/>
       <c r="N7" s="39"/>
-      <c r="O7" s="120"/>
-      <c r="P7" s="102"/>
-      <c r="Q7" s="102"/>
-      <c r="R7" s="102"/>
-      <c r="S7" s="102"/>
-      <c r="T7" s="102"/>
-      <c r="U7" s="122"/>
+      <c r="O7" s="119"/>
+      <c r="P7" s="101"/>
+      <c r="Q7" s="101"/>
+      <c r="R7" s="101"/>
+      <c r="S7" s="101"/>
+      <c r="T7" s="101"/>
+      <c r="U7" s="121"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="34">
@@ -5557,13 +5589,13 @@
       <c r="L8" s="39"/>
       <c r="M8" s="39"/>
       <c r="N8" s="39"/>
-      <c r="O8" s="120"/>
-      <c r="P8" s="102"/>
-      <c r="Q8" s="102"/>
-      <c r="R8" s="102"/>
-      <c r="S8" s="102"/>
-      <c r="T8" s="102"/>
-      <c r="U8" s="122"/>
+      <c r="O8" s="119"/>
+      <c r="P8" s="101"/>
+      <c r="Q8" s="101"/>
+      <c r="R8" s="101"/>
+      <c r="S8" s="101"/>
+      <c r="T8" s="101"/>
+      <c r="U8" s="121"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="34">
@@ -5584,13 +5616,13 @@
       <c r="L9" s="39"/>
       <c r="M9" s="39"/>
       <c r="N9" s="39"/>
-      <c r="O9" s="120"/>
-      <c r="P9" s="102"/>
-      <c r="Q9" s="102"/>
-      <c r="R9" s="102"/>
-      <c r="S9" s="102"/>
-      <c r="T9" s="102"/>
-      <c r="U9" s="122"/>
+      <c r="O9" s="119"/>
+      <c r="P9" s="101"/>
+      <c r="Q9" s="101"/>
+      <c r="R9" s="101"/>
+      <c r="S9" s="101"/>
+      <c r="T9" s="101"/>
+      <c r="U9" s="121"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="34">
@@ -5609,13 +5641,13 @@
       <c r="L10" s="39"/>
       <c r="M10" s="39"/>
       <c r="N10" s="39"/>
-      <c r="O10" s="120"/>
-      <c r="P10" s="102"/>
-      <c r="Q10" s="102"/>
-      <c r="R10" s="102"/>
-      <c r="S10" s="102"/>
-      <c r="T10" s="102"/>
-      <c r="U10" s="122"/>
+      <c r="O10" s="119"/>
+      <c r="P10" s="101"/>
+      <c r="Q10" s="101"/>
+      <c r="R10" s="101"/>
+      <c r="S10" s="101"/>
+      <c r="T10" s="101"/>
+      <c r="U10" s="121"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="34">
@@ -5634,13 +5666,13 @@
       <c r="L11" s="39"/>
       <c r="M11" s="39"/>
       <c r="N11" s="39"/>
-      <c r="O11" s="120"/>
-      <c r="P11" s="102"/>
-      <c r="Q11" s="102"/>
-      <c r="R11" s="102"/>
-      <c r="S11" s="102"/>
-      <c r="T11" s="102"/>
-      <c r="U11" s="122"/>
+      <c r="O11" s="119"/>
+      <c r="P11" s="101"/>
+      <c r="Q11" s="101"/>
+      <c r="R11" s="101"/>
+      <c r="S11" s="101"/>
+      <c r="T11" s="101"/>
+      <c r="U11" s="121"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="34">
@@ -5659,13 +5691,13 @@
       <c r="L12" s="39"/>
       <c r="M12" s="39"/>
       <c r="N12" s="39"/>
-      <c r="O12" s="120"/>
-      <c r="P12" s="102"/>
-      <c r="Q12" s="102"/>
-      <c r="R12" s="102"/>
-      <c r="S12" s="102"/>
-      <c r="T12" s="102"/>
-      <c r="U12" s="122"/>
+      <c r="O12" s="119"/>
+      <c r="P12" s="101"/>
+      <c r="Q12" s="101"/>
+      <c r="R12" s="101"/>
+      <c r="S12" s="101"/>
+      <c r="T12" s="101"/>
+      <c r="U12" s="121"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="34">
@@ -5684,13 +5716,13 @@
       <c r="L13" s="39"/>
       <c r="M13" s="39"/>
       <c r="N13" s="39"/>
-      <c r="O13" s="120"/>
-      <c r="P13" s="102"/>
-      <c r="Q13" s="102"/>
-      <c r="R13" s="102"/>
-      <c r="S13" s="102"/>
-      <c r="T13" s="102"/>
-      <c r="U13" s="122"/>
+      <c r="O13" s="119"/>
+      <c r="P13" s="101"/>
+      <c r="Q13" s="101"/>
+      <c r="R13" s="101"/>
+      <c r="S13" s="101"/>
+      <c r="T13" s="101"/>
+      <c r="U13" s="121"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="34">
@@ -5709,13 +5741,13 @@
       <c r="L14" s="39"/>
       <c r="M14" s="39"/>
       <c r="N14" s="39"/>
-      <c r="O14" s="120"/>
-      <c r="P14" s="102"/>
-      <c r="Q14" s="102"/>
-      <c r="R14" s="102"/>
-      <c r="S14" s="102"/>
-      <c r="T14" s="102"/>
-      <c r="U14" s="122"/>
+      <c r="O14" s="119"/>
+      <c r="P14" s="101"/>
+      <c r="Q14" s="101"/>
+      <c r="R14" s="101"/>
+      <c r="S14" s="101"/>
+      <c r="T14" s="101"/>
+      <c r="U14" s="121"/>
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="34">
@@ -5734,13 +5766,13 @@
       <c r="L15" s="45"/>
       <c r="M15" s="45"/>
       <c r="N15" s="45"/>
-      <c r="O15" s="121"/>
-      <c r="P15" s="102"/>
-      <c r="Q15" s="102"/>
-      <c r="R15" s="102"/>
-      <c r="S15" s="102"/>
-      <c r="T15" s="102"/>
-      <c r="U15" s="122"/>
+      <c r="O15" s="120"/>
+      <c r="P15" s="101"/>
+      <c r="Q15" s="101"/>
+      <c r="R15" s="101"/>
+      <c r="S15" s="101"/>
+      <c r="T15" s="101"/>
+      <c r="U15" s="121"/>
     </row>
     <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="46"/>
@@ -5768,12 +5800,12 @@
       <c r="M16" s="51"/>
       <c r="N16" s="51"/>
       <c r="O16" s="52"/>
-      <c r="P16" s="116"/>
-      <c r="Q16" s="116"/>
-      <c r="R16" s="116"/>
-      <c r="S16" s="116"/>
-      <c r="T16" s="116"/>
-      <c r="U16" s="116"/>
+      <c r="P16" s="115"/>
+      <c r="Q16" s="115"/>
+      <c r="R16" s="115"/>
+      <c r="S16" s="115"/>
+      <c r="T16" s="115"/>
+      <c r="U16" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Versão Final para reunião 24/02
</commit_message>
<xml_diff>
--- a/TRE_Dados_MapaRaciocinio.xlsx
+++ b/TRE_Dados_MapaRaciocinio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Historicos x Categoria" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Atas das Reuniões" sheetId="5" r:id="rId3"/>
     <sheet name="PROCESSO PADRÃO" sheetId="4" r:id="rId4"/>
     <sheet name="Controle do Projeto" sheetId="6" r:id="rId5"/>
+    <sheet name="ÁREAS PADRÃO" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="196">
   <si>
     <t>Categoria</t>
   </si>
@@ -628,6 +629,18 @@
   </si>
   <si>
     <t>* PAD com estudos preliminares para atualizar média</t>
+  </si>
+  <si>
+    <t>ÁREA RESPONSÁVEL</t>
+  </si>
+  <si>
+    <t>Secretaria de Gestão de Serviços</t>
+  </si>
+  <si>
+    <t>Coordenadoria de InfraEstrutura Predial</t>
+  </si>
+  <si>
+    <t>Coordenadoria de Segurança , Transporte e Apoio Administrativo</t>
   </si>
 </sst>
 </file>
@@ -1592,34 +1605,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1924,11 +1937,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="15542784"/>
-        <c:axId val="241013824"/>
+        <c:axId val="335196160"/>
+        <c:axId val="333043328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="15542784"/>
+        <c:axId val="335196160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1948,7 +1961,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241013824"/>
+        <c:crossAx val="333043328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1956,7 +1969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241013824"/>
+        <c:axId val="333043328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1967,7 +1980,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="15542784"/>
+        <c:crossAx val="335196160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2019,6 +2032,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2165,11 +2179,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="241620480"/>
-        <c:axId val="241015552"/>
+        <c:axId val="335199744"/>
+        <c:axId val="333045056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="241620480"/>
+        <c:axId val="335199744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2178,7 +2192,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241015552"/>
+        <c:crossAx val="333045056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2186,7 +2200,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241015552"/>
+        <c:axId val="333045056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2197,13 +2211,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241620480"/>
+        <c:crossAx val="335199744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2225,13 +2240,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>181841</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>181841</xdr:rowOff>
+      <xdr:rowOff>170635</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2782166</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>19916</xdr:rowOff>
+      <xdr:rowOff>8710</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2255,8 +2270,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="181841" y="3229841"/>
-          <a:ext cx="5483802" cy="3656734"/>
+          <a:off x="181841" y="3218635"/>
+          <a:ext cx="5491443" cy="3659281"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3103,820 +3118,912 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4:G33"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="102" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" style="102" customWidth="1"/>
-    <col min="3" max="3" width="59.140625" style="102" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" style="102" customWidth="1"/>
-    <col min="5" max="5" width="15" style="102" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="102" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" style="102" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="102" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" style="102" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="102" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" style="102" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="102" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="102"/>
+    <col min="1" max="2" width="18.28515625" style="102" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="102" customWidth="1"/>
+    <col min="4" max="4" width="59.140625" style="102" customWidth="1"/>
+    <col min="5" max="5" width="53.140625" style="102" customWidth="1"/>
+    <col min="6" max="6" width="15" style="102" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="102" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" style="102" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="102" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" style="102" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="102" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="102" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="102" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="102"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="132" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="132"/>
       <c r="C1" s="132"/>
-      <c r="D1" s="98" t="s">
+      <c r="D1" s="132"/>
+      <c r="E1" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="99" t="s">
+      <c r="F1" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="100">
+      <c r="G1" s="100">
         <f ca="1">TODAY()</f>
-        <v>42787</v>
-      </c>
-      <c r="G1" s="101" t="s">
+        <v>42789</v>
+      </c>
+      <c r="H1" s="101" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>63</v>
       </c>
       <c r="B3" s="103" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" s="103" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="104" t="s">
+      <c r="D3" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="105" t="s">
+      <c r="E3" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="105" t="s">
+      <c r="F3" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="105" t="s">
+      <c r="G3" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="106" t="s">
+      <c r="H3" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="107" t="s">
+      <c r="K3" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="108" t="s">
+      <c r="L3" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="109" t="s">
+      <c r="M3" s="109" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="110" t="s">
         <v>74</v>
       </c>
       <c r="B4" s="110" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="99" t="s">
+      <c r="D4" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="101" t="s">
+      <c r="E4" s="101" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="100">
+      <c r="F4" s="100">
         <v>42311</v>
       </c>
-      <c r="F4" s="100">
+      <c r="G4" s="100">
         <v>42446</v>
       </c>
-      <c r="G4" s="111">
-        <f t="shared" ref="G4:G12" si="0">DAYS360(E4,F4)</f>
+      <c r="H4" s="111">
+        <f t="shared" ref="H4:H12" si="0">DAYS360(F4,G4)</f>
         <v>134</v>
       </c>
-      <c r="H4" s="112"/>
-      <c r="J4" s="113">
-        <f>AVERAGE(G13,G34)</f>
+      <c r="I4" s="112"/>
+      <c r="K4" s="113">
+        <f>AVERAGE(H13,H34)</f>
         <v>169.75277777777777</v>
       </c>
-      <c r="K4" s="114">
+      <c r="L4" s="114">
         <v>0.15</v>
       </c>
-      <c r="L4" s="99">
-        <f>J4-(J4*K4)</f>
+      <c r="M4" s="99">
+        <f>K4-(K4*L4)</f>
         <v>144.28986111111109</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="110" t="s">
         <v>127</v>
       </c>
       <c r="B5" s="110" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="99" t="s">
+      <c r="D5" s="99" t="s">
         <v>129</v>
       </c>
-      <c r="D5" s="101" t="s">
+      <c r="E5" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="100">
+      <c r="F5" s="100">
         <v>42118</v>
       </c>
-      <c r="F5" s="100">
+      <c r="G5" s="100">
         <v>42221</v>
       </c>
-      <c r="G5" s="111">
+      <c r="H5" s="111">
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
-      <c r="J5" s="115"/>
-      <c r="K5" s="116"/>
-      <c r="L5" s="117"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5" s="115"/>
+      <c r="L5" s="116"/>
+      <c r="M5" s="117"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="110" t="s">
         <v>130</v>
       </c>
       <c r="B6" s="110" t="s">
+        <v>195</v>
+      </c>
+      <c r="C6" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="C6" s="99" t="s">
+      <c r="D6" s="99" t="s">
         <v>129</v>
       </c>
-      <c r="D6" s="101" t="s">
+      <c r="E6" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="E6" s="100">
+      <c r="F6" s="100">
         <v>42263</v>
       </c>
-      <c r="F6" s="100">
+      <c r="G6" s="100">
         <v>42342</v>
       </c>
-      <c r="G6" s="111">
+      <c r="H6" s="111">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
-      <c r="J6" s="115"/>
-      <c r="K6" s="116"/>
-      <c r="L6" s="117"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K6" s="115"/>
+      <c r="L6" s="116"/>
+      <c r="M6" s="117"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="110" t="s">
         <v>132</v>
       </c>
       <c r="B7" s="110" t="s">
+        <v>195</v>
+      </c>
+      <c r="C7" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="99" t="s">
+      <c r="D7" s="99" t="s">
         <v>129</v>
       </c>
-      <c r="D7" s="101" t="s">
+      <c r="E7" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="E7" s="100">
+      <c r="F7" s="100">
         <v>42633</v>
       </c>
-      <c r="F7" s="100">
+      <c r="G7" s="100">
         <v>42695</v>
       </c>
-      <c r="G7" s="111">
+      <c r="H7" s="111">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="J7" s="115"/>
-      <c r="K7" s="116"/>
-      <c r="L7" s="117"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7" s="115"/>
+      <c r="L7" s="116"/>
+      <c r="M7" s="117"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="110" t="s">
         <v>133</v>
       </c>
       <c r="B8" s="110" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="99" t="s">
+      <c r="D8" s="99" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="101" t="s">
+      <c r="E8" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="E8" s="100">
+      <c r="F8" s="100">
         <v>42422</v>
       </c>
-      <c r="F8" s="100">
+      <c r="G8" s="100">
         <v>42643</v>
       </c>
-      <c r="G8" s="111">
+      <c r="H8" s="111">
         <f t="shared" si="0"/>
         <v>218</v>
       </c>
-      <c r="J8" s="115"/>
-      <c r="K8" s="116"/>
-      <c r="L8" s="117"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8" s="115"/>
+      <c r="L8" s="116"/>
+      <c r="M8" s="117"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="110" t="s">
         <v>134</v>
       </c>
       <c r="B9" s="110" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="C9" s="99" t="s">
+      <c r="D9" s="99" t="s">
         <v>129</v>
       </c>
-      <c r="D9" s="101" t="s">
+      <c r="E9" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="E9" s="100">
+      <c r="F9" s="100">
         <v>41955</v>
       </c>
-      <c r="F9" s="100">
+      <c r="G9" s="100">
         <v>42179</v>
       </c>
-      <c r="G9" s="111">
+      <c r="H9" s="111">
         <f t="shared" si="0"/>
         <v>222</v>
       </c>
-      <c r="K9" s="118"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="118"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="110" t="s">
         <v>135</v>
       </c>
       <c r="B10" s="110" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="99" t="s">
+      <c r="D10" s="99" t="s">
         <v>129</v>
       </c>
-      <c r="D10" s="101" t="s">
+      <c r="E10" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="E10" s="100">
+      <c r="F10" s="100">
         <v>41738</v>
       </c>
-      <c r="F10" s="100">
+      <c r="G10" s="100">
         <v>41850</v>
       </c>
-      <c r="G10" s="111">
+      <c r="H10" s="111">
         <f t="shared" si="0"/>
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="110" t="s">
         <v>80</v>
       </c>
       <c r="B11" s="110" t="s">
+        <v>195</v>
+      </c>
+      <c r="C11" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="99" t="s">
+      <c r="D11" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="99" t="s">
+      <c r="E11" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="100">
+      <c r="F11" s="100">
         <v>41337</v>
       </c>
-      <c r="F11" s="100">
+      <c r="G11" s="100">
         <v>41430</v>
       </c>
-      <c r="G11" s="111">
+      <c r="H11" s="111">
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="110" t="s">
         <v>82</v>
       </c>
       <c r="B12" s="110" t="s">
+        <v>195</v>
+      </c>
+      <c r="C12" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="99" t="s">
+      <c r="D12" s="99" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="101" t="s">
+      <c r="E12" s="101" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="100">
+      <c r="F12" s="100">
         <v>42209</v>
       </c>
-      <c r="F12" s="100">
+      <c r="G12" s="100">
         <v>42683</v>
       </c>
-      <c r="G12" s="111">
+      <c r="H12" s="111">
         <f t="shared" si="0"/>
         <v>465</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="119"/>
-      <c r="B13" s="120"/>
-      <c r="C13" s="134" t="s">
+      <c r="B13" s="110"/>
+      <c r="C13" s="120"/>
+      <c r="D13" s="134" t="s">
         <v>184</v>
       </c>
-      <c r="D13" s="134"/>
       <c r="E13" s="134"/>
-      <c r="F13" s="135"/>
-      <c r="G13" s="121">
-        <f>AVERAGE(G4:G12)</f>
+      <c r="F13" s="134"/>
+      <c r="G13" s="135"/>
+      <c r="H13" s="121">
+        <f>AVERAGE(H4:H12)</f>
         <v>164.55555555555554</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="110" t="s">
         <v>85</v>
       </c>
       <c r="B14" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="99" t="s">
+      <c r="D14" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="101" t="str">
+      <c r="E14" s="101" t="str">
         <f>LOWER("CONTRATAÇÃO - SERVIÇO DE MANUTENÇÃO PREDIAL -   LIMPEZA DE VIDROS - CAPITAL/ INTERIOR")</f>
         <v>contratação - serviço de manutenção predial -   limpeza de vidros - capital/ interior</v>
       </c>
-      <c r="E14" s="100">
+      <c r="F14" s="100">
         <v>42020</v>
       </c>
-      <c r="F14" s="100">
+      <c r="G14" s="100">
         <v>42671</v>
       </c>
-      <c r="G14" s="111">
-        <f t="shared" ref="G14:G33" si="1">DAYS360(E14,F14)</f>
+      <c r="H14" s="111">
+        <f t="shared" ref="H14:H33" si="1">DAYS360(F14,G14)</f>
         <v>642</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="110" t="s">
         <v>88</v>
       </c>
       <c r="B15" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="99" t="s">
+      <c r="D15" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="101" t="s">
+      <c r="E15" s="101" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="100">
+      <c r="F15" s="100">
         <v>42439</v>
       </c>
-      <c r="F15" s="100">
+      <c r="G15" s="100">
         <v>42668</v>
       </c>
-      <c r="G15" s="111">
+      <c r="H15" s="111">
         <f t="shared" si="1"/>
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="110" t="s">
         <v>89</v>
       </c>
       <c r="B16" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="C16" s="99" t="s">
+      <c r="D16" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="101" t="s">
+      <c r="E16" s="101" t="s">
         <v>90</v>
       </c>
-      <c r="E16" s="100">
+      <c r="F16" s="100">
         <v>42521</v>
       </c>
-      <c r="F16" s="100">
+      <c r="G16" s="100">
         <v>42661</v>
       </c>
-      <c r="G16" s="111">
+      <c r="H16" s="111">
         <f t="shared" si="1"/>
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="110" t="s">
         <v>92</v>
       </c>
       <c r="B17" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C17" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="C17" s="99" t="s">
+      <c r="D17" s="99" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="101" t="s">
+      <c r="E17" s="101" t="s">
         <v>93</v>
       </c>
-      <c r="E17" s="100">
+      <c r="F17" s="100">
         <v>41242</v>
       </c>
-      <c r="F17" s="100">
+      <c r="G17" s="100">
         <v>41472</v>
       </c>
-      <c r="G17" s="111">
+      <c r="H17" s="111">
         <f t="shared" si="1"/>
         <v>228</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="110" t="s">
         <v>94</v>
       </c>
       <c r="B18" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C18" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="C18" s="99" t="s">
+      <c r="D18" s="99" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="101" t="s">
+      <c r="E18" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="100">
+      <c r="F18" s="100">
         <v>41698</v>
       </c>
-      <c r="F18" s="100">
+      <c r="G18" s="100">
         <v>41932</v>
       </c>
-      <c r="G18" s="111">
+      <c r="H18" s="111">
         <f t="shared" si="1"/>
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="110" t="s">
         <v>96</v>
       </c>
       <c r="B19" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C19" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="C19" s="99" t="s">
+      <c r="D19" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="99" t="s">
+      <c r="E19" s="99" t="s">
         <v>97</v>
       </c>
-      <c r="E19" s="100">
+      <c r="F19" s="100">
         <v>42277</v>
       </c>
-      <c r="F19" s="100">
+      <c r="G19" s="100">
         <v>42681</v>
       </c>
-      <c r="G19" s="111">
+      <c r="H19" s="111">
         <f t="shared" si="1"/>
         <v>397</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="110" t="s">
         <v>99</v>
       </c>
       <c r="B20" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C20" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="C20" s="99" t="s">
+      <c r="D20" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="101" t="s">
+      <c r="E20" s="101" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="100">
+      <c r="F20" s="100">
         <v>42136</v>
       </c>
-      <c r="F20" s="122">
+      <c r="G20" s="122">
         <v>42171</v>
       </c>
-      <c r="G20" s="111">
+      <c r="H20" s="111">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="110" t="s">
         <v>101</v>
       </c>
       <c r="B21" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="C21" s="99" t="s">
+      <c r="D21" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="101" t="s">
+      <c r="E21" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="100">
+      <c r="F21" s="100">
         <v>41541</v>
       </c>
-      <c r="F21" s="100">
+      <c r="G21" s="100">
         <v>41634</v>
       </c>
-      <c r="G21" s="111">
+      <c r="H21" s="111">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="110" t="s">
         <v>103</v>
       </c>
       <c r="B22" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C22" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="C22" s="123" t="s">
+      <c r="D22" s="123" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="101" t="s">
+      <c r="E22" s="101" t="s">
         <v>104</v>
       </c>
-      <c r="E22" s="100">
+      <c r="F22" s="100">
         <v>41575</v>
       </c>
-      <c r="F22" s="100">
+      <c r="G22" s="100">
         <v>41638</v>
       </c>
-      <c r="G22" s="111">
+      <c r="H22" s="111">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="110" t="s">
         <v>136</v>
       </c>
       <c r="B23" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C23" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="C23" s="124" t="s">
+      <c r="D23" s="124" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="125" t="s">
+      <c r="E23" s="125" t="s">
         <v>137</v>
       </c>
-      <c r="E23" s="126">
+      <c r="F23" s="126">
         <v>42580</v>
       </c>
-      <c r="F23" s="126">
+      <c r="G23" s="126">
         <v>42641</v>
       </c>
-      <c r="G23" s="127">
+      <c r="H23" s="127">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="110" t="s">
         <v>138</v>
       </c>
       <c r="B24" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C24" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="C24" s="125" t="s">
+      <c r="D24" s="125" t="s">
         <v>140</v>
       </c>
-      <c r="D24" s="128" t="s">
+      <c r="E24" s="128" t="s">
         <v>139</v>
       </c>
-      <c r="E24" s="126">
+      <c r="F24" s="126">
         <v>42612</v>
       </c>
-      <c r="F24" s="126">
+      <c r="G24" s="126">
         <v>42704</v>
       </c>
-      <c r="G24" s="127">
+      <c r="H24" s="127">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="110" t="s">
         <v>141</v>
       </c>
       <c r="B25" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C25" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="C25" s="125" t="s">
+      <c r="D25" s="125" t="s">
         <v>143</v>
       </c>
-      <c r="D25" s="128" t="s">
+      <c r="E25" s="128" t="s">
         <v>144</v>
       </c>
-      <c r="E25" s="126">
+      <c r="F25" s="126">
         <v>42068</v>
       </c>
-      <c r="F25" s="126">
+      <c r="G25" s="126">
         <v>42149</v>
       </c>
-      <c r="G25" s="127">
+      <c r="H25" s="127">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="110" t="s">
         <v>145</v>
       </c>
       <c r="B26" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C26" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="C26" s="125" t="s">
+      <c r="D26" s="125" t="s">
         <v>146</v>
       </c>
-      <c r="D26" s="128" t="s">
+      <c r="E26" s="128" t="s">
         <v>147</v>
       </c>
-      <c r="E26" s="126">
+      <c r="F26" s="126">
         <v>42410</v>
       </c>
-      <c r="F26" s="126">
+      <c r="G26" s="126">
         <v>42690</v>
       </c>
-      <c r="G26" s="127">
+      <c r="H26" s="127">
         <f t="shared" si="1"/>
         <v>276</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="110" t="s">
         <v>148</v>
       </c>
       <c r="B27" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C27" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="125" t="s">
+      <c r="D27" s="125" t="s">
         <v>149</v>
       </c>
-      <c r="D27" s="128" t="s">
+      <c r="E27" s="128" t="s">
         <v>150</v>
       </c>
-      <c r="E27" s="126">
+      <c r="F27" s="126">
         <v>41208</v>
       </c>
-      <c r="F27" s="126">
+      <c r="G27" s="126">
         <v>41348</v>
       </c>
-      <c r="G27" s="127">
+      <c r="H27" s="127">
         <f t="shared" si="1"/>
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="110" t="s">
         <v>153</v>
       </c>
       <c r="B28" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C28" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="C28" s="125" t="s">
+      <c r="D28" s="125" t="s">
         <v>151</v>
       </c>
-      <c r="D28" s="128" t="s">
+      <c r="E28" s="128" t="s">
         <v>152</v>
       </c>
-      <c r="E28" s="126">
+      <c r="F28" s="126">
         <v>40927</v>
       </c>
-      <c r="F28" s="126">
+      <c r="G28" s="126">
         <v>41012</v>
       </c>
-      <c r="G28" s="127">
+      <c r="H28" s="127">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="129" t="s">
         <v>154</v>
       </c>
       <c r="B29" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C29" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="C29" s="125" t="s">
+      <c r="D29" s="125" t="s">
         <v>143</v>
       </c>
-      <c r="D29" s="128" t="s">
+      <c r="E29" s="128" t="s">
         <v>155</v>
       </c>
-      <c r="E29" s="126">
+      <c r="F29" s="126">
         <v>41885</v>
       </c>
-      <c r="F29" s="126">
+      <c r="G29" s="126">
         <v>41996</v>
       </c>
-      <c r="G29" s="127">
+      <c r="H29" s="127">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="110" t="s">
         <v>156</v>
       </c>
       <c r="B30" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C30" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="C30" s="128" t="s">
+      <c r="D30" s="128" t="s">
         <v>157</v>
       </c>
-      <c r="D30" s="130" t="s">
+      <c r="E30" s="130" t="s">
         <v>158</v>
       </c>
-      <c r="E30" s="126">
+      <c r="F30" s="126">
         <v>40945</v>
       </c>
-      <c r="F30" s="126">
+      <c r="G30" s="126">
         <v>41093</v>
       </c>
-      <c r="G30" s="127">
+      <c r="H30" s="127">
         <f t="shared" si="1"/>
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="110" t="s">
         <v>159</v>
       </c>
       <c r="B31" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C31" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="C31" s="125" t="s">
+      <c r="D31" s="125" t="s">
         <v>160</v>
       </c>
-      <c r="D31" s="128" t="s">
+      <c r="E31" s="128" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="126">
+      <c r="F31" s="126">
         <v>41411</v>
       </c>
-      <c r="F31" s="126">
+      <c r="G31" s="126">
         <v>41666</v>
       </c>
-      <c r="G31" s="127">
+      <c r="H31" s="127">
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="110" t="s">
         <v>162</v>
       </c>
       <c r="B32" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C32" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="C32" s="125" t="s">
+      <c r="D32" s="125" t="s">
         <v>163</v>
       </c>
-      <c r="D32" s="128" t="s">
+      <c r="E32" s="128" t="s">
         <v>164</v>
       </c>
-      <c r="E32" s="126">
+      <c r="F32" s="126">
         <v>41905</v>
       </c>
-      <c r="F32" s="126">
+      <c r="G32" s="126">
         <v>41999</v>
       </c>
-      <c r="G32" s="127">
+      <c r="H32" s="127">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="110" t="s">
         <v>106</v>
       </c>
       <c r="B33" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C33" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="C33" s="99" t="s">
+      <c r="D33" s="99" t="s">
         <v>107</v>
       </c>
-      <c r="D33" s="101" t="s">
+      <c r="E33" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="E33" s="100">
+      <c r="F33" s="100">
         <v>42229</v>
       </c>
-      <c r="F33" s="100">
+      <c r="G33" s="100">
         <v>42354</v>
       </c>
-      <c r="G33" s="111">
+      <c r="H33" s="111">
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="133" t="s">
         <v>183</v>
       </c>
@@ -3924,13 +4031,14 @@
       <c r="C34" s="134"/>
       <c r="D34" s="134"/>
       <c r="E34" s="134"/>
-      <c r="F34" s="135"/>
-      <c r="G34" s="111">
-        <f>AVERAGE(G14:G33)</f>
+      <c r="F34" s="134"/>
+      <c r="G34" s="135"/>
+      <c r="H34" s="111">
+        <f>AVERAGE(H14:H33)</f>
         <v>174.95</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="99"/>
       <c r="B35" s="99"/>
       <c r="C35" s="99"/>
@@ -3938,9 +4046,10 @@
       <c r="E35" s="99"/>
       <c r="F35" s="99"/>
       <c r="G35" s="99"/>
-      <c r="H35" s="111"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H35" s="99"/>
+      <c r="I35" s="111"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="99"/>
       <c r="B36" s="99"/>
       <c r="C36" s="99"/>
@@ -3948,8 +4057,9 @@
       <c r="E36" s="99"/>
       <c r="F36" s="99"/>
       <c r="G36" s="99"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H36" s="99"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="99"/>
       <c r="B37" s="99"/>
       <c r="C37" s="99"/>
@@ -3957,8 +4067,9 @@
       <c r="E37" s="99"/>
       <c r="F37" s="99"/>
       <c r="G37" s="99"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H37" s="99"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="99"/>
       <c r="B38" s="99"/>
       <c r="C38" s="99"/>
@@ -3966,8 +4077,9 @@
       <c r="E38" s="99"/>
       <c r="F38" s="99"/>
       <c r="G38" s="99"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="99"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="99"/>
       <c r="B39" s="99"/>
       <c r="C39" s="99"/>
@@ -3975,8 +4087,9 @@
       <c r="E39" s="99"/>
       <c r="F39" s="99"/>
       <c r="G39" s="99"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H39" s="99"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="99"/>
       <c r="B40" s="99"/>
       <c r="C40" s="99"/>
@@ -3984,8 +4097,9 @@
       <c r="E40" s="99"/>
       <c r="F40" s="99"/>
       <c r="G40" s="99"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H40" s="99"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="99"/>
       <c r="B41" s="99"/>
       <c r="C41" s="99"/>
@@ -3993,8 +4107,9 @@
       <c r="E41" s="99"/>
       <c r="F41" s="99"/>
       <c r="G41" s="99"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H41" s="99"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="99"/>
       <c r="B42" s="99"/>
       <c r="C42" s="99"/>
@@ -4002,8 +4117,9 @@
       <c r="E42" s="99"/>
       <c r="F42" s="99"/>
       <c r="G42" s="99"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H42" s="99"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="99"/>
       <c r="B43" s="99"/>
       <c r="C43" s="99"/>
@@ -4011,8 +4127,9 @@
       <c r="E43" s="99"/>
       <c r="F43" s="99"/>
       <c r="G43" s="99"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H43" s="99"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="99"/>
       <c r="B44" s="99"/>
       <c r="C44" s="99"/>
@@ -4020,8 +4137,9 @@
       <c r="E44" s="99"/>
       <c r="F44" s="99"/>
       <c r="G44" s="99"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H44" s="99"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="99"/>
       <c r="B45" s="99"/>
       <c r="C45" s="99"/>
@@ -4029,8 +4147,9 @@
       <c r="E45" s="99"/>
       <c r="F45" s="99"/>
       <c r="G45" s="99"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H45" s="99"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="99"/>
       <c r="B46" s="99"/>
       <c r="C46" s="99"/>
@@ -4038,8 +4157,9 @@
       <c r="E46" s="99"/>
       <c r="F46" s="99"/>
       <c r="G46" s="99"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H46" s="99"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="99"/>
       <c r="B47" s="99"/>
       <c r="C47" s="99"/>
@@ -4047,8 +4167,9 @@
       <c r="E47" s="99"/>
       <c r="F47" s="99"/>
       <c r="G47" s="99"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H47" s="99"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="99"/>
       <c r="B48" s="99"/>
       <c r="C48" s="99"/>
@@ -4056,8 +4177,9 @@
       <c r="E48" s="99"/>
       <c r="F48" s="99"/>
       <c r="G48" s="99"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H48" s="99"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="99"/>
       <c r="B49" s="99"/>
       <c r="C49" s="99"/>
@@ -4065,8 +4187,9 @@
       <c r="E49" s="99"/>
       <c r="F49" s="99"/>
       <c r="G49" s="99"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H49" s="99"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="99"/>
       <c r="B50" s="99"/>
       <c r="C50" s="99"/>
@@ -4074,59 +4197,72 @@
       <c r="E50" s="99"/>
       <c r="F50" s="99"/>
       <c r="G50" s="99"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K58" s="102" t="s">
+      <c r="H50" s="99"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L58" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="L58" s="102">
+      <c r="M58" s="102">
         <v>1</v>
       </c>
-      <c r="M58" s="102">
-        <f>AVERAGEIF(K58:K62,K58,L58:L62)</f>
+      <c r="N58" s="102">
+        <f>AVERAGEIF(L58:L62,L58,M58:M62)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K59" s="102" t="s">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L59" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="L59" s="102">
+      <c r="M59" s="102">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K60" s="102" t="s">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L60" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="L60" s="102">
+      <c r="M60" s="102">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K61" s="102" t="s">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L61" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="L61" s="102">
+      <c r="M61" s="102">
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K62" s="102" t="s">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L62" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="L62" s="102">
+      <c r="M62" s="102">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="D13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'ÁREAS PADRÃO'!$A$1:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4:B33</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4134,8 +4270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J148"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4180,7 +4316,7 @@
         <v>112</v>
       </c>
       <c r="B4" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$33,A4,'Dados Historicos x Categoria'!$G$4:$G$33)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$C$4:$C$33,A4,'Dados Historicos x Categoria'!$H$4:$H$33)</f>
         <v>242</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -4195,7 +4331,7 @@
         <v>128</v>
       </c>
       <c r="B5" s="1">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$33,A5,'Dados Historicos x Categoria'!$G$4:$G$33)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$C$4:$C$33,A5,'Dados Historicos x Categoria'!$H$4:$H$33)</f>
         <v>103.6</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -4210,7 +4346,7 @@
         <v>142</v>
       </c>
       <c r="B6" s="79">
-        <f>AVERAGEIF('Dados Historicos x Categoria'!$B$4:$B$33,A6,'Dados Historicos x Categoria'!$G$4:$G$33)</f>
+        <f>AVERAGEIF('Dados Historicos x Categoria'!$C$4:$C$33,A6,'Dados Historicos x Categoria'!$H$4:$H$33)</f>
         <v>148.57142857142858</v>
       </c>
     </row>
@@ -5042,16 +5178,16 @@
       <c r="A2" s="139">
         <v>1</v>
       </c>
-      <c r="B2" s="141" t="s">
+      <c r="B2" s="149" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="141" t="s">
+      <c r="C2" s="149" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="141" t="s">
+      <c r="D2" s="149" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="141">
+      <c r="E2" s="149">
         <v>2</v>
       </c>
       <c r="F2" s="31" t="s">
@@ -5070,10 +5206,10 @@
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="140"/>
-      <c r="B3" s="141"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
+      <c r="B3" s="149"/>
+      <c r="C3" s="149"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="149"/>
       <c r="F3" s="31" t="s">
         <v>60</v>
       </c>
@@ -5089,16 +5225,16 @@
       <c r="J3" s="31"/>
     </row>
     <row r="4" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="141">
+      <c r="A4" s="149">
         <v>2</v>
       </c>
-      <c r="B4" s="148">
+      <c r="B4" s="150">
         <v>43042</v>
       </c>
-      <c r="C4" s="141" t="s">
+      <c r="C4" s="149" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="141" t="s">
+      <c r="D4" s="149" t="s">
         <v>53</v>
       </c>
       <c r="E4" s="139">
@@ -5139,10 +5275,10 @@
       <c r="J5" s="37"/>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="141">
+      <c r="A6" s="149">
         <v>3</v>
       </c>
-      <c r="B6" s="147">
+      <c r="B6" s="142">
         <v>42683</v>
       </c>
       <c r="C6" s="139" t="s">
@@ -5169,7 +5305,7 @@
       <c r="J6" s="31"/>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="141"/>
+      <c r="A7" s="149"/>
       <c r="B7" s="140"/>
       <c r="C7" s="140"/>
       <c r="D7" s="140"/>
@@ -5189,7 +5325,7 @@
       <c r="J7" s="31"/>
     </row>
     <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="141"/>
+      <c r="A8" s="149"/>
       <c r="B8" s="140"/>
       <c r="C8" s="140"/>
       <c r="D8" s="140"/>
@@ -5209,7 +5345,7 @@
       <c r="J8" s="53"/>
     </row>
     <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="141"/>
+      <c r="A9" s="149"/>
       <c r="B9" s="140"/>
       <c r="C9" s="140"/>
       <c r="D9" s="140"/>
@@ -5229,11 +5365,11 @@
       <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="141"/>
-      <c r="B10" s="146"/>
-      <c r="C10" s="146"/>
-      <c r="D10" s="146"/>
-      <c r="E10" s="146"/>
+      <c r="A10" s="149"/>
+      <c r="B10" s="141"/>
+      <c r="C10" s="141"/>
+      <c r="D10" s="141"/>
+      <c r="E10" s="141"/>
       <c r="F10" s="31" t="s">
         <v>70</v>
       </c>
@@ -5251,19 +5387,19 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="141">
+      <c r="A11" s="149">
         <v>4</v>
       </c>
-      <c r="B11" s="141" t="s">
+      <c r="B11" s="149" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="141" t="s">
+      <c r="C11" s="149" t="s">
         <v>115</v>
       </c>
-      <c r="D11" s="141" t="s">
+      <c r="D11" s="149" t="s">
         <v>116</v>
       </c>
-      <c r="E11" s="141">
+      <c r="E11" s="149">
         <v>2</v>
       </c>
       <c r="F11" s="53" t="s">
@@ -5281,11 +5417,11 @@
       <c r="J11" s="53"/>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="141"/>
-      <c r="B12" s="141"/>
-      <c r="C12" s="141"/>
-      <c r="D12" s="141"/>
-      <c r="E12" s="141"/>
+      <c r="A12" s="149"/>
+      <c r="B12" s="149"/>
+      <c r="C12" s="149"/>
+      <c r="D12" s="149"/>
+      <c r="E12" s="149"/>
       <c r="F12" s="55" t="s">
         <v>58</v>
       </c>
@@ -5324,7 +5460,7 @@
       <c r="A14" s="139">
         <v>5</v>
       </c>
-      <c r="B14" s="147">
+      <c r="B14" s="142">
         <v>42705</v>
       </c>
       <c r="C14" s="139"/>
@@ -5350,7 +5486,7 @@
     </row>
     <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A15" s="140"/>
-      <c r="B15" s="149"/>
+      <c r="B15" s="143"/>
       <c r="C15" s="140"/>
       <c r="D15" s="140"/>
       <c r="E15" s="140"/>
@@ -5370,9 +5506,9 @@
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="140"/>
-      <c r="B16" s="149"/>
+      <c r="B16" s="143"/>
       <c r="C16" s="140"/>
-      <c r="D16" s="146"/>
+      <c r="D16" s="141"/>
       <c r="E16" s="140"/>
       <c r="F16" s="71" t="s">
         <v>123</v>
@@ -5390,7 +5526,7 @@
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="140"/>
-      <c r="B17" s="149"/>
+      <c r="B17" s="143"/>
       <c r="C17" s="140"/>
       <c r="D17" s="67" t="s">
         <v>117</v>
@@ -5412,7 +5548,7 @@
     </row>
     <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="140"/>
-      <c r="B18" s="149"/>
+      <c r="B18" s="143"/>
       <c r="C18" s="140"/>
       <c r="D18" s="139" t="s">
         <v>118</v>
@@ -5433,20 +5569,20 @@
       <c r="J18" s="67"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="146"/>
-      <c r="B19" s="150"/>
-      <c r="C19" s="146"/>
-      <c r="D19" s="146"/>
-      <c r="E19" s="146"/>
+      <c r="A19" s="141"/>
+      <c r="B19" s="144"/>
+      <c r="C19" s="141"/>
+      <c r="D19" s="141"/>
+      <c r="E19" s="141"/>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="47">
         <v>6</v>
       </c>
-      <c r="B20" s="142">
+      <c r="B20" s="145">
         <v>42773</v>
       </c>
-      <c r="D20" s="144" t="s">
+      <c r="D20" s="147" t="s">
         <v>180</v>
       </c>
       <c r="F20" s="47" t="s">
@@ -5457,8 +5593,8 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="143"/>
-      <c r="D21" s="145"/>
+      <c r="B21" s="146"/>
+      <c r="D21" s="148"/>
       <c r="F21" s="47" t="s">
         <v>176</v>
       </c>
@@ -5470,8 +5606,8 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="143"/>
-      <c r="D22" s="145"/>
+      <c r="B22" s="146"/>
+      <c r="D22" s="148"/>
       <c r="F22" s="47" t="s">
         <v>178</v>
       </c>
@@ -5483,8 +5619,8 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B23" s="143"/>
-      <c r="D23" s="145"/>
+      <c r="B23" s="146"/>
+      <c r="D23" s="148"/>
       <c r="F23" s="47" t="s">
         <v>181</v>
       </c>
@@ -5512,11 +5648,13 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="D20:D23"/>
     <mergeCell ref="A14:A19"/>
@@ -5533,13 +5671,11 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="C11:C13"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C14:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6218,4 +6354,37 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="65.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Criada tabela com horas corrijida e adicionado arquivo do PowerBI
</commit_message>
<xml_diff>
--- a/TRE_Dados_MapaRaciocinio.xlsx
+++ b/TRE_Dados_MapaRaciocinio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Historicos x Categoria" sheetId="1" r:id="rId1"/>
@@ -1541,9 +1541,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1605,34 +1602,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1655,6 +1652,9 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1674,7 +1674,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1937,11 +1937,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="335196160"/>
-        <c:axId val="333043328"/>
+        <c:axId val="143599616"/>
+        <c:axId val="124591424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="335196160"/>
+        <c:axId val="143599616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1958,10 +1958,10 @@
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333043328"/>
+        <c:crossAx val="124591424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1969,7 +1969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="333043328"/>
+        <c:axId val="124591424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1980,7 +1980,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="335196160"/>
+        <c:crossAx val="143599616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2000,7 +2000,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2179,11 +2179,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="335199744"/>
-        <c:axId val="333045056"/>
+        <c:axId val="146435072"/>
+        <c:axId val="137745472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="335199744"/>
+        <c:axId val="146435072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2192,7 +2192,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="333045056"/>
+        <c:crossAx val="137745472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2200,7 +2200,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="333045056"/>
+        <c:axId val="137745472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2211,7 +2211,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="335199744"/>
+        <c:crossAx val="146435072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3120,35 +3120,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:H33"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.28515625" style="102" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" style="102" customWidth="1"/>
-    <col min="4" max="4" width="59.140625" style="102" customWidth="1"/>
-    <col min="5" max="5" width="53.140625" style="102" customWidth="1"/>
+    <col min="1" max="1" width="18.25" style="102" customWidth="1"/>
+    <col min="2" max="2" width="31" style="102" customWidth="1"/>
+    <col min="3" max="3" width="29.875" style="102" customWidth="1"/>
+    <col min="4" max="4" width="59.125" style="102" customWidth="1"/>
+    <col min="5" max="5" width="53.125" style="102" customWidth="1"/>
     <col min="6" max="6" width="15" style="102" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="102" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" style="102" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.125" style="102" customWidth="1"/>
+    <col min="8" max="8" width="25.375" style="102" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" style="102" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" style="102" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" style="102" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" style="102" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="102" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="102"/>
+    <col min="10" max="10" width="2.875" style="102" customWidth="1"/>
+    <col min="11" max="11" width="15.625" style="102" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.125" style="102" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.375" style="102" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.125" style="102"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
       <c r="E1" s="98" t="s">
         <v>9</v>
       </c>
@@ -3157,7 +3158,7 @@
       </c>
       <c r="G1" s="100">
         <f ca="1">TODAY()</f>
-        <v>42789</v>
+        <v>42801</v>
       </c>
       <c r="H1" s="101" t="s">
         <v>11</v>
@@ -3199,7 +3200,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="110" t="s">
         <v>74</v>
       </c>
@@ -3215,27 +3216,29 @@
       <c r="E4" s="101" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="100">
+      <c r="F4" s="157">
         <v>42311</v>
       </c>
-      <c r="G4" s="100">
+      <c r="G4" s="157">
         <v>42446</v>
       </c>
       <c r="H4" s="111">
-        <f t="shared" ref="H4:H12" si="0">DAYS360(F4,G4)</f>
+        <f t="shared" ref="H4:H14" si="0">DAYS360(F4,G4)</f>
         <v>134</v>
       </c>
-      <c r="I4" s="112"/>
+      <c r="I4" s="112">
+        <v>167</v>
+      </c>
       <c r="K4" s="113">
         <f>AVERAGE(H13,H34)</f>
-        <v>169.75277777777777</v>
+        <v>87.474999999999994</v>
       </c>
       <c r="L4" s="114">
         <v>0.15</v>
       </c>
       <c r="M4" s="99">
         <f>K4-(K4*L4)</f>
-        <v>144.28986111111109</v>
+        <v>74.353749999999991</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3254,10 +3257,10 @@
       <c r="E5" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="F5" s="100">
+      <c r="F5" s="157">
         <v>42118</v>
       </c>
-      <c r="G5" s="100">
+      <c r="G5" s="157">
         <v>42221</v>
       </c>
       <c r="H5" s="111">
@@ -3284,10 +3287,10 @@
       <c r="E6" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="F6" s="100">
+      <c r="F6" s="157">
         <v>42263</v>
       </c>
-      <c r="G6" s="100">
+      <c r="G6" s="157">
         <v>42342</v>
       </c>
       <c r="H6" s="111">
@@ -3314,10 +3317,10 @@
       <c r="E7" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="F7" s="100">
+      <c r="F7" s="157">
         <v>42633</v>
       </c>
-      <c r="G7" s="100">
+      <c r="G7" s="157">
         <v>42695</v>
       </c>
       <c r="H7" s="111">
@@ -3344,10 +3347,10 @@
       <c r="E8" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="100">
+      <c r="F8" s="157">
         <v>42422</v>
       </c>
-      <c r="G8" s="100">
+      <c r="G8" s="157">
         <v>42643</v>
       </c>
       <c r="H8" s="111">
@@ -3374,10 +3377,10 @@
       <c r="E9" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="F9" s="100">
+      <c r="F9" s="157">
         <v>41955</v>
       </c>
-      <c r="G9" s="100">
+      <c r="G9" s="157">
         <v>42179</v>
       </c>
       <c r="H9" s="111">
@@ -3402,10 +3405,10 @@
       <c r="E10" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="F10" s="100">
+      <c r="F10" s="157">
         <v>41738</v>
       </c>
-      <c r="G10" s="100">
+      <c r="G10" s="157">
         <v>41850</v>
       </c>
       <c r="H10" s="111">
@@ -3429,10 +3432,10 @@
       <c r="E11" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="100">
+      <c r="F11" s="157">
         <v>41337</v>
       </c>
-      <c r="G11" s="100">
+      <c r="G11" s="157">
         <v>41430</v>
       </c>
       <c r="H11" s="111">
@@ -3471,15 +3474,15 @@
       <c r="A13" s="119"/>
       <c r="B13" s="110"/>
       <c r="C13" s="120"/>
-      <c r="D13" s="134" t="s">
+      <c r="D13" s="133" t="s">
         <v>184</v>
       </c>
-      <c r="E13" s="134"/>
-      <c r="F13" s="134"/>
-      <c r="G13" s="135"/>
-      <c r="H13" s="121">
-        <f>AVERAGE(H4:H12)</f>
-        <v>164.55555555555554</v>
+      <c r="E13" s="133"/>
+      <c r="F13" s="133"/>
+      <c r="G13" s="134"/>
+      <c r="H13" s="111">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -3506,8 +3509,19 @@
         <v>42671</v>
       </c>
       <c r="H14" s="111">
-        <f t="shared" ref="H14:H33" si="1">DAYS360(F14,G14)</f>
+        <f t="shared" si="0"/>
         <v>642</v>
+      </c>
+      <c r="I14" s="102">
+        <v>689</v>
+      </c>
+      <c r="K14" s="112">
+        <f>I14-H14</f>
+        <v>47</v>
+      </c>
+      <c r="L14" s="102">
+        <f>K14*24</f>
+        <v>1128</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -3533,11 +3547,11 @@
         <v>42668</v>
       </c>
       <c r="H15" s="111">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H14:H33" si="1">DAYS360(F15,G15)</f>
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="110" t="s">
         <v>89</v>
       </c>
@@ -3664,7 +3678,7 @@
       <c r="F20" s="100">
         <v>42136</v>
       </c>
-      <c r="G20" s="122">
+      <c r="G20" s="121">
         <v>42171</v>
       </c>
       <c r="H20" s="111">
@@ -3672,7 +3686,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="110" t="s">
         <v>101</v>
       </c>
@@ -3699,7 +3713,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="110" t="s">
         <v>103</v>
       </c>
@@ -3709,7 +3723,7 @@
       <c r="C22" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="D22" s="123" t="s">
+      <c r="D22" s="122" t="s">
         <v>77</v>
       </c>
       <c r="E22" s="101" t="s">
@@ -3736,19 +3750,19 @@
       <c r="C23" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="124" t="s">
+      <c r="D23" s="123" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="125" t="s">
+      <c r="E23" s="124" t="s">
         <v>137</v>
       </c>
-      <c r="F23" s="126">
+      <c r="F23" s="125">
         <v>42580</v>
       </c>
-      <c r="G23" s="126">
+      <c r="G23" s="125">
         <v>42641</v>
       </c>
-      <c r="H23" s="127">
+      <c r="H23" s="126">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
@@ -3763,24 +3777,24 @@
       <c r="C24" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="D24" s="125" t="s">
+      <c r="D24" s="124" t="s">
         <v>140</v>
       </c>
-      <c r="E24" s="128" t="s">
+      <c r="E24" s="127" t="s">
         <v>139</v>
       </c>
-      <c r="F24" s="126">
+      <c r="F24" s="125">
         <v>42612</v>
       </c>
-      <c r="G24" s="126">
+      <c r="G24" s="125">
         <v>42704</v>
       </c>
-      <c r="H24" s="127">
+      <c r="H24" s="126">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="110" t="s">
         <v>141</v>
       </c>
@@ -3790,24 +3804,24 @@
       <c r="C25" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="D25" s="125" t="s">
+      <c r="D25" s="124" t="s">
         <v>143</v>
       </c>
-      <c r="E25" s="128" t="s">
+      <c r="E25" s="127" t="s">
         <v>144</v>
       </c>
-      <c r="F25" s="126">
+      <c r="F25" s="125">
         <v>42068</v>
       </c>
-      <c r="G25" s="126">
+      <c r="G25" s="125">
         <v>42149</v>
       </c>
-      <c r="H25" s="127">
+      <c r="H25" s="126">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="110" t="s">
         <v>145</v>
       </c>
@@ -3817,24 +3831,24 @@
       <c r="C26" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="D26" s="125" t="s">
+      <c r="D26" s="124" t="s">
         <v>146</v>
       </c>
-      <c r="E26" s="128" t="s">
+      <c r="E26" s="127" t="s">
         <v>147</v>
       </c>
-      <c r="F26" s="126">
+      <c r="F26" s="125">
         <v>42410</v>
       </c>
-      <c r="G26" s="126">
+      <c r="G26" s="125">
         <v>42690</v>
       </c>
-      <c r="H26" s="127">
+      <c r="H26" s="126">
         <f t="shared" si="1"/>
         <v>276</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="110" t="s">
         <v>148</v>
       </c>
@@ -3844,19 +3858,19 @@
       <c r="C27" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="D27" s="125" t="s">
+      <c r="D27" s="124" t="s">
         <v>149</v>
       </c>
-      <c r="E27" s="128" t="s">
+      <c r="E27" s="127" t="s">
         <v>150</v>
       </c>
-      <c r="F27" s="126">
+      <c r="F27" s="125">
         <v>41208</v>
       </c>
-      <c r="G27" s="126">
+      <c r="G27" s="125">
         <v>41348</v>
       </c>
-      <c r="H27" s="127">
+      <c r="H27" s="126">
         <f t="shared" si="1"/>
         <v>139</v>
       </c>
@@ -3871,25 +3885,25 @@
       <c r="C28" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="D28" s="125" t="s">
+      <c r="D28" s="124" t="s">
         <v>151</v>
       </c>
-      <c r="E28" s="128" t="s">
+      <c r="E28" s="127" t="s">
         <v>152</v>
       </c>
-      <c r="F28" s="126">
+      <c r="F28" s="125">
         <v>40927</v>
       </c>
-      <c r="G28" s="126">
+      <c r="G28" s="125">
         <v>41012</v>
       </c>
-      <c r="H28" s="127">
+      <c r="H28" s="126">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="129" t="s">
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="128" t="s">
         <v>154</v>
       </c>
       <c r="B29" s="110" t="s">
@@ -3898,19 +3912,19 @@
       <c r="C29" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="D29" s="125" t="s">
+      <c r="D29" s="124" t="s">
         <v>143</v>
       </c>
-      <c r="E29" s="128" t="s">
+      <c r="E29" s="127" t="s">
         <v>155</v>
       </c>
-      <c r="F29" s="126">
+      <c r="F29" s="125">
         <v>41885</v>
       </c>
-      <c r="G29" s="126">
+      <c r="G29" s="125">
         <v>41996</v>
       </c>
-      <c r="H29" s="127">
+      <c r="H29" s="126">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
@@ -3925,19 +3939,19 @@
       <c r="C30" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="D30" s="128" t="s">
+      <c r="D30" s="127" t="s">
         <v>157</v>
       </c>
-      <c r="E30" s="130" t="s">
+      <c r="E30" s="129" t="s">
         <v>158</v>
       </c>
-      <c r="F30" s="126">
+      <c r="F30" s="125">
         <v>40945</v>
       </c>
-      <c r="G30" s="126">
+      <c r="G30" s="125">
         <v>41093</v>
       </c>
-      <c r="H30" s="127">
+      <c r="H30" s="126">
         <f t="shared" si="1"/>
         <v>147</v>
       </c>
@@ -3952,19 +3966,19 @@
       <c r="C31" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="D31" s="125" t="s">
+      <c r="D31" s="124" t="s">
         <v>160</v>
       </c>
-      <c r="E31" s="128" t="s">
+      <c r="E31" s="127" t="s">
         <v>161</v>
       </c>
-      <c r="F31" s="126">
+      <c r="F31" s="125">
         <v>41411</v>
       </c>
-      <c r="G31" s="126">
+      <c r="G31" s="125">
         <v>41666</v>
       </c>
-      <c r="H31" s="127">
+      <c r="H31" s="126">
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
@@ -3979,24 +3993,24 @@
       <c r="C32" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="D32" s="125" t="s">
+      <c r="D32" s="124" t="s">
         <v>163</v>
       </c>
-      <c r="E32" s="128" t="s">
+      <c r="E32" s="127" t="s">
         <v>164</v>
       </c>
-      <c r="F32" s="126">
+      <c r="F32" s="125">
         <v>41905</v>
       </c>
-      <c r="G32" s="126">
+      <c r="G32" s="125">
         <v>41999</v>
       </c>
-      <c r="H32" s="127">
+      <c r="H32" s="126">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="110" t="s">
         <v>106</v>
       </c>
@@ -4024,15 +4038,15 @@
       </c>
     </row>
     <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="133" t="s">
+      <c r="A34" s="132" t="s">
         <v>183</v>
       </c>
-      <c r="B34" s="134"/>
-      <c r="C34" s="134"/>
-      <c r="D34" s="134"/>
-      <c r="E34" s="134"/>
-      <c r="F34" s="134"/>
-      <c r="G34" s="135"/>
+      <c r="B34" s="133"/>
+      <c r="C34" s="133"/>
+      <c r="D34" s="133"/>
+      <c r="E34" s="133"/>
+      <c r="F34" s="133"/>
+      <c r="G34" s="134"/>
       <c r="H34" s="111">
         <f>AVERAGE(H14:H33)</f>
         <v>174.95</v>
@@ -4270,19 +4284,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J148"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" customWidth="1"/>
+    <col min="1" max="1" width="43.25" customWidth="1"/>
+    <col min="2" max="2" width="46.375" customWidth="1"/>
+    <col min="3" max="3" width="13.125" customWidth="1"/>
+    <col min="4" max="4" width="37.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -4376,104 +4390,104 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="136" t="s">
+      <c r="C17" s="135" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="137"/>
-      <c r="E17" s="137"/>
-      <c r="F17" s="137"/>
-      <c r="G17" s="137"/>
+      <c r="D17" s="136"/>
+      <c r="E17" s="136"/>
+      <c r="F17" s="136"/>
+      <c r="G17" s="136"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="138"/>
-      <c r="D18" s="138"/>
-      <c r="E18" s="138"/>
-      <c r="F18" s="138"/>
-      <c r="G18" s="138"/>
+      <c r="C18" s="137"/>
+      <c r="D18" s="137"/>
+      <c r="E18" s="137"/>
+      <c r="F18" s="137"/>
+      <c r="G18" s="137"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="138"/>
-      <c r="D19" s="138"/>
-      <c r="E19" s="138"/>
-      <c r="F19" s="138"/>
-      <c r="G19" s="138"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="137"/>
+      <c r="E19" s="137"/>
+      <c r="F19" s="137"/>
+      <c r="G19" s="137"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="138"/>
-      <c r="D20" s="138"/>
-      <c r="E20" s="138"/>
-      <c r="F20" s="138"/>
-      <c r="G20" s="138"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="137"/>
+      <c r="E20" s="137"/>
+      <c r="F20" s="137"/>
+      <c r="G20" s="137"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="138"/>
-      <c r="D21" s="138"/>
-      <c r="E21" s="138"/>
-      <c r="F21" s="138"/>
-      <c r="G21" s="138"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="137"/>
+      <c r="E21" s="137"/>
+      <c r="F21" s="137"/>
+      <c r="G21" s="137"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="138"/>
-      <c r="D22" s="138"/>
-      <c r="E22" s="138"/>
-      <c r="F22" s="138"/>
-      <c r="G22" s="138"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="137"/>
+      <c r="E22" s="137"/>
+      <c r="F22" s="137"/>
+      <c r="G22" s="137"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="138"/>
-      <c r="D23" s="138"/>
-      <c r="E23" s="138"/>
-      <c r="F23" s="138"/>
-      <c r="G23" s="138"/>
+      <c r="C23" s="137"/>
+      <c r="D23" s="137"/>
+      <c r="E23" s="137"/>
+      <c r="F23" s="137"/>
+      <c r="G23" s="137"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="138"/>
-      <c r="D24" s="138"/>
-      <c r="E24" s="138"/>
-      <c r="F24" s="138"/>
-      <c r="G24" s="138"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="137"/>
+      <c r="E24" s="137"/>
+      <c r="F24" s="137"/>
+      <c r="G24" s="137"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="138"/>
-      <c r="D25" s="138"/>
-      <c r="E25" s="138"/>
-      <c r="F25" s="138"/>
-      <c r="G25" s="138"/>
+      <c r="C25" s="137"/>
+      <c r="D25" s="137"/>
+      <c r="E25" s="137"/>
+      <c r="F25" s="137"/>
+      <c r="G25" s="137"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="138"/>
-      <c r="D26" s="138"/>
-      <c r="E26" s="138"/>
-      <c r="F26" s="138"/>
-      <c r="G26" s="138"/>
+      <c r="C26" s="137"/>
+      <c r="D26" s="137"/>
+      <c r="E26" s="137"/>
+      <c r="F26" s="137"/>
+      <c r="G26" s="137"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="138"/>
-      <c r="D27" s="138"/>
-      <c r="E27" s="138"/>
-      <c r="F27" s="138"/>
-      <c r="G27" s="138"/>
+      <c r="C27" s="137"/>
+      <c r="D27" s="137"/>
+      <c r="E27" s="137"/>
+      <c r="F27" s="137"/>
+      <c r="G27" s="137"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="138"/>
-      <c r="D28" s="138"/>
-      <c r="E28" s="138"/>
-      <c r="F28" s="138"/>
-      <c r="G28" s="138"/>
+      <c r="C28" s="137"/>
+      <c r="D28" s="137"/>
+      <c r="E28" s="137"/>
+      <c r="F28" s="137"/>
+      <c r="G28" s="137"/>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="138"/>
-      <c r="D29" s="138"/>
-      <c r="E29" s="138"/>
-      <c r="F29" s="138"/>
-      <c r="G29" s="138"/>
+      <c r="C29" s="137"/>
+      <c r="D29" s="137"/>
+      <c r="E29" s="137"/>
+      <c r="F29" s="137"/>
+      <c r="G29" s="137"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="138"/>
-      <c r="D30" s="138"/>
-      <c r="E30" s="138"/>
-      <c r="F30" s="138"/>
-      <c r="G30" s="138"/>
+      <c r="C30" s="137"/>
+      <c r="D30" s="137"/>
+      <c r="E30" s="137"/>
+      <c r="F30" s="137"/>
+      <c r="G30" s="137"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="83" t="s">
@@ -5130,16 +5144,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="47"/>
-    <col min="2" max="2" width="15.5703125" style="47" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="47" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="47" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="47"/>
-    <col min="6" max="6" width="29.42578125" style="47" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="47" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="47" customWidth="1"/>
+    <col min="1" max="1" width="9.125" style="47"/>
+    <col min="2" max="2" width="15.625" style="47" customWidth="1"/>
+    <col min="3" max="3" width="17.875" style="47" customWidth="1"/>
+    <col min="4" max="4" width="25.875" style="47" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="47"/>
+    <col min="6" max="6" width="29.375" style="47" customWidth="1"/>
+    <col min="7" max="7" width="31.75" style="47" customWidth="1"/>
+    <col min="8" max="8" width="14.75" style="47" customWidth="1"/>
     <col min="9" max="9" width="12" style="47" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" style="47" customWidth="1"/>
+    <col min="10" max="10" width="27.375" style="47" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -5175,19 +5189,19 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="45" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="139">
+      <c r="A2" s="138">
         <v>1</v>
       </c>
-      <c r="B2" s="149" t="s">
+      <c r="B2" s="140" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="140" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="149" t="s">
+      <c r="D2" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="149">
+      <c r="E2" s="140">
         <v>2</v>
       </c>
       <c r="F2" s="31" t="s">
@@ -5204,12 +5218,12 @@
       </c>
       <c r="J2" s="31"/>
     </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="140"/>
-      <c r="B3" s="149"/>
-      <c r="C3" s="149"/>
-      <c r="D3" s="149"/>
-      <c r="E3" s="149"/>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="139"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
       <c r="F3" s="31" t="s">
         <v>60</v>
       </c>
@@ -5225,19 +5239,19 @@
       <c r="J3" s="31"/>
     </row>
     <row r="4" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="149">
+      <c r="A4" s="140">
         <v>2</v>
       </c>
-      <c r="B4" s="150">
+      <c r="B4" s="147">
         <v>43042</v>
       </c>
-      <c r="C4" s="149" t="s">
+      <c r="C4" s="140" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="149" t="s">
+      <c r="D4" s="140" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="139">
+      <c r="E4" s="138">
         <v>2</v>
       </c>
       <c r="F4" s="31" t="s">
@@ -5254,12 +5268,12 @@
       </c>
       <c r="J4" s="31"/>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="139"/>
-      <c r="B5" s="139"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="140"/>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="138"/>
+      <c r="B5" s="138"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="139"/>
       <c r="F5" s="37" t="s">
         <v>54</v>
       </c>
@@ -5274,20 +5288,20 @@
       </c>
       <c r="J5" s="37"/>
     </row>
-    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="149">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="140">
         <v>3</v>
       </c>
-      <c r="B6" s="142">
+      <c r="B6" s="146">
         <v>42683</v>
       </c>
-      <c r="C6" s="139" t="s">
+      <c r="C6" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="139" t="s">
+      <c r="D6" s="138" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="139">
+      <c r="E6" s="138">
         <v>2</v>
       </c>
       <c r="F6" s="31" t="s">
@@ -5305,11 +5319,11 @@
       <c r="J6" s="31"/>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="149"/>
-      <c r="B7" s="140"/>
-      <c r="C7" s="140"/>
-      <c r="D7" s="140"/>
-      <c r="E7" s="140"/>
+      <c r="A7" s="140"/>
+      <c r="B7" s="139"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
       <c r="F7" s="55" t="s">
         <v>67</v>
       </c>
@@ -5324,12 +5338,12 @@
       </c>
       <c r="J7" s="31"/>
     </row>
-    <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="149"/>
-      <c r="B8" s="140"/>
-      <c r="C8" s="140"/>
-      <c r="D8" s="140"/>
-      <c r="E8" s="140"/>
+    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="140"/>
+      <c r="B8" s="139"/>
+      <c r="C8" s="139"/>
+      <c r="D8" s="139"/>
+      <c r="E8" s="139"/>
       <c r="F8" s="53" t="s">
         <v>69</v>
       </c>
@@ -5344,12 +5358,12 @@
       </c>
       <c r="J8" s="53"/>
     </row>
-    <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="149"/>
-      <c r="B9" s="140"/>
-      <c r="C9" s="140"/>
-      <c r="D9" s="140"/>
-      <c r="E9" s="140"/>
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="140"/>
+      <c r="B9" s="139"/>
+      <c r="C9" s="139"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="139"/>
       <c r="F9" s="53" t="s">
         <v>73</v>
       </c>
@@ -5365,11 +5379,11 @@
       <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="149"/>
-      <c r="B10" s="141"/>
-      <c r="C10" s="141"/>
-      <c r="D10" s="141"/>
-      <c r="E10" s="141"/>
+      <c r="A10" s="140"/>
+      <c r="B10" s="145"/>
+      <c r="C10" s="145"/>
+      <c r="D10" s="145"/>
+      <c r="E10" s="145"/>
       <c r="F10" s="31" t="s">
         <v>70</v>
       </c>
@@ -5386,20 +5400,20 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="149">
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="140">
         <v>4</v>
       </c>
-      <c r="B11" s="149" t="s">
+      <c r="B11" s="140" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="149" t="s">
+      <c r="C11" s="140" t="s">
         <v>115</v>
       </c>
-      <c r="D11" s="149" t="s">
+      <c r="D11" s="140" t="s">
         <v>116</v>
       </c>
-      <c r="E11" s="149">
+      <c r="E11" s="140">
         <v>2</v>
       </c>
       <c r="F11" s="53" t="s">
@@ -5416,12 +5430,12 @@
       </c>
       <c r="J11" s="53"/>
     </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="149"/>
-      <c r="B12" s="149"/>
-      <c r="C12" s="149"/>
-      <c r="D12" s="149"/>
-      <c r="E12" s="149"/>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="140"/>
+      <c r="B12" s="140"/>
+      <c r="C12" s="140"/>
+      <c r="D12" s="140"/>
+      <c r="E12" s="140"/>
       <c r="F12" s="55" t="s">
         <v>58</v>
       </c>
@@ -5436,12 +5450,12 @@
       </c>
       <c r="J12" s="53"/>
     </row>
-    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="139"/>
-      <c r="B13" s="139"/>
-      <c r="C13" s="139"/>
-      <c r="D13" s="139"/>
-      <c r="E13" s="139"/>
+    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="138"/>
+      <c r="B13" s="138"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="138"/>
+      <c r="E13" s="138"/>
       <c r="F13" s="70" t="s">
         <v>72</v>
       </c>
@@ -5457,17 +5471,17 @@
       <c r="J13" s="66"/>
     </row>
     <row r="14" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="139">
+      <c r="A14" s="138">
         <v>5</v>
       </c>
-      <c r="B14" s="142">
+      <c r="B14" s="146">
         <v>42705</v>
       </c>
-      <c r="C14" s="139"/>
-      <c r="D14" s="139" t="s">
+      <c r="C14" s="138"/>
+      <c r="D14" s="138" t="s">
         <v>116</v>
       </c>
-      <c r="E14" s="139">
+      <c r="E14" s="138">
         <v>2</v>
       </c>
       <c r="F14" s="71" t="s">
@@ -5484,12 +5498,12 @@
       </c>
       <c r="J14" s="67"/>
     </row>
-    <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A15" s="140"/>
-      <c r="B15" s="143"/>
-      <c r="C15" s="140"/>
-      <c r="D15" s="140"/>
-      <c r="E15" s="140"/>
+    <row r="15" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="139"/>
+      <c r="B15" s="148"/>
+      <c r="C15" s="139"/>
+      <c r="D15" s="139"/>
+      <c r="E15" s="139"/>
       <c r="F15" s="71" t="s">
         <v>121</v>
       </c>
@@ -5505,11 +5519,11 @@
       <c r="J15" s="67"/>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="140"/>
-      <c r="B16" s="143"/>
-      <c r="C16" s="140"/>
-      <c r="D16" s="141"/>
-      <c r="E16" s="140"/>
+      <c r="A16" s="139"/>
+      <c r="B16" s="148"/>
+      <c r="C16" s="139"/>
+      <c r="D16" s="145"/>
+      <c r="E16" s="139"/>
       <c r="F16" s="71" t="s">
         <v>123</v>
       </c>
@@ -5525,13 +5539,13 @@
       <c r="J16" s="67"/>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="140"/>
-      <c r="B17" s="143"/>
-      <c r="C17" s="140"/>
+      <c r="A17" s="139"/>
+      <c r="B17" s="148"/>
+      <c r="C17" s="139"/>
       <c r="D17" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="140"/>
+      <c r="E17" s="139"/>
       <c r="F17" s="71" t="s">
         <v>124</v>
       </c>
@@ -5547,13 +5561,13 @@
       <c r="J17" s="67"/>
     </row>
     <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="140"/>
-      <c r="B18" s="143"/>
-      <c r="C18" s="140"/>
-      <c r="D18" s="139" t="s">
+      <c r="A18" s="139"/>
+      <c r="B18" s="148"/>
+      <c r="C18" s="139"/>
+      <c r="D18" s="138" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="140"/>
+      <c r="E18" s="139"/>
       <c r="F18" s="71" t="s">
         <v>126</v>
       </c>
@@ -5569,20 +5583,20 @@
       <c r="J18" s="67"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="141"/>
-      <c r="B19" s="144"/>
-      <c r="C19" s="141"/>
-      <c r="D19" s="141"/>
-      <c r="E19" s="141"/>
+      <c r="A19" s="145"/>
+      <c r="B19" s="149"/>
+      <c r="C19" s="145"/>
+      <c r="D19" s="145"/>
+      <c r="E19" s="145"/>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="47">
         <v>6</v>
       </c>
-      <c r="B20" s="145">
+      <c r="B20" s="141">
         <v>42773</v>
       </c>
-      <c r="D20" s="147" t="s">
+      <c r="D20" s="143" t="s">
         <v>180</v>
       </c>
       <c r="F20" s="47" t="s">
@@ -5593,8 +5607,8 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="146"/>
-      <c r="D21" s="148"/>
+      <c r="B21" s="142"/>
+      <c r="D21" s="144"/>
       <c r="F21" s="47" t="s">
         <v>176</v>
       </c>
@@ -5606,8 +5620,8 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="146"/>
-      <c r="D22" s="148"/>
+      <c r="B22" s="142"/>
+      <c r="D22" s="144"/>
       <c r="F22" s="47" t="s">
         <v>178</v>
       </c>
@@ -5618,9 +5632,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B23" s="146"/>
-      <c r="D23" s="148"/>
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B23" s="142"/>
+      <c r="D23" s="144"/>
       <c r="F23" s="47" t="s">
         <v>181</v>
       </c>
@@ -5629,17 +5643,17 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F25" s="131" t="s">
+      <c r="F25" s="130" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F26" s="131" t="s">
+      <c r="F26" s="130" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F27" s="131" t="s">
+      <c r="F27" s="130" t="s">
         <v>189</v>
       </c>
     </row>
@@ -5648,13 +5662,11 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C14:C19"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="D20:D23"/>
     <mergeCell ref="A14:A19"/>
@@ -5671,11 +5683,13 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="C11:C13"/>
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5692,13 +5706,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.25" customWidth="1"/>
+    <col min="3" max="3" width="29.875" customWidth="1"/>
+    <col min="4" max="4" width="24.875" customWidth="1"/>
+    <col min="5" max="5" width="19.25" customWidth="1"/>
+    <col min="6" max="6" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5729,7 +5743,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
@@ -5819,7 +5833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="61" t="s">
         <v>85</v>
       </c>
@@ -5859,24 +5873,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="153" t="s">
+      <c r="B1" s="152" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="155" t="s">
+      <c r="C1" s="154" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="156"/>
-      <c r="E1" s="156" t="s">
+      <c r="D1" s="155"/>
+      <c r="E1" s="155" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="157"/>
+      <c r="F1" s="156"/>
       <c r="G1" s="15" t="s">
         <v>35</v>
       </c>
@@ -5895,9 +5909,9 @@
       <c r="T1" s="16"/>
       <c r="U1" s="16"/>
     </row>
-    <row r="2" spans="1:21" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="152"/>
-      <c r="B2" s="154"/>
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="151"/>
+      <c r="B2" s="153"/>
       <c r="C2" s="17" t="s">
         <v>36</v>
       </c>
@@ -6366,7 +6380,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.5703125" customWidth="1"/>
+    <col min="1" max="1" width="65.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adicionado items pendentes na ATA de Reuniao. Novo arquivo com Somatorio sem ROUND, e registros revisados para o BD.
</commit_message>
<xml_diff>
--- a/TRE_Dados_MapaRaciocinio.xlsx
+++ b/TRE_Dados_MapaRaciocinio.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Historicos x Categoria" sheetId="1" r:id="rId1"/>
@@ -14,17 +14,17 @@
     <sheet name="Controle do Projeto" sheetId="6" r:id="rId5"/>
     <sheet name="ÁREAS PADRÃO" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -34,7 +34,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Autor:
+          <t xml:space="preserve">Author:
 </t>
         </r>
       </text>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="194">
   <si>
     <t>Categoria</t>
   </si>
@@ -601,9 +601,6 @@
     <t>A3 - Contendo , objetivo do Projeto , histórico do projeto, lead time do processo inteiro(Pareto)</t>
   </si>
   <si>
-    <t>Ruhan, Ivis e Ruhan</t>
-  </si>
-  <si>
     <t>MÉDIA SECRETARIA DE GESTÃO DE SERVIÇOS</t>
   </si>
   <si>
@@ -622,15 +619,6 @@
     <t>Média para Secretaria de Gestão de Serviços e Coordenadoria de Infraestrutura Predial</t>
   </si>
   <si>
-    <t>* Criar comparativo entre PADS sem estudo preliminar e os novos que serao coletados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Siglas antigas x atualizada </t>
-  </si>
-  <si>
-    <t>* PAD com estudos preliminares para atualizar média</t>
-  </si>
-  <si>
     <t>ÁREA RESPONSÁVEL</t>
   </si>
   <si>
@@ -641,6 +629,43 @@
   </si>
   <si>
     <t>Coordenadoria de Segurança , Transporte e Apoio Administrativo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - Conferir todos os SOMATORIOS de DIAS de TODOS os Setores Relevantes. (Através da Planilha de Banco de Dados)
+- Fazer um paralelo lado a lado mostrando os valores da planilha antiga e do calculo novo(Banco de dados) [DIAS EM DECIMAIS e tambem SOMATORIO DE HORAS]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PROBLEMAS:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Setores relevantes Duplicados no BD - Descobrir o porque.
+- Porque a média está com uma disparidade tao grande.
+(Ex. 
+CIP na xls antiga  = 14 dias
+CIP na xls nova(BD)= 4,63
+)</t>
+    </r>
+  </si>
+  <si>
+    <t>Ruhan, Ivis e André</t>
   </si>
 </sst>
 </file>
@@ -1222,7 +1247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1571,6 +1596,12 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1602,34 +1633,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1653,8 +1684,8 @@
     <xf numFmtId="165" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1667,6 +1698,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1674,7 +1708,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1937,11 +1971,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="143599616"/>
-        <c:axId val="124591424"/>
+        <c:axId val="303548032"/>
+        <c:axId val="303546856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="143599616"/>
+        <c:axId val="303548032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1961,7 +1995,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124591424"/>
+        <c:crossAx val="303546856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1969,7 +2003,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124591424"/>
+        <c:axId val="303546856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1980,7 +2014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143599616"/>
+        <c:crossAx val="303548032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2000,7 +2034,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2032,7 +2066,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2130,6 +2163,13 @@
             </c:spPr>
           </c:dPt>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
@@ -2138,6 +2178,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2179,20 +2224,21 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="146435072"/>
-        <c:axId val="137745472"/>
+        <c:axId val="174686384"/>
+        <c:axId val="174686776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146435072"/>
+        <c:axId val="174686384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137745472"/>
+        <c:crossAx val="174686776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2200,7 +2246,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137745472"/>
+        <c:axId val="174686776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2211,14 +2257,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146435072"/>
+        <c:crossAx val="174686384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2832,9 +2877,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2872,9 +2917,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2909,7 +2954,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2944,7 +2989,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3120,36 +3165,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.25" style="102" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="102" customWidth="1"/>
     <col min="2" max="2" width="31" style="102" customWidth="1"/>
-    <col min="3" max="3" width="29.875" style="102" customWidth="1"/>
-    <col min="4" max="4" width="59.125" style="102" customWidth="1"/>
-    <col min="5" max="5" width="53.125" style="102" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="102" customWidth="1"/>
+    <col min="4" max="4" width="59.140625" style="102" customWidth="1"/>
+    <col min="5" max="5" width="53.140625" style="102" customWidth="1"/>
     <col min="6" max="6" width="15" style="102" customWidth="1"/>
-    <col min="7" max="7" width="15.125" style="102" customWidth="1"/>
-    <col min="8" max="8" width="25.375" style="102" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="102" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" style="102" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" style="102" customWidth="1"/>
-    <col min="10" max="10" width="2.875" style="102" customWidth="1"/>
-    <col min="11" max="11" width="15.625" style="102" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.125" style="102" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.375" style="102" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.125" style="102"/>
+    <col min="10" max="10" width="2.85546875" style="102" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="102" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="102" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="102" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="102"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
       <c r="E1" s="98" t="s">
         <v>9</v>
       </c>
@@ -3158,7 +3203,7 @@
       </c>
       <c r="G1" s="100">
         <f ca="1">TODAY()</f>
-        <v>42801</v>
+        <v>42807</v>
       </c>
       <c r="H1" s="101" t="s">
         <v>11</v>
@@ -3170,7 +3215,7 @@
         <v>63</v>
       </c>
       <c r="B3" s="103" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C3" s="103" t="s">
         <v>113</v>
@@ -3200,12 +3245,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="110" t="s">
         <v>74</v>
       </c>
       <c r="B4" s="110" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C4" s="110" t="s">
         <v>112</v>
@@ -3216,10 +3261,10 @@
       <c r="E4" s="101" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="157">
+      <c r="F4" s="132">
         <v>42311</v>
       </c>
-      <c r="G4" s="157">
+      <c r="G4" s="132">
         <v>42446</v>
       </c>
       <c r="H4" s="111">
@@ -3246,7 +3291,7 @@
         <v>127</v>
       </c>
       <c r="B5" s="110" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C5" s="110" t="s">
         <v>128</v>
@@ -3257,10 +3302,10 @@
       <c r="E5" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="F5" s="157">
+      <c r="F5" s="132">
         <v>42118</v>
       </c>
-      <c r="G5" s="157">
+      <c r="G5" s="132">
         <v>42221</v>
       </c>
       <c r="H5" s="111">
@@ -3276,7 +3321,7 @@
         <v>130</v>
       </c>
       <c r="B6" s="110" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C6" s="110" t="s">
         <v>128</v>
@@ -3287,10 +3332,10 @@
       <c r="E6" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="F6" s="157">
+      <c r="F6" s="132">
         <v>42263</v>
       </c>
-      <c r="G6" s="157">
+      <c r="G6" s="132">
         <v>42342</v>
       </c>
       <c r="H6" s="111">
@@ -3306,7 +3351,7 @@
         <v>132</v>
       </c>
       <c r="B7" s="110" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C7" s="110" t="s">
         <v>128</v>
@@ -3317,10 +3362,10 @@
       <c r="E7" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="F7" s="157">
+      <c r="F7" s="132">
         <v>42633</v>
       </c>
-      <c r="G7" s="157">
+      <c r="G7" s="132">
         <v>42695</v>
       </c>
       <c r="H7" s="111">
@@ -3336,7 +3381,7 @@
         <v>133</v>
       </c>
       <c r="B8" s="110" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C8" s="110" t="s">
         <v>128</v>
@@ -3347,10 +3392,10 @@
       <c r="E8" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="157">
+      <c r="F8" s="132">
         <v>42422</v>
       </c>
-      <c r="G8" s="157">
+      <c r="G8" s="132">
         <v>42643</v>
       </c>
       <c r="H8" s="111">
@@ -3366,7 +3411,7 @@
         <v>134</v>
       </c>
       <c r="B9" s="110" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C9" s="110" t="s">
         <v>128</v>
@@ -3377,10 +3422,10 @@
       <c r="E9" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="F9" s="157">
+      <c r="F9" s="132">
         <v>41955</v>
       </c>
-      <c r="G9" s="157">
+      <c r="G9" s="132">
         <v>42179</v>
       </c>
       <c r="H9" s="111">
@@ -3394,7 +3439,7 @@
         <v>135</v>
       </c>
       <c r="B10" s="110" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C10" s="110" t="s">
         <v>128</v>
@@ -3405,10 +3450,10 @@
       <c r="E10" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="F10" s="157">
+      <c r="F10" s="132">
         <v>41738</v>
       </c>
-      <c r="G10" s="157">
+      <c r="G10" s="132">
         <v>41850</v>
       </c>
       <c r="H10" s="111">
@@ -3421,7 +3466,7 @@
         <v>80</v>
       </c>
       <c r="B11" s="110" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C11" s="110" t="s">
         <v>112</v>
@@ -3432,10 +3477,10 @@
       <c r="E11" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="157">
+      <c r="F11" s="132">
         <v>41337</v>
       </c>
-      <c r="G11" s="157">
+      <c r="G11" s="132">
         <v>41430</v>
       </c>
       <c r="H11" s="111">
@@ -3448,7 +3493,7 @@
         <v>82</v>
       </c>
       <c r="B12" s="110" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C12" s="110" t="s">
         <v>112</v>
@@ -3474,12 +3519,12 @@
       <c r="A13" s="119"/>
       <c r="B13" s="110"/>
       <c r="C13" s="120"/>
-      <c r="D13" s="133" t="s">
-        <v>184</v>
-      </c>
-      <c r="E13" s="133"/>
-      <c r="F13" s="133"/>
-      <c r="G13" s="134"/>
+      <c r="D13" s="135" t="s">
+        <v>183</v>
+      </c>
+      <c r="E13" s="135"/>
+      <c r="F13" s="135"/>
+      <c r="G13" s="136"/>
       <c r="H13" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3490,7 +3535,7 @@
         <v>85</v>
       </c>
       <c r="B14" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C14" s="110" t="s">
         <v>112</v>
@@ -3529,7 +3574,7 @@
         <v>88</v>
       </c>
       <c r="B15" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C15" s="110" t="s">
         <v>112</v>
@@ -3547,16 +3592,16 @@
         <v>42668</v>
       </c>
       <c r="H15" s="111">
-        <f t="shared" ref="H14:H33" si="1">DAYS360(F15,G15)</f>
+        <f t="shared" ref="H15:H33" si="1">DAYS360(F15,G15)</f>
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="110" t="s">
         <v>89</v>
       </c>
       <c r="B16" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C16" s="110" t="s">
         <v>112</v>
@@ -3583,7 +3628,7 @@
         <v>92</v>
       </c>
       <c r="B17" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C17" s="110" t="s">
         <v>112</v>
@@ -3610,7 +3655,7 @@
         <v>94</v>
       </c>
       <c r="B18" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C18" s="110" t="s">
         <v>112</v>
@@ -3637,7 +3682,7 @@
         <v>96</v>
       </c>
       <c r="B19" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C19" s="110" t="s">
         <v>112</v>
@@ -3664,7 +3709,7 @@
         <v>99</v>
       </c>
       <c r="B20" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C20" s="110" t="s">
         <v>128</v>
@@ -3686,12 +3731,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="110" t="s">
         <v>101</v>
       </c>
       <c r="B21" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C21" s="110" t="s">
         <v>112</v>
@@ -3713,12 +3758,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="110" t="s">
         <v>103</v>
       </c>
       <c r="B22" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C22" s="110" t="s">
         <v>128</v>
@@ -3745,7 +3790,7 @@
         <v>136</v>
       </c>
       <c r="B23" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C23" s="110" t="s">
         <v>128</v>
@@ -3772,7 +3817,7 @@
         <v>138</v>
       </c>
       <c r="B24" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C24" s="110" t="s">
         <v>128</v>
@@ -3794,12 +3839,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="110" t="s">
         <v>141</v>
       </c>
       <c r="B25" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C25" s="110" t="s">
         <v>142</v>
@@ -3821,12 +3866,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="110" t="s">
         <v>145</v>
       </c>
       <c r="B26" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C26" s="110" t="s">
         <v>142</v>
@@ -3848,12 +3893,12 @@
         <v>276</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="110" t="s">
         <v>148</v>
       </c>
       <c r="B27" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C27" s="110" t="s">
         <v>112</v>
@@ -3880,7 +3925,7 @@
         <v>153</v>
       </c>
       <c r="B28" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C28" s="110" t="s">
         <v>142</v>
@@ -3902,12 +3947,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="128" t="s">
         <v>154</v>
       </c>
       <c r="B29" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C29" s="110" t="s">
         <v>142</v>
@@ -3934,7 +3979,7 @@
         <v>156</v>
       </c>
       <c r="B30" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C30" s="110" t="s">
         <v>142</v>
@@ -3961,7 +4006,7 @@
         <v>159</v>
       </c>
       <c r="B31" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C31" s="110" t="s">
         <v>142</v>
@@ -3988,7 +4033,7 @@
         <v>162</v>
       </c>
       <c r="B32" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C32" s="110" t="s">
         <v>142</v>
@@ -4010,12 +4055,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="110" t="s">
         <v>106</v>
       </c>
       <c r="B33" s="110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C33" s="110" t="s">
         <v>112</v>
@@ -4038,15 +4083,15 @@
       </c>
     </row>
     <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="132" t="s">
-        <v>183</v>
-      </c>
-      <c r="B34" s="133"/>
-      <c r="C34" s="133"/>
-      <c r="D34" s="133"/>
-      <c r="E34" s="133"/>
-      <c r="F34" s="133"/>
-      <c r="G34" s="134"/>
+      <c r="A34" s="134" t="s">
+        <v>182</v>
+      </c>
+      <c r="B34" s="135"/>
+      <c r="C34" s="135"/>
+      <c r="D34" s="135"/>
+      <c r="E34" s="135"/>
+      <c r="F34" s="135"/>
+      <c r="G34" s="136"/>
       <c r="H34" s="111">
         <f>AVERAGE(H14:H33)</f>
         <v>174.95</v>
@@ -4290,13 +4335,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.25" customWidth="1"/>
-    <col min="2" max="2" width="46.375" customWidth="1"/>
-    <col min="3" max="3" width="13.125" customWidth="1"/>
-    <col min="4" max="4" width="37.25" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -4305,7 +4350,7 @@
       </c>
       <c r="C2" s="65"/>
       <c r="D2" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>5</v>
@@ -4319,7 +4364,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E3" s="1">
         <v>165</v>
@@ -4334,7 +4379,7 @@
         <v>242</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E4" s="1">
         <v>175</v>
@@ -4349,7 +4394,7 @@
         <v>103.6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E5" s="1">
         <v>169</v>
@@ -4390,104 +4435,104 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="135" t="s">
+      <c r="C17" s="137" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="136"/>
-      <c r="E17" s="136"/>
-      <c r="F17" s="136"/>
-      <c r="G17" s="136"/>
+      <c r="D17" s="138"/>
+      <c r="E17" s="138"/>
+      <c r="F17" s="138"/>
+      <c r="G17" s="138"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="137"/>
-      <c r="D18" s="137"/>
-      <c r="E18" s="137"/>
-      <c r="F18" s="137"/>
-      <c r="G18" s="137"/>
+      <c r="C18" s="139"/>
+      <c r="D18" s="139"/>
+      <c r="E18" s="139"/>
+      <c r="F18" s="139"/>
+      <c r="G18" s="139"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="137"/>
-      <c r="D19" s="137"/>
-      <c r="E19" s="137"/>
-      <c r="F19" s="137"/>
-      <c r="G19" s="137"/>
+      <c r="C19" s="139"/>
+      <c r="D19" s="139"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="139"/>
+      <c r="G19" s="139"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="137"/>
-      <c r="D20" s="137"/>
-      <c r="E20" s="137"/>
-      <c r="F20" s="137"/>
-      <c r="G20" s="137"/>
+      <c r="C20" s="139"/>
+      <c r="D20" s="139"/>
+      <c r="E20" s="139"/>
+      <c r="F20" s="139"/>
+      <c r="G20" s="139"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="137"/>
-      <c r="D21" s="137"/>
-      <c r="E21" s="137"/>
-      <c r="F21" s="137"/>
-      <c r="G21" s="137"/>
+      <c r="C21" s="139"/>
+      <c r="D21" s="139"/>
+      <c r="E21" s="139"/>
+      <c r="F21" s="139"/>
+      <c r="G21" s="139"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="137"/>
-      <c r="D22" s="137"/>
-      <c r="E22" s="137"/>
-      <c r="F22" s="137"/>
-      <c r="G22" s="137"/>
+      <c r="C22" s="139"/>
+      <c r="D22" s="139"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="139"/>
+      <c r="G22" s="139"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="137"/>
-      <c r="D23" s="137"/>
-      <c r="E23" s="137"/>
-      <c r="F23" s="137"/>
-      <c r="G23" s="137"/>
+      <c r="C23" s="139"/>
+      <c r="D23" s="139"/>
+      <c r="E23" s="139"/>
+      <c r="F23" s="139"/>
+      <c r="G23" s="139"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="137"/>
-      <c r="D24" s="137"/>
-      <c r="E24" s="137"/>
-      <c r="F24" s="137"/>
-      <c r="G24" s="137"/>
+      <c r="C24" s="139"/>
+      <c r="D24" s="139"/>
+      <c r="E24" s="139"/>
+      <c r="F24" s="139"/>
+      <c r="G24" s="139"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="137"/>
-      <c r="D25" s="137"/>
-      <c r="E25" s="137"/>
-      <c r="F25" s="137"/>
-      <c r="G25" s="137"/>
+      <c r="C25" s="139"/>
+      <c r="D25" s="139"/>
+      <c r="E25" s="139"/>
+      <c r="F25" s="139"/>
+      <c r="G25" s="139"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="137"/>
-      <c r="D26" s="137"/>
-      <c r="E26" s="137"/>
-      <c r="F26" s="137"/>
-      <c r="G26" s="137"/>
+      <c r="C26" s="139"/>
+      <c r="D26" s="139"/>
+      <c r="E26" s="139"/>
+      <c r="F26" s="139"/>
+      <c r="G26" s="139"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="137"/>
-      <c r="D27" s="137"/>
-      <c r="E27" s="137"/>
-      <c r="F27" s="137"/>
-      <c r="G27" s="137"/>
+      <c r="C27" s="139"/>
+      <c r="D27" s="139"/>
+      <c r="E27" s="139"/>
+      <c r="F27" s="139"/>
+      <c r="G27" s="139"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="137"/>
-      <c r="D28" s="137"/>
-      <c r="E28" s="137"/>
-      <c r="F28" s="137"/>
-      <c r="G28" s="137"/>
+      <c r="C28" s="139"/>
+      <c r="D28" s="139"/>
+      <c r="E28" s="139"/>
+      <c r="F28" s="139"/>
+      <c r="G28" s="139"/>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="137"/>
-      <c r="D29" s="137"/>
-      <c r="E29" s="137"/>
-      <c r="F29" s="137"/>
-      <c r="G29" s="137"/>
+      <c r="C29" s="139"/>
+      <c r="D29" s="139"/>
+      <c r="E29" s="139"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="139"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="137"/>
-      <c r="D30" s="137"/>
-      <c r="E30" s="137"/>
-      <c r="F30" s="137"/>
-      <c r="G30" s="137"/>
+      <c r="C30" s="139"/>
+      <c r="D30" s="139"/>
+      <c r="E30" s="139"/>
+      <c r="F30" s="139"/>
+      <c r="G30" s="139"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="83" t="s">
@@ -5138,22 +5183,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="47"/>
-    <col min="2" max="2" width="15.625" style="47" customWidth="1"/>
-    <col min="3" max="3" width="17.875" style="47" customWidth="1"/>
-    <col min="4" max="4" width="25.875" style="47" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="47"/>
-    <col min="6" max="6" width="29.375" style="47" customWidth="1"/>
-    <col min="7" max="7" width="31.75" style="47" customWidth="1"/>
-    <col min="8" max="8" width="14.75" style="47" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="47"/>
+    <col min="2" max="2" width="15.5703125" style="47" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="47" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="47" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="47"/>
+    <col min="6" max="6" width="29.42578125" style="47" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" style="47" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="47" customWidth="1"/>
     <col min="9" max="9" width="12" style="47" customWidth="1"/>
-    <col min="10" max="10" width="27.375" style="47" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" style="47" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.25">
@@ -5189,19 +5234,19 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="45" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="138">
+      <c r="A2" s="140">
         <v>1</v>
       </c>
-      <c r="B2" s="140" t="s">
+      <c r="B2" s="150" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="140" t="s">
+      <c r="C2" s="150" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="140" t="s">
+      <c r="D2" s="150" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="140">
+      <c r="E2" s="150">
         <v>2</v>
       </c>
       <c r="F2" s="31" t="s">
@@ -5218,12 +5263,12 @@
       </c>
       <c r="J2" s="31"/>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="139"/>
-      <c r="B3" s="140"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="141"/>
+      <c r="B3" s="150"/>
+      <c r="C3" s="150"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
       <c r="F3" s="31" t="s">
         <v>60</v>
       </c>
@@ -5239,19 +5284,19 @@
       <c r="J3" s="31"/>
     </row>
     <row r="4" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="140">
+      <c r="A4" s="150">
         <v>2</v>
       </c>
-      <c r="B4" s="147">
+      <c r="B4" s="151">
         <v>43042</v>
       </c>
-      <c r="C4" s="140" t="s">
+      <c r="C4" s="150" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="140" t="s">
+      <c r="D4" s="150" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="138">
+      <c r="E4" s="140">
         <v>2</v>
       </c>
       <c r="F4" s="31" t="s">
@@ -5268,12 +5313,12 @@
       </c>
       <c r="J4" s="31"/>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="138"/>
-      <c r="B5" s="138"/>
-      <c r="C5" s="138"/>
-      <c r="D5" s="138"/>
-      <c r="E5" s="139"/>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="140"/>
+      <c r="B5" s="140"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="141"/>
       <c r="F5" s="37" t="s">
         <v>54</v>
       </c>
@@ -5288,20 +5333,20 @@
       </c>
       <c r="J5" s="37"/>
     </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="140">
+    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="150">
         <v>3</v>
       </c>
-      <c r="B6" s="146">
+      <c r="B6" s="143">
         <v>42683</v>
       </c>
-      <c r="C6" s="138" t="s">
+      <c r="C6" s="140" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="138" t="s">
+      <c r="D6" s="140" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="138">
+      <c r="E6" s="140">
         <v>2</v>
       </c>
       <c r="F6" s="31" t="s">
@@ -5319,11 +5364,11 @@
       <c r="J6" s="31"/>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="140"/>
-      <c r="B7" s="139"/>
-      <c r="C7" s="139"/>
-      <c r="D7" s="139"/>
-      <c r="E7" s="139"/>
+      <c r="A7" s="150"/>
+      <c r="B7" s="141"/>
+      <c r="C7" s="141"/>
+      <c r="D7" s="141"/>
+      <c r="E7" s="141"/>
       <c r="F7" s="55" t="s">
         <v>67</v>
       </c>
@@ -5338,12 +5383,12 @@
       </c>
       <c r="J7" s="31"/>
     </row>
-    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="140"/>
-      <c r="B8" s="139"/>
-      <c r="C8" s="139"/>
-      <c r="D8" s="139"/>
-      <c r="E8" s="139"/>
+    <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="150"/>
+      <c r="B8" s="141"/>
+      <c r="C8" s="141"/>
+      <c r="D8" s="141"/>
+      <c r="E8" s="141"/>
       <c r="F8" s="53" t="s">
         <v>69</v>
       </c>
@@ -5358,12 +5403,12 @@
       </c>
       <c r="J8" s="53"/>
     </row>
-    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="140"/>
-      <c r="B9" s="139"/>
-      <c r="C9" s="139"/>
-      <c r="D9" s="139"/>
-      <c r="E9" s="139"/>
+    <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="150"/>
+      <c r="B9" s="141"/>
+      <c r="C9" s="141"/>
+      <c r="D9" s="141"/>
+      <c r="E9" s="141"/>
       <c r="F9" s="53" t="s">
         <v>73</v>
       </c>
@@ -5379,11 +5424,11 @@
       <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="140"/>
-      <c r="B10" s="145"/>
-      <c r="C10" s="145"/>
-      <c r="D10" s="145"/>
-      <c r="E10" s="145"/>
+      <c r="A10" s="150"/>
+      <c r="B10" s="142"/>
+      <c r="C10" s="142"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="142"/>
       <c r="F10" s="31" t="s">
         <v>70</v>
       </c>
@@ -5400,20 +5445,20 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="140">
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="150">
         <v>4</v>
       </c>
-      <c r="B11" s="140" t="s">
+      <c r="B11" s="150" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="140" t="s">
+      <c r="C11" s="150" t="s">
         <v>115</v>
       </c>
-      <c r="D11" s="140" t="s">
+      <c r="D11" s="150" t="s">
         <v>116</v>
       </c>
-      <c r="E11" s="140">
+      <c r="E11" s="150">
         <v>2</v>
       </c>
       <c r="F11" s="53" t="s">
@@ -5430,12 +5475,12 @@
       </c>
       <c r="J11" s="53"/>
     </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="140"/>
-      <c r="B12" s="140"/>
-      <c r="C12" s="140"/>
-      <c r="D12" s="140"/>
-      <c r="E12" s="140"/>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="150"/>
+      <c r="B12" s="150"/>
+      <c r="C12" s="150"/>
+      <c r="D12" s="150"/>
+      <c r="E12" s="150"/>
       <c r="F12" s="55" t="s">
         <v>58</v>
       </c>
@@ -5450,12 +5495,12 @@
       </c>
       <c r="J12" s="53"/>
     </row>
-    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="138"/>
-      <c r="B13" s="138"/>
-      <c r="C13" s="138"/>
-      <c r="D13" s="138"/>
-      <c r="E13" s="138"/>
+    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="140"/>
+      <c r="B13" s="140"/>
+      <c r="C13" s="140"/>
+      <c r="D13" s="140"/>
+      <c r="E13" s="140"/>
       <c r="F13" s="70" t="s">
         <v>72</v>
       </c>
@@ -5471,17 +5516,17 @@
       <c r="J13" s="66"/>
     </row>
     <row r="14" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="138">
+      <c r="A14" s="140">
         <v>5</v>
       </c>
-      <c r="B14" s="146">
+      <c r="B14" s="143">
         <v>42705</v>
       </c>
-      <c r="C14" s="138"/>
-      <c r="D14" s="138" t="s">
+      <c r="C14" s="140"/>
+      <c r="D14" s="140" t="s">
         <v>116</v>
       </c>
-      <c r="E14" s="138">
+      <c r="E14" s="140">
         <v>2</v>
       </c>
       <c r="F14" s="71" t="s">
@@ -5498,12 +5543,12 @@
       </c>
       <c r="J14" s="67"/>
     </row>
-    <row r="15" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="139"/>
-      <c r="B15" s="148"/>
-      <c r="C15" s="139"/>
-      <c r="D15" s="139"/>
-      <c r="E15" s="139"/>
+    <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+      <c r="A15" s="141"/>
+      <c r="B15" s="144"/>
+      <c r="C15" s="141"/>
+      <c r="D15" s="141"/>
+      <c r="E15" s="141"/>
       <c r="F15" s="71" t="s">
         <v>121</v>
       </c>
@@ -5519,11 +5564,11 @@
       <c r="J15" s="67"/>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="139"/>
-      <c r="B16" s="148"/>
-      <c r="C16" s="139"/>
-      <c r="D16" s="145"/>
-      <c r="E16" s="139"/>
+      <c r="A16" s="141"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="141"/>
+      <c r="D16" s="142"/>
+      <c r="E16" s="141"/>
       <c r="F16" s="71" t="s">
         <v>123</v>
       </c>
@@ -5539,13 +5584,13 @@
       <c r="J16" s="67"/>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="139"/>
-      <c r="B17" s="148"/>
-      <c r="C17" s="139"/>
+      <c r="A17" s="141"/>
+      <c r="B17" s="144"/>
+      <c r="C17" s="141"/>
       <c r="D17" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="139"/>
+      <c r="E17" s="141"/>
       <c r="F17" s="71" t="s">
         <v>124</v>
       </c>
@@ -5561,13 +5606,13 @@
       <c r="J17" s="67"/>
     </row>
     <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="139"/>
-      <c r="B18" s="148"/>
-      <c r="C18" s="139"/>
-      <c r="D18" s="138" t="s">
+      <c r="A18" s="141"/>
+      <c r="B18" s="144"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="140" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="139"/>
+      <c r="E18" s="141"/>
       <c r="F18" s="71" t="s">
         <v>126</v>
       </c>
@@ -5583,20 +5628,20 @@
       <c r="J18" s="67"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="145"/>
-      <c r="B19" s="149"/>
-      <c r="C19" s="145"/>
-      <c r="D19" s="145"/>
-      <c r="E19" s="145"/>
+      <c r="A19" s="142"/>
+      <c r="B19" s="145"/>
+      <c r="C19" s="142"/>
+      <c r="D19" s="142"/>
+      <c r="E19" s="142"/>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="47">
         <v>6</v>
       </c>
-      <c r="B20" s="141">
+      <c r="B20" s="146">
         <v>42773</v>
       </c>
-      <c r="D20" s="143" t="s">
+      <c r="D20" s="148" t="s">
         <v>180</v>
       </c>
       <c r="F20" s="47" t="s">
@@ -5607,8 +5652,8 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="142"/>
-      <c r="D21" s="144"/>
+      <c r="B21" s="147"/>
+      <c r="D21" s="149"/>
       <c r="F21" s="47" t="s">
         <v>176</v>
       </c>
@@ -5620,8 +5665,8 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="142"/>
-      <c r="D22" s="144"/>
+      <c r="B22" s="147"/>
+      <c r="D22" s="149"/>
       <c r="F22" s="47" t="s">
         <v>178</v>
       </c>
@@ -5632,41 +5677,51 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B23" s="142"/>
-      <c r="D23" s="144"/>
+    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B23" s="147"/>
+      <c r="D23" s="149"/>
       <c r="F23" s="47" t="s">
         <v>181</v>
       </c>
       <c r="G23" s="47" t="s">
-        <v>182</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="345" x14ac:dyDescent="0.25">
+      <c r="B24" s="131">
+        <v>42809</v>
+      </c>
+      <c r="F24" s="159" t="s">
+        <v>192</v>
+      </c>
+      <c r="G24" s="47" t="s">
+        <v>193</v>
+      </c>
+      <c r="I24" s="47" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F25" s="130" t="s">
-        <v>191</v>
-      </c>
+      <c r="F25" s="130"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F26" s="130" t="s">
-        <v>190</v>
-      </c>
+      <c r="F26" s="130"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F27" s="130" t="s">
-        <v>189</v>
-      </c>
+      <c r="F27" s="130"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F28"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="D20:D23"/>
     <mergeCell ref="A14:A19"/>
@@ -5683,13 +5738,11 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="C11:C13"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C14:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5706,13 +5759,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.25" customWidth="1"/>
-    <col min="3" max="3" width="29.875" customWidth="1"/>
-    <col min="4" max="4" width="24.875" customWidth="1"/>
-    <col min="5" max="5" width="19.25" customWidth="1"/>
-    <col min="6" max="6" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.375" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5743,7 +5796,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
@@ -5833,7 +5886,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="61" t="s">
         <v>85</v>
       </c>
@@ -5873,24 +5926,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="152" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="154" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="154" t="s">
+      <c r="C1" s="156" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155" t="s">
+      <c r="D1" s="157"/>
+      <c r="E1" s="157" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="156"/>
+      <c r="F1" s="158"/>
       <c r="G1" s="15" t="s">
         <v>35</v>
       </c>
@@ -5909,9 +5962,9 @@
       <c r="T1" s="16"/>
       <c r="U1" s="16"/>
     </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="151"/>
-      <c r="B2" s="153"/>
+    <row r="2" spans="1:21" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="153"/>
+      <c r="B2" s="155"/>
       <c r="C2" s="17" t="s">
         <v>36</v>
       </c>
@@ -6380,22 +6433,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.625" customWidth="1"/>
+    <col min="1" max="1" width="65.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ata atualizada nome da pasta Apresentações atualizada
</commit_message>
<xml_diff>
--- a/TRE_Dados_MapaRaciocinio.xlsx
+++ b/TRE_Dados_MapaRaciocinio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="11760" windowHeight="5205" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Historicos x Categoria" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="196">
   <si>
     <t>Categoria</t>
   </si>
@@ -383,9 +383,6 @@
   <si>
     <t xml:space="preserve">Conclusão 
 </t>
-  </si>
-  <si>
-    <t>Em Progresso</t>
   </si>
   <si>
     <t>Analisar SIPOC e FluxoGrama , se for possível usar um bypass para chegar a um ponto comum poderemos aplicar soluções semelhantes que abordem as 2 áreas.</t>
@@ -670,6 +667,18 @@
   <si>
     <t>*Resolvido problemas de duplicados na planilha de Banco de Dados    
 *Descoberta a razão da diferença nas médias( Motivo  Média por PAD e não por  total ocorrência)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Apresentação dos novos valores em horas para os PADs para o grupo;
+-          Na apresentação alterar de secretaria para coordenadoria nos quadros que tem as medias divididas pela meta;
+-          Foi decidido aplicar a meta de 15%;
+-          Foi decidido que iremos usar o quadro da direita que utiliza os dias em forma fracionada;
+-          Silmara precisa enviar mais PADs de sua coordenadoria;
+-          Iva deve fazer o levantamento de valores para os PADs para sabermos o ganho financeiro da redução da media de dias;
+-          Entrega do Define dia 30/03;</t>
+  </si>
+  <si>
+    <t>Silmara, Eva, Alceu, Julian, Yuri, Pedro,Ivanilda, Flavio,Ruhan, Ivis, André</t>
   </si>
 </sst>
 </file>
@@ -821,7 +830,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1237,21 +1246,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1433,15 +1433,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1600,14 +1591,14 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1640,36 +1631,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1690,6 +1666,15 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1975,11 +1960,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="315138048"/>
-        <c:axId val="349416256"/>
+        <c:axId val="199507968"/>
+        <c:axId val="199298432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="315138048"/>
+        <c:axId val="199507968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1999,7 +1984,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349416256"/>
+        <c:crossAx val="199298432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2007,7 +1992,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="349416256"/>
+        <c:axId val="199298432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2018,7 +2003,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="315138048"/>
+        <c:crossAx val="199507968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2070,7 +2055,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2229,11 +2213,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="315141632"/>
-        <c:axId val="349420288"/>
+        <c:axId val="199509504"/>
+        <c:axId val="199300160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="315141632"/>
+        <c:axId val="199509504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2243,7 +2227,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="349420288"/>
+        <c:crossAx val="199300160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2251,7 +2235,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="349420288"/>
+        <c:axId val="199300160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2262,14 +2246,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="315141632"/>
+        <c:crossAx val="199509504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3178,1133 +3161,1133 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.25" style="102" customWidth="1"/>
-    <col min="2" max="2" width="31" style="102" customWidth="1"/>
-    <col min="3" max="3" width="29.875" style="102" customWidth="1"/>
-    <col min="4" max="4" width="59.125" style="102" customWidth="1"/>
-    <col min="5" max="5" width="53.125" style="102" customWidth="1"/>
-    <col min="6" max="6" width="15" style="102" customWidth="1"/>
-    <col min="7" max="7" width="15.125" style="102" customWidth="1"/>
-    <col min="8" max="8" width="25.375" style="102" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" style="102" customWidth="1"/>
-    <col min="10" max="10" width="2.875" style="102" customWidth="1"/>
-    <col min="11" max="11" width="15.625" style="102" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.125" style="102" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.375" style="102" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.125" style="102"/>
+    <col min="1" max="1" width="18.25" style="99" customWidth="1"/>
+    <col min="2" max="2" width="31" style="99" customWidth="1"/>
+    <col min="3" max="3" width="29.875" style="99" customWidth="1"/>
+    <col min="4" max="4" width="59.125" style="99" customWidth="1"/>
+    <col min="5" max="5" width="53.125" style="99" customWidth="1"/>
+    <col min="6" max="6" width="15" style="99" customWidth="1"/>
+    <col min="7" max="7" width="15.125" style="99" customWidth="1"/>
+    <col min="8" max="8" width="25.375" style="99" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="99" customWidth="1"/>
+    <col min="10" max="10" width="2.875" style="99" customWidth="1"/>
+    <col min="11" max="11" width="15.625" style="99" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.125" style="99" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.375" style="99" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.125" style="99"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="98" t="s">
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="99" t="s">
+      <c r="F1" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="100">
+      <c r="G1" s="97">
         <f ca="1">TODAY()</f>
-        <v>42807</v>
-      </c>
-      <c r="H1" s="101" t="s">
+        <v>42809</v>
+      </c>
+      <c r="H1" s="98" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="103" t="s">
-        <v>188</v>
-      </c>
-      <c r="C3" s="103" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="104" t="s">
+      <c r="B3" s="100" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="100" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="105" t="s">
+      <c r="E3" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="105" t="s">
+      <c r="F3" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="105" t="s">
+      <c r="G3" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="106" t="s">
+      <c r="H3" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="107" t="s">
+      <c r="K3" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="108" t="s">
+      <c r="L3" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="109" t="s">
+      <c r="M3" s="106" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="107" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="110" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="110" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="99" t="s">
+      <c r="B4" s="107" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="101" t="s">
+      <c r="E4" s="98" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="132">
+      <c r="F4" s="128">
         <v>42311</v>
       </c>
-      <c r="G4" s="132">
+      <c r="G4" s="128">
         <v>42446</v>
       </c>
-      <c r="H4" s="111">
+      <c r="H4" s="108">
         <f t="shared" ref="H4:H14" si="0">DAYS360(F4,G4)</f>
         <v>134</v>
       </c>
-      <c r="I4" s="112">
+      <c r="I4" s="109">
         <v>167</v>
       </c>
-      <c r="K4" s="113">
+      <c r="K4" s="110">
         <f>AVERAGE(H13,H34)</f>
         <v>87.474999999999994</v>
       </c>
-      <c r="L4" s="114">
+      <c r="L4" s="111">
         <v>0.15</v>
       </c>
-      <c r="M4" s="99">
+      <c r="M4" s="96">
         <f>K4-(K4*L4)</f>
         <v>74.353749999999991</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="110" t="s">
+      <c r="A5" s="107" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="107" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" s="107" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="110" t="s">
-        <v>191</v>
-      </c>
-      <c r="C5" s="110" t="s">
+      <c r="D5" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="D5" s="99" t="s">
-        <v>129</v>
-      </c>
-      <c r="E5" s="101" t="s">
-        <v>131</v>
-      </c>
-      <c r="F5" s="132">
+      <c r="E5" s="98" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="128">
         <v>42118</v>
       </c>
-      <c r="G5" s="132">
+      <c r="G5" s="128">
         <v>42221</v>
       </c>
-      <c r="H5" s="111">
+      <c r="H5" s="108">
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
-      <c r="K5" s="115"/>
-      <c r="L5" s="116"/>
-      <c r="M5" s="117"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="113"/>
+      <c r="M5" s="114"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="110" t="s">
+      <c r="A6" s="107" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="107" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" s="107" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="96" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="98" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="110" t="s">
-        <v>191</v>
-      </c>
-      <c r="C6" s="110" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="99" t="s">
-        <v>129</v>
-      </c>
-      <c r="E6" s="101" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" s="132">
+      <c r="F6" s="128">
         <v>42263</v>
       </c>
-      <c r="G6" s="132">
+      <c r="G6" s="128">
         <v>42342</v>
       </c>
-      <c r="H6" s="111">
+      <c r="H6" s="108">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
-      <c r="K6" s="115"/>
-      <c r="L6" s="116"/>
-      <c r="M6" s="117"/>
+      <c r="K6" s="112"/>
+      <c r="L6" s="113"/>
+      <c r="M6" s="114"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="110" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" s="110" t="s">
-        <v>191</v>
-      </c>
-      <c r="C7" s="110" t="s">
+      <c r="A7" s="107" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="107" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="107" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="D7" s="99" t="s">
-        <v>129</v>
-      </c>
-      <c r="E7" s="101" t="s">
-        <v>131</v>
-      </c>
-      <c r="F7" s="132">
+      <c r="E7" s="98" t="s">
+        <v>130</v>
+      </c>
+      <c r="F7" s="128">
         <v>42633</v>
       </c>
-      <c r="G7" s="132">
+      <c r="G7" s="128">
         <v>42695</v>
       </c>
-      <c r="H7" s="111">
+      <c r="H7" s="108">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="K7" s="115"/>
-      <c r="L7" s="116"/>
-      <c r="M7" s="117"/>
+      <c r="K7" s="112"/>
+      <c r="L7" s="113"/>
+      <c r="M7" s="114"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="110" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="110" t="s">
-        <v>191</v>
-      </c>
-      <c r="C8" s="110" t="s">
+      <c r="A8" s="107" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="107" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="107" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="99" t="s">
-        <v>129</v>
-      </c>
-      <c r="E8" s="101" t="s">
-        <v>131</v>
-      </c>
-      <c r="F8" s="132">
+      <c r="E8" s="98" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="128">
         <v>42422</v>
       </c>
-      <c r="G8" s="132">
+      <c r="G8" s="128">
         <v>42643</v>
       </c>
-      <c r="H8" s="111">
+      <c r="H8" s="108">
         <f t="shared" si="0"/>
         <v>218</v>
       </c>
-      <c r="K8" s="115"/>
-      <c r="L8" s="116"/>
-      <c r="M8" s="117"/>
+      <c r="K8" s="112"/>
+      <c r="L8" s="113"/>
+      <c r="M8" s="114"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="110" t="s">
-        <v>134</v>
-      </c>
-      <c r="B9" s="110" t="s">
-        <v>191</v>
-      </c>
-      <c r="C9" s="110" t="s">
+      <c r="A9" s="107" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="107" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="107" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="D9" s="99" t="s">
-        <v>129</v>
-      </c>
-      <c r="E9" s="101" t="s">
-        <v>131</v>
-      </c>
-      <c r="F9" s="132">
+      <c r="E9" s="98" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="128">
         <v>41955</v>
       </c>
-      <c r="G9" s="132">
+      <c r="G9" s="128">
         <v>42179</v>
       </c>
-      <c r="H9" s="111">
+      <c r="H9" s="108">
         <f t="shared" si="0"/>
         <v>222</v>
       </c>
-      <c r="L9" s="118"/>
+      <c r="L9" s="115"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="110" t="s">
-        <v>135</v>
-      </c>
-      <c r="B10" s="110" t="s">
-        <v>191</v>
-      </c>
-      <c r="C10" s="110" t="s">
+      <c r="A10" s="107" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="107" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" s="107" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="D10" s="99" t="s">
-        <v>129</v>
-      </c>
-      <c r="E10" s="101" t="s">
-        <v>131</v>
-      </c>
-      <c r="F10" s="132">
+      <c r="E10" s="98" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="128">
         <v>41738</v>
       </c>
-      <c r="G10" s="132">
+      <c r="G10" s="128">
         <v>41850</v>
       </c>
-      <c r="H10" s="111">
+      <c r="H10" s="108">
         <f t="shared" si="0"/>
         <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="110" t="s">
+      <c r="A11" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="110" t="s">
-        <v>191</v>
-      </c>
-      <c r="C11" s="110" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" s="99" t="s">
+      <c r="B11" s="107" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="99" t="s">
+      <c r="E11" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="132">
+      <c r="F11" s="128">
         <v>41337</v>
       </c>
-      <c r="G11" s="132">
+      <c r="G11" s="128">
         <v>41430</v>
       </c>
-      <c r="H11" s="111">
+      <c r="H11" s="108">
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="110" t="s">
+      <c r="A12" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="110" t="s">
-        <v>191</v>
-      </c>
-      <c r="C12" s="110" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="99" t="s">
+      <c r="B12" s="107" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="101" t="s">
+      <c r="E12" s="98" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="100">
+      <c r="F12" s="97">
         <v>42209</v>
       </c>
-      <c r="G12" s="100">
+      <c r="G12" s="97">
         <v>42683</v>
       </c>
-      <c r="H12" s="111">
+      <c r="H12" s="108">
         <f t="shared" si="0"/>
         <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="119"/>
-      <c r="B13" s="110"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="136" t="s">
-        <v>183</v>
-      </c>
-      <c r="E13" s="136"/>
-      <c r="F13" s="136"/>
-      <c r="G13" s="137"/>
-      <c r="H13" s="111">
+      <c r="A13" s="116"/>
+      <c r="B13" s="107"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="133" t="s">
+        <v>182</v>
+      </c>
+      <c r="E13" s="133"/>
+      <c r="F13" s="133"/>
+      <c r="G13" s="134"/>
+      <c r="H13" s="108">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="110" t="s">
+      <c r="A14" s="107" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C14" s="110" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" s="99" t="s">
+      <c r="B14" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C14" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="96" t="s">
         <v>86</v>
       </c>
-      <c r="E14" s="101" t="str">
+      <c r="E14" s="98" t="str">
         <f>LOWER("CONTRATAÇÃO - SERVIÇO DE MANUTENÇÃO PREDIAL -   LIMPEZA DE VIDROS - CAPITAL/ INTERIOR")</f>
         <v>contratação - serviço de manutenção predial -   limpeza de vidros - capital/ interior</v>
       </c>
-      <c r="F14" s="100">
+      <c r="F14" s="97">
         <v>42020</v>
       </c>
-      <c r="G14" s="100">
+      <c r="G14" s="97">
         <v>42671</v>
       </c>
-      <c r="H14" s="111">
+      <c r="H14" s="108">
         <f t="shared" si="0"/>
         <v>642</v>
       </c>
-      <c r="I14" s="102">
+      <c r="I14" s="99">
         <v>689</v>
       </c>
-      <c r="K14" s="112">
+      <c r="K14" s="109">
         <f>I14-H14</f>
         <v>47</v>
       </c>
-      <c r="L14" s="102">
+      <c r="L14" s="99">
         <f>K14*24</f>
         <v>1128</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="110" t="s">
+      <c r="A15" s="107" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C15" s="110" t="s">
-        <v>112</v>
-      </c>
-      <c r="D15" s="99" t="s">
+      <c r="B15" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C15" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="96" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="101" t="s">
+      <c r="E15" s="98" t="s">
         <v>87</v>
       </c>
-      <c r="F15" s="100">
+      <c r="F15" s="97">
         <v>42439</v>
       </c>
-      <c r="G15" s="100">
+      <c r="G15" s="97">
         <v>42668</v>
       </c>
-      <c r="H15" s="111">
+      <c r="H15" s="108">
         <f t="shared" ref="H15:H33" si="1">DAYS360(F15,G15)</f>
         <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="110" t="s">
+      <c r="A16" s="107" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C16" s="110" t="s">
-        <v>112</v>
-      </c>
-      <c r="D16" s="99" t="s">
+      <c r="B16" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C16" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="96" t="s">
         <v>91</v>
       </c>
-      <c r="E16" s="101" t="s">
+      <c r="E16" s="98" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="100">
+      <c r="F16" s="97">
         <v>42521</v>
       </c>
-      <c r="G16" s="100">
+      <c r="G16" s="97">
         <v>42661</v>
       </c>
-      <c r="H16" s="111">
+      <c r="H16" s="108">
         <f t="shared" si="1"/>
         <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="110" t="s">
+      <c r="A17" s="107" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C17" s="110" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" s="99" t="s">
+      <c r="B17" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C17" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="101" t="s">
+      <c r="E17" s="98" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="100">
+      <c r="F17" s="97">
         <v>41242</v>
       </c>
-      <c r="G17" s="100">
+      <c r="G17" s="97">
         <v>41472</v>
       </c>
-      <c r="H17" s="111">
+      <c r="H17" s="108">
         <f t="shared" si="1"/>
         <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="110" t="s">
+      <c r="A18" s="107" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C18" s="110" t="s">
-        <v>112</v>
-      </c>
-      <c r="D18" s="99" t="s">
+      <c r="B18" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="101" t="s">
+      <c r="E18" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="F18" s="100">
+      <c r="F18" s="97">
         <v>41698</v>
       </c>
-      <c r="G18" s="100">
+      <c r="G18" s="97">
         <v>41932</v>
       </c>
-      <c r="H18" s="111">
+      <c r="H18" s="108">
         <f t="shared" si="1"/>
         <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="110" t="s">
+      <c r="A19" s="107" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C19" s="110" t="s">
-        <v>112</v>
-      </c>
-      <c r="D19" s="99" t="s">
+      <c r="B19" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C19" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="96" t="s">
         <v>98</v>
       </c>
-      <c r="E19" s="99" t="s">
+      <c r="E19" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="F19" s="100">
+      <c r="F19" s="97">
         <v>42277</v>
       </c>
-      <c r="G19" s="100">
+      <c r="G19" s="97">
         <v>42681</v>
       </c>
-      <c r="H19" s="111">
+      <c r="H19" s="108">
         <f t="shared" si="1"/>
         <v>397</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="110" t="s">
+      <c r="A20" s="107" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C20" s="110" t="s">
-        <v>128</v>
-      </c>
-      <c r="D20" s="99" t="s">
+      <c r="B20" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" s="107" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="101" t="s">
+      <c r="E20" s="98" t="s">
         <v>100</v>
       </c>
-      <c r="F20" s="100">
+      <c r="F20" s="97">
         <v>42136</v>
       </c>
-      <c r="G20" s="121">
+      <c r="G20" s="118">
         <v>42171</v>
       </c>
-      <c r="H20" s="111">
+      <c r="H20" s="108">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="110" t="s">
+      <c r="A21" s="107" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C21" s="110" t="s">
-        <v>112</v>
-      </c>
-      <c r="D21" s="99" t="s">
+      <c r="B21" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C21" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="101" t="s">
+      <c r="E21" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="F21" s="100">
+      <c r="F21" s="97">
         <v>41541</v>
       </c>
-      <c r="G21" s="100">
+      <c r="G21" s="97">
         <v>41634</v>
       </c>
-      <c r="H21" s="111">
+      <c r="H21" s="108">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="110" t="s">
+      <c r="A22" s="107" t="s">
         <v>103</v>
       </c>
-      <c r="B22" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C22" s="110" t="s">
-        <v>128</v>
-      </c>
-      <c r="D22" s="122" t="s">
+      <c r="B22" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C22" s="107" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="119" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="101" t="s">
+      <c r="E22" s="98" t="s">
         <v>104</v>
       </c>
-      <c r="F22" s="100">
+      <c r="F22" s="97">
         <v>41575</v>
       </c>
-      <c r="G22" s="100">
+      <c r="G22" s="97">
         <v>41638</v>
       </c>
-      <c r="H22" s="111">
+      <c r="H22" s="108">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="110" t="s">
+      <c r="A23" s="107" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C23" s="107" t="s">
+        <v>127</v>
+      </c>
+      <c r="D23" s="120" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="121" t="s">
         <v>136</v>
       </c>
-      <c r="B23" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C23" s="110" t="s">
-        <v>128</v>
-      </c>
-      <c r="D23" s="123" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="124" t="s">
-        <v>137</v>
-      </c>
-      <c r="F23" s="125">
+      <c r="F23" s="122">
         <v>42580</v>
       </c>
-      <c r="G23" s="125">
+      <c r="G23" s="122">
         <v>42641</v>
       </c>
-      <c r="H23" s="126">
+      <c r="H23" s="123">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="110" t="s">
+      <c r="A24" s="107" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C24" s="107" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" s="121" t="s">
+        <v>139</v>
+      </c>
+      <c r="E24" s="124" t="s">
         <v>138</v>
       </c>
-      <c r="B24" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C24" s="110" t="s">
-        <v>128</v>
-      </c>
-      <c r="D24" s="124" t="s">
-        <v>140</v>
-      </c>
-      <c r="E24" s="127" t="s">
-        <v>139</v>
-      </c>
-      <c r="F24" s="125">
+      <c r="F24" s="122">
         <v>42612</v>
       </c>
-      <c r="G24" s="125">
+      <c r="G24" s="122">
         <v>42704</v>
       </c>
-      <c r="H24" s="126">
+      <c r="H24" s="123">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="110" t="s">
+      <c r="A25" s="107" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C25" s="107" t="s">
         <v>141</v>
       </c>
-      <c r="B25" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C25" s="110" t="s">
+      <c r="D25" s="121" t="s">
         <v>142</v>
       </c>
-      <c r="D25" s="124" t="s">
+      <c r="E25" s="124" t="s">
         <v>143</v>
       </c>
-      <c r="E25" s="127" t="s">
-        <v>144</v>
-      </c>
-      <c r="F25" s="125">
+      <c r="F25" s="122">
         <v>42068</v>
       </c>
-      <c r="G25" s="125">
+      <c r="G25" s="122">
         <v>42149</v>
       </c>
-      <c r="H25" s="126">
+      <c r="H25" s="123">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="110" t="s">
+      <c r="A26" s="107" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C26" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="D26" s="121" t="s">
         <v>145</v>
       </c>
-      <c r="B26" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C26" s="110" t="s">
-        <v>142</v>
-      </c>
-      <c r="D26" s="124" t="s">
+      <c r="E26" s="124" t="s">
         <v>146</v>
       </c>
-      <c r="E26" s="127" t="s">
-        <v>147</v>
-      </c>
-      <c r="F26" s="125">
+      <c r="F26" s="122">
         <v>42410</v>
       </c>
-      <c r="G26" s="125">
+      <c r="G26" s="122">
         <v>42690</v>
       </c>
-      <c r="H26" s="126">
+      <c r="H26" s="123">
         <f t="shared" si="1"/>
         <v>276</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="110" t="s">
+      <c r="A27" s="107" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C27" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="121" t="s">
         <v>148</v>
       </c>
-      <c r="B27" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C27" s="110" t="s">
-        <v>112</v>
-      </c>
-      <c r="D27" s="124" t="s">
+      <c r="E27" s="124" t="s">
         <v>149</v>
       </c>
-      <c r="E27" s="127" t="s">
-        <v>150</v>
-      </c>
-      <c r="F27" s="125">
+      <c r="F27" s="122">
         <v>41208</v>
       </c>
-      <c r="G27" s="125">
+      <c r="G27" s="122">
         <v>41348</v>
       </c>
-      <c r="H27" s="126">
+      <c r="H27" s="123">
         <f t="shared" si="1"/>
         <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="110" t="s">
-        <v>153</v>
-      </c>
-      <c r="B28" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C28" s="110" t="s">
-        <v>142</v>
-      </c>
-      <c r="D28" s="124" t="s">
+      <c r="A28" s="107" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C28" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" s="121" t="s">
+        <v>150</v>
+      </c>
+      <c r="E28" s="124" t="s">
         <v>151</v>
       </c>
-      <c r="E28" s="127" t="s">
-        <v>152</v>
-      </c>
-      <c r="F28" s="125">
+      <c r="F28" s="122">
         <v>40927</v>
       </c>
-      <c r="G28" s="125">
+      <c r="G28" s="122">
         <v>41012</v>
       </c>
-      <c r="H28" s="126">
+      <c r="H28" s="123">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="128" t="s">
+      <c r="A29" s="125" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C29" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="121" t="s">
+        <v>142</v>
+      </c>
+      <c r="E29" s="124" t="s">
         <v>154</v>
       </c>
-      <c r="B29" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C29" s="110" t="s">
-        <v>142</v>
-      </c>
-      <c r="D29" s="124" t="s">
-        <v>143</v>
-      </c>
-      <c r="E29" s="127" t="s">
-        <v>155</v>
-      </c>
-      <c r="F29" s="125">
+      <c r="F29" s="122">
         <v>41885</v>
       </c>
-      <c r="G29" s="125">
+      <c r="G29" s="122">
         <v>41996</v>
       </c>
-      <c r="H29" s="126">
+      <c r="H29" s="123">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="110" t="s">
+      <c r="A30" s="107" t="s">
+        <v>155</v>
+      </c>
+      <c r="B30" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C30" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="D30" s="124" t="s">
         <v>156</v>
       </c>
-      <c r="B30" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C30" s="110" t="s">
-        <v>142</v>
-      </c>
-      <c r="D30" s="127" t="s">
+      <c r="E30" s="126" t="s">
         <v>157</v>
       </c>
-      <c r="E30" s="129" t="s">
-        <v>158</v>
-      </c>
-      <c r="F30" s="125">
+      <c r="F30" s="122">
         <v>40945</v>
       </c>
-      <c r="G30" s="125">
+      <c r="G30" s="122">
         <v>41093</v>
       </c>
-      <c r="H30" s="126">
+      <c r="H30" s="123">
         <f t="shared" si="1"/>
         <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="110" t="s">
+      <c r="A31" s="107" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C31" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="D31" s="121" t="s">
         <v>159</v>
       </c>
-      <c r="B31" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C31" s="110" t="s">
-        <v>142</v>
-      </c>
-      <c r="D31" s="124" t="s">
+      <c r="E31" s="124" t="s">
         <v>160</v>
       </c>
-      <c r="E31" s="127" t="s">
-        <v>161</v>
-      </c>
-      <c r="F31" s="125">
+      <c r="F31" s="122">
         <v>41411</v>
       </c>
-      <c r="G31" s="125">
+      <c r="G31" s="122">
         <v>41666</v>
       </c>
-      <c r="H31" s="126">
+      <c r="H31" s="123">
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="110" t="s">
+      <c r="A32" s="107" t="s">
+        <v>161</v>
+      </c>
+      <c r="B32" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C32" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="D32" s="121" t="s">
         <v>162</v>
       </c>
-      <c r="B32" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C32" s="110" t="s">
-        <v>142</v>
-      </c>
-      <c r="D32" s="124" t="s">
+      <c r="E32" s="124" t="s">
         <v>163</v>
       </c>
-      <c r="E32" s="127" t="s">
-        <v>164</v>
-      </c>
-      <c r="F32" s="125">
+      <c r="F32" s="122">
         <v>41905</v>
       </c>
-      <c r="G32" s="125">
+      <c r="G32" s="122">
         <v>41999</v>
       </c>
-      <c r="H32" s="126">
+      <c r="H32" s="123">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="110" t="s">
+      <c r="A33" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="B33" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C33" s="110" t="s">
-        <v>112</v>
-      </c>
-      <c r="D33" s="99" t="s">
+      <c r="B33" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C33" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="96" t="s">
         <v>107</v>
       </c>
-      <c r="E33" s="101" t="s">
+      <c r="E33" s="98" t="s">
         <v>108</v>
       </c>
-      <c r="F33" s="100">
+      <c r="F33" s="97">
         <v>42229</v>
       </c>
-      <c r="G33" s="100">
+      <c r="G33" s="97">
         <v>42354</v>
       </c>
-      <c r="H33" s="111">
+      <c r="H33" s="108">
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="135" t="s">
-        <v>182</v>
-      </c>
-      <c r="B34" s="136"/>
-      <c r="C34" s="136"/>
-      <c r="D34" s="136"/>
-      <c r="E34" s="136"/>
-      <c r="F34" s="136"/>
-      <c r="G34" s="137"/>
-      <c r="H34" s="111">
+      <c r="A34" s="132" t="s">
+        <v>181</v>
+      </c>
+      <c r="B34" s="133"/>
+      <c r="C34" s="133"/>
+      <c r="D34" s="133"/>
+      <c r="E34" s="133"/>
+      <c r="F34" s="133"/>
+      <c r="G34" s="134"/>
+      <c r="H34" s="108">
         <f>AVERAGE(H14:H33)</f>
         <v>174.95</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="99"/>
-      <c r="B35" s="99"/>
-      <c r="C35" s="99"/>
-      <c r="D35" s="99"/>
-      <c r="E35" s="99"/>
-      <c r="F35" s="99"/>
-      <c r="G35" s="99"/>
-      <c r="H35" s="99"/>
-      <c r="I35" s="111"/>
+      <c r="A35" s="96"/>
+      <c r="B35" s="96"/>
+      <c r="C35" s="96"/>
+      <c r="D35" s="96"/>
+      <c r="E35" s="96"/>
+      <c r="F35" s="96"/>
+      <c r="G35" s="96"/>
+      <c r="H35" s="96"/>
+      <c r="I35" s="108"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="99"/>
-      <c r="B36" s="99"/>
-      <c r="C36" s="99"/>
-      <c r="D36" s="99"/>
-      <c r="E36" s="99"/>
-      <c r="F36" s="99"/>
-      <c r="G36" s="99"/>
-      <c r="H36" s="99"/>
+      <c r="A36" s="96"/>
+      <c r="B36" s="96"/>
+      <c r="C36" s="96"/>
+      <c r="D36" s="96"/>
+      <c r="E36" s="96"/>
+      <c r="F36" s="96"/>
+      <c r="G36" s="96"/>
+      <c r="H36" s="96"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="99"/>
-      <c r="B37" s="99"/>
-      <c r="C37" s="99"/>
-      <c r="D37" s="99"/>
-      <c r="E37" s="99"/>
-      <c r="F37" s="99"/>
-      <c r="G37" s="99"/>
-      <c r="H37" s="99"/>
+      <c r="A37" s="96"/>
+      <c r="B37" s="96"/>
+      <c r="C37" s="96"/>
+      <c r="D37" s="96"/>
+      <c r="E37" s="96"/>
+      <c r="F37" s="96"/>
+      <c r="G37" s="96"/>
+      <c r="H37" s="96"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="99"/>
-      <c r="B38" s="99"/>
-      <c r="C38" s="99"/>
-      <c r="D38" s="99"/>
-      <c r="E38" s="99"/>
-      <c r="F38" s="99"/>
-      <c r="G38" s="99"/>
-      <c r="H38" s="99"/>
+      <c r="A38" s="96"/>
+      <c r="B38" s="96"/>
+      <c r="C38" s="96"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="96"/>
+      <c r="F38" s="96"/>
+      <c r="G38" s="96"/>
+      <c r="H38" s="96"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="99"/>
-      <c r="B39" s="99"/>
-      <c r="C39" s="99"/>
-      <c r="D39" s="99"/>
-      <c r="E39" s="99"/>
-      <c r="F39" s="99"/>
-      <c r="G39" s="99"/>
-      <c r="H39" s="99"/>
+      <c r="A39" s="96"/>
+      <c r="B39" s="96"/>
+      <c r="C39" s="96"/>
+      <c r="D39" s="96"/>
+      <c r="E39" s="96"/>
+      <c r="F39" s="96"/>
+      <c r="G39" s="96"/>
+      <c r="H39" s="96"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="99"/>
-      <c r="B40" s="99"/>
-      <c r="C40" s="99"/>
-      <c r="D40" s="99"/>
-      <c r="E40" s="99"/>
-      <c r="F40" s="99"/>
-      <c r="G40" s="99"/>
-      <c r="H40" s="99"/>
+      <c r="A40" s="96"/>
+      <c r="B40" s="96"/>
+      <c r="C40" s="96"/>
+      <c r="D40" s="96"/>
+      <c r="E40" s="96"/>
+      <c r="F40" s="96"/>
+      <c r="G40" s="96"/>
+      <c r="H40" s="96"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="99"/>
-      <c r="B41" s="99"/>
-      <c r="C41" s="99"/>
-      <c r="D41" s="99"/>
-      <c r="E41" s="99"/>
-      <c r="F41" s="99"/>
-      <c r="G41" s="99"/>
-      <c r="H41" s="99"/>
+      <c r="A41" s="96"/>
+      <c r="B41" s="96"/>
+      <c r="C41" s="96"/>
+      <c r="D41" s="96"/>
+      <c r="E41" s="96"/>
+      <c r="F41" s="96"/>
+      <c r="G41" s="96"/>
+      <c r="H41" s="96"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="99"/>
-      <c r="B42" s="99"/>
-      <c r="C42" s="99"/>
-      <c r="D42" s="99"/>
-      <c r="E42" s="99"/>
-      <c r="F42" s="99"/>
-      <c r="G42" s="99"/>
-      <c r="H42" s="99"/>
+      <c r="A42" s="96"/>
+      <c r="B42" s="96"/>
+      <c r="C42" s="96"/>
+      <c r="D42" s="96"/>
+      <c r="E42" s="96"/>
+      <c r="F42" s="96"/>
+      <c r="G42" s="96"/>
+      <c r="H42" s="96"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="99"/>
-      <c r="B43" s="99"/>
-      <c r="C43" s="99"/>
-      <c r="D43" s="99"/>
-      <c r="E43" s="99"/>
-      <c r="F43" s="99"/>
-      <c r="G43" s="99"/>
-      <c r="H43" s="99"/>
+      <c r="A43" s="96"/>
+      <c r="B43" s="96"/>
+      <c r="C43" s="96"/>
+      <c r="D43" s="96"/>
+      <c r="E43" s="96"/>
+      <c r="F43" s="96"/>
+      <c r="G43" s="96"/>
+      <c r="H43" s="96"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="99"/>
-      <c r="B44" s="99"/>
-      <c r="C44" s="99"/>
-      <c r="D44" s="99"/>
-      <c r="E44" s="99"/>
-      <c r="F44" s="99"/>
-      <c r="G44" s="99"/>
-      <c r="H44" s="99"/>
+      <c r="A44" s="96"/>
+      <c r="B44" s="96"/>
+      <c r="C44" s="96"/>
+      <c r="D44" s="96"/>
+      <c r="E44" s="96"/>
+      <c r="F44" s="96"/>
+      <c r="G44" s="96"/>
+      <c r="H44" s="96"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="99"/>
-      <c r="B45" s="99"/>
-      <c r="C45" s="99"/>
-      <c r="D45" s="99"/>
-      <c r="E45" s="99"/>
-      <c r="F45" s="99"/>
-      <c r="G45" s="99"/>
-      <c r="H45" s="99"/>
+      <c r="A45" s="96"/>
+      <c r="B45" s="96"/>
+      <c r="C45" s="96"/>
+      <c r="D45" s="96"/>
+      <c r="E45" s="96"/>
+      <c r="F45" s="96"/>
+      <c r="G45" s="96"/>
+      <c r="H45" s="96"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="99"/>
-      <c r="B46" s="99"/>
-      <c r="C46" s="99"/>
-      <c r="D46" s="99"/>
-      <c r="E46" s="99"/>
-      <c r="F46" s="99"/>
-      <c r="G46" s="99"/>
-      <c r="H46" s="99"/>
+      <c r="A46" s="96"/>
+      <c r="B46" s="96"/>
+      <c r="C46" s="96"/>
+      <c r="D46" s="96"/>
+      <c r="E46" s="96"/>
+      <c r="F46" s="96"/>
+      <c r="G46" s="96"/>
+      <c r="H46" s="96"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="99"/>
-      <c r="B47" s="99"/>
-      <c r="C47" s="99"/>
-      <c r="D47" s="99"/>
-      <c r="E47" s="99"/>
-      <c r="F47" s="99"/>
-      <c r="G47" s="99"/>
-      <c r="H47" s="99"/>
+      <c r="A47" s="96"/>
+      <c r="B47" s="96"/>
+      <c r="C47" s="96"/>
+      <c r="D47" s="96"/>
+      <c r="E47" s="96"/>
+      <c r="F47" s="96"/>
+      <c r="G47" s="96"/>
+      <c r="H47" s="96"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="99"/>
-      <c r="B48" s="99"/>
-      <c r="C48" s="99"/>
-      <c r="D48" s="99"/>
-      <c r="E48" s="99"/>
-      <c r="F48" s="99"/>
-      <c r="G48" s="99"/>
-      <c r="H48" s="99"/>
+      <c r="A48" s="96"/>
+      <c r="B48" s="96"/>
+      <c r="C48" s="96"/>
+      <c r="D48" s="96"/>
+      <c r="E48" s="96"/>
+      <c r="F48" s="96"/>
+      <c r="G48" s="96"/>
+      <c r="H48" s="96"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="99"/>
-      <c r="B49" s="99"/>
-      <c r="C49" s="99"/>
-      <c r="D49" s="99"/>
-      <c r="E49" s="99"/>
-      <c r="F49" s="99"/>
-      <c r="G49" s="99"/>
-      <c r="H49" s="99"/>
+      <c r="A49" s="96"/>
+      <c r="B49" s="96"/>
+      <c r="C49" s="96"/>
+      <c r="D49" s="96"/>
+      <c r="E49" s="96"/>
+      <c r="F49" s="96"/>
+      <c r="G49" s="96"/>
+      <c r="H49" s="96"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="99"/>
-      <c r="B50" s="99"/>
-      <c r="C50" s="99"/>
-      <c r="D50" s="99"/>
-      <c r="E50" s="99"/>
-      <c r="F50" s="99"/>
-      <c r="G50" s="99"/>
-      <c r="H50" s="99"/>
+      <c r="A50" s="96"/>
+      <c r="B50" s="96"/>
+      <c r="C50" s="96"/>
+      <c r="D50" s="96"/>
+      <c r="E50" s="96"/>
+      <c r="F50" s="96"/>
+      <c r="G50" s="96"/>
+      <c r="H50" s="96"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L58" s="102" t="s">
+      <c r="L58" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="M58" s="102">
+      <c r="M58" s="99">
         <v>1</v>
       </c>
-      <c r="N58" s="102">
+      <c r="N58" s="99">
         <f>AVERAGEIF(L58:L62,L58,M58:M62)</f>
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L59" s="102" t="s">
+      <c r="L59" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="M59" s="102">
+      <c r="M59" s="99">
         <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L60" s="102" t="s">
+      <c r="L60" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="M60" s="102">
+      <c r="M60" s="99">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L61" s="102" t="s">
+      <c r="L61" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="M61" s="102">
+      <c r="M61" s="99">
         <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L62" s="102" t="s">
+      <c r="L62" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="M62" s="102">
+      <c r="M62" s="99">
         <v>3</v>
       </c>
     </row>
@@ -4335,7 +4318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J148"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E3" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>
@@ -4356,7 +4339,7 @@
       </c>
       <c r="C2" s="65"/>
       <c r="D2" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>5</v>
@@ -4370,7 +4353,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E3" s="1">
         <v>165</v>
@@ -4378,14 +4361,14 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="1">
         <f>AVERAGEIF('Dados Historicos x Categoria'!$C$4:$C$33,A4,'Dados Historicos x Categoria'!$H$4:$H$33)</f>
         <v>242</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E4" s="1">
         <v>175</v>
@@ -4393,14 +4376,14 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" s="1">
         <f>AVERAGEIF('Dados Historicos x Categoria'!$C$4:$C$33,A5,'Dados Historicos x Categoria'!$H$4:$H$33)</f>
         <v>103.6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E5" s="1">
         <v>169</v>
@@ -4408,9 +4391,9 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B6" s="79">
+        <v>141</v>
+      </c>
+      <c r="B6" s="76">
         <f>AVERAGEIF('Dados Historicos x Categoria'!$C$4:$C$33,A6,'Dados Historicos x Categoria'!$H$4:$H$33)</f>
         <v>148.57142857142858</v>
       </c>
@@ -4441,522 +4424,522 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="138" t="s">
+      <c r="C17" s="135" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="139"/>
-      <c r="E17" s="139"/>
-      <c r="F17" s="139"/>
-      <c r="G17" s="139"/>
+      <c r="D17" s="136"/>
+      <c r="E17" s="136"/>
+      <c r="F17" s="136"/>
+      <c r="G17" s="136"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="140"/>
-      <c r="D18" s="140"/>
-      <c r="E18" s="140"/>
-      <c r="F18" s="140"/>
-      <c r="G18" s="140"/>
+      <c r="C18" s="137"/>
+      <c r="D18" s="137"/>
+      <c r="E18" s="137"/>
+      <c r="F18" s="137"/>
+      <c r="G18" s="137"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="140"/>
-      <c r="D19" s="140"/>
-      <c r="E19" s="140"/>
-      <c r="F19" s="140"/>
-      <c r="G19" s="140"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="137"/>
+      <c r="E19" s="137"/>
+      <c r="F19" s="137"/>
+      <c r="G19" s="137"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="140"/>
-      <c r="D20" s="140"/>
-      <c r="E20" s="140"/>
-      <c r="F20" s="140"/>
-      <c r="G20" s="140"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="137"/>
+      <c r="E20" s="137"/>
+      <c r="F20" s="137"/>
+      <c r="G20" s="137"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="140"/>
-      <c r="D21" s="140"/>
-      <c r="E21" s="140"/>
-      <c r="F21" s="140"/>
-      <c r="G21" s="140"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="137"/>
+      <c r="E21" s="137"/>
+      <c r="F21" s="137"/>
+      <c r="G21" s="137"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="140"/>
-      <c r="D22" s="140"/>
-      <c r="E22" s="140"/>
-      <c r="F22" s="140"/>
-      <c r="G22" s="140"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="137"/>
+      <c r="E22" s="137"/>
+      <c r="F22" s="137"/>
+      <c r="G22" s="137"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="140"/>
-      <c r="D23" s="140"/>
-      <c r="E23" s="140"/>
-      <c r="F23" s="140"/>
-      <c r="G23" s="140"/>
+      <c r="C23" s="137"/>
+      <c r="D23" s="137"/>
+      <c r="E23" s="137"/>
+      <c r="F23" s="137"/>
+      <c r="G23" s="137"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="140"/>
-      <c r="D24" s="140"/>
-      <c r="E24" s="140"/>
-      <c r="F24" s="140"/>
-      <c r="G24" s="140"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="137"/>
+      <c r="E24" s="137"/>
+      <c r="F24" s="137"/>
+      <c r="G24" s="137"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="140"/>
-      <c r="D25" s="140"/>
-      <c r="E25" s="140"/>
-      <c r="F25" s="140"/>
-      <c r="G25" s="140"/>
+      <c r="C25" s="137"/>
+      <c r="D25" s="137"/>
+      <c r="E25" s="137"/>
+      <c r="F25" s="137"/>
+      <c r="G25" s="137"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="140"/>
-      <c r="D26" s="140"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="140"/>
-      <c r="G26" s="140"/>
+      <c r="C26" s="137"/>
+      <c r="D26" s="137"/>
+      <c r="E26" s="137"/>
+      <c r="F26" s="137"/>
+      <c r="G26" s="137"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="140"/>
-      <c r="D27" s="140"/>
-      <c r="E27" s="140"/>
-      <c r="F27" s="140"/>
-      <c r="G27" s="140"/>
+      <c r="C27" s="137"/>
+      <c r="D27" s="137"/>
+      <c r="E27" s="137"/>
+      <c r="F27" s="137"/>
+      <c r="G27" s="137"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="140"/>
-      <c r="D28" s="140"/>
-      <c r="E28" s="140"/>
-      <c r="F28" s="140"/>
-      <c r="G28" s="140"/>
+      <c r="C28" s="137"/>
+      <c r="D28" s="137"/>
+      <c r="E28" s="137"/>
+      <c r="F28" s="137"/>
+      <c r="G28" s="137"/>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="140"/>
-      <c r="D29" s="140"/>
-      <c r="E29" s="140"/>
-      <c r="F29" s="140"/>
-      <c r="G29" s="140"/>
+      <c r="C29" s="137"/>
+      <c r="D29" s="137"/>
+      <c r="E29" s="137"/>
+      <c r="F29" s="137"/>
+      <c r="G29" s="137"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="140"/>
-      <c r="D30" s="140"/>
-      <c r="E30" s="140"/>
-      <c r="F30" s="140"/>
-      <c r="G30" s="140"/>
+      <c r="C30" s="137"/>
+      <c r="D30" s="137"/>
+      <c r="E30" s="137"/>
+      <c r="F30" s="137"/>
+      <c r="G30" s="137"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="83" t="s">
+      <c r="A47" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="84" t="s">
+      <c r="B47" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="84" t="s">
+      <c r="C47" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="85" t="s">
+      <c r="D47" s="82" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="80" t="s">
+      <c r="A48" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="81">
+      <c r="B48" s="78">
         <v>42311</v>
       </c>
-      <c r="C48" s="81">
+      <c r="C48" s="78">
         <v>42446</v>
       </c>
-      <c r="D48" s="82">
+      <c r="D48" s="79">
         <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="80" t="s">
-        <v>129</v>
-      </c>
-      <c r="B49" s="81">
+      <c r="A49" s="77" t="s">
+        <v>128</v>
+      </c>
+      <c r="B49" s="78">
         <v>42118</v>
       </c>
-      <c r="C49" s="81">
+      <c r="C49" s="78">
         <v>42221</v>
       </c>
-      <c r="D49" s="82">
+      <c r="D49" s="79">
         <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="80" t="s">
-        <v>129</v>
-      </c>
-      <c r="B50" s="81">
+      <c r="A50" s="77" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="78">
         <v>42263</v>
       </c>
-      <c r="C50" s="81">
+      <c r="C50" s="78">
         <v>42342</v>
       </c>
-      <c r="D50" s="82">
+      <c r="D50" s="79">
         <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="80" t="s">
-        <v>129</v>
-      </c>
-      <c r="B51" s="81">
+      <c r="A51" s="77" t="s">
+        <v>128</v>
+      </c>
+      <c r="B51" s="78">
         <v>42633</v>
       </c>
-      <c r="C51" s="81">
+      <c r="C51" s="78">
         <v>42695</v>
       </c>
-      <c r="D51" s="82">
+      <c r="D51" s="79">
         <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="80" t="s">
-        <v>129</v>
-      </c>
-      <c r="B52" s="81">
+      <c r="A52" s="77" t="s">
+        <v>128</v>
+      </c>
+      <c r="B52" s="78">
         <v>42422</v>
       </c>
-      <c r="C52" s="81">
+      <c r="C52" s="78">
         <v>42643</v>
       </c>
-      <c r="D52" s="82">
+      <c r="D52" s="79">
         <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="80" t="s">
-        <v>129</v>
-      </c>
-      <c r="B53" s="81">
+      <c r="A53" s="77" t="s">
+        <v>128</v>
+      </c>
+      <c r="B53" s="78">
         <v>41955</v>
       </c>
-      <c r="C53" s="81">
+      <c r="C53" s="78">
         <v>42179</v>
       </c>
-      <c r="D53" s="82">
+      <c r="D53" s="79">
         <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="80" t="s">
-        <v>129</v>
-      </c>
-      <c r="B54" s="81">
+      <c r="A54" s="77" t="s">
+        <v>128</v>
+      </c>
+      <c r="B54" s="78">
         <v>41738</v>
       </c>
-      <c r="C54" s="81">
+      <c r="C54" s="78">
         <v>41850</v>
       </c>
-      <c r="D54" s="82">
+      <c r="D54" s="79">
         <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="80" t="s">
+      <c r="A55" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="B55" s="81">
+      <c r="B55" s="78">
         <v>41337</v>
       </c>
-      <c r="C55" s="81">
+      <c r="C55" s="78">
         <v>41430</v>
       </c>
-      <c r="D55" s="82">
+      <c r="D55" s="79">
         <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="80" t="s">
+      <c r="A56" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="B56" s="81">
+      <c r="B56" s="78">
         <v>42209</v>
       </c>
-      <c r="C56" s="81">
+      <c r="C56" s="78">
         <v>42683</v>
       </c>
-      <c r="D56" s="82">
+      <c r="D56" s="79">
         <v>465</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="80" t="s">
+      <c r="A57" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="B57" s="81">
+      <c r="B57" s="78">
         <v>42020</v>
       </c>
-      <c r="C57" s="81">
+      <c r="C57" s="78">
         <v>42671</v>
       </c>
-      <c r="D57" s="82">
+      <c r="D57" s="79">
         <v>642</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="80" t="s">
+      <c r="A58" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="B58" s="81">
+      <c r="B58" s="78">
         <v>42439</v>
       </c>
-      <c r="C58" s="81">
+      <c r="C58" s="78">
         <v>42668</v>
       </c>
-      <c r="D58" s="82">
+      <c r="D58" s="79">
         <v>225</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="80" t="s">
+      <c r="A59" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="B59" s="81">
+      <c r="B59" s="78">
         <v>42521</v>
       </c>
-      <c r="C59" s="81">
+      <c r="C59" s="78">
         <v>42661</v>
       </c>
-      <c r="D59" s="82">
+      <c r="D59" s="79">
         <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="80" t="s">
+      <c r="A60" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="81">
+      <c r="B60" s="78">
         <v>41242</v>
       </c>
-      <c r="C60" s="81">
+      <c r="C60" s="78">
         <v>41472</v>
       </c>
-      <c r="D60" s="82">
+      <c r="D60" s="79">
         <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="80" t="s">
+      <c r="A61" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="B61" s="81">
+      <c r="B61" s="78">
         <v>41698</v>
       </c>
-      <c r="C61" s="81">
+      <c r="C61" s="78">
         <v>41932</v>
       </c>
-      <c r="D61" s="82">
+      <c r="D61" s="79">
         <v>230</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="80" t="s">
+      <c r="A62" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="B62" s="81">
+      <c r="B62" s="78">
         <v>42277</v>
       </c>
-      <c r="C62" s="81">
+      <c r="C62" s="78">
         <v>42681</v>
       </c>
-      <c r="D62" s="82">
+      <c r="D62" s="79">
         <v>397</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="80" t="s">
+      <c r="A63" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="B63" s="81">
+      <c r="B63" s="78">
         <v>42136</v>
       </c>
-      <c r="C63" s="81">
+      <c r="C63" s="78">
         <v>42171</v>
       </c>
-      <c r="D63" s="82">
+      <c r="D63" s="79">
         <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="80" t="s">
+      <c r="A64" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="B64" s="81">
+      <c r="B64" s="78">
         <v>41541</v>
       </c>
-      <c r="C64" s="81">
+      <c r="C64" s="78">
         <v>41634</v>
       </c>
-      <c r="D64" s="82">
+      <c r="D64" s="79">
         <v>92</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="80" t="s">
+      <c r="A65" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="B65" s="81">
+      <c r="B65" s="78">
         <v>41575</v>
       </c>
-      <c r="C65" s="81">
+      <c r="C65" s="78">
         <v>41638</v>
       </c>
-      <c r="D65" s="82">
+      <c r="D65" s="79">
         <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="80" t="s">
+      <c r="A66" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="B66" s="81">
+      <c r="B66" s="78">
         <v>42580</v>
       </c>
-      <c r="C66" s="81">
+      <c r="C66" s="78">
         <v>42641</v>
       </c>
-      <c r="D66" s="82">
+      <c r="D66" s="79">
         <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="80" t="s">
-        <v>140</v>
-      </c>
-      <c r="B67" s="81">
+      <c r="A67" s="77" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="78">
         <v>42612</v>
       </c>
-      <c r="C67" s="81">
+      <c r="C67" s="78">
         <v>42704</v>
       </c>
-      <c r="D67" s="82">
+      <c r="D67" s="79">
         <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="80" t="s">
-        <v>143</v>
-      </c>
-      <c r="B68" s="81">
+      <c r="A68" s="77" t="s">
+        <v>142</v>
+      </c>
+      <c r="B68" s="78">
         <v>42068</v>
       </c>
-      <c r="C68" s="81">
+      <c r="C68" s="78">
         <v>42149</v>
       </c>
-      <c r="D68" s="82">
+      <c r="D68" s="79">
         <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="80" t="s">
-        <v>146</v>
-      </c>
-      <c r="B69" s="81">
+      <c r="A69" s="77" t="s">
+        <v>145</v>
+      </c>
+      <c r="B69" s="78">
         <v>42410</v>
       </c>
-      <c r="C69" s="81">
+      <c r="C69" s="78">
         <v>42690</v>
       </c>
-      <c r="D69" s="82">
+      <c r="D69" s="79">
         <v>276</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="80" t="s">
-        <v>149</v>
-      </c>
-      <c r="B70" s="81">
+      <c r="A70" s="77" t="s">
+        <v>148</v>
+      </c>
+      <c r="B70" s="78">
         <v>41208</v>
       </c>
-      <c r="C70" s="81">
+      <c r="C70" s="78">
         <v>41348</v>
       </c>
-      <c r="D70" s="82">
+      <c r="D70" s="79">
         <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="80" t="s">
-        <v>151</v>
-      </c>
-      <c r="B71" s="81">
+      <c r="A71" s="77" t="s">
+        <v>150</v>
+      </c>
+      <c r="B71" s="78">
         <v>40927</v>
       </c>
-      <c r="C71" s="81">
+      <c r="C71" s="78">
         <v>41012</v>
       </c>
-      <c r="D71" s="82">
+      <c r="D71" s="79">
         <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="80" t="s">
-        <v>143</v>
-      </c>
-      <c r="B72" s="81">
+      <c r="A72" s="77" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="78">
         <v>41885</v>
       </c>
-      <c r="C72" s="81">
+      <c r="C72" s="78">
         <v>41996</v>
       </c>
-      <c r="D72" s="82">
+      <c r="D72" s="79">
         <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="80" t="s">
-        <v>165</v>
-      </c>
-      <c r="B73" s="81">
+      <c r="A73" s="77" t="s">
+        <v>164</v>
+      </c>
+      <c r="B73" s="78">
         <v>40945</v>
       </c>
-      <c r="C73" s="81">
+      <c r="C73" s="78">
         <v>41093</v>
       </c>
-      <c r="D73" s="82">
+      <c r="D73" s="79">
         <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="80" t="s">
-        <v>160</v>
-      </c>
-      <c r="B74" s="81">
+      <c r="A74" s="77" t="s">
+        <v>159</v>
+      </c>
+      <c r="B74" s="78">
         <v>41411</v>
       </c>
-      <c r="C74" s="81">
+      <c r="C74" s="78">
         <v>41666</v>
       </c>
-      <c r="D74" s="82">
+      <c r="D74" s="79">
         <v>250</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="80" t="s">
-        <v>163</v>
-      </c>
-      <c r="B75" s="81">
+      <c r="A75" s="77" t="s">
+        <v>162</v>
+      </c>
+      <c r="B75" s="78">
         <v>41905</v>
       </c>
-      <c r="C75" s="81">
+      <c r="C75" s="78">
         <v>41999</v>
       </c>
-      <c r="D75" s="82">
+      <c r="D75" s="79">
         <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="80" t="s">
+      <c r="A76" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="B76" s="81">
+      <c r="B76" s="78">
         <v>42229</v>
       </c>
-      <c r="C76" s="81">
+      <c r="C76" s="78">
         <v>42354</v>
       </c>
-      <c r="D76" s="82">
+      <c r="D76" s="79">
         <v>123</v>
       </c>
     </row>
@@ -5189,8 +5172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5240,7 +5223,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="45" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="141">
+      <c r="A2" s="138">
         <v>1</v>
       </c>
       <c r="B2" s="143" t="s">
@@ -5270,7 +5253,7 @@
       <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="142"/>
+      <c r="A3" s="139"/>
       <c r="B3" s="143"/>
       <c r="C3" s="143"/>
       <c r="D3" s="143"/>
@@ -5293,7 +5276,7 @@
       <c r="A4" s="143">
         <v>2</v>
       </c>
-      <c r="B4" s="150">
+      <c r="B4" s="144">
         <v>43042</v>
       </c>
       <c r="C4" s="143" t="s">
@@ -5302,7 +5285,7 @@
       <c r="D4" s="143" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="141">
+      <c r="E4" s="138">
         <v>2</v>
       </c>
       <c r="F4" s="31" t="s">
@@ -5320,11 +5303,11 @@
       <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="141"/>
-      <c r="B5" s="141"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="141"/>
-      <c r="E5" s="142"/>
+      <c r="A5" s="138"/>
+      <c r="B5" s="138"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="139"/>
       <c r="F5" s="37" t="s">
         <v>54</v>
       </c>
@@ -5343,16 +5326,16 @@
       <c r="A6" s="143">
         <v>3</v>
       </c>
-      <c r="B6" s="149">
+      <c r="B6" s="141">
         <v>42683</v>
       </c>
-      <c r="C6" s="141" t="s">
+      <c r="C6" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="141" t="s">
+      <c r="D6" s="138" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="141">
+      <c r="E6" s="138">
         <v>2</v>
       </c>
       <c r="F6" s="31" t="s">
@@ -5371,10 +5354,10 @@
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="143"/>
-      <c r="B7" s="142"/>
-      <c r="C7" s="142"/>
-      <c r="D7" s="142"/>
-      <c r="E7" s="142"/>
+      <c r="B7" s="139"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
       <c r="F7" s="55" t="s">
         <v>67</v>
       </c>
@@ -5391,10 +5374,10 @@
     </row>
     <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="143"/>
-      <c r="B8" s="142"/>
-      <c r="C8" s="142"/>
-      <c r="D8" s="142"/>
-      <c r="E8" s="142"/>
+      <c r="B8" s="139"/>
+      <c r="C8" s="139"/>
+      <c r="D8" s="139"/>
+      <c r="E8" s="139"/>
       <c r="F8" s="53" t="s">
         <v>69</v>
       </c>
@@ -5411,10 +5394,10 @@
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="143"/>
-      <c r="B9" s="142"/>
-      <c r="C9" s="142"/>
-      <c r="D9" s="142"/>
-      <c r="E9" s="142"/>
+      <c r="B9" s="139"/>
+      <c r="C9" s="139"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="139"/>
       <c r="F9" s="53" t="s">
         <v>73</v>
       </c>
@@ -5431,10 +5414,10 @@
     </row>
     <row r="10" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="143"/>
-      <c r="B10" s="148"/>
-      <c r="C10" s="148"/>
-      <c r="D10" s="148"/>
-      <c r="E10" s="148"/>
+      <c r="B10" s="140"/>
+      <c r="C10" s="140"/>
+      <c r="D10" s="140"/>
+      <c r="E10" s="140"/>
       <c r="F10" s="31" t="s">
         <v>70</v>
       </c>
@@ -5448,7 +5431,7 @@
         <v>57</v>
       </c>
       <c r="J10" s="59" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -5459,10 +5442,10 @@
         <v>48</v>
       </c>
       <c r="C11" s="143" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="143" t="s">
         <v>115</v>
-      </c>
-      <c r="D11" s="143" t="s">
-        <v>116</v>
       </c>
       <c r="E11" s="143">
         <v>2</v>
@@ -5502,11 +5485,11 @@
       <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="141"/>
-      <c r="B13" s="141"/>
-      <c r="C13" s="141"/>
-      <c r="D13" s="141"/>
-      <c r="E13" s="141"/>
+      <c r="A13" s="138"/>
+      <c r="B13" s="138"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="138"/>
+      <c r="E13" s="138"/>
       <c r="F13" s="70" t="s">
         <v>72</v>
       </c>
@@ -5516,67 +5499,67 @@
       <c r="H13" s="68">
         <v>42690</v>
       </c>
-      <c r="I13" s="73" t="s">
-        <v>51</v>
+      <c r="I13" s="154" t="s">
+        <v>57</v>
       </c>
       <c r="J13" s="66"/>
     </row>
     <row r="14" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="141">
+      <c r="A14" s="138">
         <v>5</v>
       </c>
-      <c r="B14" s="149">
+      <c r="B14" s="141">
         <v>42705</v>
       </c>
-      <c r="C14" s="141"/>
-      <c r="D14" s="141" t="s">
-        <v>116</v>
-      </c>
-      <c r="E14" s="141">
+      <c r="C14" s="138"/>
+      <c r="D14" s="138" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="138">
         <v>2</v>
       </c>
       <c r="F14" s="71" t="s">
+        <v>118</v>
+      </c>
+      <c r="G14" s="71" t="s">
         <v>119</v>
-      </c>
-      <c r="G14" s="71" t="s">
-        <v>120</v>
       </c>
       <c r="H14" s="72">
         <v>42705</v>
       </c>
-      <c r="I14" s="74" t="s">
-        <v>51</v>
+      <c r="I14" s="73" t="s">
+        <v>57</v>
       </c>
       <c r="J14" s="67"/>
     </row>
     <row r="15" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="142"/>
-      <c r="B15" s="151"/>
-      <c r="C15" s="142"/>
-      <c r="D15" s="142"/>
-      <c r="E15" s="142"/>
+      <c r="A15" s="139"/>
+      <c r="B15" s="142"/>
+      <c r="C15" s="139"/>
+      <c r="D15" s="139"/>
+      <c r="E15" s="139"/>
       <c r="F15" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="G15" s="71" t="s">
         <v>121</v>
-      </c>
-      <c r="G15" s="71" t="s">
-        <v>122</v>
       </c>
       <c r="H15" s="72">
         <v>42705</v>
       </c>
-      <c r="I15" s="75" t="s">
-        <v>110</v>
+      <c r="I15" s="73" t="s">
+        <v>57</v>
       </c>
       <c r="J15" s="67"/>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="142"/>
-      <c r="B16" s="151"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="148"/>
-      <c r="E16" s="142"/>
+      <c r="A16" s="139"/>
+      <c r="B16" s="142"/>
+      <c r="C16" s="139"/>
+      <c r="D16" s="140"/>
+      <c r="E16" s="139"/>
       <c r="F16" s="71" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G16" s="71" t="s">
         <v>49</v>
@@ -5584,43 +5567,43 @@
       <c r="H16" s="72">
         <v>42705</v>
       </c>
-      <c r="I16" s="74" t="s">
+      <c r="I16" s="73" t="s">
         <v>51</v>
       </c>
       <c r="J16" s="67"/>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="142"/>
-      <c r="B17" s="151"/>
-      <c r="C17" s="142"/>
+      <c r="A17" s="139"/>
+      <c r="B17" s="142"/>
+      <c r="C17" s="139"/>
       <c r="D17" s="67" t="s">
-        <v>117</v>
-      </c>
-      <c r="E17" s="142"/>
+        <v>116</v>
+      </c>
+      <c r="E17" s="139"/>
       <c r="F17" s="71" t="s">
+        <v>123</v>
+      </c>
+      <c r="G17" s="71" t="s">
         <v>124</v>
-      </c>
-      <c r="G17" s="71" t="s">
-        <v>125</v>
       </c>
       <c r="H17" s="72">
         <v>42705</v>
       </c>
-      <c r="I17" s="74" t="s">
+      <c r="I17" s="73" t="s">
         <v>51</v>
       </c>
       <c r="J17" s="67"/>
     </row>
     <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="142"/>
-      <c r="B18" s="151"/>
-      <c r="C18" s="142"/>
-      <c r="D18" s="141" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18" s="142"/>
+      <c r="A18" s="139"/>
+      <c r="B18" s="142"/>
+      <c r="C18" s="139"/>
+      <c r="D18" s="138" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="139"/>
       <c r="F18" s="71" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G18" s="71" t="s">
         <v>49</v>
@@ -5628,107 +5611,150 @@
       <c r="H18" s="72">
         <v>42705</v>
       </c>
-      <c r="I18" s="76" t="s">
+      <c r="I18" s="73" t="s">
         <v>57</v>
       </c>
       <c r="J18" s="67"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="148"/>
-      <c r="B19" s="152"/>
-      <c r="C19" s="148"/>
-      <c r="D19" s="148"/>
-      <c r="E19" s="148"/>
+      <c r="A19" s="139"/>
+      <c r="B19" s="142"/>
+      <c r="C19" s="139"/>
+      <c r="D19" s="139"/>
+      <c r="E19" s="139"/>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="47">
+      <c r="A20" s="143">
         <v>6</v>
       </c>
       <c r="B20" s="144">
         <v>42773</v>
       </c>
-      <c r="D20" s="146" t="s">
+      <c r="C20" s="143"/>
+      <c r="D20" s="143" t="s">
+        <v>179</v>
+      </c>
+      <c r="E20" s="143">
+        <v>2</v>
+      </c>
+      <c r="F20" s="129" t="s">
+        <v>174</v>
+      </c>
+      <c r="G20" s="129"/>
+      <c r="H20" s="129"/>
+      <c r="I20" s="73" t="s">
+        <v>57</v>
+      </c>
+      <c r="J20" s="129"/>
+    </row>
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="143"/>
+      <c r="B21" s="144"/>
+      <c r="C21" s="143"/>
+      <c r="D21" s="143"/>
+      <c r="E21" s="143"/>
+      <c r="F21" s="129" t="s">
+        <v>175</v>
+      </c>
+      <c r="G21" s="129" t="s">
+        <v>176</v>
+      </c>
+      <c r="H21" s="129"/>
+      <c r="I21" s="73" t="s">
+        <v>57</v>
+      </c>
+      <c r="J21" s="129"/>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="143"/>
+      <c r="B22" s="144"/>
+      <c r="C22" s="143"/>
+      <c r="D22" s="143"/>
+      <c r="E22" s="143"/>
+      <c r="F22" s="129" t="s">
+        <v>177</v>
+      </c>
+      <c r="G22" s="129" t="s">
+        <v>178</v>
+      </c>
+      <c r="H22" s="129"/>
+      <c r="I22" s="73" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22" s="129"/>
+    </row>
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="143"/>
+      <c r="B23" s="144"/>
+      <c r="C23" s="143"/>
+      <c r="D23" s="143"/>
+      <c r="E23" s="143"/>
+      <c r="F23" s="129" t="s">
         <v>180</v>
       </c>
-      <c r="F20" s="47" t="s">
-        <v>175</v>
-      </c>
-      <c r="I20" s="47" t="s">
+      <c r="G23" s="129" t="s">
+        <v>192</v>
+      </c>
+      <c r="H23" s="129"/>
+      <c r="I23" s="153" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" s="129"/>
+    </row>
+    <row r="24" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+      <c r="A24" s="129">
+        <v>7</v>
+      </c>
+      <c r="B24" s="130">
+        <v>42809</v>
+      </c>
+      <c r="C24" s="129" t="s">
+        <v>195</v>
+      </c>
+      <c r="D24" s="129" t="s">
+        <v>194</v>
+      </c>
+      <c r="E24" s="129">
+        <v>2</v>
+      </c>
+      <c r="F24" s="152" t="s">
+        <v>191</v>
+      </c>
+      <c r="G24" s="129" t="s">
+        <v>192</v>
+      </c>
+      <c r="H24" s="129" t="s">
+        <v>193</v>
+      </c>
+      <c r="I24" s="58" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="145"/>
-      <c r="D21" s="147"/>
-      <c r="F21" s="47" t="s">
-        <v>176</v>
-      </c>
-      <c r="G21" s="47" t="s">
-        <v>177</v>
-      </c>
-      <c r="I21" s="47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="145"/>
-      <c r="D22" s="147"/>
-      <c r="F22" s="47" t="s">
-        <v>178</v>
-      </c>
-      <c r="G22" s="47" t="s">
-        <v>179</v>
-      </c>
-      <c r="I22" s="47" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B23" s="145"/>
-      <c r="D23" s="147"/>
-      <c r="F23" s="47" t="s">
-        <v>181</v>
-      </c>
-      <c r="G23" s="47" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="315" x14ac:dyDescent="0.25">
-      <c r="B24" s="131">
-        <v>42809</v>
-      </c>
-      <c r="F24" s="133" t="s">
-        <v>192</v>
-      </c>
-      <c r="G24" s="47" t="s">
-        <v>193</v>
-      </c>
-      <c r="H24" s="47" t="s">
-        <v>194</v>
-      </c>
-      <c r="I24" s="47" t="s">
-        <v>51</v>
-      </c>
+      <c r="J24" s="129"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F25" s="130"/>
+      <c r="F25" s="127"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F26" s="130"/>
+      <c r="F26" s="127"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F27" s="130"/>
+      <c r="F27" s="127"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F28"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C14:C19"/>
+  <mergeCells count="31">
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="D20:D23"/>
     <mergeCell ref="A14:A19"/>
@@ -5745,13 +5771,11 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="C11:C13"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C14:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5854,7 +5878,7 @@
         <v>76</v>
       </c>
       <c r="B5" s="69" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="46" t="s">
         <v>77</v>
@@ -5900,7 +5924,7 @@
         <v>85</v>
       </c>
       <c r="B7" s="61" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>86</v>
@@ -5939,20 +5963,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="145" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="155" t="s">
+      <c r="B1" s="147" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="157" t="s">
+      <c r="C1" s="149" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158" t="s">
+      <c r="D1" s="150"/>
+      <c r="E1" s="150" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="159"/>
+      <c r="F1" s="151"/>
       <c r="G1" s="15" t="s">
         <v>35</v>
       </c>
@@ -5972,8 +5996,8 @@
       <c r="U1" s="16"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="154"/>
-      <c r="B2" s="156"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="148"/>
       <c r="C2" s="17" t="s">
         <v>36</v>
       </c>
@@ -5987,13 +6011,13 @@
         <v>37</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H2" s="20">
         <v>42675</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J2" s="20">
         <v>42736</v>
@@ -6005,31 +6029,31 @@
         <v>42795</v>
       </c>
       <c r="M2" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="N2" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="N2" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="O2" s="92">
+      <c r="O2" s="89">
         <v>42887</v>
       </c>
       <c r="P2" s="20">
         <v>42917</v>
       </c>
       <c r="Q2" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="S2" s="20" t="s">
         <v>171</v>
-      </c>
-      <c r="R2" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="S2" s="20" t="s">
-        <v>172</v>
       </c>
       <c r="T2" s="20">
         <v>43040</v>
       </c>
-      <c r="U2" s="92" t="s">
-        <v>174</v>
+      <c r="U2" s="89" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -6059,48 +6083,48 @@
       <c r="L3" s="25"/>
       <c r="M3" s="25"/>
       <c r="N3" s="25"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="77"/>
-      <c r="S3" s="77"/>
-      <c r="T3" s="77"/>
-      <c r="U3" s="97"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="74"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="94"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="86">
+      <c r="A4" s="83">
         <v>2</v>
       </c>
-      <c r="B4" s="87" t="s">
-        <v>166</v>
-      </c>
-      <c r="C4" s="88">
+      <c r="B4" s="84" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="85">
         <v>42670</v>
       </c>
-      <c r="D4" s="89">
+      <c r="D4" s="86">
         <v>42794</v>
       </c>
-      <c r="E4" s="89">
+      <c r="E4" s="86">
         <v>42670</v>
       </c>
-      <c r="F4" s="90">
+      <c r="F4" s="87">
         <v>42794</v>
       </c>
-      <c r="G4" s="86"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="94"/>
-      <c r="P4" s="77"/>
-      <c r="Q4" s="77"/>
-      <c r="R4" s="77"/>
-      <c r="S4" s="77"/>
-      <c r="T4" s="77"/>
-      <c r="U4" s="97"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="75"/>
+      <c r="M4" s="75"/>
+      <c r="N4" s="75"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="94"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
@@ -6121,13 +6145,13 @@
       <c r="L5" s="31"/>
       <c r="M5" s="31"/>
       <c r="N5" s="31"/>
-      <c r="O5" s="95"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="77"/>
-      <c r="S5" s="77"/>
-      <c r="T5" s="77"/>
-      <c r="U5" s="97"/>
+      <c r="O5" s="92"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="74"/>
+      <c r="R5" s="74"/>
+      <c r="S5" s="74"/>
+      <c r="T5" s="74"/>
+      <c r="U5" s="94"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="26">
@@ -6148,13 +6172,13 @@
       <c r="L6" s="31"/>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
-      <c r="O6" s="95"/>
-      <c r="P6" s="77"/>
-      <c r="Q6" s="77"/>
-      <c r="R6" s="77"/>
-      <c r="S6" s="77"/>
-      <c r="T6" s="77"/>
-      <c r="U6" s="97"/>
+      <c r="O6" s="92"/>
+      <c r="P6" s="74"/>
+      <c r="Q6" s="74"/>
+      <c r="R6" s="74"/>
+      <c r="S6" s="74"/>
+      <c r="T6" s="74"/>
+      <c r="U6" s="94"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="26">
@@ -6175,13 +6199,13 @@
       <c r="L7" s="31"/>
       <c r="M7" s="31"/>
       <c r="N7" s="31"/>
-      <c r="O7" s="95"/>
-      <c r="P7" s="77"/>
-      <c r="Q7" s="77"/>
-      <c r="R7" s="77"/>
-      <c r="S7" s="77"/>
-      <c r="T7" s="77"/>
-      <c r="U7" s="97"/>
+      <c r="O7" s="92"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="94"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
@@ -6202,13 +6226,13 @@
       <c r="L8" s="31"/>
       <c r="M8" s="31"/>
       <c r="N8" s="31"/>
-      <c r="O8" s="95"/>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="77"/>
-      <c r="R8" s="77"/>
-      <c r="S8" s="77"/>
-      <c r="T8" s="77"/>
-      <c r="U8" s="97"/>
+      <c r="O8" s="92"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="74"/>
+      <c r="T8" s="74"/>
+      <c r="U8" s="94"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="26">
@@ -6229,13 +6253,13 @@
       <c r="L9" s="31"/>
       <c r="M9" s="31"/>
       <c r="N9" s="31"/>
-      <c r="O9" s="95"/>
-      <c r="P9" s="77"/>
-      <c r="Q9" s="77"/>
-      <c r="R9" s="77"/>
-      <c r="S9" s="77"/>
-      <c r="T9" s="77"/>
-      <c r="U9" s="97"/>
+      <c r="O9" s="92"/>
+      <c r="P9" s="74"/>
+      <c r="Q9" s="74"/>
+      <c r="R9" s="74"/>
+      <c r="S9" s="74"/>
+      <c r="T9" s="74"/>
+      <c r="U9" s="94"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
@@ -6254,13 +6278,13 @@
       <c r="L10" s="31"/>
       <c r="M10" s="31"/>
       <c r="N10" s="31"/>
-      <c r="O10" s="95"/>
-      <c r="P10" s="77"/>
-      <c r="Q10" s="77"/>
-      <c r="R10" s="77"/>
-      <c r="S10" s="77"/>
-      <c r="T10" s="77"/>
-      <c r="U10" s="97"/>
+      <c r="O10" s="92"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="74"/>
+      <c r="S10" s="74"/>
+      <c r="T10" s="74"/>
+      <c r="U10" s="94"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="26">
@@ -6279,13 +6303,13 @@
       <c r="L11" s="31"/>
       <c r="M11" s="31"/>
       <c r="N11" s="31"/>
-      <c r="O11" s="95"/>
-      <c r="P11" s="77"/>
-      <c r="Q11" s="77"/>
-      <c r="R11" s="77"/>
-      <c r="S11" s="77"/>
-      <c r="T11" s="77"/>
-      <c r="U11" s="97"/>
+      <c r="O11" s="92"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
+      <c r="R11" s="74"/>
+      <c r="S11" s="74"/>
+      <c r="T11" s="74"/>
+      <c r="U11" s="94"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
@@ -6304,13 +6328,13 @@
       <c r="L12" s="31"/>
       <c r="M12" s="31"/>
       <c r="N12" s="31"/>
-      <c r="O12" s="95"/>
-      <c r="P12" s="77"/>
-      <c r="Q12" s="77"/>
-      <c r="R12" s="77"/>
-      <c r="S12" s="77"/>
-      <c r="T12" s="77"/>
-      <c r="U12" s="97"/>
+      <c r="O12" s="92"/>
+      <c r="P12" s="74"/>
+      <c r="Q12" s="74"/>
+      <c r="R12" s="74"/>
+      <c r="S12" s="74"/>
+      <c r="T12" s="74"/>
+      <c r="U12" s="94"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="26">
@@ -6329,13 +6353,13 @@
       <c r="L13" s="31"/>
       <c r="M13" s="31"/>
       <c r="N13" s="31"/>
-      <c r="O13" s="95"/>
-      <c r="P13" s="77"/>
-      <c r="Q13" s="77"/>
-      <c r="R13" s="77"/>
-      <c r="S13" s="77"/>
-      <c r="T13" s="77"/>
-      <c r="U13" s="97"/>
+      <c r="O13" s="92"/>
+      <c r="P13" s="74"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="74"/>
+      <c r="S13" s="74"/>
+      <c r="T13" s="74"/>
+      <c r="U13" s="94"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
@@ -6354,13 +6378,13 @@
       <c r="L14" s="31"/>
       <c r="M14" s="31"/>
       <c r="N14" s="31"/>
-      <c r="O14" s="95"/>
-      <c r="P14" s="77"/>
-      <c r="Q14" s="77"/>
-      <c r="R14" s="77"/>
-      <c r="S14" s="77"/>
-      <c r="T14" s="77"/>
-      <c r="U14" s="97"/>
+      <c r="O14" s="92"/>
+      <c r="P14" s="74"/>
+      <c r="Q14" s="74"/>
+      <c r="R14" s="74"/>
+      <c r="S14" s="74"/>
+      <c r="T14" s="74"/>
+      <c r="U14" s="94"/>
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26">
@@ -6379,13 +6403,13 @@
       <c r="L15" s="37"/>
       <c r="M15" s="37"/>
       <c r="N15" s="37"/>
-      <c r="O15" s="96"/>
-      <c r="P15" s="77"/>
-      <c r="Q15" s="77"/>
-      <c r="R15" s="77"/>
-      <c r="S15" s="77"/>
-      <c r="T15" s="77"/>
-      <c r="U15" s="97"/>
+      <c r="O15" s="93"/>
+      <c r="P15" s="74"/>
+      <c r="Q15" s="74"/>
+      <c r="R15" s="74"/>
+      <c r="S15" s="74"/>
+      <c r="T15" s="74"/>
+      <c r="U15" s="94"/>
     </row>
     <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="38"/>
@@ -6413,12 +6437,12 @@
       <c r="M16" s="43"/>
       <c r="N16" s="43"/>
       <c r="O16" s="44"/>
-      <c r="P16" s="91"/>
-      <c r="Q16" s="91"/>
-      <c r="R16" s="91"/>
-      <c r="S16" s="91"/>
-      <c r="T16" s="91"/>
-      <c r="U16" s="91"/>
+      <c r="P16" s="88"/>
+      <c r="Q16" s="88"/>
+      <c r="R16" s="88"/>
+      <c r="S16" s="88"/>
+      <c r="T16" s="88"/>
+      <c r="U16" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6447,17 +6471,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>